<commit_message>
Include command code in V2 result to align with request formation
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="149">
   <si>
     <t>Offset</t>
   </si>
@@ -334,21 +334,12 @@
     <t>A9 9A 06 31 01 00 02 01 3B ED</t>
   </si>
   <si>
-    <t>Read action header</t>
-  </si>
-  <si>
     <t>A9 9A 03 61 01 65 ED</t>
   </si>
   <si>
-    <t>Read action detail</t>
-  </si>
-  <si>
     <t>A9 9A 03 62 01 66 ED</t>
   </si>
   <si>
-    <t>Read action pose</t>
-  </si>
-  <si>
     <t>Yes {4}</t>
   </si>
   <si>
@@ -419,24 +410,12 @@
   </si>
   <si>
     <t>Action Header</t>
-  </si>
-  <si>
-    <t>{cmd}{success}</t>
-  </si>
-  <si>
-    <t>Yes {10}</t>
   </si>
   <si>
     <t>5 bytes of command enable flag
 {V1, V2, BT, CB, SV}</t>
   </si>
   <si>
-    <t>Yes {37}</t>
-  </si>
-  <si>
-    <t>Yes {8}</t>
-  </si>
-  <si>
     <t>&lt;id, anlge, lock&gt;</t>
   </si>
   <si>
@@ -450,6 +429,42 @@
   </si>
   <si>
     <t>{cnt} + ({id},{angle},{time})</t>
+  </si>
+  <si>
+    <t>Get action header</t>
+  </si>
+  <si>
+    <t>Get action detail</t>
+  </si>
+  <si>
+    <t>Get action pose</t>
+  </si>
+  <si>
+    <t>Yes {11}</t>
+  </si>
+  <si>
+    <t>0x61</t>
+  </si>
+  <si>
+    <t>Reserved (command code get header)</t>
+  </si>
+  <si>
+    <t>Yes {38}</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Yes {9}</t>
+  </si>
+  <si>
+    <t>Yes {7}</t>
+  </si>
+  <si>
+    <t>Yes {1}</t>
+  </si>
+  <si>
+    <t>{success}</t>
   </si>
 </sst>
 </file>
@@ -483,7 +498,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,12 +508,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -530,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -556,56 +565,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -911,7 +917,7 @@
   <dimension ref="A2:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +930,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>38</v>
       </c>
     </row>
@@ -946,7 +952,7 @@
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="24" t="s">
         <v>3</v>
       </c>
     </row>
@@ -957,7 +963,7 @@
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="24"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -966,7 +972,7 @@
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -975,10 +981,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>6</v>
+        <v>141</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -988,7 +994,7 @@
       <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -999,7 +1005,7 @@
       <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1010,7 +1016,7 @@
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1021,7 +1027,7 @@
       <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1032,7 +1038,7 @@
       <c r="C13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1043,7 +1049,7 @@
       <c r="C14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1054,7 +1060,7 @@
       <c r="C15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1065,7 +1071,7 @@
       <c r="C16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1076,7 +1082,7 @@
       <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1087,7 +1093,7 @@
       <c r="C18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1098,7 +1104,7 @@
       <c r="C19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1109,7 +1115,7 @@
       <c r="C20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1120,12 +1126,12 @@
       <c r="C21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1147,7 +1153,7 @@
       <c r="C26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1158,7 +1164,7 @@
       <c r="C27" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="8" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1169,7 +1175,7 @@
       <c r="C28" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="8" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1180,7 +1186,7 @@
       <c r="C29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="8" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1191,7 +1197,7 @@
       <c r="C30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="8" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1202,7 +1208,7 @@
       <c r="C31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1213,19 +1219,19 @@
       <c r="C32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="11"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="13"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="12"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="11"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="13"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1241,10 +1247,10 @@
   <dimension ref="B2:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
+      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1259,7 @@
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="31" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" style="17" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="13.85546875" style="1" customWidth="1"/>
@@ -1277,9 +1283,9 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="G3" s="15"/>
-      <c r="K3" s="16"/>
+      <c r="E3" s="18"/>
+      <c r="G3" s="14"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -1288,11 +1294,11 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
+      <c r="E4" s="18"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
@@ -1301,11 +1307,11 @@
       <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
+      <c r="E5" s="18"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
@@ -1314,15 +1320,15 @@
       <c r="C6" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
+      <c r="E6" s="18"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -1331,7 +1337,7 @@
       <c r="C7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="19"/>
+      <c r="E7" s="18"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -1340,7 +1346,7 @@
       <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="19"/>
+      <c r="E8" s="18"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -1349,7 +1355,7 @@
       <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="19"/>
+      <c r="E9" s="18"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
@@ -1361,7 +1367,7 @@
       <c r="D12" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F12" s="7" t="s">
@@ -1374,10 +1380,10 @@
         <v>79</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
@@ -1387,21 +1393,21 @@
       <c r="C13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="20" t="s">
         <v>68</v>
       </c>
       <c r="G13" s="4"/>
       <c r="I13" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>67</v>
@@ -1417,20 +1423,20 @@
       <c r="D14" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="19" t="s">
         <v>73</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>70</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>67</v>
@@ -1446,18 +1452,18 @@
       <c r="D15" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="19" t="s">
         <v>73</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="14"/>
+      <c r="G15" s="13"/>
       <c r="I15" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>67</v>
@@ -1470,26 +1476,26 @@
       <c r="C16" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="22" t="s">
         <v>78</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>77</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>136</v>
+        <v>123</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -1502,7 +1508,7 @@
       <c r="D17" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="19" t="s">
         <v>67</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -1510,13 +1516,13 @@
       </c>
       <c r="G17" s="4"/>
       <c r="I17" s="4" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1529,7 +1535,7 @@
       <c r="D18" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="19" t="s">
         <v>102</v>
       </c>
       <c r="F18" s="4" t="s">
@@ -1537,13 +1543,13 @@
       </c>
       <c r="G18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>81</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1556,7 +1562,7 @@
       <c r="D19" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="19" t="s">
         <v>67</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -1564,13 +1570,13 @@
       </c>
       <c r="G19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1583,7 +1589,7 @@
       <c r="D20" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="19" t="s">
         <v>102</v>
       </c>
       <c r="F20" s="4" t="s">
@@ -1591,13 +1597,13 @@
       </c>
       <c r="G20" s="4"/>
       <c r="I20" s="4" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>81</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1610,7 +1616,7 @@
       <c r="D21" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="19" t="s">
         <v>101</v>
       </c>
       <c r="F21" s="4" t="s">
@@ -1621,10 +1627,10 @@
         <v>92</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1637,7 +1643,7 @@
       <c r="D22" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="19" t="s">
         <v>101</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -1648,10 +1654,10 @@
         <v>92</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
@@ -1664,21 +1670,24 @@
       <c r="D23" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="19" t="s">
         <v>100</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>97</v>
       </c>
       <c r="G23" s="4"/>
+      <c r="H23" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="I23" s="4" t="s">
         <v>92</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -1691,7 +1700,7 @@
       <c r="D24" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="19" t="s">
         <v>99</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -1699,10 +1708,10 @@
       </c>
       <c r="G24" s="4"/>
       <c r="I24" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>67</v>
@@ -1713,26 +1722,29 @@
         <v>61</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="20" t="s">
-        <v>111</v>
+      <c r="E25" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G25" s="4"/>
+      <c r="H25" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="I25" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -1740,16 +1752,16 @@
         <v>62</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="20" t="s">
-        <v>111</v>
+      <c r="E26" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G26" s="4"/>
       <c r="I26" s="4"/>
@@ -1761,16 +1773,16 @@
         <v>63</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="G27" s="4"/>
       <c r="I27" s="4"/>
@@ -1779,58 +1791,58 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E28" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="I28" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="J28" s="25" t="s">
-        <v>92</v>
+        <v>146</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E29" s="20" t="s">
-        <v>122</v>
+      <c r="E29" s="19" t="s">
+        <v>119</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G29" s="4"/>
       <c r="I29" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="J29" s="25" t="s">
-        <v>92</v>
+        <v>146</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update action name ready
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="ActionData" sheetId="1" r:id="rId1"/>
-    <sheet name="V2 Command" sheetId="2" r:id="rId2"/>
+    <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
+    <sheet name="ActionData" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="161">
   <si>
     <t>Offset</t>
   </si>
@@ -337,9 +337,6 @@
     <t>A9 9A 03 61 01 65 ED</t>
   </si>
   <si>
-    <t>A9 9A 03 62 01 66 ED</t>
-  </si>
-  <si>
     <t>Yes {4}</t>
   </si>
   <si>
@@ -349,9 +346,6 @@
     <t>actionId, poseId</t>
   </si>
   <si>
-    <t>A9 9A 04 63 01 02 6A ED</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
@@ -382,9 +376,6 @@
     <t>A9 9A 02 F2 F4 ED</t>
   </si>
   <si>
-    <t>Result</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -407,9 +398,6 @@
   </si>
   <si>
     <t>Yes {124}</t>
-  </si>
-  <si>
-    <t>Action Header</t>
   </si>
   <si>
     <t>5 bytes of command enable flag
@@ -434,9 +422,6 @@
     <t>Get action header</t>
   </si>
   <si>
-    <t>Get action detail</t>
-  </si>
-  <si>
     <t>Get action pose</t>
   </si>
   <si>
@@ -452,9 +437,6 @@
     <t>Yes {38}</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Yes {9}</t>
   </si>
   <si>
@@ -465,6 +447,61 @@
   </si>
   <si>
     <t>{success}</t>
+  </si>
+  <si>
+    <t>** {len} {cmd} {len_H} {len_L} {aId} {poseCnt} {data}</t>
+  </si>
+  <si>
+    <t>Yes {40}</t>
+  </si>
+  <si>
+    <t>Yes {34}</t>
+  </si>
+  <si>
+    <t>{aId} {pId} {poseData}</t>
+  </si>
+  <si>
+    <t>** full result = {header}</t>
+  </si>
+  <si>
+    <t>Result (i.e. {parm} is result format)</t>
+  </si>
+  <si>
+    <t>Get fall action detail</t>
+  </si>
+  <si>
+    <t>A9 9A 04 62 01 02 69 ED</t>
+  </si>
+  <si>
+    <t>A9 9A 03 63 01 67 ED</t>
+  </si>
+  <si>
+    <t>Full record as Header</t>
+  </si>
+  <si>
+    <t>{Refer to ActionData}</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Update action header (all pose cleared)</t>
+  </si>
+  <si>
+    <t>Update action pose (pose count updated)</t>
+  </si>
+  <si>
+    <t>Update action name</t>
+  </si>
+  <si>
+    <t>{id}{len}({actionName})</t>
+  </si>
+  <si>
+    <t>A9 9A 03 03 01 07 ED</t>
+  </si>
+  <si>
+    <t>A9 9A 0A 74 01 07  44 65 66 61 75 6C 74 D7 ED
+Action name = "Default"</t>
   </si>
 </sst>
 </file>
@@ -589,15 +626,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -605,13 +633,22 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -914,10 +951,696 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" style="21" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="13.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="47.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="G3" s="14"/>
+      <c r="K3" s="15"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="22"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="22"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <v>11</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="5">
+        <v>12</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="I18" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>13</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="I19" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="I20" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <v>21</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="I21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>22</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="I22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>23</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="I23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
+        <v>31</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="I24" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
+        <v>61</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="I25" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
+        <v>62</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="I26" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
+        <v>63</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="I27" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
+        <v>71</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
+        <v>72</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E29" s="19"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B30" s="3">
+        <v>74</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="I33" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +1675,7 @@
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="20" t="s">
         <v>3</v>
       </c>
     </row>
@@ -963,7 +1686,7 @@
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24"/>
+      <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -981,10 +1704,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1239,614 +1962,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O29"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="13.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="18"/>
-      <c r="G3" s="14"/>
-      <c r="K3" s="15"/>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="18"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="18"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="18"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="I13" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="I15" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="K16" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="5">
-        <v>11</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="4"/>
-      <c r="I17" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="5">
-        <v>12</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="I18" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="5">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="I19" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="3">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="I20" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="3">
-        <v>21</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="I21" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="3">
-        <v>22</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="I22" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="3">
-        <v>23</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="3">
-        <v>31</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="4"/>
-      <c r="I24" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="3">
-        <v>61</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="3">
-        <v>62</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="3">
-        <v>63</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="G29" s="4"/>
-      <c r="I29" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Reduce header size to 60 to met serial buffer size limit
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="178">
   <si>
     <t>Offset</t>
   </si>
@@ -397,9 +397,6 @@
     <t>Yes {128}</t>
   </si>
   <si>
-    <t>Yes {124}</t>
-  </si>
-  <si>
     <t>5 bytes of command enable flag
 {V1, V2, BT, CB, SV}</t>
   </si>
@@ -500,8 +497,63 @@
     <t>A9 9A 03 03 01 07 ED</t>
   </si>
   <si>
-    <t>A9 9A 0A 74 01 07  44 65 66 61 75 6C 74 D7 ED
+    <t xml:space="preserve">A9 9A 7C 61 01 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 DF ED
+</t>
+  </si>
+  <si>
+    <t>Reserved for command code</t>
+  </si>
+  <si>
+    <t>Action name (max 20, fill zero at end)</t>
+  </si>
+  <si>
+    <t>Serial buffer only 63 available, so reduce size to 60 for safety</t>
+  </si>
+  <si>
+    <t>34~35</t>
+  </si>
+  <si>
+    <t>Reserved for affected servo</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06~25</t>
+  </si>
+  <si>
+    <t>26~27</t>
+  </si>
+  <si>
+    <t>Reserved terminator</t>
+  </si>
+  <si>
+    <t>30~33</t>
+  </si>
+  <si>
+    <t>36~37</t>
+  </si>
+  <si>
+    <t>38~57</t>
+  </si>
+  <si>
+    <t>Length of header data = 56</t>
+  </si>
+  <si>
+    <t>0x38</t>
+  </si>
+  <si>
+    <t>Yes {60}</t>
+  </si>
+  <si>
+    <t>Yes {56}</t>
+  </si>
+  <si>
+    <t>A9 9A 0B 74 01 07  44 65 66 61 75 6C 74 D7 ED
 Action name = "Default"</t>
+  </si>
+  <si>
+    <t>A9 9A 38 71 01 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 00 00 00 AB ED</t>
   </si>
 </sst>
 </file>
@@ -535,7 +587,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,6 +597,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -649,6 +707,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -954,10 +1021,10 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1157,7 @@
         <v>122</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
@@ -1165,8 +1232,8 @@
       <c r="F15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>159</v>
+      <c r="G15" s="26" t="s">
+        <v>158</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>119</v>
@@ -1198,13 +1265,13 @@
         <v>77</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>120</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -1225,13 +1292,13 @@
       </c>
       <c r="G17" s="4"/>
       <c r="I17" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>121</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1252,13 +1319,13 @@
       </c>
       <c r="G18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>81</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1279,13 +1346,13 @@
       </c>
       <c r="G19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>121</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1306,13 +1373,13 @@
       </c>
       <c r="G20" s="4"/>
       <c r="I20" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>81</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1393,7 +1460,7 @@
         <v>123</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -1428,7 +1495,7 @@
         <v>61</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>81</v>
@@ -1441,13 +1508,13 @@
       </c>
       <c r="G25" s="4"/>
       <c r="I25" s="4" t="s">
-        <v>125</v>
+        <v>174</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -1455,7 +1522,7 @@
         <v>62</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>106</v>
@@ -1464,17 +1531,17 @@
         <v>108</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G26" s="4"/>
       <c r="I26" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="K26" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -1482,7 +1549,7 @@
         <v>63</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>81</v>
@@ -1491,7 +1558,7 @@
         <v>107</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G27" s="4"/>
       <c r="I27" s="4" t="s">
@@ -1501,7 +1568,7 @@
         <v>123</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -1509,16 +1576,16 @@
         <v>71</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>125</v>
       </c>
       <c r="E28" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>153</v>
       </c>
       <c r="G28" s="4"/>
       <c r="I28" s="4"/>
@@ -1530,10 +1597,10 @@
         <v>72</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="4"/>
@@ -1542,26 +1609,32 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>74</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E30" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>158</v>
-      </c>
       <c r="F30" s="18" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="G30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
+      <c r="I30" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
@@ -1594,13 +1667,13 @@
         <v>113</v>
       </c>
       <c r="I32" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="K32" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
@@ -1621,13 +1694,13 @@
       </c>
       <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="K33" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1637,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D34"/>
+  <dimension ref="A2:D55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1748,7 @@
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="27" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1686,7 +1759,7 @@
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -1704,10 +1777,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1853,10 +1926,23 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>39</v>
-      </c>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
@@ -1874,10 +1960,10 @@
         <v>30</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>56</v>
+        <v>1</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1885,80 +1971,276 @@
         <v>31</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>42</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D27" s="27"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>45</v>
+        <v>173</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>52</v>
+      <c r="B29" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>46</v>
+        <v>135</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
-        <v>53</v>
+      <c r="B30" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>48</v>
+        <v>8</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
-        <v>54</v>
+      <c r="B31" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>50</v>
+        <v>5</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="3">
+        <v>28</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
+        <v>29</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="3">
+        <v>58</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <v>59</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="10"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="12"/>
+    </row>
+    <row r="44" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D53" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="10"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="12"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="12"/>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="10"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="12"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="10"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D26:D27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
@@ -1967,12 +2249,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C2:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="158.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="C2" s="25" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fix on some command parameters
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="ActionData" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -464,9 +464,6 @@
     <t>Result (i.e. {parm} is result format)</t>
   </si>
   <si>
-    <t>Get fall action detail</t>
-  </si>
-  <si>
     <t>A9 9A 04 62 01 02 69 ED</t>
   </si>
   <si>
@@ -554,12 +551,15 @@
   </si>
   <si>
     <t>A9 9A 38 71 01 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 00 00 00 AB ED</t>
+  </si>
+  <si>
+    <t>Get full action detail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -727,6 +727,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -774,7 +777,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -809,7 +812,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1021,10 +1024,10 @@
   <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,7 +1236,7 @@
         <v>74</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>119</v>
@@ -1508,10 +1511,10 @@
       </c>
       <c r="G25" s="4"/>
       <c r="I25" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>175</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>146</v>
@@ -1531,7 +1534,7 @@
         <v>108</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G26" s="4"/>
       <c r="I26" s="4" t="s">
@@ -1549,7 +1552,7 @@
         <v>63</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>81</v>
@@ -1558,7 +1561,7 @@
         <v>107</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G27" s="4"/>
       <c r="I27" s="4" t="s">
@@ -1576,16 +1579,16 @@
         <v>71</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>125</v>
       </c>
       <c r="E28" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="G28" s="4"/>
       <c r="I28" s="4"/>
@@ -1597,10 +1600,10 @@
         <v>72</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="4"/>
@@ -1614,16 +1617,16 @@
         <v>74</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E30" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>157</v>
-      </c>
       <c r="F30" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G30" s="4"/>
       <c r="I30" s="4" t="s">
@@ -1933,7 +1936,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
@@ -1980,10 +1983,10 @@
         <v>32</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1994,7 +1997,7 @@
         <v>135</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2010,7 +2013,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>5</v>
@@ -2021,24 +2024,24 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2065,7 +2068,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>20</v>
@@ -2076,7 +2079,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>23</v>
@@ -2087,18 +2090,18 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>5</v>
@@ -2262,12 +2265,12 @@
   <sheetData>
     <row r="2" spans="3:3" ht="60" x14ac:dyDescent="0.25">
       <c r="C2" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add RobotMaintenance tools - It will jump to maintenance after reset, just for testing during development - should be change to check GPIO before entering Maintenance mode
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="ActionData" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="184">
   <si>
     <t>Offset</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>{w. time}</t>
-  </si>
-  <si>
-    <t>Servo execution time in ms</t>
   </si>
   <si>
     <t>Wait time in ms</t>
@@ -504,9 +501,6 @@
     <t>Action name (max 20, fill zero at end)</t>
   </si>
   <si>
-    <t>Serial buffer only 63 available, so reduce size to 60 for safety</t>
-  </si>
-  <si>
     <t>34~35</t>
   </si>
   <si>
@@ -553,14 +547,38 @@
     <t>A9 9A 38 71 01 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 00 00 00 AB ED</t>
   </si>
   <si>
-    <t>Get full action detail</t>
+    <t>Get full action detail (not recommended)</t>
+  </si>
+  <si>
+    <t>Serial buffer only has 63 bytes available, so reduce size to 60 bytes for safety</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Servo execution time in ms(*)</t>
+  </si>
+  <si>
+    <t>Time in servo command is not in ms</t>
+  </si>
+  <si>
+    <t>Will allow user to change this factor in PC</t>
+  </si>
+  <si>
+    <t>Or add command to speed up/slow down action</t>
+  </si>
+  <si>
+    <t>The factor 20 seems not a perfect value</t>
+  </si>
+  <si>
+    <t>Return</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,8 +604,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -603,6 +631,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -716,6 +750,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,7 +820,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -812,7 +855,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1021,13 +1064,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O33"/>
+  <dimension ref="B2:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,674 +1079,735 @@
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" style="21" customWidth="1"/>
-    <col min="6" max="6" width="39.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="13.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="47.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="8.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" style="21" customWidth="1"/>
+    <col min="7" max="7" width="39.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="13.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="47.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="G3" s="14"/>
-      <c r="K3" s="15"/>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F3" s="22"/>
+      <c r="H3" s="14"/>
+      <c r="L3" s="15"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="L4" s="14"/>
+      <c r="F4" s="22"/>
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
       <c r="O4" s="14"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="14"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="L5" s="14"/>
+      <c r="F5" s="22"/>
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="14"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="G6" s="16"/>
+        <v>56</v>
+      </c>
+      <c r="F6" s="22"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
-      <c r="L6" s="14"/>
+      <c r="K6" s="16"/>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
       <c r="O6" s="14"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="14"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="22"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="22"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F9" s="22"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="J12" s="7" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="I13" s="4" t="s">
-        <v>119</v>
-      </c>
+      <c r="H13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="J14" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="I15" s="4" t="s">
+      <c r="E16" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="K16" s="18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="4"/>
-      <c r="I17" s="4" t="s">
-        <v>137</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>12</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="I18" s="4" t="s">
-        <v>138</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>13</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="I19" s="4" t="s">
-        <v>137</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H19" s="4"/>
       <c r="J19" s="4" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>14</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="I20" s="4" t="s">
-        <v>138</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="4"/>
       <c r="J20" s="4" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="I21" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="H21" s="4"/>
       <c r="J21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="K21" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>22</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="I22" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="H22" s="4"/>
       <c r="J22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="K22" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>23</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G23" s="4"/>
-      <c r="I23" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="H23" s="4"/>
       <c r="J23" s="4" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <v>31</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="4"/>
-      <c r="I24" s="4" t="s">
-        <v>119</v>
-      </c>
+      <c r="G24" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="4"/>
       <c r="J24" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <v>61</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" s="4"/>
-      <c r="I25" s="4" t="s">
-        <v>173</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H25" s="4"/>
       <c r="J25" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>62</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G26" s="4"/>
-      <c r="I26" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="J26" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K26" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="L26" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="K26" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <v>63</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="G27" s="4"/>
-      <c r="I27" s="4" t="s">
-        <v>92</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H27" s="4"/>
       <c r="J27" s="4" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <v>71</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E28" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="G28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="H28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <v>72</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="4"/>
+        <v>151</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="19"/>
       <c r="G29" s="4"/>
-      <c r="I29" s="4"/>
+      <c r="H29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
-    </row>
-    <row r="30" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>74</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="F30" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="G30" s="4"/>
-      <c r="I30" s="4" t="s">
+      <c r="G30" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="H30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K30" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="L30" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="K30" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="19"/>
       <c r="G31" s="4"/>
-      <c r="I31" s="4"/>
+      <c r="H31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="E32" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F33" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="I32" s="4" t="s">
+      <c r="G33" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H33" s="4"/>
+      <c r="J33" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K33" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="L33" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G33" s="4"/>
-      <c r="I33" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1713,10 +1817,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D55"/>
+  <dimension ref="A2:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,8 +1828,10 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="36.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="46" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="56.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
@@ -1780,10 +1886,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1934,9 +2040,9 @@
       <c r="C22" s="11"/>
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>161</v>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>176</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
@@ -1983,10 +2089,10 @@
         <v>32</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1994,10 +2100,10 @@
         <v>33</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2013,7 +2119,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>5</v>
@@ -2024,24 +2130,24 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2068,7 +2174,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>20</v>
@@ -2079,7 +2185,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>23</v>
@@ -2090,18 +2196,18 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>5</v>
@@ -2161,7 +2267,7 @@
         <v>40</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2177,51 +2283,51 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>45</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C51" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C52" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>5</v>
@@ -2239,6 +2345,29 @@
       <c r="B55" s="10"/>
       <c r="C55" s="11"/>
       <c r="D55" s="12"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2265,12 +2394,12 @@
   <sheetData>
     <row r="2" spans="3:3" ht="60" x14ac:dyDescent="0.25">
       <c r="C2" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MP3 related command ready & tested
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="225">
   <si>
     <t>Offset</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>22~25</t>
-  </si>
-  <si>
-    <t>26~31</t>
   </si>
   <si>
     <t>Pose sequence no.</t>
@@ -328,9 +325,6 @@
     <t>Command enable (enquiry / set)</t>
   </si>
   <si>
-    <t>A9 9A 06 31 01 00 02 01 3B ED</t>
-  </si>
-  <si>
     <t>A9 9A 03 61 01 65 ED</t>
   </si>
   <si>
@@ -571,9 +565,6 @@
     <t>{head}</t>
   </si>
   <si>
-    <t>Head Light flag</t>
-  </si>
-  <si>
     <t>Play action</t>
   </si>
   <si>
@@ -608,12 +599,108 @@
   </si>
   <si>
     <t>A9 9A 03 01 01 05 ED</t>
+  </si>
+  <si>
+    <t>Head Light flag (0xff - do nothing)</t>
+  </si>
+  <si>
+    <t>{mp3.d}</t>
+  </si>
+  <si>
+    <t>{mp3.f}</t>
+  </si>
+  <si>
+    <t>MP3 directory (0xff - do nothing)</t>
+  </si>
+  <si>
+    <t>MP3 file (0x00 - stop, 0xff - do nothing)</t>
+  </si>
+  <si>
+    <t>29~31</t>
+  </si>
+  <si>
+    <t>Set Head LED</t>
+  </si>
+  <si>
+    <t>A9 9A 03 31 00 34 ED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A9 9A 03 31 01 35 ED </t>
+  </si>
+  <si>
+    <t>A9 9A 06 24 01 00 02 01 2E ED</t>
+  </si>
+  <si>
+    <t>Stop MP3</t>
+  </si>
+  <si>
+    <t>A9 9A 02 32 34 ED</t>
+  </si>
+  <si>
+    <t>Play File</t>
+  </si>
+  <si>
+    <t>A9 9A 04 33 00 01 38 ED</t>
+  </si>
+  <si>
+    <t>Play MP3 File</t>
+  </si>
+  <si>
+    <t>&lt;file&gt;</t>
+  </si>
+  <si>
+    <t>A9 9A 03 34 01 38 ED</t>
+  </si>
+  <si>
+    <t>Play Avert File</t>
+  </si>
+  <si>
+    <t>A9 9A 03 35 01 39 ED</t>
+  </si>
+  <si>
+    <t>MP3 Set Volume</t>
+  </si>
+  <si>
+    <t>&lt;option&gt;&lt;volume&gt;</t>
+  </si>
+  <si>
+    <t>A9 9A 04 36 00 0F 49 ED</t>
+  </si>
+  <si>
+    <t>A9 9A 04 36 01 01 3C ED</t>
+  </si>
+  <si>
+    <t>{volume}</t>
+  </si>
+  <si>
+    <t>&lt;folder&gt;&lt;file&gt;  (folder = 0xff =&gt; root)</t>
+  </si>
+  <si>
+    <t>A9 9A 04 33 ff 02 38 ED</t>
+  </si>
+  <si>
+    <t>06~37</t>
+  </si>
+  <si>
+    <t>38~47</t>
+  </si>
+  <si>
+    <t>Servo angle (32 bytes)</t>
+  </si>
+  <si>
+    <t>LED control flag (8 bytes)</t>
+  </si>
+  <si>
+    <t>49~63</t>
+  </si>
+  <si>
+    <t>Pose Data (60 bytes) - extend to 32 servo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -698,7 +785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -783,6 +870,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -847,7 +940,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -882,7 +975,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1091,13 +1184,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O37"/>
+  <dimension ref="B2:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1213,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -1165,7 +1258,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="22"/>
       <c r="G6" s="16"/>
@@ -1179,16 +1272,16 @@
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="22"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>26</v>
@@ -1197,7 +1290,7 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>28</v>
@@ -1206,31 +1299,31 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>71</v>
-      </c>
       <c r="I12" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
@@ -1238,28 +1331,28 @@
         <v>31</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
@@ -1267,28 +1360,28 @@
         <v>32</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>69</v>
-      </c>
       <c r="I14" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
@@ -1296,57 +1389,57 @@
         <v>33</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E15" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="G15" s="26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I15" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>76</v>
-      </c>
       <c r="I16" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -1354,26 +1447,26 @@
         <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" s="4"/>
       <c r="I17" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1381,26 +1474,26 @@
         <v>12</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1408,26 +1501,26 @@
         <v>13</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1435,26 +1528,26 @@
         <v>14</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G20" s="4"/>
       <c r="I20" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1462,26 +1555,26 @@
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="G21" s="4"/>
       <c r="I21" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1489,26 +1582,26 @@
         <v>22</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="G22" s="4"/>
       <c r="I22" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
@@ -1516,358 +1609,526 @@
         <v>23</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="G23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>98</v>
-      </c>
       <c r="F24" s="4" t="s">
-        <v>103</v>
+        <v>202</v>
       </c>
       <c r="G24" s="4"/>
       <c r="I24" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K24" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>7</v>
+        <v>136</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>71</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="G25" s="4"/>
+        <v>200</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>201</v>
+      </c>
       <c r="I25" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K25" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" s="27" t="s">
-        <v>186</v>
+        <v>78</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>65</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="G26" s="4"/>
+        <v>204</v>
+      </c>
+      <c r="G26" s="13"/>
       <c r="I26" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K26" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="J26" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>190</v>
+      <c r="B27" s="3">
+        <v>33</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" s="27" t="s">
-        <v>66</v>
+        <v>103</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>217</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="G27" s="4"/>
+        <v>206</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>218</v>
+      </c>
       <c r="I27" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K27" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>130</v>
+        <v>207</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>106</v>
+        <v>79</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>208</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G28" s="4"/>
+        <v>209</v>
+      </c>
+      <c r="G28" s="13"/>
       <c r="I28" s="4" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>131</v>
+        <v>210</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>107</v>
+        <v>79</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>208</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="G29" s="4"/>
+        <v>211</v>
+      </c>
+      <c r="G29" s="13"/>
       <c r="I29" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>213</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G30" s="4"/>
+        <v>214</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>215</v>
+      </c>
       <c r="I30" s="4" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>140</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>148</v>
+        <v>79</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>7</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
       <c r="G31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="I31" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E32" s="19"/>
-      <c r="F32" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="G32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" s="3">
-        <v>74</v>
+      <c r="I32" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>172</v>
+        <v>78</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>189</v>
       </c>
       <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K33" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="J33" s="4" t="s">
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="3">
+        <v>61</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G34" s="4"/>
+      <c r="I34" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
+        <v>62</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G35" s="4"/>
+      <c r="I35" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="3">
+        <v>63</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G36" s="4"/>
+      <c r="I36" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="K36" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="K33" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
+        <v>71</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
+        <v>72</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E38" s="19"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+    </row>
+    <row r="39" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
+        <v>74</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="G39" s="4"/>
+      <c r="I39" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="F42" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="I36" s="4" t="s">
+      <c r="G43" s="4"/>
+      <c r="I43" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K43" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G37" s="4"/>
-      <c r="I37" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1877,10 +2138,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D60"/>
+  <dimension ref="A2:D80"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1917,7 +2178,7 @@
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="31" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1928,7 +2189,7 @@
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="29"/>
+      <c r="D6" s="31"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -1946,10 +2207,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2102,7 +2363,7 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
@@ -2131,7 +2392,7 @@
       <c r="C26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="31" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2142,17 +2403,17 @@
       <c r="C27" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="29"/>
+      <c r="D27" s="31"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2160,10 +2421,10 @@
         <v>33</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2179,7 +2440,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>5</v>
@@ -2190,24 +2451,24 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2234,7 +2495,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>20</v>
@@ -2245,7 +2506,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>23</v>
@@ -2256,18 +2517,18 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>5</v>
@@ -2327,7 +2588,7 @@
         <v>40</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2341,7 +2602,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>50</v>
       </c>
@@ -2349,10 +2610,10 @@
         <v>43</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>51</v>
       </c>
@@ -2363,7 +2624,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>52</v>
       </c>
@@ -2374,7 +2635,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>53</v>
       </c>
@@ -2385,59 +2646,230 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="3">
         <v>26</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="3" t="s">
-        <v>54</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="3">
+        <v>27</v>
       </c>
       <c r="C54" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D54" s="29" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="3">
+        <v>28</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D55" s="29" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D56" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="10"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="12"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="10"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="12"/>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="1" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="10"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="12"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D59" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D60" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" s="30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D68" s="30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D69" s="30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D70" s="30" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D71" s="30" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="3">
+        <v>46</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>180</v>
+      </c>
+      <c r="D72" s="30" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="3">
+        <v>47</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D73" s="30" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="3">
+        <v>48</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D74" s="30" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="10"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="12"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C77" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2465,12 +2897,12 @@
   <sheetData>
     <row r="2" spans="3:3" ht="60" x14ac:dyDescent="0.25">
       <c r="C2" s="25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Servo LED setting follow UBT (i.e. 0 - ON, 1 - OFF) - Head LED Setting as normal (i.e. 0 - OFF, 1 - ON)
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -310,9 +310,6 @@
     <t>Set LED</t>
   </si>
   <si>
-    <t>List&lt;id, on/off&gt;</t>
-  </si>
-  <si>
     <t>List&lt;id, angle,time&gt;</t>
   </si>
   <si>
@@ -695,6 +692,9 @@
   </si>
   <si>
     <t>Pose Data (60 bytes) - extend to 32 servo</t>
+  </si>
+  <si>
+    <t>List&lt;id, on/off&gt;  (0 - ON, else - OFF)</t>
   </si>
 </sst>
 </file>
@@ -1186,11 +1186,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,13 +1317,13 @@
         <v>70</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
@@ -1337,22 +1337,22 @@
         <v>79</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>66</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J13" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
@@ -1375,13 +1375,13 @@
         <v>68</v>
       </c>
       <c r="I14" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
@@ -1401,16 +1401,16 @@
         <v>72</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I15" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="45" x14ac:dyDescent="0.25">
@@ -1418,7 +1418,7 @@
         <v>73</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>80</v>
@@ -1433,13 +1433,13 @@
         <v>75</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -1460,13 +1460,13 @@
       </c>
       <c r="G17" s="4"/>
       <c r="I17" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1480,20 +1480,20 @@
         <v>79</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>82</v>
       </c>
       <c r="G18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>79</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1514,13 +1514,13 @@
       </c>
       <c r="G19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1534,20 +1534,20 @@
         <v>79</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>88</v>
       </c>
       <c r="G20" s="4"/>
       <c r="I20" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>79</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1561,7 +1561,7 @@
         <v>90</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>91</v>
@@ -1571,10 +1571,10 @@
         <v>90</v>
       </c>
       <c r="J21" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="K21" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1588,7 +1588,7 @@
         <v>90</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>93</v>
@@ -1598,10 +1598,10 @@
         <v>90</v>
       </c>
       <c r="J22" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
@@ -1615,7 +1615,7 @@
         <v>90</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>95</v>
@@ -1625,10 +1625,10 @@
         <v>90</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -1642,20 +1642,20 @@
         <v>90</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>97</v>
+        <v>224</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G24" s="4"/>
       <c r="I24" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J24" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="K24" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
@@ -1663,28 +1663,28 @@
         <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E25" s="29" t="s">
         <v>71</v>
       </c>
       <c r="F25" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G25" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="G25" s="13" t="s">
-        <v>201</v>
-      </c>
       <c r="I25" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="K25" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -1692,7 +1692,7 @@
         <v>32</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>78</v>
@@ -1701,17 +1701,17 @@
         <v>65</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G26" s="13"/>
       <c r="I26" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="K26" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -1719,28 +1719,28 @@
         <v>33</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E27" s="29" t="s">
+      <c r="G27" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>218</v>
-      </c>
       <c r="I27" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J27" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="K27" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -1748,26 +1748,26 @@
         <v>34</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E28" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>209</v>
       </c>
       <c r="G28" s="13"/>
       <c r="I28" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J28" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="K28" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -1775,26 +1775,26 @@
         <v>35</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G29" s="13"/>
       <c r="I29" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="K29" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -1802,28 +1802,28 @@
         <v>36</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="29" t="s">
         <v>212</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E30" s="29" t="s">
+      <c r="F30" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="G30" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="I30" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K30" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -1831,7 +1831,7 @@
         <v>41</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>79</v>
@@ -1840,17 +1840,17 @@
         <v>7</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G31" s="4"/>
       <c r="I31" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J31" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="K31" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
@@ -1858,34 +1858,34 @@
         <v>42</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G32" s="4"/>
       <c r="I32" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="K32" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>78</v>
@@ -1894,17 +1894,17 @@
         <v>65</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="K33" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
@@ -1912,26 +1912,26 @@
         <v>61</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G34" s="4"/>
       <c r="I34" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="J34" s="4" t="s">
-        <v>169</v>
-      </c>
       <c r="K34" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
@@ -1939,26 +1939,26 @@
         <v>62</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G35" s="4"/>
       <c r="I35" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J35" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="K35" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
@@ -1966,26 +1966,26 @@
         <v>63</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G36" s="4"/>
       <c r="I36" s="4" t="s">
         <v>90</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
@@ -1993,16 +1993,16 @@
         <v>71</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E37" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>147</v>
       </c>
       <c r="G37" s="4"/>
       <c r="I37" s="4"/>
@@ -2014,10 +2014,10 @@
         <v>72</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E38" s="19"/>
       <c r="F38" s="4"/>
@@ -2031,26 +2031,26 @@
         <v>74</v>
       </c>
       <c r="C39" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>152</v>
-      </c>
       <c r="F39" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G39" s="4"/>
       <c r="I39" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J39" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="K39" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
@@ -2077,58 +2077,58 @@
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" s="4" t="s">
+      <c r="E42" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="F42" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>110</v>
-      </c>
       <c r="I42" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J42" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J42" s="4" t="s">
+      <c r="K42" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>78</v>
       </c>
       <c r="E43" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="G43" s="4"/>
       <c r="I43" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J43" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="K43" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K43" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2140,7 +2140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -2207,10 +2207,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2363,7 +2363,7 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
@@ -2410,10 +2410,10 @@
         <v>32</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2421,10 +2421,10 @@
         <v>33</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2440,7 +2440,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>5</v>
@@ -2451,24 +2451,24 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2495,7 +2495,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>20</v>
@@ -2506,7 +2506,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>23</v>
@@ -2517,18 +2517,18 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>5</v>
@@ -2610,7 +2610,7 @@
         <v>43</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2651,10 +2651,10 @@
         <v>26</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2662,10 +2662,10 @@
         <v>27</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2673,15 +2673,15 @@
         <v>28</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>5</v>
@@ -2697,30 +2697,30 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C58" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D59" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D60" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D61" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
@@ -2764,7 +2764,7 @@
         <v>43</v>
       </c>
       <c r="D68" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
@@ -2780,24 +2780,24 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D70" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D71" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
@@ -2805,10 +2805,10 @@
         <v>46</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D72" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
@@ -2816,10 +2816,10 @@
         <v>47</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
@@ -2827,15 +2827,15 @@
         <v>48</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>5</v>
@@ -2851,25 +2851,25 @@
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C77" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D78" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D79" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D80" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2897,12 +2897,12 @@
   <sheetData>
     <row r="2" spans="3:3" ht="60" x14ac:dyDescent="0.25">
       <c r="C2" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on ActionData - add sample data
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="233">
   <si>
     <t>Offset</t>
   </si>
@@ -679,22 +679,46 @@
     <t>06~37</t>
   </si>
   <si>
-    <t>38~47</t>
-  </si>
-  <si>
     <t>Servo angle (32 bytes)</t>
   </si>
   <si>
     <t>LED control flag (8 bytes)</t>
   </si>
   <si>
-    <t>49~63</t>
-  </si>
-  <si>
     <t>Pose Data (60 bytes) - extend to 32 servo</t>
   </si>
   <si>
     <t>List&lt;id, on/off&gt;  (0 - ON, else - OFF)</t>
+  </si>
+  <si>
+    <t>49~59</t>
+  </si>
+  <si>
+    <t>0x62</t>
+  </si>
+  <si>
+    <t>{actionId}</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07~08</t>
+  </si>
+  <si>
+    <t>09~10</t>
+  </si>
+  <si>
+    <t>11~42</t>
+  </si>
+  <si>
+    <t>43~50</t>
+  </si>
+  <si>
+    <t>38~45</t>
+  </si>
+  <si>
+    <t>54~59</t>
   </si>
 </sst>
 </file>
@@ -785,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -870,6 +894,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1186,11 +1213,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,7 +1669,7 @@
         <v>90</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>201</v>
@@ -2138,10 +2165,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D80"/>
+  <dimension ref="A2:D85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2178,7 +2205,7 @@
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2189,7 +2216,7 @@
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="31"/>
+      <c r="D6" s="32"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -2392,7 +2419,7 @@
       <c r="C26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="32" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2403,7 +2430,7 @@
       <c r="C27" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="31"/>
+      <c r="D27" s="32"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
@@ -2720,10 +2747,10 @@
     </row>
     <row r="63" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" s="6" t="s">
         <v>0</v>
       </c>
@@ -2734,148 +2761,232 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D66" s="30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D66" s="32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C67" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" s="32"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D68" s="31" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D69" s="31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D70" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D71" s="31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D67" s="30" t="s">
+      <c r="D72" s="30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="5" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="B73" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D68" s="30" t="s">
+      <c r="D73" s="30" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="3" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="B74" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D69" s="30" t="s">
+      <c r="D74" s="30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="3" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="B75" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D70" s="30" t="s">
+      <c r="D75" s="30" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D76" s="30" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C71" s="4" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
+        <v>46</v>
+      </c>
+      <c r="B77" s="3">
+        <v>51</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D77" s="30" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>47</v>
+      </c>
+      <c r="B78" s="3">
+        <v>52</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D78" s="30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
         <v>48</v>
       </c>
-      <c r="D71" s="30" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="3">
-        <v>46</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D72" s="30" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="3">
-        <v>47</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D73" s="30" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="3">
-        <v>48</v>
-      </c>
-      <c r="C74" s="4" t="s">
+      <c r="B79" s="3">
+        <v>53</v>
+      </c>
+      <c r="C79" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="D74" s="30" t="s">
+      <c r="D79" s="30" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C75" s="4" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D75" s="30" t="s">
+      <c r="D80" s="30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="10"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="12"/>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="1" t="s">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="10"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="12"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C82" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D78" s="1" t="s">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D79" s="1" t="s">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D80" s="1" t="s">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="1" t="s">
         <v>177</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D66:D67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>

</xml_diff>

<commit_message>
- always end MP3 after use (9600bps not stable) - action data add mp3 volume
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="236">
   <si>
     <t>Offset</t>
   </si>
@@ -613,9 +613,6 @@
     <t>MP3 file (0x00 - stop, 0xff - do nothing)</t>
   </si>
   <si>
-    <t>29~31</t>
-  </si>
-  <si>
     <t>Set Head LED</t>
   </si>
   <si>
@@ -658,9 +655,6 @@
     <t>MP3 Set Volume</t>
   </si>
   <si>
-    <t>&lt;option&gt;&lt;volume&gt;</t>
-  </si>
-  <si>
     <t>A9 9A 04 36 00 0F 49 ED</t>
   </si>
   <si>
@@ -718,7 +712,22 @@
     <t>38~45</t>
   </si>
   <si>
-    <t>54~59</t>
+    <t>&lt;mode&gt;&lt;volume&gt;</t>
+  </si>
+  <si>
+    <t>{mp3.vol}</t>
+  </si>
+  <si>
+    <t>MP3 volume</t>
+  </si>
+  <si>
+    <t>30~31</t>
+  </si>
+  <si>
+    <t>MP3 volume (0xff - no change)</t>
+  </si>
+  <si>
+    <t>55~57</t>
   </si>
 </sst>
 </file>
@@ -809,7 +818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -894,6 +903,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1214,10 +1226,10 @@
   <dimension ref="B2:O43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,10 +1681,10 @@
         <v>90</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G24" s="4"/>
       <c r="I24" s="4" t="s">
@@ -1690,7 +1702,7 @@
         <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>135</v>
@@ -1699,10 +1711,10 @@
         <v>71</v>
       </c>
       <c r="F25" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="G25" s="13" t="s">
         <v>199</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>200</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>134</v>
@@ -1719,7 +1731,7 @@
         <v>32</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>78</v>
@@ -1728,7 +1740,7 @@
         <v>65</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G26" s="13"/>
       <c r="I26" s="4" t="s">
@@ -1746,19 +1758,19 @@
         <v>33</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>102</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>134</v>
@@ -1775,16 +1787,16 @@
         <v>34</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E28" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>207</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>208</v>
       </c>
       <c r="G28" s="13"/>
       <c r="I28" s="4" t="s">
@@ -1802,16 +1814,16 @@
         <v>35</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G29" s="13"/>
       <c r="I29" s="4" t="s">
@@ -1829,19 +1841,19 @@
         <v>36</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>102</v>
       </c>
       <c r="E30" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>214</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>134</v>
@@ -1850,7 +1862,7 @@
         <v>135</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -2165,10 +2177,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D85"/>
+  <dimension ref="A2:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,7 +2217,7 @@
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2216,7 +2228,7 @@
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="32"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -2419,7 +2431,7 @@
       <c r="C26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2430,7 +2442,7 @@
       <c r="C27" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="32"/>
+      <c r="D27" s="33"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
@@ -2707,278 +2719,331 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="3" t="s">
-        <v>197</v>
+      <c r="B56" s="3">
+        <v>39</v>
       </c>
       <c r="C56" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D56" s="32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D57" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="10"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="12"/>
-    </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="1" t="s">
+      <c r="B58" s="10"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="12"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D60" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D61" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="6" t="s">
+    <row r="64" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C66" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D66" s="7" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D66" s="32" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D67" s="32"/>
+        <v>1</v>
+      </c>
+      <c r="D67" s="33" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D68" s="31" t="s">
-        <v>165</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D68" s="33"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>224</v>
+        <v>166</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D70" s="31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="D70" s="31" t="s">
+      <c r="C71" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D71" s="31" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D71" s="31" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>226</v>
+        <v>158</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D72" s="30" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="D72" s="31" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D73" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C73" s="4" t="s">
+      <c r="B74" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D73" s="30" t="s">
+      <c r="D74" s="30" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D74" s="30" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>218</v>
+        <v>51</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D75" s="30" t="s">
-        <v>219</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C76" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D76" s="30" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D76" s="30" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="3">
-        <v>46</v>
-      </c>
-      <c r="B77" s="3">
-        <v>51</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>179</v>
-      </c>
       <c r="D77" s="30" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B78" s="3">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="D78" s="30" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
+        <v>47</v>
+      </c>
+      <c r="B79" s="3">
+        <v>52</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D79" s="30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
         <v>48</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B80" s="3">
         <v>53</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="C80" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="D79" s="30" t="s">
+      <c r="D80" s="30" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C80" s="4" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3">
+        <v>54</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D81" s="32" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C82" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="30" t="s">
+      <c r="D82" s="32" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="10"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="12"/>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="1" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3">
+        <v>58</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D83" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3">
+        <v>59</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D84" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="10"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="12"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="10"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="12"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C87" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D83" s="1" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D84" s="1" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D85" s="1" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="1" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2986,7 +3051,7 @@
   <mergeCells count="3">
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="D67:D68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Working - for backup only
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="212">
   <si>
     <t>Offset</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Start code</t>
   </si>
   <si>
-    <t>0x7C</t>
-  </si>
-  <si>
     <t>0x00</t>
   </si>
   <si>
@@ -48,54 +45,24 @@
     <t>{len}</t>
   </si>
   <si>
-    <t>Length of action name</t>
-  </si>
-  <si>
-    <t>Length of header data = 124 (128 - 4)</t>
-  </si>
-  <si>
-    <t>11~40</t>
-  </si>
-  <si>
     <t>{name}</t>
   </si>
   <si>
-    <t>Action name (max 30, zero terminate)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terminator </t>
-  </si>
-  <si>
-    <t>42~47</t>
-  </si>
-  <si>
     <t>{step}</t>
   </si>
   <si>
     <t>Step count</t>
   </si>
   <si>
-    <t>50~53</t>
-  </si>
-  <si>
     <t>{time}</t>
   </si>
   <si>
-    <t>Execution time in ms (32bit)</t>
-  </si>
-  <si>
-    <t>54~69</t>
-  </si>
-  <si>
     <t>{servo}</t>
   </si>
   <si>
     <t>Affected servo</t>
   </si>
   <si>
-    <t>70~125</t>
-  </si>
-  <si>
     <t>{sum}</t>
   </si>
   <si>
@@ -123,21 +90,12 @@
     <t>04</t>
   </si>
   <si>
-    <t>05~09</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Header (128 bytes)</t>
-  </si>
-  <si>
-    <t>Pose Data (32 bytes)</t>
-  </si>
-  <si>
     <t>{seq}</t>
   </si>
   <si>
@@ -159,25 +117,7 @@
     <t>{angle}</t>
   </si>
   <si>
-    <t>Servo angle</t>
-  </si>
-  <si>
     <t>{led}</t>
-  </si>
-  <si>
-    <t>LED control flag</t>
-  </si>
-  <si>
-    <t>02~03</t>
-  </si>
-  <si>
-    <t>04~05</t>
-  </si>
-  <si>
-    <t>06~21</t>
-  </si>
-  <si>
-    <t>22~25</t>
   </si>
   <si>
     <t>Pose sequence no.</t>
@@ -310,9 +250,6 @@
     <t>Set LED</t>
   </si>
   <si>
-    <t>List&lt;id, angle,time&gt;</t>
-  </si>
-  <si>
     <t>List&lt;id&gt;</t>
   </si>
   <si>
@@ -413,9 +350,6 @@
     <t>0x61</t>
   </si>
   <si>
-    <t>Reserved (command code get header)</t>
-  </si>
-  <si>
     <t>Yes {38}</t>
   </si>
   <si>
@@ -670,9 +604,6 @@
     <t>A9 9A 04 33 ff 02 38 ED</t>
   </si>
   <si>
-    <t>06~37</t>
-  </si>
-  <si>
     <t>Servo angle (32 bytes)</t>
   </si>
   <si>
@@ -685,9 +616,6 @@
     <t>List&lt;id, on/off&gt;  (0 - ON, else - OFF)</t>
   </si>
   <si>
-    <t>49~59</t>
-  </si>
-  <si>
     <t>0x62</t>
   </si>
   <si>
@@ -709,25 +637,26 @@
     <t>43~50</t>
   </si>
   <si>
-    <t>38~45</t>
-  </si>
-  <si>
     <t>&lt;mode&gt;&lt;volume&gt;</t>
   </si>
   <si>
     <t>{mp3.vol}</t>
   </si>
   <si>
-    <t>MP3 volume</t>
-  </si>
-  <si>
-    <t>30~31</t>
-  </si>
-  <si>
     <t>MP3 volume (0xff - no change)</t>
   </si>
   <si>
     <t>55~57</t>
+  </si>
+  <si>
+    <t>Execution time in ms (32bit) - Total Wait Time</t>
+  </si>
+  <si>
+    <t>Header (60 bytes)</t>
+  </si>
+  <si>
+    <t>List&lt;id, angle,time&gt; 
+(due to 64byte buffer, max 19 servo)</t>
   </si>
 </sst>
 </file>
@@ -818,7 +747,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -840,9 +769,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1225,11 +1151,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,7 +1164,7 @@
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" style="20" customWidth="1"/>
     <col min="6" max="6" width="39.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="29" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="13.85546875" style="1" customWidth="1"/>
@@ -1252,233 +1178,233 @@
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="G3" s="14"/>
-      <c r="K3" s="15"/>
+      <c r="E3" s="21"/>
+      <c r="G3" s="13"/>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
+      <c r="E4" s="21"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="22"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
+        <v>8</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
+        <v>35</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="22"/>
+        <v>36</v>
+      </c>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="22"/>
+        <v>15</v>
+      </c>
+      <c r="E8" s="21"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="22"/>
+        <v>17</v>
+      </c>
+      <c r="E9" s="21"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>64</v>
+        <v>57</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>191</v>
+        <v>40</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>169</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>68</v>
+        <v>47</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>71</v>
+        <v>59</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="26" t="s">
-        <v>152</v>
+        <v>52</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>130</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K16" s="17" t="s">
         <v>100</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="K16" s="18" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -1486,26 +1412,26 @@
         <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>65</v>
+        <v>58</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="G17" s="4"/>
       <c r="I17" s="4" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1513,26 +1439,26 @@
         <v>12</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>99</v>
+        <v>59</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>78</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="G18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1540,26 +1466,26 @@
         <v>13</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="G19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1567,26 +1493,26 @@
         <v>14</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>99</v>
+        <v>59</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>78</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="G20" s="4"/>
       <c r="I20" s="4" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1594,26 +1520,26 @@
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>98</v>
+        <v>70</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="G21" s="4"/>
       <c r="I21" s="4" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1621,53 +1547,53 @@
         <v>22</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>98</v>
+        <v>70</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="G22" s="4"/>
       <c r="I22" s="4" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>23</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>97</v>
+        <v>70</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>211</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="G23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -1675,26 +1601,26 @@
         <v>24</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>220</v>
+        <v>70</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>197</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="G24" s="4"/>
       <c r="I24" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
@@ -1702,28 +1628,28 @@
         <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>71</v>
+        <v>113</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>199</v>
+        <v>176</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>177</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -1731,26 +1657,26 @@
         <v>32</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>65</v>
+        <v>58</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>45</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="G26" s="13"/>
+        <v>180</v>
+      </c>
+      <c r="G26" s="12"/>
       <c r="I26" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -1758,28 +1684,28 @@
         <v>33</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>214</v>
+        <v>81</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>192</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -1787,26 +1713,26 @@
         <v>34</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>206</v>
+        <v>59</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>184</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="G28" s="13"/>
+        <v>185</v>
+      </c>
+      <c r="G28" s="12"/>
       <c r="I28" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -1814,26 +1740,26 @@
         <v>35</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>206</v>
+        <v>59</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>184</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="G29" s="13"/>
+        <v>187</v>
+      </c>
+      <c r="G29" s="12"/>
       <c r="I29" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -1841,28 +1767,28 @@
         <v>36</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>230</v>
+        <v>81</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>205</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -1870,26 +1796,26 @@
         <v>41</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>7</v>
+        <v>59</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>6</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="G31" s="4"/>
       <c r="I31" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
@@ -1897,53 +1823,53 @@
         <v>42</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E32" s="27" t="s">
-        <v>182</v>
+        <v>59</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>160</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="G32" s="4"/>
       <c r="I32" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="27" t="s">
-        <v>65</v>
+        <v>58</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>45</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
@@ -1951,26 +1877,26 @@
         <v>61</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>103</v>
+        <v>59</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>82</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="G34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
@@ -1978,26 +1904,26 @@
         <v>62</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>104</v>
+        <v>81</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>83</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="G35" s="4"/>
       <c r="I35" s="4" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
@@ -2005,26 +1931,26 @@
         <v>63</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>103</v>
+        <v>59</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>82</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="G36" s="4"/>
       <c r="I36" s="4" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
@@ -2032,16 +1958,16 @@
         <v>71</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>145</v>
+        <v>99</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>123</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="G37" s="4"/>
       <c r="I37" s="4"/>
@@ -2053,12 +1979,12 @@
         <v>72</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E38" s="19"/>
+        <v>125</v>
+      </c>
+      <c r="E38" s="18"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="I38" s="4"/>
@@ -2070,34 +1996,34 @@
         <v>74</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="D39" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F39" s="17" t="s">
         <v>147</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>169</v>
       </c>
       <c r="G39" s="4"/>
       <c r="I39" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="18"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="17"/>
       <c r="G40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -2107,7 +2033,7 @@
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="19"/>
+      <c r="E41" s="18"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="I41" s="4"/>
@@ -2116,58 +2042,58 @@
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I42" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="J42" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>113</v>
+        <v>58</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>92</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="G43" s="4"/>
       <c r="I43" s="4" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2177,10 +2103,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D90"/>
+  <dimension ref="A2:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2195,863 +2121,462 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="A2" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="33"/>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>131</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D8" s="32"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="D11" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
-        <v>41</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>15</v>
+      <c r="D13" s="19" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>5</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>141</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="19" t="s">
         <v>5</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="3">
-        <v>126</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>29</v>
+        <v>15</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
+      <c r="B22" s="3">
+        <v>59</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="33" t="s">
-        <v>3</v>
+      <c r="C26" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="33"/>
+        <v>1</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>165</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D28" s="32"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>154</v>
+        <v>144</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>7</v>
+        <v>198</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>158</v>
+        <v>23</v>
       </c>
       <c r="C31" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
+        <v>51</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
+        <v>52</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="3">
+        <v>53</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <v>54</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="20" t="s">
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="3">
+        <v>58</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="3">
+        <v>59</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="9"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="11"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="9"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="11"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="3">
-        <v>28</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="3">
-        <v>29</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="3">
-        <v>58</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="3">
-        <v>59</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="12"/>
-    </row>
-    <row r="44" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="3">
-        <v>26</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D53" s="27" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="3">
-        <v>27</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D54" s="29" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="3">
-        <v>28</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D55" s="29" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="3">
-        <v>39</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="D56" s="32" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="10"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="12"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D62" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D67" s="33" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D68" s="33"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D69" s="31" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="D70" s="31" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="D71" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D72" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D73" s="30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D74" s="30" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D75" s="30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D76" s="30" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D77" s="30" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="3">
-        <v>46</v>
-      </c>
-      <c r="B78" s="3">
-        <v>51</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D78" s="30" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="3">
-        <v>47</v>
-      </c>
-      <c r="B79" s="3">
-        <v>52</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D79" s="30" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="3">
-        <v>48</v>
-      </c>
-      <c r="B80" s="3">
-        <v>53</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D80" s="30" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3">
-        <v>54</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="D81" s="32" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D82" s="32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3">
-        <v>58</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D83" s="32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3">
-        <v>59</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D84" s="32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="10"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="12"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="10"/>
-      <c r="C86" s="11"/>
-      <c r="D86" s="12"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C87" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D88" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D89" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D90" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D67:D68"/>
+  <mergeCells count="2">
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D27:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
@@ -3072,13 +2597,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="C2" s="25" t="s">
-        <v>153</v>
+      <c r="C2" s="24" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ready to save and retrieve action from SPIFFS
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="215">
   <si>
     <t>Offset</t>
   </si>
@@ -435,9 +435,6 @@
     <t>06~25</t>
   </si>
   <si>
-    <t>26~27</t>
-  </si>
-  <si>
     <t>Reserved terminator</t>
   </si>
   <si>
@@ -666,12 +663,15 @@
   </si>
   <si>
     <t xml:space="preserve">Bit-wise flag </t>
+  </si>
+  <si>
+    <t>Length of action name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -756,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -838,6 +838,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -917,7 +920,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -952,7 +955,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1163,11 +1166,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,7 +1297,7 @@
         <v>50</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>96</v>
@@ -1314,16 +1317,16 @@
         <v>59</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>46</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>113</v>
@@ -1592,7 +1595,7 @@
         <v>70</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>75</v>
@@ -1619,10 +1622,10 @@
         <v>70</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G24" s="4"/>
       <c r="I24" s="4" t="s">
@@ -1640,7 +1643,7 @@
         <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>113</v>
@@ -1649,10 +1652,10 @@
         <v>51</v>
       </c>
       <c r="F25" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G25" s="12" t="s">
         <v>176</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>177</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>112</v>
@@ -1669,7 +1672,7 @@
         <v>32</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>58</v>
@@ -1678,7 +1681,7 @@
         <v>45</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G26" s="12"/>
       <c r="I26" s="4" t="s">
@@ -1696,19 +1699,19 @@
         <v>33</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E27" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>193</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>112</v>
@@ -1725,16 +1728,16 @@
         <v>34</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E28" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>185</v>
       </c>
       <c r="G28" s="12"/>
       <c r="I28" s="4" t="s">
@@ -1752,16 +1755,16 @@
         <v>35</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G29" s="12"/>
       <c r="I29" s="4" t="s">
@@ -1779,19 +1782,19 @@
         <v>36</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F30" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>190</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>112</v>
@@ -1800,7 +1803,7 @@
         <v>113</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -1808,7 +1811,7 @@
         <v>41</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>59</v>
@@ -1817,7 +1820,7 @@
         <v>6</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G31" s="4"/>
       <c r="I31" s="4" t="s">
@@ -1835,16 +1838,16 @@
         <v>42</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G32" s="4"/>
       <c r="I32" s="4" t="s">
@@ -1859,10 +1862,10 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>165</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>58</v>
@@ -1871,7 +1874,7 @@
         <v>45</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
@@ -1889,7 +1892,7 @@
         <v>60</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>58</v>
@@ -1898,7 +1901,7 @@
         <v>45</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G34" s="4"/>
       <c r="I34" s="4" t="s">
@@ -1908,7 +1911,7 @@
         <v>95</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
@@ -1929,10 +1932,10 @@
       </c>
       <c r="G35" s="4"/>
       <c r="I35" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J35" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>119</v>
@@ -1970,7 +1973,7 @@
         <v>63</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>59</v>
@@ -2044,7 +2047,7 @@
         <v>129</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G40" s="4"/>
       <c r="I40" s="4" t="s">
@@ -2142,10 +2145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D50"/>
+  <dimension ref="A2:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,12 +2164,12 @@
   <sheetData>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
@@ -2195,7 +2198,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="34" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2206,17 +2209,17 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="33"/>
+      <c r="D8" s="34"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2264,325 +2267,331 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>138</v>
+      <c r="B14" s="3">
+        <v>26</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
+        <v>28</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
         <v>29</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D17" s="19" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>14</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>135</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="19" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="3">
-        <v>58</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
+        <v>58</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
         <v>59</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D23" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-    </row>
-    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="33" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="33"/>
+        <v>1</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>143</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D29" s="34"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>198</v>
+        <v>143</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>136</v>
+        <v>23</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>26</v>
+        <v>198</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>200</v>
+        <v>136</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="29" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="D35" s="29" t="s">
-        <v>31</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>194</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C37" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D37" s="29" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="3">
-        <v>51</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>157</v>
-      </c>
       <c r="D38" s="29" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D40" s="29" t="s">
         <v>172</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
+        <v>53</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="3">
         <v>54</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C42" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D42" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="D41" s="31" t="s">
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D42" s="31" t="s">
+      <c r="D43" s="31" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="3">
-        <v>58</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" s="31" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
+        <v>58</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="3">
         <v>59</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="31" t="s">
+      <c r="D45" s="31" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="9"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="11"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="9"/>
@@ -2590,32 +2599,37 @@
       <c r="D46" s="11"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C47" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>153</v>
-      </c>
+      <c r="B47" s="9"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="11"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="D48" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D28:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
@@ -2642,7 +2656,7 @@
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working - extend poseId & porinter to double byte, 65535 steps allowed - Split readActionFile to readActionHeader & readActionPose, where readActionPose only read the size based on buffer size, and start point based on _poseOffset - Ready for single batch upload only, - next: handling of large batch : write to disk when a batch is full - when to truncate file - write header?  append file - write pose? - poseCnt : how to handle enable flag for poseCnt, include disabled action?  if not, may affect the calculation of data size, or another count is needed.
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="219">
   <si>
     <t>Offset</t>
   </si>
@@ -268,9 +268,6 @@
     <t>actionId</t>
   </si>
   <si>
-    <t>actionId, poseId</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
@@ -383,9 +380,6 @@
     <t>Result (i.e. {parm} is result format)</t>
   </si>
   <si>
-    <t>A9 9A 04 62 01 02 69 ED</t>
-  </si>
-  <si>
     <t>A9 9A 03 63 01 67 ED</t>
   </si>
   <si>
@@ -643,9 +637,6 @@
     <t>MP3 volume (0xff - no change)</t>
   </si>
   <si>
-    <t>55~57</t>
-  </si>
-  <si>
     <t>Execution time in ms (32bit) - Total Wait Time</t>
   </si>
   <si>
@@ -666,6 +657,27 @@
   </si>
   <si>
     <t>Length of action name</t>
+  </si>
+  <si>
+    <t>{seq.high}</t>
+  </si>
+  <si>
+    <t>High byte of pose sequence no.</t>
+  </si>
+  <si>
+    <t>56~57</t>
+  </si>
+  <si>
+    <t>{step.high}</t>
+  </si>
+  <si>
+    <t>Step count HIGH byte</t>
+  </si>
+  <si>
+    <t>A9 9A 05 62 01 00 02 6A ED</t>
+  </si>
+  <si>
+    <t>actionId, poseId (2 byte HIGH, LOW)</t>
   </si>
 </sst>
 </file>
@@ -709,7 +721,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -725,6 +737,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -756,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -859,6 +877,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1167,10 +1200,10 @@
   <dimension ref="B2:O44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,13 +1330,13 @@
         <v>50</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
@@ -1317,22 +1350,22 @@
         <v>59</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>46</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J13" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
@@ -1355,13 +1388,13 @@
         <v>48</v>
       </c>
       <c r="I14" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
@@ -1381,16 +1414,16 @@
         <v>52</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I15" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="45" x14ac:dyDescent="0.25">
@@ -1413,13 +1446,13 @@
         <v>55</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -1440,13 +1473,13 @@
       </c>
       <c r="G17" s="4"/>
       <c r="I17" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1467,13 +1500,13 @@
       </c>
       <c r="G18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>59</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1494,13 +1527,13 @@
       </c>
       <c r="G19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1521,13 +1554,13 @@
       </c>
       <c r="G20" s="4"/>
       <c r="I20" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>59</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1551,10 +1584,10 @@
         <v>70</v>
       </c>
       <c r="J21" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K21" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1578,10 +1611,10 @@
         <v>70</v>
       </c>
       <c r="J22" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1595,7 +1628,7 @@
         <v>70</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>75</v>
@@ -1605,10 +1638,10 @@
         <v>70</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -1622,20 +1655,20 @@
         <v>70</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G24" s="4"/>
       <c r="I24" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J24" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="K24" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
@@ -1643,28 +1676,28 @@
         <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E25" s="28" t="s">
         <v>51</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I25" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="K25" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -1672,7 +1705,7 @@
         <v>32</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>58</v>
@@ -1681,17 +1714,17 @@
         <v>45</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G26" s="12"/>
       <c r="I26" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="K26" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -1699,28 +1732,28 @@
         <v>33</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I27" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J27" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="K27" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -1728,26 +1761,26 @@
         <v>34</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G28" s="12"/>
       <c r="I28" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J28" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="K28" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -1755,26 +1788,26 @@
         <v>35</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G29" s="12"/>
       <c r="I29" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="K29" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -1782,28 +1815,28 @@
         <v>36</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F30" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K30" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -1811,7 +1844,7 @@
         <v>41</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>59</v>
@@ -1820,17 +1853,17 @@
         <v>6</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G31" s="4"/>
       <c r="I31" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J31" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="K31" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
@@ -1838,34 +1871,34 @@
         <v>42</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E32" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>161</v>
       </c>
       <c r="G32" s="4"/>
       <c r="I32" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="K32" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>58</v>
@@ -1874,17 +1907,17 @@
         <v>45</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="K33" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
@@ -1892,7 +1925,7 @@
         <v>60</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>58</v>
@@ -1901,17 +1934,17 @@
         <v>45</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
@@ -1919,7 +1952,7 @@
         <v>61</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>59</v>
@@ -1932,13 +1965,13 @@
       </c>
       <c r="G35" s="4"/>
       <c r="I35" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
@@ -1946,53 +1979,53 @@
         <v>62</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>81</v>
+        <v>106</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>93</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>83</v>
+        <v>218</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>121</v>
+        <v>217</v>
       </c>
       <c r="G36" s="4"/>
       <c r="I36" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="J36" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="K36" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="K36" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="3">
+    </row>
+    <row r="37" spans="2:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="36">
         <v>63</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="C37" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="18" t="s">
+      <c r="E37" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G37" s="4"/>
-      <c r="I37" s="4" t="s">
+      <c r="F37" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="G37" s="37"/>
+      <c r="I37" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="J37" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>115</v>
+      <c r="J37" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="K37" s="37" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
@@ -2000,16 +2033,16 @@
         <v>71</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G38" s="4"/>
       <c r="I38" s="4"/>
@@ -2021,10 +2054,10 @@
         <v>72</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E39" s="18"/>
       <c r="F39" s="4"/>
@@ -2038,26 +2071,26 @@
         <v>74</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G40" s="4"/>
       <c r="I40" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J40" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="K40" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
@@ -2084,58 +2117,58 @@
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D43" s="4" t="s">
+      <c r="E43" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="F43" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="G43" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G43" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="I43" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J43" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="K43" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K43" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>58</v>
       </c>
       <c r="E44" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F44" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="G44" s="4"/>
       <c r="I44" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J44" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J44" s="4" t="s">
+      <c r="K44" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2145,10 +2178,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D51"/>
+  <dimension ref="A2:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,12 +2197,12 @@
   <sheetData>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
@@ -2198,7 +2231,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="35" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2209,17 +2242,17 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="35"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2227,10 +2260,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2246,7 +2279,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>4</v>
@@ -2257,13 +2290,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2274,7 +2307,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2285,7 +2318,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2304,26 +2337,26 @@
         <v>29</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>4</v>
+        <v>215</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>5</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>13</v>
@@ -2334,18 +2367,18 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>4</v>
@@ -2383,7 +2416,7 @@
     </row>
     <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2404,7 +2437,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="35" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2415,17 +2448,17 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="34"/>
+      <c r="D29" s="35"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2433,10 +2466,10 @@
         <v>22</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2444,7 +2477,7 @@
         <v>23</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>6</v>
@@ -2452,7 +2485,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>26</v>
@@ -2463,7 +2496,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>27</v>
@@ -2474,18 +2507,18 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>30</v>
@@ -2496,24 +2529,24 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
@@ -2521,10 +2554,10 @@
         <v>51</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -2532,10 +2565,10 @@
         <v>52</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D40" s="29" t="s">
         <v>170</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
@@ -2543,10 +2576,10 @@
         <v>53</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D41" s="29" t="s">
         <v>171</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
@@ -2554,49 +2587,55 @@
         <v>54</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
-        <v>207</v>
+      <c r="B43" s="3">
+        <v>55</v>
       </c>
       <c r="C43" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D43" s="34" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="31" t="s">
+      <c r="D44" s="31" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="3">
-        <v>58</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D44" s="31" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
+        <v>58</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="3">
         <v>59</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D45" s="31" t="s">
+      <c r="D46" s="31" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="11"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
@@ -2604,26 +2643,31 @@
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C48" s="1" t="s">
+      <c r="B48" s="9"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="11"/>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D50" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D51" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2651,12 +2695,12 @@
   <sheetData>
     <row r="2" spans="3:3" ht="60" x14ac:dyDescent="0.25">
       <c r="C2" s="24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ready for testing with long long action - e.g. 402 steps 江南 style.
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -878,20 +878,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1199,11 +1199,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,30 +2001,30 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="2:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="36">
+    <row r="37" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="35">
         <v>63</v>
       </c>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="D37" s="37" t="s">
+      <c r="D37" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="38" t="s">
+      <c r="E37" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="F37" s="37" t="s">
+      <c r="F37" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="G37" s="37"/>
-      <c r="I37" s="37" t="s">
+      <c r="G37" s="36"/>
+      <c r="I37" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="J37" s="37" t="s">
+      <c r="J37" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="K37" s="37" t="s">
+      <c r="K37" s="36" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2115,59 +2115,59 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
+    <row r="43" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="E43" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F43" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G43" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="I43" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="J43" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="K43" s="4" t="s">
+      <c r="K43" s="36" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
+    <row r="44" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="18" t="s">
+      <c r="E44" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="G44" s="4"/>
-      <c r="I44" s="4" t="s">
+      <c r="G44" s="36"/>
+      <c r="I44" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="J44" s="4" t="s">
+      <c r="J44" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="K44" s="4" t="s">
+      <c r="K44" s="36" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2180,7 +2180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -2231,7 +2231,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="39" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2242,7 +2242,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="39"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -2437,7 +2437,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="39" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2448,7 +2448,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="35"/>
+      <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">

</xml_diff>

<commit_message>
New command to retrieve batter level
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="224">
   <si>
     <t>Offset</t>
   </si>
@@ -592,9 +592,6 @@
     <t>&lt;folder&gt;&lt;file&gt;  (folder = 0xff =&gt; root)</t>
   </si>
   <si>
-    <t>A9 9A 04 33 ff 02 38 ED</t>
-  </si>
-  <si>
     <t>Servo angle (32 bytes)</t>
   </si>
   <si>
@@ -626,9 +623,6 @@
   </si>
   <si>
     <t>43~50</t>
-  </si>
-  <si>
-    <t>&lt;mode&gt;&lt;volume&gt;</t>
   </si>
   <si>
     <t>{mp3.vol}</t>
@@ -678,12 +672,33 @@
   </si>
   <si>
     <t>actionId, poseId (2 byte HIGH, LOW)</t>
+  </si>
+  <si>
+    <t>0B</t>
+  </si>
+  <si>
+    <t>Get batter level</t>
+  </si>
+  <si>
+    <t>A9 9A 02 0B 0D ED</t>
+  </si>
+  <si>
+    <t>Yes{3}</t>
+  </si>
+  <si>
+    <t>{%}{A0-value&lt;high,low&gt;}</t>
+  </si>
+  <si>
+    <t>A9 9A 04 33 FF 02 38 ED</t>
+  </si>
+  <si>
+    <t>&lt;mode&gt;&lt;volume&gt; (0 - set, 1 - ^, 2 - v )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -953,7 +968,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -988,7 +1003,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1197,13 +1212,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O44"/>
+  <dimension ref="B2:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,146 +1471,146 @@
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="5">
-        <v>11</v>
+      <c r="B17" s="5" t="s">
+        <v>217</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="23" t="s">
         <v>45</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="4"/>
+        <v>219</v>
+      </c>
+      <c r="G17" s="12"/>
       <c r="I17" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>101</v>
+        <v>220</v>
+      </c>
+      <c r="K17" s="17" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="3">
-        <v>14</v>
+      <c r="B20" s="5">
+        <v>13</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G20" s="4"/>
       <c r="I20" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G21" s="4"/>
       <c r="I21" s="4" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>70</v>
@@ -1604,7 +1619,7 @@
         <v>77</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G22" s="4"/>
       <c r="I22" s="4" t="s">
@@ -1617,21 +1632,21 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="23" t="s">
-        <v>207</v>
+      <c r="E23" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G23" s="4"/>
       <c r="I23" s="4" t="s">
@@ -1641,55 +1656,53 @@
         <v>96</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>194</v>
+      <c r="E24" s="23" t="s">
+        <v>205</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>175</v>
+        <v>75</v>
       </c>
       <c r="G24" s="4"/>
       <c r="I24" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>172</v>
+        <v>76</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E25" s="28" t="s">
-        <v>51</v>
+        <v>70</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>193</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>174</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="G25" s="4"/>
       <c r="I25" s="4" t="s">
         <v>111</v>
       </c>
@@ -1702,21 +1715,23 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G26" s="12"/>
+        <v>173</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>174</v>
+      </c>
       <c r="I26" s="4" t="s">
         <v>111</v>
       </c>
@@ -1729,23 +1744,21 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>189</v>
+        <v>45</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>190</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="G27" s="12"/>
       <c r="I27" s="4" t="s">
         <v>111</v>
       </c>
@@ -1758,21 +1771,23 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G28" s="12"/>
+        <v>179</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>222</v>
+      </c>
       <c r="I28" s="4" t="s">
         <v>111</v>
       </c>
@@ -1785,10 +1800,10 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>59</v>
@@ -1797,7 +1812,7 @@
         <v>181</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G29" s="12"/>
       <c r="I29" s="4" t="s">
@@ -1812,23 +1827,21 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>187</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="G30" s="12"/>
       <c r="I30" s="4" t="s">
         <v>111</v>
       </c>
@@ -1836,26 +1849,28 @@
         <v>112</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>188</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>6</v>
+        <v>81</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>223</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="G31" s="4"/>
+        <v>186</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>187</v>
+      </c>
       <c r="I31" s="4" t="s">
         <v>111</v>
       </c>
@@ -1863,24 +1878,24 @@
         <v>112</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>113</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>157</v>
+        <v>6</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G32" s="4"/>
       <c r="I32" s="4" t="s">
@@ -1894,20 +1909,20 @@
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
-        <v>161</v>
+      <c r="B33" s="3">
+        <v>42</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
@@ -1921,246 +1936,246 @@
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="3">
-        <v>60</v>
+      <c r="B34" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>208</v>
+        <v>162</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="32" t="s">
+      <c r="E34" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>209</v>
+        <v>163</v>
       </c>
       <c r="G34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>210</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>82</v>
+        <v>58</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>80</v>
+        <v>207</v>
       </c>
       <c r="G35" s="4"/>
       <c r="I35" s="4" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>118</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="25" t="s">
-        <v>93</v>
+        <v>105</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>218</v>
+        <v>82</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>217</v>
+        <v>80</v>
       </c>
       <c r="G36" s="4"/>
       <c r="I36" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
+        <v>62</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G37" s="4"/>
+      <c r="I37" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="J37" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="K36" s="4" t="s">
+      <c r="K37" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="35">
+    <row r="38" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="35">
         <v>63</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C38" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="D37" s="36" t="s">
+      <c r="D38" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="37" t="s">
+      <c r="E38" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="F37" s="36" t="s">
+      <c r="F38" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="G37" s="36"/>
-      <c r="I37" s="36" t="s">
+      <c r="G38" s="36"/>
+      <c r="I38" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="J37" s="36" t="s">
+      <c r="J38" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="K37" s="36" t="s">
+      <c r="K38" s="36" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="3">
-        <v>71</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="G39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
     </row>
-    <row r="40" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="E40" s="18"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <v>74</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E41" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="F41" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="G40" s="4"/>
-      <c r="I40" s="4" t="s">
+      <c r="G41" s="4"/>
+      <c r="I41" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="J41" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="K40" s="4" t="s">
+      <c r="K41" s="4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="4"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="17"/>
       <c r="G42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D43" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="E43" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="F43" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="G43" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="I43" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="J43" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="K43" s="36" t="s">
-        <v>113</v>
-      </c>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
     </row>
     <row r="44" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="35" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C44" s="36" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="E44" s="37" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F44" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="G44" s="36"/>
+        <v>86</v>
+      </c>
+      <c r="G44" s="36" t="s">
+        <v>87</v>
+      </c>
       <c r="I44" s="36" t="s">
         <v>111</v>
       </c>
@@ -2168,6 +2183,33 @@
         <v>112</v>
       </c>
       <c r="K44" s="36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" s="36"/>
+      <c r="I45" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="J45" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="K45" s="36" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2197,7 +2239,7 @@
   <sheetData>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2318,7 +2360,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2337,10 +2379,10 @@
         <v>29</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2351,7 +2393,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2416,7 +2458,7 @@
     </row>
     <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2466,7 +2508,7 @@
         <v>22</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D31" s="30" t="s">
         <v>130</v>
@@ -2477,7 +2519,7 @@
         <v>23</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>6</v>
@@ -2496,7 +2538,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>27</v>
@@ -2507,7 +2549,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>29</v>
@@ -2518,7 +2560,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>30</v>
@@ -2529,24 +2571,24 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
@@ -2587,10 +2629,10 @@
         <v>54</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
@@ -2598,15 +2640,15 @@
         <v>55</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D43" s="34" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
New command to delete action file
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="227">
   <si>
     <t>Offset</t>
   </si>
@@ -693,12 +693,21 @@
   </si>
   <si>
     <t>&lt;mode&gt;&lt;volume&gt; (0 - set, 1 - ^, 2 - v )</t>
+  </si>
+  <si>
+    <t>Delete action file</t>
+  </si>
+  <si>
+    <t>A9 9A 03 75 00 78 ED</t>
+  </si>
+  <si>
+    <t>{result}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -968,7 +977,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1003,7 +1012,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1215,10 +1224,10 @@
   <dimension ref="B2:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,8 +1235,8 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" style="20" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="39.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="29" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="13.85546875" style="1" customWidth="1"/>
@@ -2136,15 +2145,31 @@
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="3"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="17"/>
+      <c r="B42" s="3">
+        <v>75</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>225</v>
+      </c>
       <c r="G42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
+      <c r="I42" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>

</xml_diff>

<commit_message>
Make some command available even when action is playing, e.g. battery check, mp3 volume, stop mp3
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -496,12 +496,6 @@
     <t>Combo ID</t>
   </si>
   <si>
-    <t>A9 9A 03 41 00 43 ED</t>
-  </si>
-  <si>
-    <t>A9 9A 03 42 00 44 ED</t>
-  </si>
-  <si>
     <t>Fix {full-len}</t>
   </si>
   <si>
@@ -702,6 +696,12 @@
   </si>
   <si>
     <t>{result}</t>
+  </si>
+  <si>
+    <t>A9 9A 03 41 00 44 ED</t>
+  </si>
+  <si>
+    <t>A9 9A 03 42 00 45 ED</t>
   </si>
 </sst>
 </file>
@@ -1224,10 +1224,10 @@
   <dimension ref="B2:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B39" sqref="B39:F42"/>
+      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,7 +1354,7 @@
         <v>50</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>95</v>
@@ -1374,16 +1374,16 @@
         <v>59</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>46</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>112</v>
@@ -1481,10 +1481,10 @@
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>58</v>
@@ -1493,17 +1493,17 @@
         <v>45</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G17" s="12"/>
       <c r="I17" s="4" t="s">
         <v>110</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1679,7 +1679,7 @@
         <v>70</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>75</v>
@@ -1706,10 +1706,10 @@
         <v>70</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G25" s="4"/>
       <c r="I25" s="4" t="s">
@@ -1727,7 +1727,7 @@
         <v>31</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>112</v>
@@ -1736,10 +1736,10 @@
         <v>51</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>111</v>
@@ -1756,7 +1756,7 @@
         <v>32</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>58</v>
@@ -1765,7 +1765,7 @@
         <v>45</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G27" s="12"/>
       <c r="I27" s="4" t="s">
@@ -1783,19 +1783,19 @@
         <v>33</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>111</v>
@@ -1812,16 +1812,16 @@
         <v>34</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G29" s="12"/>
       <c r="I29" s="4" t="s">
@@ -1839,16 +1839,16 @@
         <v>35</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G30" s="12"/>
       <c r="I30" s="4" t="s">
@@ -1866,19 +1866,19 @@
         <v>36</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>111</v>
@@ -1887,7 +1887,7 @@
         <v>112</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
@@ -1904,7 +1904,7 @@
         <v>6</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>158</v>
+        <v>225</v>
       </c>
       <c r="G32" s="4"/>
       <c r="I32" s="4" t="s">
@@ -1931,7 +1931,7 @@
         <v>157</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>159</v>
+        <v>226</v>
       </c>
       <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
@@ -1946,10 +1946,10 @@
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>58</v>
@@ -1958,7 +1958,7 @@
         <v>45</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G34" s="4"/>
       <c r="I34" s="4" t="s">
@@ -1976,7 +1976,7 @@
         <v>60</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>58</v>
@@ -1985,7 +1985,7 @@
         <v>45</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G35" s="4"/>
       <c r="I35" s="4" t="s">
@@ -1995,7 +1995,7 @@
         <v>94</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
@@ -2036,10 +2036,10 @@
         <v>93</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G37" s="4"/>
       <c r="I37" s="4" t="s">
@@ -2149,7 +2149,7 @@
         <v>75</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>59</v>
@@ -2158,7 +2158,7 @@
         <v>6</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G42" s="4"/>
       <c r="I42" s="4" t="s">
@@ -2168,7 +2168,7 @@
         <v>112</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
@@ -2264,7 +2264,7 @@
   <sheetData>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2385,7 +2385,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2404,10 +2404,10 @@
         <v>29</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2418,7 +2418,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2483,7 +2483,7 @@
     </row>
     <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2533,7 +2533,7 @@
         <v>22</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D31" s="30" t="s">
         <v>130</v>
@@ -2544,7 +2544,7 @@
         <v>23</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>6</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>27</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>29</v>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>30</v>
@@ -2596,24 +2596,24 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
@@ -2624,7 +2624,7 @@
         <v>154</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -2632,10 +2632,10 @@
         <v>52</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D40" s="29" t="s">
         <v>168</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
@@ -2643,10 +2643,10 @@
         <v>53</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D41" s="29" t="s">
         <v>169</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
@@ -2654,10 +2654,10 @@
         <v>54</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
@@ -2665,15 +2665,15 @@
         <v>55</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D43" s="34" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Update for common method
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
     <sheet name="ActionData" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="CommonMethod" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="345">
   <si>
     <t>Offset</t>
   </si>
@@ -702,6 +703,360 @@
   </si>
   <si>
     <t>A9 9A 03 42 00 45 ED</t>
+  </si>
+  <si>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>init</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method </t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Close connection</t>
+  </si>
+  <si>
+    <t>Open connection</t>
+  </si>
+  <si>
+    <t>SoftwareSerial *ssData, HardwareSerial *hsDebug</t>
+  </si>
+  <si>
+    <t>Initialization</t>
+  </si>
+  <si>
+    <t>byte max_id, byte maxRetry</t>
+  </si>
+  <si>
+    <t>Constructor</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>getVersion</t>
+  </si>
+  <si>
+    <t>Get firmware version</t>
+  </si>
+  <si>
+    <t>byte id</t>
+  </si>
+  <si>
+    <t>move</t>
+  </si>
+  <si>
+    <t>Move servo</t>
+  </si>
+  <si>
+    <t>byte id, byte angle, byte time</t>
+  </si>
+  <si>
+    <t>byte cnt, byte *[{servo, angle, time}]</t>
+  </si>
+  <si>
+    <t>moveX</t>
+  </si>
+  <si>
+    <t>lock</t>
+  </si>
+  <si>
+    <t>lockX</t>
+  </si>
+  <si>
+    <t>Move multiple servos</t>
+  </si>
+  <si>
+    <t>Lock multiple servos</t>
+  </si>
+  <si>
+    <t>byte cnt, byte *[{id}]</t>
+  </si>
+  <si>
+    <t>lockAll</t>
+  </si>
+  <si>
+    <t>moveAll</t>
+  </si>
+  <si>
+    <t>Move all servos</t>
+  </si>
+  <si>
+    <t>byte angle, byte time</t>
+  </si>
+  <si>
+    <t>unlock</t>
+  </si>
+  <si>
+    <t>unlockX</t>
+  </si>
+  <si>
+    <t>unlockAll</t>
+  </si>
+  <si>
+    <t>byte id, byte mode</t>
+  </si>
+  <si>
+    <t>byte cnt, byte *[{id}], byte mode</t>
+  </si>
+  <si>
+    <t>byte mode</t>
+  </si>
+  <si>
+    <t>getPos</t>
+  </si>
+  <si>
+    <t>Get posistion</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>uint16</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>setDebug</t>
+  </si>
+  <si>
+    <t>setReturn</t>
+  </si>
+  <si>
+    <t>Set optional return</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>UBT Implementation</t>
+  </si>
+  <si>
+    <t>Set LED status</t>
+  </si>
+  <si>
+    <t>setLed</t>
+  </si>
+  <si>
+    <t>setLedX</t>
+  </si>
+  <si>
+    <t>Set multiple LED</t>
+  </si>
+  <si>
+    <t>setLedAll</t>
+  </si>
+  <si>
+    <t>Set all LED</t>
+  </si>
+  <si>
+    <t>isLocked</t>
+  </si>
+  <si>
+    <t>isExists</t>
+  </si>
+  <si>
+    <t>Check if servo is locked</t>
+  </si>
+  <si>
+    <t>Check if servo exists</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>getAdjAngle</t>
+  </si>
+  <si>
+    <t>Get current position adjustment</t>
+  </si>
+  <si>
+    <t>setAdjAngle</t>
+  </si>
+  <si>
+    <t>Set position adjustion</t>
+  </si>
+  <si>
+    <t>byte id, uint16 value</t>
+  </si>
+  <si>
+    <t>resetServo</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>detectServo</t>
+  </si>
+  <si>
+    <t>Internal detect servo status</t>
+  </si>
+  <si>
+    <t>Reset all servo</t>
+  </si>
+  <si>
+    <t>Full reset</t>
+  </si>
+  <si>
+    <t>(send get version to detect)</t>
+  </si>
+  <si>
+    <t>(seems not available)</t>
+  </si>
+  <si>
+    <t>resetServoX</t>
+  </si>
+  <si>
+    <t>Reset one servo</t>
+  </si>
+  <si>
+    <t>N/A - internal operation</t>
+  </si>
+  <si>
+    <t>N/A - internal operation ??</t>
+  </si>
+  <si>
+    <t>Not available</t>
+  </si>
+  <si>
+    <t>HiLZD</t>
+  </si>
+  <si>
+    <t>New Servo Board</t>
+  </si>
+  <si>
+    <t>** Required</t>
+  </si>
+  <si>
+    <t>FC CF {id} 01 00 00 00 00 {sum} ED</t>
+  </si>
+  <si>
+    <t>FA AF 00 01 {pos} {time} {} {} {sum} ED</t>
+  </si>
+  <si>
+    <t>NO, by result of detectServo</t>
+  </si>
+  <si>
+    <t>NO, by result of latest move/getPos operation</t>
+  </si>
+  <si>
+    <t>FA AF {id} D4 00 00 00 {sum} ED</t>
+  </si>
+  <si>
+    <t>FA AF {id} D2 {+H} {+L} {-H} {-L} {sum} ED</t>
+  </si>
+  <si>
+    <t>FA AF {id} 01 {pos} {time} {TH} {TL} {sum} ED</t>
+  </si>
+  <si>
+    <t>FA AF {id} 04 {mode} 00 00 {sum} ED</t>
+  </si>
+  <si>
+    <t>FA AF {id} 00 {mode} 00 00 {sum} ED</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>#{id}P{pos}T{time}\r\n</t>
+  </si>
+  <si>
+    <t>#{id}PRAD\r\n</t>
+  </si>
+  <si>
+    <t>Lock all servos</t>
+  </si>
+  <si>
+    <t>NO, use [getPos] then [move]</t>
+  </si>
+  <si>
+    <t>NO, use [getPos]</t>
+  </si>
+  <si>
+    <t>NO, use N x [move]</t>
+  </si>
+  <si>
+    <t>NO, use N x [setLed]</t>
+  </si>
+  <si>
+    <t>Unlock multiple servos</t>
+  </si>
+  <si>
+    <t>Unlock all servos</t>
+  </si>
+  <si>
+    <t>FA AF {id} 02 00 00 00 {sum} ED, but also unlocked</t>
+  </si>
+  <si>
+    <t>#{id}PULR\r\n</t>
+  </si>
+  <si>
+    <t>[#{id}PULR]*\r\n</t>
+  </si>
+  <si>
+    <t>[#{id}P{pos}T{time}]*\r\n</t>
+  </si>
+  <si>
+    <t>#{id}PULK\r\n</t>
+  </si>
+  <si>
+    <t>[#{id}PULK]*\r\n</t>
+  </si>
+  <si>
+    <t>Stop servo</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>stopX</t>
+  </si>
+  <si>
+    <t>stopAll</t>
+  </si>
+  <si>
+    <t>Stop multiple servo</t>
+  </si>
+  <si>
+    <t>Stop all servo</t>
+  </si>
+  <si>
+    <t>#{id}PVER\r\n</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>***?? PSCK</t>
+  </si>
+  <si>
+    <t>setBaud</t>
+  </si>
+  <si>
+    <t>Set baud rate (default 115200)</t>
+  </si>
+  <si>
+    <t>uint32 baud</t>
+  </si>
+  <si>
+    <t>getBaud</t>
+  </si>
+  <si>
+    <t>Get baud rate</t>
+  </si>
+  <si>
+    <t>uint32</t>
   </si>
 </sst>
 </file>
@@ -798,7 +1153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -914,6 +1269,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1223,8 +1580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
@@ -2298,7 +2655,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="41" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2309,7 +2666,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="39"/>
+      <c r="D8" s="41"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -2504,7 +2861,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="39" t="s">
+      <c r="D28" s="41" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2515,7 +2872,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="41"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
@@ -2773,4 +3130,787 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:J41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="40" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="J3" s="40" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E4" t="s">
+        <v>265</v>
+      </c>
+      <c r="F4" t="s">
+        <v>265</v>
+      </c>
+      <c r="H4" t="s">
+        <v>299</v>
+      </c>
+      <c r="I4" t="s">
+        <v>299</v>
+      </c>
+      <c r="J4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F5" t="s">
+        <v>265</v>
+      </c>
+      <c r="H5" t="s">
+        <v>299</v>
+      </c>
+      <c r="I5" t="s">
+        <v>299</v>
+      </c>
+      <c r="J5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>339</v>
+      </c>
+      <c r="C6" t="s">
+        <v>340</v>
+      </c>
+      <c r="D6" t="s">
+        <v>341</v>
+      </c>
+      <c r="E6" t="s">
+        <v>283</v>
+      </c>
+      <c r="F6" t="s">
+        <v>265</v>
+      </c>
+      <c r="H6" t="s">
+        <v>299</v>
+      </c>
+      <c r="I6" t="s">
+        <v>299</v>
+      </c>
+      <c r="J6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" t="s">
+        <v>343</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>344</v>
+      </c>
+      <c r="F7" t="s">
+        <v>265</v>
+      </c>
+      <c r="H7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I7" t="s">
+        <v>299</v>
+      </c>
+      <c r="J7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" t="s">
+        <v>233</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>283</v>
+      </c>
+      <c r="F8" t="s">
+        <v>265</v>
+      </c>
+      <c r="H8" t="s">
+        <v>299</v>
+      </c>
+      <c r="I8" t="s">
+        <v>299</v>
+      </c>
+      <c r="J8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>283</v>
+      </c>
+      <c r="F9" t="s">
+        <v>265</v>
+      </c>
+      <c r="H9" t="s">
+        <v>299</v>
+      </c>
+      <c r="I9" t="s">
+        <v>299</v>
+      </c>
+      <c r="J9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>290</v>
+      </c>
+      <c r="C10" t="s">
+        <v>294</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>283</v>
+      </c>
+      <c r="F10" t="s">
+        <v>265</v>
+      </c>
+      <c r="H10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" t="s">
+        <v>292</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>283</v>
+      </c>
+      <c r="F11" t="s">
+        <v>265</v>
+      </c>
+      <c r="H11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>289</v>
+      </c>
+      <c r="C12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D12" t="s">
+        <v>241</v>
+      </c>
+      <c r="E12" t="s">
+        <v>283</v>
+      </c>
+      <c r="F12" t="s">
+        <v>265</v>
+      </c>
+      <c r="H12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>297</v>
+      </c>
+      <c r="C13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>283</v>
+      </c>
+      <c r="F13" t="s">
+        <v>265</v>
+      </c>
+      <c r="H13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>268</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>261</v>
+      </c>
+      <c r="F15" t="s">
+        <v>265</v>
+      </c>
+      <c r="H15" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>269</v>
+      </c>
+      <c r="C16" t="s">
+        <v>270</v>
+      </c>
+      <c r="D16" t="s">
+        <v>261</v>
+      </c>
+      <c r="F16" t="s">
+        <v>265</v>
+      </c>
+      <c r="H16" t="s">
+        <v>301</v>
+      </c>
+      <c r="J16" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C18" t="s">
+        <v>240</v>
+      </c>
+      <c r="D18" t="s">
+        <v>241</v>
+      </c>
+      <c r="E18" t="s">
+        <v>266</v>
+      </c>
+      <c r="F18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18" t="s">
+        <v>305</v>
+      </c>
+      <c r="I18" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>242</v>
+      </c>
+      <c r="C20" t="s">
+        <v>243</v>
+      </c>
+      <c r="D20" t="s">
+        <v>244</v>
+      </c>
+      <c r="E20" t="s">
+        <v>267</v>
+      </c>
+      <c r="F20" t="s">
+        <v>123</v>
+      </c>
+      <c r="H20" t="s">
+        <v>311</v>
+      </c>
+      <c r="I20" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C21" t="s">
+        <v>249</v>
+      </c>
+      <c r="D21" t="s">
+        <v>245</v>
+      </c>
+      <c r="E21" t="s">
+        <v>267</v>
+      </c>
+      <c r="F21" t="s">
+        <v>123</v>
+      </c>
+      <c r="H21" t="s">
+        <v>320</v>
+      </c>
+      <c r="I21" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>253</v>
+      </c>
+      <c r="C22" t="s">
+        <v>254</v>
+      </c>
+      <c r="D22" t="s">
+        <v>255</v>
+      </c>
+      <c r="E22" t="s">
+        <v>267</v>
+      </c>
+      <c r="F22" t="s">
+        <v>123</v>
+      </c>
+      <c r="H22" t="s">
+        <v>306</v>
+      </c>
+      <c r="I22" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>331</v>
+      </c>
+      <c r="C23" t="s">
+        <v>330</v>
+      </c>
+      <c r="D23" t="s">
+        <v>241</v>
+      </c>
+      <c r="E23" t="s">
+        <v>267</v>
+      </c>
+      <c r="F23" t="s">
+        <v>123</v>
+      </c>
+      <c r="H23" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>332</v>
+      </c>
+      <c r="C24" t="s">
+        <v>334</v>
+      </c>
+      <c r="D24" t="s">
+        <v>251</v>
+      </c>
+      <c r="E24" t="s">
+        <v>267</v>
+      </c>
+      <c r="F24" t="s">
+        <v>123</v>
+      </c>
+      <c r="H24" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>333</v>
+      </c>
+      <c r="C25" t="s">
+        <v>335</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>267</v>
+      </c>
+      <c r="F25" t="s">
+        <v>123</v>
+      </c>
+      <c r="H25" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>247</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>241</v>
+      </c>
+      <c r="E27" t="s">
+        <v>267</v>
+      </c>
+      <c r="F27" t="s">
+        <v>123</v>
+      </c>
+      <c r="H27" t="s">
+        <v>318</v>
+      </c>
+      <c r="I27" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>248</v>
+      </c>
+      <c r="C28" t="s">
+        <v>250</v>
+      </c>
+      <c r="D28" t="s">
+        <v>251</v>
+      </c>
+      <c r="E28" t="s">
+        <v>267</v>
+      </c>
+      <c r="F28" t="s">
+        <v>123</v>
+      </c>
+      <c r="H28" t="s">
+        <v>318</v>
+      </c>
+      <c r="I28" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>252</v>
+      </c>
+      <c r="C29" t="s">
+        <v>317</v>
+      </c>
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" t="s">
+        <v>267</v>
+      </c>
+      <c r="F29" t="s">
+        <v>123</v>
+      </c>
+      <c r="H29" t="s">
+        <v>318</v>
+      </c>
+      <c r="I29" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>256</v>
+      </c>
+      <c r="C30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" t="s">
+        <v>241</v>
+      </c>
+      <c r="E30" t="s">
+        <v>267</v>
+      </c>
+      <c r="F30" t="s">
+        <v>123</v>
+      </c>
+      <c r="H30" t="s">
+        <v>319</v>
+      </c>
+      <c r="I30" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>257</v>
+      </c>
+      <c r="C31" t="s">
+        <v>322</v>
+      </c>
+      <c r="D31" t="s">
+        <v>251</v>
+      </c>
+      <c r="E31" t="s">
+        <v>267</v>
+      </c>
+      <c r="F31" t="s">
+        <v>123</v>
+      </c>
+      <c r="H31" t="s">
+        <v>319</v>
+      </c>
+      <c r="I31" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>258</v>
+      </c>
+      <c r="C32" t="s">
+        <v>323</v>
+      </c>
+      <c r="D32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" t="s">
+        <v>267</v>
+      </c>
+      <c r="F32" t="s">
+        <v>123</v>
+      </c>
+      <c r="H32" t="s">
+        <v>319</v>
+      </c>
+      <c r="I32" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>274</v>
+      </c>
+      <c r="C33" t="s">
+        <v>273</v>
+      </c>
+      <c r="D33" t="s">
+        <v>259</v>
+      </c>
+      <c r="E33" t="s">
+        <v>267</v>
+      </c>
+      <c r="F33" t="s">
+        <v>123</v>
+      </c>
+      <c r="H33" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>275</v>
+      </c>
+      <c r="C34" t="s">
+        <v>276</v>
+      </c>
+      <c r="D34" t="s">
+        <v>260</v>
+      </c>
+      <c r="E34" t="s">
+        <v>267</v>
+      </c>
+      <c r="F34" t="s">
+        <v>123</v>
+      </c>
+      <c r="H34" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>277</v>
+      </c>
+      <c r="C35" t="s">
+        <v>278</v>
+      </c>
+      <c r="D35" t="s">
+        <v>261</v>
+      </c>
+      <c r="E35" t="s">
+        <v>267</v>
+      </c>
+      <c r="F35" t="s">
+        <v>123</v>
+      </c>
+      <c r="H35" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>286</v>
+      </c>
+      <c r="C36" t="s">
+        <v>287</v>
+      </c>
+      <c r="D36" t="s">
+        <v>288</v>
+      </c>
+      <c r="E36" t="s">
+        <v>267</v>
+      </c>
+      <c r="F36" t="s">
+        <v>123</v>
+      </c>
+      <c r="H36" t="s">
+        <v>310</v>
+      </c>
+      <c r="I36" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>262</v>
+      </c>
+      <c r="C38" t="s">
+        <v>263</v>
+      </c>
+      <c r="D38" t="s">
+        <v>241</v>
+      </c>
+      <c r="E38" t="s">
+        <v>267</v>
+      </c>
+      <c r="F38" t="s">
+        <v>70</v>
+      </c>
+      <c r="H38" t="s">
+        <v>324</v>
+      </c>
+      <c r="I38" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>279</v>
+      </c>
+      <c r="C39" t="s">
+        <v>281</v>
+      </c>
+      <c r="D39" t="s">
+        <v>241</v>
+      </c>
+      <c r="E39" t="s">
+        <v>283</v>
+      </c>
+      <c r="F39" t="s">
+        <v>70</v>
+      </c>
+      <c r="H39" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>280</v>
+      </c>
+      <c r="C40" t="s">
+        <v>282</v>
+      </c>
+      <c r="D40" t="s">
+        <v>241</v>
+      </c>
+      <c r="E40" t="s">
+        <v>283</v>
+      </c>
+      <c r="F40" t="s">
+        <v>70</v>
+      </c>
+      <c r="H40" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>284</v>
+      </c>
+      <c r="C41" t="s">
+        <v>285</v>
+      </c>
+      <c r="D41" t="s">
+        <v>241</v>
+      </c>
+      <c r="E41" t="s">
+        <v>266</v>
+      </c>
+      <c r="F41" t="s">
+        <v>70</v>
+      </c>
+      <c r="H41" t="s">
+        <v>309</v>
+      </c>
+      <c r="I41" t="s">
+        <v>337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Missing feature: Set adjust angle
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="347">
   <si>
     <t>Offset</t>
   </si>
@@ -1057,6 +1057,12 @@
   </si>
   <si>
     <t>uint32</t>
+  </si>
+  <si>
+    <t>Set adjustment</t>
+  </si>
+  <si>
+    <t>A9 9A 05 15 01 FF E8 02 ED</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1271,6 +1277,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1578,13 +1587,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O45"/>
+  <dimension ref="B2:O46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,37 +1982,31 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>77</v>
-      </c>
+        <v>345</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="41"/>
       <c r="F22" s="4" t="s">
-        <v>71</v>
+        <v>346</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="I22" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="I22" s="4"/>
       <c r="J22" s="4" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>70</v>
@@ -2012,7 +2015,7 @@
         <v>77</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G23" s="4"/>
       <c r="I23" s="4" t="s">
@@ -2025,21 +2028,21 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="23" t="s">
-        <v>203</v>
+      <c r="E24" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G24" s="4"/>
       <c r="I24" s="4" t="s">
@@ -2049,55 +2052,53 @@
         <v>96</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="18" t="s">
-        <v>191</v>
+      <c r="E25" s="23" t="s">
+        <v>203</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>173</v>
+        <v>75</v>
       </c>
       <c r="G25" s="4"/>
       <c r="I25" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>170</v>
+        <v>76</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>51</v>
+        <v>70</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>172</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="G26" s="4"/>
       <c r="I26" s="4" t="s">
         <v>111</v>
       </c>
@@ -2110,21 +2111,23 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G27" s="12"/>
+        <v>171</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>172</v>
+      </c>
       <c r="I27" s="4" t="s">
         <v>111</v>
       </c>
@@ -2137,23 +2140,21 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>187</v>
+        <v>45</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>220</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="G28" s="12"/>
       <c r="I28" s="4" t="s">
         <v>111</v>
       </c>
@@ -2166,21 +2167,23 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="G29" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>220</v>
+      </c>
       <c r="I29" s="4" t="s">
         <v>111</v>
       </c>
@@ -2193,10 +2196,10 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>59</v>
@@ -2205,7 +2208,7 @@
         <v>179</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G30" s="12"/>
       <c r="I30" s="4" t="s">
@@ -2220,23 +2223,21 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>185</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="G31" s="12"/>
       <c r="I31" s="4" t="s">
         <v>111</v>
       </c>
@@ -2244,26 +2245,28 @@
         <v>112</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>186</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E32" s="26" t="s">
-        <v>6</v>
+        <v>81</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>221</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="G32" s="4"/>
+        <v>184</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="I32" s="4" t="s">
         <v>111</v>
       </c>
@@ -2271,24 +2274,24 @@
         <v>112</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>157</v>
+        <v>6</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
@@ -2302,20 +2305,20 @@
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
-        <v>159</v>
+      <c r="B34" s="3">
+        <v>42</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>161</v>
+        <v>226</v>
       </c>
       <c r="G34" s="4"/>
       <c r="I34" s="4" t="s">
@@ -2329,193 +2332,193 @@
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="3">
-        <v>60</v>
+      <c r="B35" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>204</v>
+        <v>160</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="32" t="s">
+      <c r="E35" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>205</v>
+        <v>161</v>
       </c>
       <c r="G35" s="4"/>
       <c r="I35" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>206</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>82</v>
+        <v>58</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>80</v>
+        <v>205</v>
       </c>
       <c r="G36" s="4"/>
       <c r="I36" s="4" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>118</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>93</v>
+        <v>105</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>214</v>
+        <v>82</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>213</v>
+        <v>80</v>
       </c>
       <c r="G37" s="4"/>
       <c r="I37" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
+        <v>62</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="I38" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="J38" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="K37" s="4" t="s">
+      <c r="K38" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="35">
+    <row r="39" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="35">
         <v>63</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C39" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="D38" s="36" t="s">
+      <c r="D39" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E38" s="37" t="s">
+      <c r="E39" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="F38" s="36" t="s">
+      <c r="F39" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="G38" s="36"/>
-      <c r="I38" s="36" t="s">
+      <c r="G39" s="36"/>
+      <c r="I39" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="J38" s="36" t="s">
+      <c r="J39" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="K38" s="36" t="s">
+      <c r="K39" s="36" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="3">
-        <v>71</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E39" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E40" s="18"/>
-      <c r="F40" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="G40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
     </row>
-    <row r="41" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E41" s="18"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="3">
+        <v>74</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="F42" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="G41" s="4"/>
-      <c r="I41" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="3">
-        <v>75</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E42" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>223</v>
       </c>
       <c r="G42" s="4"/>
       <c r="I42" s="4" t="s">
@@ -2525,66 +2528,66 @@
         <v>112</v>
       </c>
       <c r="K42" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="3">
+        <v>75</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G43" s="4"/>
+      <c r="I43" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K43" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="3"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-    </row>
-    <row r="44" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D44" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="E44" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="F44" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="G44" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="I44" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="J44" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="K44" s="36" t="s">
-        <v>113</v>
-      </c>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
     </row>
     <row r="45" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="35" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D45" s="36" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="E45" s="37" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F45" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="G45" s="36"/>
+        <v>86</v>
+      </c>
+      <c r="G45" s="36" t="s">
+        <v>87</v>
+      </c>
       <c r="I45" s="36" t="s">
         <v>111</v>
       </c>
@@ -2592,6 +2595,33 @@
         <v>112</v>
       </c>
       <c r="K45" s="36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="F46" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" s="36"/>
+      <c r="I46" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="J46" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="K46" s="36" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2655,7 +2685,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="42" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2666,7 +2696,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="41"/>
+      <c r="D8" s="42"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -2861,7 +2891,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="41" t="s">
+      <c r="D28" s="42" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2872,7 +2902,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="41"/>
+      <c r="D29" s="42"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
@@ -3136,7 +3166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- Working on combo - Clean up obsolete V1 code
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
-    <sheet name="ActionData" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="CommonMethod" sheetId="4" r:id="rId4"/>
+    <sheet name="Combo" sheetId="5" r:id="rId2"/>
+    <sheet name="ActionData" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="CommonMethod" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="359">
   <si>
     <t>Offset</t>
   </si>
@@ -1063,6 +1064,42 @@
   </si>
   <si>
     <t>A9 9A 05 15 01 FF E8 02 ED</t>
+  </si>
+  <si>
+    <t>Get combo detail</t>
+  </si>
+  <si>
+    <t>A9 9A 03 68 01 6B ED</t>
+  </si>
+  <si>
+    <t>** full result = {comboData}</t>
+  </si>
+  <si>
+    <t>0x68</t>
+  </si>
+  <si>
+    <t>Combo Seq No</t>
+  </si>
+  <si>
+    <t>10~49</t>
+  </si>
+  <si>
+    <t>50~57</t>
+  </si>
+  <si>
+    <t>Combo Detail {actionId, repeatCount}</t>
+  </si>
+  <si>
+    <t>{actionId, repeatCount} x 20</t>
+  </si>
+  <si>
+    <t>05~09</t>
+  </si>
+  <si>
+    <t>Set combo detail</t>
+  </si>
+  <si>
+    <t>A9 9A 03 69 01 6C ED</t>
   </si>
 </sst>
 </file>
@@ -1159,7 +1196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1277,6 +1314,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1587,13 +1627,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O46"/>
+  <dimension ref="B2:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
+      <selection pane="bottomRight" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2468,160 +2508,210 @@
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>121</v>
+        <v>347</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" s="42" t="s">
+        <v>214</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>122</v>
+        <v>348</v>
       </c>
       <c r="G40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
+      <c r="I40" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E41" s="18"/>
-      <c r="F41" s="4"/>
+        <v>357</v>
+      </c>
+      <c r="D41" s="25"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="4" t="s">
+        <v>358</v>
+      </c>
       <c r="G41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-    </row>
-    <row r="42" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="I41" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="3">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="F42" s="17" t="s">
-        <v>144</v>
+        <v>121</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="G42" s="4"/>
-      <c r="I42" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>113</v>
-      </c>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
+        <v>72</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E43" s="18"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="3">
+        <v>74</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G44" s="4"/>
+      <c r="I44" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="3">
         <v>75</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="26" t="s">
+      <c r="E45" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F45" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="G43" s="4"/>
-      <c r="I43" s="4" t="s">
+      <c r="G45" s="4"/>
+      <c r="I45" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="J45" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="K43" s="4" t="s">
+      <c r="K45" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="3"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-    </row>
-    <row r="45" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="35" t="s">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="3"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C45" s="36" t="s">
+      <c r="C47" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D45" s="36" t="s">
+      <c r="D47" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="E45" s="37" t="s">
+      <c r="E47" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="F45" s="36" t="s">
+      <c r="F47" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="G45" s="36" t="s">
+      <c r="G47" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="I45" s="36" t="s">
+      <c r="I47" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="J45" s="36" t="s">
+      <c r="J47" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="K45" s="36" t="s">
+      <c r="K47" s="36" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="35" t="s">
+    <row r="48" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="36" t="s">
+      <c r="C48" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="36" t="s">
+      <c r="D48" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E46" s="37" t="s">
+      <c r="E48" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="F46" s="36" t="s">
+      <c r="F48" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="G46" s="36"/>
-      <c r="I46" s="36" t="s">
+      <c r="G48" s="36"/>
+      <c r="I48" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="J46" s="36" t="s">
+      <c r="J48" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="K46" s="36" t="s">
+      <c r="K48" s="36" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2632,10 +2722,152 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="43"/>
+    </row>
+    <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>58</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>59</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2685,7 +2917,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="43" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2696,7 +2928,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="42"/>
+      <c r="D8" s="43"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -2891,7 +3123,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="43" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2902,7 +3134,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="42"/>
+      <c r="D29" s="43"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
@@ -3134,7 +3366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:C5"/>
   <sheetViews>
@@ -3162,7 +3394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J41"/>
   <sheetViews>

</xml_diff>

<commit_message>
Enhace robot config with more config options, will be added into Windows UI later
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -2,23 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
-    <sheet name="Combo" sheetId="5" r:id="rId2"/>
-    <sheet name="ActionData" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
-    <sheet name="CommonMethod" sheetId="4" r:id="rId5"/>
+    <sheet name="ConfigData" sheetId="6" r:id="rId2"/>
+    <sheet name="ComboData" sheetId="5" r:id="rId3"/>
+    <sheet name="ActionData" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="CommonMethod" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="424">
   <si>
     <t>Offset</t>
   </si>
@@ -1072,9 +1073,6 @@
     <t>A9 9A 03 68 01 6B ED</t>
   </si>
   <si>
-    <t>** full result = {comboData}</t>
-  </si>
-  <si>
     <t>0x68</t>
   </si>
   <si>
@@ -1099,7 +1097,205 @@
     <t>Set combo detail</t>
   </si>
   <si>
-    <t>A9 9A 03 69 01 6C ED</t>
+    <t>{version}</t>
+  </si>
+  <si>
+    <t>Version No.</t>
+  </si>
+  <si>
+    <t>{debug}</t>
+  </si>
+  <si>
+    <t>Enable debug at startup</t>
+  </si>
+  <si>
+    <t>10~11</t>
+  </si>
+  <si>
+    <t>{refVol}</t>
+  </si>
+  <si>
+    <t>Reference voltage</t>
+  </si>
+  <si>
+    <t>12~13</t>
+  </si>
+  <si>
+    <t>{minVol}</t>
+  </si>
+  <si>
+    <t>14~15</t>
+  </si>
+  <si>
+    <t>{maxVol}</t>
+  </si>
+  <si>
+    <t>Voltage Low = 0%</t>
+  </si>
+  <si>
+    <t>Voltage High = 100%</t>
+  </si>
+  <si>
+    <t>16~17</t>
+  </si>
+  <si>
+    <t>{almVol}</t>
+  </si>
+  <si>
+    <t>Alarm if voltage less than this v alue</t>
+  </si>
+  <si>
+    <t>{maxServo}</t>
+  </si>
+  <si>
+    <t>Maximum number of servo</t>
+  </si>
+  <si>
+    <t>{maxDetect}</t>
+  </si>
+  <si>
+    <t>Maximum retry in detecting servo</t>
+  </si>
+  <si>
+    <t>{cmdTimeout}</t>
+  </si>
+  <si>
+    <t>Wait ms for command time</t>
+  </si>
+  <si>
+    <t>{cmdRetry}</t>
+  </si>
+  <si>
+    <t>Maximum number of retry for caommand failture</t>
+  </si>
+  <si>
+    <t>{MP3}</t>
+  </si>
+  <si>
+    <t>MP3 enable</t>
+  </si>
+  <si>
+    <t>{MP3Vol}</t>
+  </si>
+  <si>
+    <t>Default MP3 volume</t>
+  </si>
+  <si>
+    <t>{MP3Start}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MP3 to be play at startup </t>
+  </si>
+  <si>
+    <t>{router}</t>
+  </si>
+  <si>
+    <t>Try to connect router at startup</t>
+  </si>
+  <si>
+    <t>{autoStand}</t>
+  </si>
+  <si>
+    <t>Try to standup if fall down</t>
+  </si>
+  <si>
+    <t>{faceUp}</t>
+  </si>
+  <si>
+    <t>{faceDown}</t>
+  </si>
+  <si>
+    <t>Standup action for face down</t>
+  </si>
+  <si>
+    <t>Standup action for face up</t>
+  </si>
+  <si>
+    <t>#define</t>
+  </si>
+  <si>
+    <t>RC_VERSION</t>
+  </si>
+  <si>
+    <t>RC_ENABLE_DEBUG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC_REF_VOLTAGE         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC_MIN_VOLTAGE         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC_MAX_VOLTAGE         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC_ALARM_VOLTAGE       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC_MAX_SERVO           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC_MAX_DETECT_RETRY    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC_MAX_COMMAND_WAIT_MS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC_MAX_COMMAND_RETRY   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC_MP3_ENABLED         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC_MP3_VOLUME          </t>
+  </si>
+  <si>
+    <t>RC_MP3_STARTUP</t>
+  </si>
+  <si>
+    <t>RC_AUTO_STAND</t>
+  </si>
+  <si>
+    <t>RC_CONNECT_ROUTER</t>
+  </si>
+  <si>
+    <t>RC_AUTO_FACE_UP</t>
+  </si>
+  <si>
+    <t>RC_AUTO_FACE_DOWN</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>{OLED}</t>
+  </si>
+  <si>
+    <t>Enable OLED (I2C connected)</t>
+  </si>
+  <si>
+    <t>RC_ENABLE_OLED</t>
+  </si>
+  <si>
+    <t>Get robot config</t>
+  </si>
+  <si>
+    <t>Set robot config</t>
+  </si>
+  <si>
+    <t>{Refer to ComboData}</t>
+  </si>
+  <si>
+    <t>A9 9A 02 04 06 ED</t>
+  </si>
+  <si>
+    <t>{amInterval}</t>
+  </si>
+  <si>
+    <t>Alarm interval in second</t>
+  </si>
+  <si>
+    <t>RC_ARARM_INTERVAL</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1320,6 +1516,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1627,13 +1830,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O48"/>
+  <dimension ref="B2:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A42" sqref="A42"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,7 +2046,7 @@
       <c r="F15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="4" t="s">
         <v>128</v>
       </c>
       <c r="I15" s="4" t="s">
@@ -1856,122 +2059,114 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>56</v>
-      </c>
+        <v>417</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>55</v>
-      </c>
+        <v>420</v>
+      </c>
+      <c r="G16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>99</v>
+        <v>143</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D19" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E19" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="I17" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="5">
-        <v>11</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="I18" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="5">
-        <v>12</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="12"/>
       <c r="I19" s="4" t="s">
         <v>110</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>100</v>
+        <v>218</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>58</v>
@@ -1980,7 +2175,7 @@
         <v>45</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G20" s="4"/>
       <c r="I20" s="4" t="s">
@@ -1990,15 +2185,15 @@
         <v>94</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="3">
-        <v>14</v>
+      <c r="B21" s="5">
+        <v>12</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>59</v>
@@ -2007,7 +2202,7 @@
         <v>78</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G21" s="4"/>
       <c r="I21" s="4" t="s">
@@ -2017,99 +2212,99 @@
         <v>59</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="3">
-        <v>15</v>
+      <c r="B22" s="5">
+        <v>13</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="41"/>
+        <v>63</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="F22" s="4" t="s">
-        <v>346</v>
+        <v>65</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="I22" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="J22" s="4" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>77</v>
-      </c>
+        <v>345</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="41"/>
       <c r="F24" s="4" t="s">
-        <v>73</v>
+        <v>346</v>
       </c>
       <c r="G24" s="4"/>
-      <c r="I24" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="23" t="s">
-        <v>203</v>
+      <c r="E25" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G25" s="4"/>
       <c r="I25" s="4" t="s">
@@ -2119,82 +2314,80 @@
         <v>96</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>70</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>191</v>
+        <v>77</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="G26" s="4"/>
       <c r="I26" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>170</v>
+        <v>74</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>51</v>
+        <v>70</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>203</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>172</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="G27" s="4"/>
       <c r="I27" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>174</v>
+        <v>76</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>45</v>
+        <v>70</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G28" s="12"/>
+        <v>173</v>
+      </c>
+      <c r="G28" s="4"/>
       <c r="I28" s="4" t="s">
         <v>111</v>
       </c>
@@ -2207,22 +2400,22 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>187</v>
+        <v>51</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>220</v>
+        <v>171</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>172</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>111</v>
@@ -2236,19 +2429,19 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>179</v>
+        <v>45</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="G30" s="12"/>
       <c r="I30" s="4" t="s">
@@ -2263,21 +2456,23 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G31" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>220</v>
+      </c>
       <c r="I31" s="4" t="s">
         <v>111</v>
       </c>
@@ -2290,23 +2485,21 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>185</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="G32" s="12"/>
       <c r="I32" s="4" t="s">
         <v>111</v>
       </c>
@@ -2314,26 +2507,26 @@
         <v>112</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>186</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="26" t="s">
-        <v>6</v>
+      <c r="E33" s="28" t="s">
+        <v>179</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="G33" s="4"/>
+        <v>182</v>
+      </c>
+      <c r="G33" s="12"/>
       <c r="I33" s="4" t="s">
         <v>111</v>
       </c>
@@ -2346,21 +2539,23 @@
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>156</v>
+        <v>183</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="26" t="s">
-        <v>157</v>
+        <v>81</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>221</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="G34" s="4"/>
+        <v>184</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="I34" s="4" t="s">
         <v>111</v>
       </c>
@@ -2368,24 +2563,24 @@
         <v>112</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="3" t="s">
-        <v>159</v>
+      <c r="B35" s="3">
+        <v>41</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>161</v>
+        <v>225</v>
       </c>
       <c r="G35" s="4"/>
       <c r="I35" s="4" t="s">
@@ -2400,318 +2595,372 @@
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E36" s="32" t="s">
-        <v>45</v>
+        <v>59</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>157</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="G36" s="4"/>
       <c r="I36" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>206</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="3">
-        <v>61</v>
+      <c r="B37" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>105</v>
+        <v>160</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>82</v>
+        <v>58</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>45</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>80</v>
+        <v>161</v>
       </c>
       <c r="G37" s="4"/>
       <c r="I37" s="4" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="3">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>214</v>
+        <v>204</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="G38" s="4"/>
       <c r="I38" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="35">
-        <v>63</v>
-      </c>
-      <c r="C39" s="36" t="s">
-        <v>146</v>
-      </c>
-      <c r="D39" s="36" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
+        <v>61</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="37" t="s">
+      <c r="E39" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F39" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="G39" s="36"/>
-      <c r="I39" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="J39" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="K39" s="36" t="s">
-        <v>114</v>
+      <c r="F39" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G39" s="4"/>
+      <c r="I39" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>347</v>
+        <v>106</v>
       </c>
       <c r="D40" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="E40" s="42" t="s">
+      <c r="E40" s="18" t="s">
         <v>214</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>348</v>
+        <v>213</v>
       </c>
       <c r="G40" s="4"/>
       <c r="I40" s="4" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="3">
-        <v>69</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D41" s="25"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="G41" s="4"/>
-      <c r="I41" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>349</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="35">
+        <v>63</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="G41" s="36"/>
+      <c r="I41" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="J41" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="K41" s="36" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="3">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E42" s="18" t="s">
-        <v>121</v>
+        <v>347</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" s="42" t="s">
+        <v>214</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>122</v>
+        <v>348</v>
       </c>
       <c r="G42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
+      <c r="I42" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E43" s="18"/>
-      <c r="F43" s="4"/>
+        <v>356</v>
+      </c>
+      <c r="D43" s="25"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="4" t="s">
+        <v>419</v>
+      </c>
       <c r="G43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-    </row>
-    <row r="44" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="I43" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>144</v>
+        <v>121</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="G44" s="4"/>
-      <c r="I44" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>113</v>
-      </c>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
+        <v>72</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E45" s="18"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+    </row>
+    <row r="46" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="3">
+        <v>74</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G46" s="4"/>
+      <c r="I46" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="3">
         <v>75</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C47" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="26" t="s">
+      <c r="E47" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F47" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="G45" s="4"/>
-      <c r="I45" s="4" t="s">
+      <c r="G47" s="4"/>
+      <c r="I47" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="J45" s="4" t="s">
+      <c r="J47" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="K47" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-    </row>
-    <row r="47" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="35" t="s">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+    </row>
+    <row r="49" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="36" t="s">
+      <c r="C49" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D47" s="36" t="s">
+      <c r="D49" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="E47" s="37" t="s">
+      <c r="E49" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="F47" s="36" t="s">
+      <c r="F49" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="G47" s="36" t="s">
+      <c r="G49" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="I47" s="36" t="s">
+      <c r="I49" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="J47" s="36" t="s">
+      <c r="J49" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="K47" s="36" t="s">
+      <c r="K49" s="36" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="35" t="s">
+    <row r="50" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="36" t="s">
+      <c r="C50" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="D48" s="36" t="s">
+      <c r="D50" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E48" s="37" t="s">
+      <c r="E50" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="F48" s="36" t="s">
+      <c r="F50" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="G48" s="36"/>
-      <c r="I48" s="36" t="s">
+      <c r="G50" s="36"/>
+      <c r="I50" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="J48" s="36" t="s">
+      <c r="J50" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="K48" s="36" t="s">
+      <c r="K50" s="36" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2722,10 +2971,384 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="45"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="45"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="45"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="45"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>358</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>360</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>388</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>415</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>363</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>368</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>369</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>372</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <v>18</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>422</v>
+      </c>
+      <c r="E15" s="45" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <v>21</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>374</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>22</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>376</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>23</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>378</v>
+      </c>
+      <c r="E18" s="45" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>24</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>380</v>
+      </c>
+      <c r="E19" s="45" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>31</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="D20" s="43" t="s">
+        <v>382</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <v>32</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>384</v>
+      </c>
+      <c r="E21" s="45" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>33</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>386</v>
+      </c>
+      <c r="E22" s="45" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>41</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="D23" s="43" t="s">
+        <v>390</v>
+      </c>
+      <c r="E23" s="45" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
+        <v>42</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>394</v>
+      </c>
+      <c r="E24" s="45" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
+        <v>43</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D25" s="43" t="s">
+        <v>393</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
+        <v>58</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="45"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
+        <v>59</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="45"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2753,7 +3376,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="46" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2764,7 +3387,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="43"/>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
@@ -2782,7 +3405,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D6" s="42" t="s">
         <v>130</v>
@@ -2796,12 +3419,12 @@
         <v>26</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
@@ -2812,18 +3435,18 @@
     </row>
     <row r="9" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
@@ -2862,7 +3485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D52"/>
   <sheetViews>
@@ -2917,7 +3540,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="46" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2928,7 +3551,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="43"/>
+      <c r="D8" s="46"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -3123,7 +3746,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="43" t="s">
+      <c r="D28" s="46" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3134,7 +3757,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="43"/>
+      <c r="D29" s="46"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
@@ -3366,7 +3989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:C5"/>
   <sheetViews>
@@ -3394,7 +4017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J41"/>
   <sheetViews>

</xml_diff>

<commit_message>
Working on Combo - get combo ready
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -1094,9 +1094,6 @@
     <t>05~09</t>
   </si>
   <si>
-    <t>Set combo detail</t>
-  </si>
-  <si>
     <t>{version}</t>
   </si>
   <si>
@@ -1296,6 +1293,9 @@
   </si>
   <si>
     <t>RC_ARARM_INTERVAL</t>
+  </si>
+  <si>
+    <t>Update combo</t>
   </si>
 </sst>
 </file>
@@ -1836,7 +1836,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,12 +2064,12 @@
         <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="43"/>
       <c r="F16" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G16" s="4"/>
       <c r="I16" s="4" t="s">
@@ -2079,7 +2079,7 @@
         <v>143</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -2087,12 +2087,12 @@
         <v>134</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="43"/>
       <c r="F17" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G17" s="4"/>
       <c r="I17" s="4" t="s">
@@ -2779,7 +2779,7 @@
         <v>143</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
@@ -2787,12 +2787,12 @@
         <v>69</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>356</v>
+        <v>423</v>
       </c>
       <c r="D43" s="25"/>
       <c r="E43" s="42"/>
       <c r="F43" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G43" s="4"/>
       <c r="I43" s="4" t="s">
@@ -2973,8 +2973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,7 +2996,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -3050,13 +3050,13 @@
         <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D7" s="43" t="s">
         <v>357</v>
       </c>
-      <c r="D7" s="43" t="s">
-        <v>358</v>
-      </c>
       <c r="E7" s="45" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -3064,13 +3064,13 @@
         <v>134</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="D8" s="43" t="s">
         <v>359</v>
       </c>
-      <c r="D8" s="43" t="s">
-        <v>360</v>
-      </c>
       <c r="E8" s="45" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -3078,83 +3078,83 @@
         <v>194</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="D9" s="43" t="s">
         <v>387</v>
       </c>
-      <c r="D9" s="43" t="s">
-        <v>388</v>
-      </c>
       <c r="E9" s="45" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="43" t="s">
         <v>414</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="E10" s="45" t="s">
         <v>415</v>
-      </c>
-      <c r="E10" s="45" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="43" t="s">
         <v>362</v>
       </c>
-      <c r="D11" s="43" t="s">
-        <v>363</v>
-      </c>
       <c r="E11" s="45" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>365</v>
-      </c>
       <c r="D12" s="43" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E12" s="45" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>367</v>
-      </c>
       <c r="D13" s="43" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E13" s="45" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="43" t="s">
         <v>371</v>
       </c>
-      <c r="D14" s="43" t="s">
-        <v>372</v>
-      </c>
       <c r="E14" s="45" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -3162,13 +3162,13 @@
         <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="D15" s="44" t="s">
         <v>421</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="E15" s="45" t="s">
         <v>422</v>
-      </c>
-      <c r="E15" s="45" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -3176,13 +3176,13 @@
         <v>21</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="D16" s="43" t="s">
         <v>373</v>
       </c>
-      <c r="D16" s="43" t="s">
-        <v>374</v>
-      </c>
       <c r="E16" s="45" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -3190,13 +3190,13 @@
         <v>22</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D17" s="43" t="s">
         <v>375</v>
       </c>
-      <c r="D17" s="43" t="s">
-        <v>376</v>
-      </c>
       <c r="E17" s="45" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -3204,13 +3204,13 @@
         <v>23</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D18" s="43" t="s">
         <v>377</v>
       </c>
-      <c r="D18" s="43" t="s">
-        <v>378</v>
-      </c>
       <c r="E18" s="45" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -3218,13 +3218,13 @@
         <v>24</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="D19" s="43" t="s">
         <v>379</v>
       </c>
-      <c r="D19" s="43" t="s">
-        <v>380</v>
-      </c>
       <c r="E19" s="45" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -3232,13 +3232,13 @@
         <v>31</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D20" s="43" t="s">
         <v>381</v>
       </c>
-      <c r="D20" s="43" t="s">
-        <v>382</v>
-      </c>
       <c r="E20" s="45" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -3246,13 +3246,13 @@
         <v>32</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="D21" s="43" t="s">
         <v>383</v>
       </c>
-      <c r="D21" s="43" t="s">
-        <v>384</v>
-      </c>
       <c r="E21" s="45" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -3260,13 +3260,13 @@
         <v>33</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="D22" s="43" t="s">
         <v>385</v>
       </c>
-      <c r="D22" s="43" t="s">
-        <v>386</v>
-      </c>
       <c r="E22" s="45" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -3274,13 +3274,13 @@
         <v>41</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="D23" s="43" t="s">
         <v>389</v>
       </c>
-      <c r="D23" s="43" t="s">
-        <v>390</v>
-      </c>
       <c r="E23" s="45" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -3288,13 +3288,13 @@
         <v>42</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E24" s="45" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -3302,13 +3302,13 @@
         <v>43</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="D25" s="43" t="s">
         <v>392</v>
       </c>
-      <c r="D25" s="43" t="s">
-        <v>393</v>
-      </c>
       <c r="E25" s="45" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -3347,8 +3347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Default to nodemcuv2 - Voltage based on L's command board - New command to reset factory default
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="426">
   <si>
     <t>Offset</t>
   </si>
@@ -674,9 +674,6 @@
     <t>0B</t>
   </si>
   <si>
-    <t>Get batter level</t>
-  </si>
-  <si>
     <t>A9 9A 02 0B 0D ED</t>
   </si>
   <si>
@@ -1296,6 +1293,15 @@
   </si>
   <si>
     <t>Update combo</t>
+  </si>
+  <si>
+    <t>Get battery level</t>
+  </si>
+  <si>
+    <t>Reset robot config</t>
+  </si>
+  <si>
+    <t>A9 9A 02 06 08 ED</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1523,6 +1529,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1830,13 +1839,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O50"/>
+  <dimension ref="B2:O51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
+      <selection pane="bottomRight" activeCell="I18" sqref="I18:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,12 +2073,12 @@
         <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="43"/>
       <c r="F16" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G16" s="4"/>
       <c r="I16" s="4" t="s">
@@ -2079,7 +2088,7 @@
         <v>143</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -2087,12 +2096,12 @@
         <v>134</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="43"/>
       <c r="F17" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G17" s="4"/>
       <c r="I17" s="4" t="s">
@@ -2105,224 +2114,220 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="I18" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D19" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E19" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G19" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I19" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J19" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="K18" s="17" t="s">
+      <c r="K19" s="17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="4" t="s">
+      <c r="G20" s="12"/>
+      <c r="I20" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="G19" s="12"/>
-      <c r="I19" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="J19" s="4" t="s">
+      <c r="K20" s="17" t="s">
         <v>218</v>
-      </c>
-      <c r="K19" s="17" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="5">
-        <v>11</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="I20" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G21" s="4"/>
       <c r="I21" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G22" s="4"/>
       <c r="I22" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="3">
-        <v>14</v>
+      <c r="B23" s="5">
+        <v>13</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="41"/>
+        <v>66</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>78</v>
+      </c>
       <c r="F24" s="4" t="s">
-        <v>346</v>
+        <v>68</v>
       </c>
       <c r="G24" s="4"/>
-      <c r="I24" s="4"/>
+      <c r="I24" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="J24" s="4" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>77</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="41"/>
       <c r="F25" s="4" t="s">
-        <v>71</v>
+        <v>345</v>
       </c>
       <c r="G25" s="4"/>
-      <c r="I25" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>70</v>
@@ -2331,7 +2336,7 @@
         <v>77</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G26" s="4"/>
       <c r="I26" s="4" t="s">
@@ -2344,21 +2349,21 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E27" s="23" t="s">
-        <v>203</v>
+      <c r="E27" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G27" s="4"/>
       <c r="I27" s="4" t="s">
@@ -2368,55 +2373,53 @@
         <v>96</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="18" t="s">
-        <v>191</v>
+      <c r="E28" s="23" t="s">
+        <v>203</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>173</v>
+        <v>75</v>
       </c>
       <c r="G28" s="4"/>
       <c r="I28" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>170</v>
+        <v>76</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E29" s="28" t="s">
-        <v>51</v>
+        <v>70</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>172</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="G29" s="4"/>
       <c r="I29" s="4" t="s">
         <v>111</v>
       </c>
@@ -2429,21 +2432,23 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G30" s="12"/>
+        <v>171</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>172</v>
+      </c>
       <c r="I30" s="4" t="s">
         <v>111</v>
       </c>
@@ -2456,23 +2461,21 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>187</v>
+        <v>45</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>220</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="G31" s="12"/>
       <c r="I31" s="4" t="s">
         <v>111</v>
       </c>
@@ -2485,21 +2488,23 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="G32" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>219</v>
+      </c>
       <c r="I32" s="4" t="s">
         <v>111</v>
       </c>
@@ -2512,10 +2517,10 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>59</v>
@@ -2524,7 +2529,7 @@
         <v>179</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G33" s="12"/>
       <c r="I33" s="4" t="s">
@@ -2539,23 +2544,21 @@
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>185</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="G34" s="12"/>
       <c r="I34" s="4" t="s">
         <v>111</v>
       </c>
@@ -2563,26 +2566,28 @@
         <v>112</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>186</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E35" s="26" t="s">
-        <v>6</v>
+        <v>81</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>220</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="G35" s="4"/>
+        <v>184</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="I35" s="4" t="s">
         <v>111</v>
       </c>
@@ -2590,24 +2595,24 @@
         <v>112</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>157</v>
+        <v>6</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G36" s="4"/>
       <c r="I36" s="4" t="s">
@@ -2621,20 +2626,20 @@
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
-        <v>159</v>
+      <c r="B37" s="3">
+        <v>42</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>161</v>
+        <v>225</v>
       </c>
       <c r="G37" s="4"/>
       <c r="I37" s="4" t="s">
@@ -2648,243 +2653,243 @@
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="3">
-        <v>60</v>
+      <c r="B38" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>204</v>
+        <v>160</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E38" s="32" t="s">
+      <c r="E38" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>205</v>
+        <v>161</v>
       </c>
       <c r="G38" s="4"/>
       <c r="I38" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>206</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E39" s="18" t="s">
-        <v>82</v>
+        <v>58</v>
+      </c>
+      <c r="E39" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>80</v>
+        <v>205</v>
       </c>
       <c r="G39" s="4"/>
       <c r="I39" s="4" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>118</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>93</v>
+        <v>105</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>214</v>
+        <v>82</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>213</v>
+        <v>80</v>
       </c>
       <c r="G40" s="4"/>
       <c r="I40" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <v>62</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G41" s="4"/>
+      <c r="I41" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="J41" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="K40" s="4" t="s">
+      <c r="K41" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="35">
+    <row r="42" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="35">
         <v>63</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C42" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="D41" s="36" t="s">
+      <c r="D42" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="37" t="s">
+      <c r="E42" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="F41" s="36" t="s">
+      <c r="F42" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="G41" s="36"/>
-      <c r="I41" s="36" t="s">
+      <c r="G42" s="36"/>
+      <c r="I42" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="J41" s="36" t="s">
+      <c r="J42" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="K41" s="36" t="s">
+      <c r="K42" s="36" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="3">
-        <v>68</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="E42" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="G42" s="4"/>
-      <c r="I42" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>423</v>
-      </c>
-      <c r="D43" s="25"/>
-      <c r="E43" s="42"/>
+        <v>346</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E43" s="42" t="s">
+        <v>214</v>
+      </c>
       <c r="F43" s="4" t="s">
-        <v>418</v>
+        <v>347</v>
       </c>
       <c r="G43" s="4"/>
       <c r="I43" s="4" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>113</v>
+        <v>417</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>121</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="D44" s="25"/>
+      <c r="E44" s="42"/>
       <c r="F44" s="4" t="s">
-        <v>122</v>
+        <v>417</v>
       </c>
       <c r="G44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
+      <c r="I44" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E45" s="18"/>
-      <c r="F45" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="G45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
     </row>
-    <row r="46" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E46" s="18"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="3">
+        <v>74</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="F46" s="17" t="s">
+      <c r="F47" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="G46" s="4"/>
-      <c r="I46" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="3">
-        <v>75</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E47" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>223</v>
       </c>
       <c r="G47" s="4"/>
       <c r="I47" s="4" t="s">
@@ -2894,66 +2899,66 @@
         <v>112</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>224</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="4"/>
+      <c r="B48" s="3">
+        <v>75</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>222</v>
+      </c>
       <c r="G48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-    </row>
-    <row r="49" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D49" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="E49" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="F49" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="G49" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="I49" s="36" t="s">
+      <c r="I48" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="J49" s="36" t="s">
+      <c r="J48" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="K49" s="36" t="s">
-        <v>113</v>
-      </c>
+      <c r="K48" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="3"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
     </row>
     <row r="50" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="35" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C50" s="36" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="E50" s="37" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F50" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="G50" s="36"/>
+        <v>86</v>
+      </c>
+      <c r="G50" s="36" t="s">
+        <v>87</v>
+      </c>
       <c r="I50" s="36" t="s">
         <v>111</v>
       </c>
@@ -2961,6 +2966,33 @@
         <v>112</v>
       </c>
       <c r="K50" s="36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="F51" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="G51" s="36"/>
+      <c r="I51" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="J51" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="K51" s="36" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2996,7 +3028,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -3006,7 +3038,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="47" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="45"/>
@@ -3018,7 +3050,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="46"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="45"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -3038,7 +3070,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D6" s="43" t="s">
         <v>130</v>
@@ -3050,13 +3082,13 @@
         <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D7" s="43" t="s">
         <v>356</v>
       </c>
-      <c r="D7" s="43" t="s">
-        <v>357</v>
-      </c>
       <c r="E7" s="45" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -3064,13 +3096,13 @@
         <v>134</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="D8" s="43" t="s">
         <v>358</v>
       </c>
-      <c r="D8" s="43" t="s">
-        <v>359</v>
-      </c>
       <c r="E8" s="45" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -3078,83 +3110,83 @@
         <v>194</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="D9" s="43" t="s">
         <v>386</v>
       </c>
-      <c r="D9" s="43" t="s">
-        <v>387</v>
-      </c>
       <c r="E9" s="45" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="43" t="s">
         <v>413</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="E10" s="45" t="s">
         <v>414</v>
-      </c>
-      <c r="E10" s="45" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="43" t="s">
         <v>361</v>
       </c>
-      <c r="D11" s="43" t="s">
-        <v>362</v>
-      </c>
       <c r="E11" s="45" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>364</v>
-      </c>
       <c r="D12" s="43" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E12" s="45" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>366</v>
-      </c>
       <c r="D13" s="43" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E13" s="45" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="43" t="s">
         <v>370</v>
       </c>
-      <c r="D14" s="43" t="s">
-        <v>371</v>
-      </c>
       <c r="E14" s="45" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -3162,13 +3194,13 @@
         <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="D15" s="44" t="s">
         <v>420</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="E15" s="45" t="s">
         <v>421</v>
-      </c>
-      <c r="E15" s="45" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -3176,13 +3208,13 @@
         <v>21</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D16" s="43" t="s">
         <v>372</v>
       </c>
-      <c r="D16" s="43" t="s">
-        <v>373</v>
-      </c>
       <c r="E16" s="45" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -3190,13 +3222,13 @@
         <v>22</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="D17" s="43" t="s">
         <v>374</v>
       </c>
-      <c r="D17" s="43" t="s">
-        <v>375</v>
-      </c>
       <c r="E17" s="45" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -3204,13 +3236,13 @@
         <v>23</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D18" s="43" t="s">
         <v>376</v>
       </c>
-      <c r="D18" s="43" t="s">
-        <v>377</v>
-      </c>
       <c r="E18" s="45" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -3218,13 +3250,13 @@
         <v>24</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="D19" s="43" t="s">
         <v>378</v>
       </c>
-      <c r="D19" s="43" t="s">
-        <v>379</v>
-      </c>
       <c r="E19" s="45" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -3232,13 +3264,13 @@
         <v>31</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D20" s="43" t="s">
         <v>380</v>
       </c>
-      <c r="D20" s="43" t="s">
-        <v>381</v>
-      </c>
       <c r="E20" s="45" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -3246,13 +3278,13 @@
         <v>32</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="D21" s="43" t="s">
         <v>382</v>
       </c>
-      <c r="D21" s="43" t="s">
-        <v>383</v>
-      </c>
       <c r="E21" s="45" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -3260,13 +3292,13 @@
         <v>33</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="D22" s="43" t="s">
         <v>384</v>
       </c>
-      <c r="D22" s="43" t="s">
-        <v>385</v>
-      </c>
       <c r="E22" s="45" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -3274,13 +3306,13 @@
         <v>41</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="D23" s="43" t="s">
         <v>388</v>
       </c>
-      <c r="D23" s="43" t="s">
-        <v>389</v>
-      </c>
       <c r="E23" s="45" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -3288,13 +3320,13 @@
         <v>42</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E24" s="45" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -3302,13 +3334,13 @@
         <v>43</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="D25" s="43" t="s">
         <v>391</v>
       </c>
-      <c r="D25" s="43" t="s">
-        <v>392</v>
-      </c>
       <c r="E25" s="45" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -3347,7 +3379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -3376,7 +3408,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="47" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3387,7 +3419,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="46"/>
+      <c r="D4" s="47"/>
     </row>
     <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
@@ -3405,7 +3437,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D6" s="42" t="s">
         <v>130</v>
@@ -3419,12 +3451,12 @@
         <v>26</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
@@ -3435,18 +3467,18 @@
     </row>
     <row r="9" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
@@ -3540,7 +3572,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="47" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3551,7 +3583,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="46"/>
+      <c r="D8" s="47"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -3746,7 +3778,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="46" t="s">
+      <c r="D28" s="47" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3757,7 +3789,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="46"/>
+      <c r="D29" s="47"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
@@ -4037,761 +4069,761 @@
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="40" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C3" s="40" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G3" s="40"/>
       <c r="H3" s="40" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I3" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="J3" s="40" t="s">
         <v>302</v>
-      </c>
-      <c r="J3" s="40" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="39" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" t="s">
         <v>235</v>
       </c>
-      <c r="D5" t="s">
-        <v>236</v>
-      </c>
       <c r="E5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>338</v>
+      </c>
+      <c r="C6" t="s">
         <v>339</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>340</v>
       </c>
-      <c r="D6" t="s">
-        <v>341</v>
-      </c>
       <c r="E6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C7" t="s">
         <v>342</v>
-      </c>
-      <c r="C7" t="s">
-        <v>343</v>
       </c>
       <c r="D7" t="s">
         <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D8" t="s">
         <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D9" t="s">
         <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D10" t="s">
         <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>290</v>
+      </c>
+      <c r="C11" t="s">
         <v>291</v>
-      </c>
-      <c r="C11" t="s">
-        <v>292</v>
       </c>
       <c r="D11" t="s">
         <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D13" t="s">
         <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C15" t="s">
         <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>268</v>
+      </c>
+      <c r="C16" t="s">
         <v>269</v>
       </c>
-      <c r="C16" t="s">
-        <v>270</v>
-      </c>
       <c r="D16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>238</v>
+      </c>
+      <c r="C18" t="s">
         <v>239</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>240</v>
       </c>
-      <c r="D18" t="s">
-        <v>241</v>
-      </c>
       <c r="E18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F18" t="s">
         <v>70</v>
       </c>
       <c r="H18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>241</v>
+      </c>
+      <c r="C20" t="s">
         <v>242</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>243</v>
       </c>
-      <c r="D20" t="s">
-        <v>244</v>
-      </c>
       <c r="E20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F20" t="s">
         <v>123</v>
       </c>
       <c r="H20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D21" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F21" t="s">
         <v>123</v>
       </c>
       <c r="H21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>252</v>
+      </c>
+      <c r="C22" t="s">
         <v>253</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>254</v>
       </c>
-      <c r="D22" t="s">
-        <v>255</v>
-      </c>
       <c r="E22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F22" t="s">
         <v>123</v>
       </c>
       <c r="H22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C23" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F23" t="s">
         <v>123</v>
       </c>
       <c r="H23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E24" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F24" t="s">
         <v>123</v>
       </c>
       <c r="H24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D25" t="s">
         <v>45</v>
       </c>
       <c r="E25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F25" t="s">
         <v>123</v>
       </c>
       <c r="H25" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C27" t="s">
         <v>69</v>
       </c>
       <c r="D27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F27" t="s">
         <v>123</v>
       </c>
       <c r="H27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C28" t="s">
+        <v>249</v>
+      </c>
+      <c r="D28" t="s">
         <v>250</v>
       </c>
-      <c r="D28" t="s">
-        <v>251</v>
-      </c>
       <c r="E28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F28" t="s">
         <v>123</v>
       </c>
       <c r="H28" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C29" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D29" t="s">
         <v>45</v>
       </c>
       <c r="E29" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F29" t="s">
         <v>123</v>
       </c>
       <c r="H29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C30" t="s">
         <v>72</v>
       </c>
       <c r="D30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F30" t="s">
         <v>123</v>
       </c>
       <c r="H30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C31" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F31" t="s">
         <v>123</v>
       </c>
       <c r="H31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I31" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C32" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D32" t="s">
         <v>45</v>
       </c>
       <c r="E32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F32" t="s">
         <v>123</v>
       </c>
       <c r="H32" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E33" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F33" t="s">
         <v>123</v>
       </c>
       <c r="H33" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>274</v>
+      </c>
+      <c r="C34" t="s">
         <v>275</v>
       </c>
-      <c r="C34" t="s">
-        <v>276</v>
-      </c>
       <c r="D34" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E34" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F34" t="s">
         <v>123</v>
       </c>
       <c r="H34" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>276</v>
+      </c>
+      <c r="C35" t="s">
         <v>277</v>
       </c>
-      <c r="C35" t="s">
-        <v>278</v>
-      </c>
       <c r="D35" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E35" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F35" t="s">
         <v>123</v>
       </c>
       <c r="H35" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>285</v>
+      </c>
+      <c r="C36" t="s">
         <v>286</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>287</v>
       </c>
-      <c r="D36" t="s">
-        <v>288</v>
-      </c>
       <c r="E36" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F36" t="s">
         <v>123</v>
       </c>
       <c r="H36" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>261</v>
+      </c>
+      <c r="C38" t="s">
         <v>262</v>
       </c>
-      <c r="C38" t="s">
-        <v>263</v>
-      </c>
       <c r="D38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E38" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F38" t="s">
         <v>70</v>
       </c>
       <c r="H38" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I38" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D39" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E39" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F39" t="s">
         <v>70</v>
       </c>
       <c r="H39" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C40" t="s">
+        <v>281</v>
+      </c>
+      <c r="D40" t="s">
+        <v>240</v>
+      </c>
+      <c r="E40" t="s">
         <v>282</v>
-      </c>
-      <c r="D40" t="s">
-        <v>241</v>
-      </c>
-      <c r="E40" t="s">
-        <v>283</v>
       </c>
       <c r="F40" t="s">
         <v>70</v>
       </c>
       <c r="H40" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>283</v>
+      </c>
+      <c r="C41" t="s">
         <v>284</v>
       </c>
-      <c r="C41" t="s">
-        <v>285</v>
-      </c>
       <c r="D41" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F41" t="s">
         <v>70</v>
       </c>
       <c r="H41" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I41" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New feature to GetNetwork
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -9,17 +9,18 @@
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
     <sheet name="ConfigData" sheetId="6" r:id="rId2"/>
-    <sheet name="ComboData" sheetId="5" r:id="rId3"/>
-    <sheet name="ActionData" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
-    <sheet name="CommonMethod" sheetId="4" r:id="rId6"/>
+    <sheet name="GetNetwork" sheetId="7" r:id="rId3"/>
+    <sheet name="ComboData" sheetId="5" r:id="rId4"/>
+    <sheet name="ActionData" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="CommonMethod" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="443">
   <si>
     <t>Offset</t>
   </si>
@@ -1302,6 +1303,57 @@
   </si>
   <si>
     <t>A9 9A 02 06 08 ED</t>
+  </si>
+  <si>
+    <t>0C</t>
+  </si>
+  <si>
+    <t>Get current network setting</t>
+  </si>
+  <si>
+    <t>A9 9A 02 0C 0E ED</t>
+  </si>
+  <si>
+    <t>0x0C</t>
+  </si>
+  <si>
+    <t>{Mode}</t>
+  </si>
+  <si>
+    <t>Network mode</t>
+  </si>
+  <si>
+    <t>05~24</t>
+  </si>
+  <si>
+    <t>{SSID/SP}</t>
+  </si>
+  <si>
+    <t>SSID or AP Name</t>
+  </si>
+  <si>
+    <t>25~44</t>
+  </si>
+  <si>
+    <t>{IP}</t>
+  </si>
+  <si>
+    <t>Robot IP</t>
+  </si>
+  <si>
+    <t>45~46</t>
+  </si>
+  <si>
+    <t>{Port}</t>
+  </si>
+  <si>
+    <t>Robot Port</t>
+  </si>
+  <si>
+    <t>47~57</t>
+  </si>
+  <si>
+    <t>{mode}{AP}{IP}{Port} - see GetNetwork</t>
   </si>
 </sst>
 </file>
@@ -1398,7 +1450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1529,6 +1581,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1839,13 +1894,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O51"/>
+  <dimension ref="B2:O52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I18" sqref="I18:K18"/>
+      <selection pane="bottomRight" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,167 +2249,163 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="5">
-        <v>11</v>
+      <c r="B21" s="5" t="s">
+        <v>426</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>45</v>
-      </c>
+        <v>427</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="4"/>
+        <v>428</v>
+      </c>
+      <c r="G21" s="12"/>
       <c r="I21" s="4" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>101</v>
+        <v>143</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G22" s="4"/>
       <c r="I22" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="3">
-        <v>14</v>
+      <c r="B24" s="5">
+        <v>13</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G24" s="4"/>
       <c r="I24" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="41"/>
+        <v>66</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>78</v>
+      </c>
       <c r="F25" s="4" t="s">
-        <v>345</v>
+        <v>68</v>
       </c>
       <c r="G25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="I25" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="J25" s="4" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>77</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="41"/>
       <c r="F26" s="4" t="s">
-        <v>71</v>
+        <v>345</v>
       </c>
       <c r="G26" s="4"/>
-      <c r="I26" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>70</v>
@@ -2363,7 +2414,7 @@
         <v>77</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G27" s="4"/>
       <c r="I27" s="4" t="s">
@@ -2376,21 +2427,21 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="23" t="s">
-        <v>203</v>
+      <c r="E28" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G28" s="4"/>
       <c r="I28" s="4" t="s">
@@ -2400,55 +2451,53 @@
         <v>96</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="18" t="s">
-        <v>191</v>
+      <c r="E29" s="23" t="s">
+        <v>203</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>173</v>
+        <v>75</v>
       </c>
       <c r="G29" s="4"/>
       <c r="I29" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>170</v>
+        <v>76</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>51</v>
+        <v>70</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>172</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="G30" s="4"/>
       <c r="I30" s="4" t="s">
         <v>111</v>
       </c>
@@ -2461,21 +2510,23 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G31" s="12"/>
+        <v>171</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>172</v>
+      </c>
       <c r="I31" s="4" t="s">
         <v>111</v>
       </c>
@@ -2488,23 +2539,21 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>187</v>
+        <v>45</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>219</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="G32" s="12"/>
       <c r="I32" s="4" t="s">
         <v>111</v>
       </c>
@@ -2517,21 +2566,23 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="G33" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>219</v>
+      </c>
       <c r="I33" s="4" t="s">
         <v>111</v>
       </c>
@@ -2544,10 +2595,10 @@
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>59</v>
@@ -2556,7 +2607,7 @@
         <v>179</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G34" s="12"/>
       <c r="I34" s="4" t="s">
@@ -2571,23 +2622,21 @@
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>185</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="G35" s="12"/>
       <c r="I35" s="4" t="s">
         <v>111</v>
       </c>
@@ -2595,26 +2644,28 @@
         <v>112</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>186</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E36" s="26" t="s">
-        <v>6</v>
+        <v>81</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>220</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="G36" s="4"/>
+        <v>184</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="I36" s="4" t="s">
         <v>111</v>
       </c>
@@ -2622,24 +2673,24 @@
         <v>112</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>157</v>
+        <v>6</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G37" s="4"/>
       <c r="I37" s="4" t="s">
@@ -2653,20 +2704,20 @@
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>159</v>
+      <c r="B38" s="3">
+        <v>42</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>161</v>
+        <v>225</v>
       </c>
       <c r="G38" s="4"/>
       <c r="I38" s="4" t="s">
@@ -2680,243 +2731,243 @@
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="3">
-        <v>60</v>
+      <c r="B39" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>204</v>
+        <v>160</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="32" t="s">
+      <c r="E39" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>205</v>
+        <v>161</v>
       </c>
       <c r="G39" s="4"/>
       <c r="I39" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>206</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>82</v>
+        <v>58</v>
+      </c>
+      <c r="E40" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>80</v>
+        <v>205</v>
       </c>
       <c r="G40" s="4"/>
       <c r="I40" s="4" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>118</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>93</v>
+        <v>105</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>214</v>
+        <v>82</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>213</v>
+        <v>80</v>
       </c>
       <c r="G41" s="4"/>
       <c r="I41" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="3">
+        <v>62</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G42" s="4"/>
+      <c r="I42" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="J41" s="4" t="s">
+      <c r="J42" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="K41" s="4" t="s">
+      <c r="K42" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="35">
+    <row r="43" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="35">
         <v>63</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C43" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="D42" s="36" t="s">
+      <c r="D43" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="37" t="s">
+      <c r="E43" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="F42" s="36" t="s">
+      <c r="F43" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="G42" s="36"/>
-      <c r="I42" s="36" t="s">
+      <c r="G43" s="36"/>
+      <c r="I43" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="J42" s="36" t="s">
+      <c r="J43" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="K42" s="36" t="s">
+      <c r="K43" s="36" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="3">
-        <v>68</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="D43" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="E43" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="G43" s="4"/>
-      <c r="I43" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="K43" s="4" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="42"/>
+        <v>346</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="42" t="s">
+        <v>214</v>
+      </c>
       <c r="F44" s="4" t="s">
-        <v>417</v>
+        <v>347</v>
       </c>
       <c r="G44" s="4"/>
       <c r="I44" s="4" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>113</v>
+        <v>417</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E45" s="18" t="s">
-        <v>121</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="D45" s="25"/>
+      <c r="E45" s="42"/>
       <c r="F45" s="4" t="s">
-        <v>122</v>
+        <v>417</v>
       </c>
       <c r="G45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
+      <c r="I45" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E46" s="18"/>
-      <c r="F46" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="G46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E47" s="18" t="s">
+      <c r="E47" s="18"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+    </row>
+    <row r="48" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="3">
+        <v>74</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="F48" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="G47" s="4"/>
-      <c r="I47" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="3">
-        <v>75</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E48" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>222</v>
       </c>
       <c r="G48" s="4"/>
       <c r="I48" s="4" t="s">
@@ -2926,66 +2977,66 @@
         <v>112</v>
       </c>
       <c r="K48" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="3">
+        <v>75</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="G49" s="4"/>
+      <c r="I49" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K49" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="3"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-    </row>
-    <row r="50" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C50" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D50" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="E50" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="F50" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="G50" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="I50" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="J50" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="K50" s="36" t="s">
-        <v>113</v>
-      </c>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="3"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
     </row>
     <row r="51" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="35" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C51" s="36" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D51" s="36" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="E51" s="37" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F51" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="G51" s="36"/>
+        <v>86</v>
+      </c>
+      <c r="G51" s="36" t="s">
+        <v>87</v>
+      </c>
       <c r="I51" s="36" t="s">
         <v>111</v>
       </c>
@@ -2993,6 +3044,33 @@
         <v>112</v>
       </c>
       <c r="K51" s="36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="F52" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="G52" s="36"/>
+      <c r="I52" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="J52" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="K52" s="36" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3006,7 +3084,7 @@
   <dimension ref="B2:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B2" sqref="B2:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3038,7 +3116,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="48" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="45"/>
@@ -3050,7 +3128,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="47"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="45"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -3376,6 +3454,159 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="48"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>58</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>59</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D12"/>
   <sheetViews>
@@ -3408,7 +3639,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="48" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3419,7 +3650,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="47"/>
+      <c r="D4" s="48"/>
     </row>
     <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
@@ -3517,7 +3748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D52"/>
   <sheetViews>
@@ -3572,7 +3803,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="48" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3583,7 +3814,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="47"/>
+      <c r="D8" s="48"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -3778,7 +4009,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="D28" s="48" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3789,7 +4020,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="47"/>
+      <c r="D29" s="48"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
@@ -4021,7 +4252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:C5"/>
   <sheetViews>
@@ -4049,7 +4280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J41"/>
   <sheetViews>

</xml_diff>

<commit_message>
New command to get & save wifi config
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -9,18 +9,19 @@
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
     <sheet name="ConfigData" sheetId="6" r:id="rId2"/>
-    <sheet name="GetNetwork" sheetId="7" r:id="rId3"/>
-    <sheet name="ComboData" sheetId="5" r:id="rId4"/>
-    <sheet name="ActionData" sheetId="1" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
-    <sheet name="CommonMethod" sheetId="4" r:id="rId7"/>
+    <sheet name="NetworkConfig" sheetId="8" r:id="rId3"/>
+    <sheet name="GetNetwork" sheetId="7" r:id="rId4"/>
+    <sheet name="ComboData" sheetId="5" r:id="rId5"/>
+    <sheet name="ActionData" sheetId="1" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId7"/>
+    <sheet name="CommonMethod" sheetId="4" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="512">
   <si>
     <t>Offset</t>
   </si>
@@ -1354,13 +1355,220 @@
   </si>
   <si>
     <t>{mode}{AP}{IP}{Port} - see GetNetwork</t>
+  </si>
+  <si>
+    <t>0D</t>
+  </si>
+  <si>
+    <t>Get network config</t>
+  </si>
+  <si>
+    <t>Yes {120}</t>
+  </si>
+  <si>
+    <t>Yes {116}</t>
+  </si>
+  <si>
+    <t>0E</t>
+  </si>
+  <si>
+    <t>Set network config</t>
+  </si>
+  <si>
+    <t>{Refer to NetworkConfig}</t>
+  </si>
+  <si>
+    <t>0x74</t>
+  </si>
+  <si>
+    <t>Length of header data = 116</t>
+  </si>
+  <si>
+    <t>            uint8_t</t>
+  </si>
+  <si>
+    <t>            bool ena</t>
+  </si>
+  <si>
+    <t>            char ssi</t>
+  </si>
+  <si>
+    <t>            char pas</t>
+  </si>
+  <si>
+    <t>            char apN</t>
+  </si>
+  <si>
+    <t>            char apK</t>
+  </si>
+  <si>
+    <t>            uint16_t</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>headerA9       </t>
+  </si>
+  <si>
+    <t>header9A       </t>
+  </si>
+  <si>
+    <t>size           </t>
+  </si>
+  <si>
+    <t>command        </t>
+  </si>
+  <si>
+    <t>ver_major      </t>
+  </si>
+  <si>
+    <t>ver_minor      </t>
+  </si>
+  <si>
+    <t>filler_01[2]   </t>
+  </si>
+  <si>
+    <t>bleRouter      </t>
+  </si>
+  <si>
+    <t>filler_02[1]   </t>
+  </si>
+  <si>
+    <t>d[30]          </t>
+  </si>
+  <si>
+    <t>sword[20]      </t>
+  </si>
+  <si>
+    <t>routerTimeout  </t>
+  </si>
+  <si>
+    <t>filler_03[1]   </t>
+  </si>
+  <si>
+    <t>bleAP          </t>
+  </si>
+  <si>
+    <t>filler_04[1]   </t>
+  </si>
+  <si>
+    <t>ame[20]        </t>
+  </si>
+  <si>
+    <t>ey[20]         </t>
+  </si>
+  <si>
+    <t>bleServer      </t>
+  </si>
+  <si>
+    <t>filler_05[1]   </t>
+  </si>
+  <si>
+    <t>serverPort    </t>
+  </si>
+  <si>
+    <t>bleUDP         </t>
+  </si>
+  <si>
+    <t>filler_06[1]   </t>
+  </si>
+  <si>
+    <t>udpRxPort     </t>
+  </si>
+  <si>
+    <t>udpTxPort     </t>
+  </si>
+  <si>
+    <t>filler_07[4]   </t>
+  </si>
+  <si>
+    <t>sum            </t>
+  </si>
+  <si>
+    <t>endEA          </t>
+  </si>
+  <si>
+    <t>Version major (not allow to read if not match)</t>
+  </si>
+  <si>
+    <t>Version minor (allow to read even not match)</t>
+  </si>
+  <si>
+    <t>enbleRouter      </t>
+  </si>
+  <si>
+    <t>ssid</t>
+  </si>
+  <si>
+    <t>SSID</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Byte(s)</t>
+  </si>
+  <si>
+    <t>Router timeout (seconds)</t>
+  </si>
+  <si>
+    <t>enableAP</t>
+  </si>
+  <si>
+    <t>Router enable flag</t>
+  </si>
+  <si>
+    <t>AP enable flag</t>
+  </si>
+  <si>
+    <t>apName</t>
+  </si>
+  <si>
+    <t>Name of AP</t>
+  </si>
+  <si>
+    <t>apKey</t>
+  </si>
+  <si>
+    <t>Key of AP</t>
+  </si>
+  <si>
+    <t>enableServer</t>
+  </si>
+  <si>
+    <t>Setting server enable flag</t>
+  </si>
+  <si>
+    <t>Setting server port</t>
+  </si>
+  <si>
+    <t>enableUDP</t>
+  </si>
+  <si>
+    <t>UDP enable flag</t>
+  </si>
+  <si>
+    <t>UDP receive port</t>
+  </si>
+  <si>
+    <t>UDP transmit port</t>
+  </si>
+  <si>
+    <t>A9 9A 02 0D 0F ED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A9 9A 74 E 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 F 0 1 0 45 53 50 31 35 35 36 36 37 31 37 0 0 0 0 0 0 0 0 0 31 32 33 34 35 36 37 38 0 0 0 0 0 0 0 0 0 0 0 0 1 0 50 0 1 0 34 23 3C 23 0 0 0 0 CD ED </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1392,6 +1600,12 @@
       <u/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1450,7 +1664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1586,6 +1800,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1894,13 +2131,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O52"/>
+  <dimension ref="B2:N54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K22" sqref="K22"/>
+      <selection pane="bottomRight" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1914,11 +2151,10 @@
     <col min="7" max="7" width="29" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="13.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="47.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1926,7 +2162,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -1937,7 +2173,7 @@
       <c r="G3" s="13"/>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -1948,9 +2184,8 @@
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1961,9 +2196,8 @@
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1978,9 +2212,8 @@
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -1989,7 +2222,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
@@ -1998,7 +2231,7 @@
       </c>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
@@ -2007,7 +2240,7 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
@@ -2036,7 +2269,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
@@ -2065,7 +2298,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
@@ -2094,7 +2327,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
@@ -2123,7 +2356,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
@@ -2146,7 +2379,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>134</v>
       </c>
@@ -2169,7 +2402,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>194</v>
       </c>
@@ -2192,7 +2425,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>53</v>
       </c>
@@ -2221,7 +2454,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>215</v>
       </c>
@@ -2248,7 +2481,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>426</v>
       </c>
@@ -2271,66 +2504,61 @@
         <v>442</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="5">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="G22" s="12"/>
+      <c r="I22" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="G23" s="12"/>
+      <c r="I23" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="5">
         <v>11</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="I22" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="5">
-        <v>12</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G23" s="4"/>
-      <c r="I23" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="5">
-        <v>13</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>58</v>
@@ -2339,7 +2567,7 @@
         <v>45</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G24" s="4"/>
       <c r="I24" s="4" t="s">
@@ -2349,15 +2577,15 @@
         <v>94</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="3">
-        <v>14</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
+        <v>12</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>59</v>
@@ -2366,7 +2594,7 @@
         <v>78</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G25" s="4"/>
       <c r="I25" s="4" t="s">
@@ -2376,99 +2604,99 @@
         <v>59</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="3">
-        <v>15</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
+        <v>13</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="41"/>
+        <v>63</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="F26" s="4" t="s">
-        <v>345</v>
+        <v>65</v>
       </c>
       <c r="G26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="I26" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="J26" s="4" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G27" s="4"/>
       <c r="I27" s="4" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>77</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="41"/>
       <c r="F28" s="4" t="s">
-        <v>73</v>
+        <v>345</v>
       </c>
       <c r="G28" s="4"/>
-      <c r="I28" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="23" t="s">
-        <v>203</v>
+      <c r="E29" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G29" s="4"/>
       <c r="I29" s="4" t="s">
@@ -2478,82 +2706,80 @@
         <v>96</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>70</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>191</v>
+        <v>77</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="G30" s="4"/>
       <c r="I30" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>170</v>
+        <v>74</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E31" s="28" t="s">
-        <v>51</v>
+        <v>70</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>203</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>172</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="G31" s="4"/>
       <c r="I31" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>174</v>
+        <v>76</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E32" s="28" t="s">
-        <v>45</v>
+        <v>70</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G32" s="12"/>
+        <v>173</v>
+      </c>
+      <c r="G32" s="4"/>
       <c r="I32" s="4" t="s">
         <v>111</v>
       </c>
@@ -2566,22 +2792,22 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>187</v>
+        <v>51</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>219</v>
+        <v>171</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>172</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>111</v>
@@ -2595,19 +2821,19 @@
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>179</v>
+        <v>45</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="G34" s="12"/>
       <c r="I34" s="4" t="s">
@@ -2622,21 +2848,23 @@
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G35" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>219</v>
+      </c>
       <c r="I35" s="4" t="s">
         <v>111</v>
       </c>
@@ -2649,23 +2877,21 @@
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>185</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="G36" s="12"/>
       <c r="I36" s="4" t="s">
         <v>111</v>
       </c>
@@ -2673,26 +2899,26 @@
         <v>112</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>186</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="26" t="s">
-        <v>6</v>
+      <c r="E37" s="28" t="s">
+        <v>179</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="G37" s="4"/>
+        <v>182</v>
+      </c>
+      <c r="G37" s="12"/>
       <c r="I37" s="4" t="s">
         <v>111</v>
       </c>
@@ -2705,21 +2931,23 @@
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="3">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>156</v>
+        <v>183</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E38" s="26" t="s">
-        <v>157</v>
+        <v>81</v>
+      </c>
+      <c r="E38" s="28" t="s">
+        <v>220</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="G38" s="4"/>
+        <v>184</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="I38" s="4" t="s">
         <v>111</v>
       </c>
@@ -2727,24 +2955,24 @@
         <v>112</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
-        <v>159</v>
+      <c r="B39" s="3">
+        <v>41</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>161</v>
+        <v>224</v>
       </c>
       <c r="G39" s="4"/>
       <c r="I39" s="4" t="s">
@@ -2759,318 +2987,372 @@
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E40" s="32" t="s">
-        <v>45</v>
+        <v>59</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>157</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="G40" s="4"/>
       <c r="I40" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>206</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="3">
-        <v>61</v>
+      <c r="B41" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>105</v>
+        <v>160</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>82</v>
+        <v>58</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>45</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>80</v>
+        <v>161</v>
       </c>
       <c r="G41" s="4"/>
       <c r="I41" s="4" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="3">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="E42" s="18" t="s">
-        <v>214</v>
+        <v>204</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="G42" s="4"/>
       <c r="I42" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="35">
-        <v>63</v>
-      </c>
-      <c r="C43" s="36" t="s">
-        <v>146</v>
-      </c>
-      <c r="D43" s="36" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="3">
+        <v>61</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="37" t="s">
+      <c r="E43" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F43" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="G43" s="36"/>
-      <c r="I43" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="J43" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="K43" s="36" t="s">
-        <v>114</v>
+      <c r="F43" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G43" s="4"/>
+      <c r="I43" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>346</v>
+        <v>106</v>
       </c>
       <c r="D44" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="42" t="s">
+      <c r="E44" s="18" t="s">
         <v>214</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>347</v>
+        <v>213</v>
       </c>
       <c r="G44" s="4"/>
       <c r="I44" s="4" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="3">
-        <v>69</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="D45" s="25"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="G45" s="4"/>
-      <c r="I45" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K45" s="4" t="s">
-        <v>113</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="35">
+        <v>63</v>
+      </c>
+      <c r="C45" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="D45" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E45" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F45" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="G45" s="36"/>
+      <c r="I45" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="J45" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="K45" s="36" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E46" s="18" t="s">
-        <v>121</v>
+        <v>346</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E46" s="42" t="s">
+        <v>214</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>122</v>
+        <v>347</v>
       </c>
       <c r="G46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
+      <c r="I46" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="3">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E47" s="18"/>
-      <c r="F47" s="4"/>
+        <v>422</v>
+      </c>
+      <c r="D47" s="25"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="4" t="s">
+        <v>417</v>
+      </c>
       <c r="G47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-    </row>
-    <row r="48" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="I47" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="3">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="F48" s="17" t="s">
-        <v>144</v>
+        <v>121</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="G48" s="4"/>
-      <c r="I48" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K48" s="4" t="s">
-        <v>113</v>
-      </c>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="3">
+        <v>72</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E49" s="18"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+    </row>
+    <row r="50" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="3">
+        <v>74</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G50" s="4"/>
+      <c r="I50" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="3">
         <v>75</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E49" s="26" t="s">
+      <c r="E51" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="F51" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="G49" s="4"/>
-      <c r="I49" s="4" t="s">
+      <c r="G51" s="4"/>
+      <c r="I51" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="J49" s="4" t="s">
+      <c r="J51" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="K49" s="4" t="s">
+      <c r="K51" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="3"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-    </row>
-    <row r="51" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="35" t="s">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+    </row>
+    <row r="53" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="36" t="s">
+      <c r="C53" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D51" s="36" t="s">
+      <c r="D53" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="E51" s="37" t="s">
+      <c r="E53" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="F51" s="36" t="s">
+      <c r="F53" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="G51" s="36" t="s">
+      <c r="G53" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="I51" s="36" t="s">
+      <c r="I53" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="J51" s="36" t="s">
+      <c r="J53" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="K51" s="36" t="s">
+      <c r="K53" s="36" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="35" t="s">
+    <row r="54" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="36" t="s">
+      <c r="C54" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="D52" s="36" t="s">
+      <c r="D54" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E52" s="37" t="s">
+      <c r="E54" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="F52" s="36" t="s">
+      <c r="F54" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="G52" s="36"/>
-      <c r="I52" s="36" t="s">
+      <c r="G54" s="36"/>
+      <c r="I54" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="J52" s="36" t="s">
+      <c r="J54" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="K52" s="36" t="s">
+      <c r="K54" s="36" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3084,7 +3366,7 @@
   <dimension ref="B2:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D27"/>
+      <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3116,7 +3398,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="57" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="45"/>
@@ -3128,7 +3410,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="45"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -3454,6 +3736,1709 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AV31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="50"/>
+    <col min="9" max="9" width="14" style="52" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="52"/>
+    <col min="12" max="12" width="9.140625" style="53"/>
+    <col min="13" max="17" width="9.140625" style="52"/>
+    <col min="18" max="48" width="9.140625" style="50"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="I1" s="52" t="s">
+        <v>452</v>
+      </c>
+      <c r="J1" s="52" t="s">
+        <v>460</v>
+      </c>
+      <c r="K1" s="52" t="s">
+        <v>459</v>
+      </c>
+      <c r="L1" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="I2" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J2" s="51" t="s">
+        <v>461</v>
+      </c>
+      <c r="K2" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L2" s="54">
+        <v>1</v>
+      </c>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="11"/>
+      <c r="AJ2" s="11"/>
+      <c r="AK2" s="11"/>
+      <c r="AL2" s="11"/>
+      <c r="AM2" s="11"/>
+      <c r="AN2" s="11"/>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="11"/>
+    </row>
+    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B3" s="55">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="48">
+        <v>1</v>
+      </c>
+      <c r="F3" s="45"/>
+      <c r="I3" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J3" s="51" t="s">
+        <v>462</v>
+      </c>
+      <c r="K3" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L3" s="54">
+        <v>2</v>
+      </c>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="11"/>
+      <c r="AI3" s="11"/>
+      <c r="AJ3" s="11"/>
+      <c r="AK3" s="11"/>
+      <c r="AL3" s="11"/>
+      <c r="AM3" s="11"/>
+      <c r="AN3" s="11"/>
+      <c r="AO3" s="11"/>
+      <c r="AP3" s="11"/>
+    </row>
+    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B4" s="56">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="57"/>
+      <c r="E4" s="48">
+        <v>1</v>
+      </c>
+      <c r="F4" s="45"/>
+      <c r="I4" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>463</v>
+      </c>
+      <c r="K4" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L4" s="54">
+        <v>3</v>
+      </c>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="11"/>
+      <c r="AI4" s="11"/>
+      <c r="AJ4" s="11"/>
+      <c r="AK4" s="11"/>
+      <c r="AL4" s="11"/>
+      <c r="AM4" s="11"/>
+      <c r="AN4" s="11"/>
+      <c r="AO4" s="11"/>
+      <c r="AP4" s="11"/>
+    </row>
+    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B5" s="56">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>451</v>
+      </c>
+      <c r="E5" s="48">
+        <v>1</v>
+      </c>
+      <c r="F5" s="45"/>
+      <c r="I5" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>464</v>
+      </c>
+      <c r="K5" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L5" s="54">
+        <v>4</v>
+      </c>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="11"/>
+      <c r="AH5" s="11"/>
+      <c r="AI5" s="11"/>
+      <c r="AJ5" s="11"/>
+      <c r="AK5" s="11"/>
+      <c r="AL5" s="11"/>
+      <c r="AM5" s="11"/>
+      <c r="AN5" s="11"/>
+      <c r="AO5" s="11"/>
+      <c r="AP5" s="11"/>
+    </row>
+    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B6" s="56">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="48">
+        <v>1</v>
+      </c>
+      <c r="F6" s="45"/>
+      <c r="I6" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J6" s="51" t="s">
+        <v>465</v>
+      </c>
+      <c r="K6" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L6" s="54">
+        <v>5</v>
+      </c>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="51"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="11"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="11"/>
+      <c r="AM6" s="11"/>
+      <c r="AN6" s="11"/>
+      <c r="AO6" s="11"/>
+      <c r="AP6" s="11"/>
+    </row>
+    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B7" s="56">
+        <v>4</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>464</v>
+      </c>
+      <c r="D7" s="49" t="s">
+        <v>487</v>
+      </c>
+      <c r="E7" s="49">
+        <v>1</v>
+      </c>
+      <c r="F7" s="45"/>
+      <c r="I7" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J7" s="51" t="s">
+        <v>466</v>
+      </c>
+      <c r="K7" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L7" s="54">
+        <v>6</v>
+      </c>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="11"/>
+      <c r="AG7" s="11"/>
+      <c r="AH7" s="11"/>
+      <c r="AI7" s="11"/>
+      <c r="AJ7" s="11"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="11"/>
+      <c r="AM7" s="11"/>
+      <c r="AN7" s="11"/>
+      <c r="AO7" s="11"/>
+      <c r="AP7" s="11"/>
+    </row>
+    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B8" s="56">
+        <v>5</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>465</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>488</v>
+      </c>
+      <c r="E8" s="49">
+        <v>1</v>
+      </c>
+      <c r="F8" s="45"/>
+      <c r="I8" s="51" t="s">
+        <v>453</v>
+      </c>
+      <c r="J8" s="51" t="s">
+        <v>467</v>
+      </c>
+      <c r="K8" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L8" s="54">
+        <v>8</v>
+      </c>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="11"/>
+      <c r="AI8" s="11"/>
+      <c r="AJ8" s="11"/>
+      <c r="AK8" s="11"/>
+      <c r="AL8" s="11"/>
+      <c r="AM8" s="11"/>
+      <c r="AN8" s="11"/>
+      <c r="AO8" s="11"/>
+      <c r="AP8" s="11"/>
+    </row>
+    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B9" s="56">
+        <v>6</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>466</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>466</v>
+      </c>
+      <c r="E9" s="49">
+        <v>2</v>
+      </c>
+      <c r="F9" s="45"/>
+      <c r="I9" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J9" s="51" t="s">
+        <v>468</v>
+      </c>
+      <c r="K9" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L9" s="54">
+        <v>9</v>
+      </c>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="11"/>
+      <c r="AG9" s="11"/>
+      <c r="AH9" s="11"/>
+      <c r="AI9" s="11"/>
+      <c r="AJ9" s="11"/>
+      <c r="AK9" s="11"/>
+      <c r="AL9" s="11"/>
+      <c r="AM9" s="11"/>
+      <c r="AN9" s="11"/>
+      <c r="AO9" s="11"/>
+      <c r="AP9" s="11"/>
+    </row>
+    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B10" s="56">
+        <v>8</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>489</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>497</v>
+      </c>
+      <c r="E10" s="49">
+        <v>1</v>
+      </c>
+      <c r="F10" s="45"/>
+      <c r="I10" s="51" t="s">
+        <v>454</v>
+      </c>
+      <c r="J10" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="K10" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L10" s="54">
+        <v>10</v>
+      </c>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11"/>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="11"/>
+      <c r="AI10" s="11"/>
+      <c r="AJ10" s="11"/>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="11"/>
+      <c r="AM10" s="11"/>
+      <c r="AN10" s="11"/>
+      <c r="AO10" s="11"/>
+      <c r="AP10" s="11"/>
+    </row>
+    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B11" s="56">
+        <v>9</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>468</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>468</v>
+      </c>
+      <c r="E11" s="49">
+        <v>1</v>
+      </c>
+      <c r="F11" s="45"/>
+      <c r="I11" s="51" t="s">
+        <v>455</v>
+      </c>
+      <c r="J11" s="51" t="s">
+        <v>470</v>
+      </c>
+      <c r="K11" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L11" s="54">
+        <v>40</v>
+      </c>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="11"/>
+      <c r="AH11" s="11"/>
+      <c r="AI11" s="11"/>
+      <c r="AJ11" s="11"/>
+      <c r="AK11" s="11"/>
+      <c r="AL11" s="11"/>
+      <c r="AM11" s="11"/>
+      <c r="AN11" s="11"/>
+      <c r="AO11" s="11"/>
+      <c r="AP11" s="11"/>
+    </row>
+    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B12" s="56">
+        <v>10</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>490</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>491</v>
+      </c>
+      <c r="E12" s="49">
+        <v>30</v>
+      </c>
+      <c r="F12" s="45"/>
+      <c r="I12" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J12" s="51" t="s">
+        <v>471</v>
+      </c>
+      <c r="K12" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L12" s="54">
+        <v>60</v>
+      </c>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="11"/>
+      <c r="AG12" s="11"/>
+      <c r="AH12" s="11"/>
+      <c r="AI12" s="11"/>
+      <c r="AJ12" s="11"/>
+      <c r="AK12" s="11"/>
+      <c r="AL12" s="11"/>
+      <c r="AM12" s="11"/>
+      <c r="AN12" s="11"/>
+      <c r="AO12" s="11"/>
+      <c r="AP12" s="11"/>
+    </row>
+    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B13" s="56">
+        <v>40</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>492</v>
+      </c>
+      <c r="D13" s="49" t="s">
+        <v>493</v>
+      </c>
+      <c r="E13" s="49">
+        <v>20</v>
+      </c>
+      <c r="F13" s="45"/>
+      <c r="I13" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J13" s="51" t="s">
+        <v>472</v>
+      </c>
+      <c r="K13" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L13" s="54">
+        <v>61</v>
+      </c>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="11"/>
+      <c r="AG13" s="11"/>
+      <c r="AH13" s="11"/>
+      <c r="AI13" s="11"/>
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="11"/>
+      <c r="AL13" s="11"/>
+      <c r="AM13" s="11"/>
+      <c r="AN13" s="11"/>
+      <c r="AO13" s="11"/>
+      <c r="AP13" s="11"/>
+    </row>
+    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B14" s="56">
+        <v>60</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>471</v>
+      </c>
+      <c r="D14" s="49" t="s">
+        <v>495</v>
+      </c>
+      <c r="E14" s="49">
+        <v>1</v>
+      </c>
+      <c r="F14" s="45"/>
+      <c r="I14" s="51" t="s">
+        <v>453</v>
+      </c>
+      <c r="J14" s="51" t="s">
+        <v>473</v>
+      </c>
+      <c r="K14" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L14" s="54">
+        <v>62</v>
+      </c>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="11"/>
+      <c r="AG14" s="11"/>
+      <c r="AH14" s="11"/>
+      <c r="AI14" s="11"/>
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="11"/>
+      <c r="AL14" s="11"/>
+      <c r="AM14" s="11"/>
+      <c r="AN14" s="11"/>
+      <c r="AO14" s="11"/>
+      <c r="AP14" s="11"/>
+    </row>
+    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B15" s="56">
+        <v>61</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>472</v>
+      </c>
+      <c r="D15" s="49" t="s">
+        <v>472</v>
+      </c>
+      <c r="E15" s="49">
+        <v>1</v>
+      </c>
+      <c r="F15" s="45"/>
+      <c r="I15" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J15" s="51" t="s">
+        <v>474</v>
+      </c>
+      <c r="K15" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L15" s="54">
+        <v>63</v>
+      </c>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="51"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="11"/>
+      <c r="AG15" s="11"/>
+      <c r="AH15" s="11"/>
+      <c r="AI15" s="11"/>
+      <c r="AJ15" s="11"/>
+      <c r="AK15" s="11"/>
+      <c r="AL15" s="11"/>
+      <c r="AM15" s="11"/>
+      <c r="AN15" s="11"/>
+      <c r="AO15" s="11"/>
+      <c r="AP15" s="11"/>
+    </row>
+    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B16" s="56">
+        <v>62</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>496</v>
+      </c>
+      <c r="D16" s="49" t="s">
+        <v>498</v>
+      </c>
+      <c r="E16" s="49">
+        <v>1</v>
+      </c>
+      <c r="F16" s="45"/>
+      <c r="I16" s="51" t="s">
+        <v>456</v>
+      </c>
+      <c r="J16" s="51" t="s">
+        <v>475</v>
+      </c>
+      <c r="K16" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L16" s="54">
+        <v>64</v>
+      </c>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="51"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="11"/>
+      <c r="AF16" s="11"/>
+      <c r="AG16" s="11"/>
+      <c r="AH16" s="11"/>
+      <c r="AI16" s="11"/>
+      <c r="AJ16" s="11"/>
+      <c r="AK16" s="11"/>
+      <c r="AL16" s="11"/>
+      <c r="AM16" s="11"/>
+      <c r="AN16" s="11"/>
+      <c r="AO16" s="11"/>
+      <c r="AP16" s="11"/>
+    </row>
+    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B17" s="56">
+        <v>63</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>474</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>474</v>
+      </c>
+      <c r="E17" s="49">
+        <v>1</v>
+      </c>
+      <c r="F17" s="45"/>
+      <c r="I17" s="51" t="s">
+        <v>457</v>
+      </c>
+      <c r="J17" s="51" t="s">
+        <v>476</v>
+      </c>
+      <c r="K17" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L17" s="54">
+        <v>84</v>
+      </c>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="11"/>
+      <c r="AE17" s="11"/>
+      <c r="AF17" s="11"/>
+      <c r="AG17" s="11"/>
+      <c r="AH17" s="11"/>
+      <c r="AI17" s="11"/>
+      <c r="AJ17" s="11"/>
+      <c r="AK17" s="11"/>
+      <c r="AL17" s="11"/>
+      <c r="AM17" s="11"/>
+      <c r="AN17" s="11"/>
+      <c r="AO17" s="11"/>
+      <c r="AP17" s="11"/>
+    </row>
+    <row r="18" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B18" s="56">
+        <v>64</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>499</v>
+      </c>
+      <c r="D18" s="49" t="s">
+        <v>500</v>
+      </c>
+      <c r="E18" s="49">
+        <v>20</v>
+      </c>
+      <c r="F18" s="45"/>
+      <c r="I18" s="51" t="s">
+        <v>453</v>
+      </c>
+      <c r="J18" s="51" t="s">
+        <v>477</v>
+      </c>
+      <c r="K18" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L18" s="54">
+        <v>104</v>
+      </c>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="51"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="11"/>
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="11"/>
+      <c r="AI18" s="11"/>
+      <c r="AJ18" s="11"/>
+      <c r="AK18" s="11"/>
+      <c r="AL18" s="11"/>
+      <c r="AM18" s="11"/>
+      <c r="AN18" s="11"/>
+      <c r="AO18" s="11"/>
+      <c r="AP18" s="11"/>
+    </row>
+    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B19" s="56">
+        <v>84</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>501</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>502</v>
+      </c>
+      <c r="E19" s="49">
+        <v>20</v>
+      </c>
+      <c r="F19" s="45"/>
+      <c r="I19" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J19" s="51" t="s">
+        <v>478</v>
+      </c>
+      <c r="K19" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L19" s="54">
+        <v>105</v>
+      </c>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="11"/>
+      <c r="AF19" s="11"/>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="11"/>
+      <c r="AI19" s="11"/>
+      <c r="AJ19" s="11"/>
+      <c r="AK19" s="11"/>
+      <c r="AL19" s="11"/>
+      <c r="AM19" s="11"/>
+      <c r="AN19" s="11"/>
+      <c r="AO19" s="11"/>
+      <c r="AP19" s="11"/>
+    </row>
+    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B20" s="56">
+        <v>104</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="D20" s="49" t="s">
+        <v>504</v>
+      </c>
+      <c r="E20" s="49">
+        <v>1</v>
+      </c>
+      <c r="F20" s="45"/>
+      <c r="I20" s="51" t="s">
+        <v>458</v>
+      </c>
+      <c r="J20" s="51" t="s">
+        <v>479</v>
+      </c>
+      <c r="K20" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L20" s="54">
+        <v>106</v>
+      </c>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="11"/>
+      <c r="AD20" s="11"/>
+      <c r="AE20" s="11"/>
+      <c r="AF20" s="11"/>
+      <c r="AG20" s="11"/>
+      <c r="AH20" s="11"/>
+      <c r="AI20" s="11"/>
+      <c r="AJ20" s="11"/>
+      <c r="AK20" s="11"/>
+      <c r="AL20" s="11"/>
+      <c r="AM20" s="11"/>
+      <c r="AN20" s="11"/>
+      <c r="AO20" s="11"/>
+      <c r="AP20" s="11"/>
+    </row>
+    <row r="21" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B21" s="56">
+        <v>105</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>478</v>
+      </c>
+      <c r="D21" s="49" t="s">
+        <v>478</v>
+      </c>
+      <c r="E21" s="49">
+        <v>1</v>
+      </c>
+      <c r="F21" s="45"/>
+      <c r="I21" s="51" t="s">
+        <v>453</v>
+      </c>
+      <c r="J21" s="51" t="s">
+        <v>480</v>
+      </c>
+      <c r="K21" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L21" s="54">
+        <v>108</v>
+      </c>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51"/>
+      <c r="Q21" s="51"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11"/>
+      <c r="AE21" s="11"/>
+      <c r="AF21" s="11"/>
+      <c r="AG21" s="11"/>
+      <c r="AH21" s="11"/>
+      <c r="AI21" s="11"/>
+      <c r="AJ21" s="11"/>
+      <c r="AK21" s="11"/>
+      <c r="AL21" s="11"/>
+      <c r="AM21" s="11"/>
+      <c r="AN21" s="11"/>
+      <c r="AO21" s="11"/>
+      <c r="AP21" s="11"/>
+    </row>
+    <row r="22" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B22" s="56">
+        <v>106</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>479</v>
+      </c>
+      <c r="D22" s="49" t="s">
+        <v>505</v>
+      </c>
+      <c r="E22" s="49">
+        <v>2</v>
+      </c>
+      <c r="F22" s="45"/>
+      <c r="I22" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J22" s="51" t="s">
+        <v>481</v>
+      </c>
+      <c r="K22" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L22" s="54">
+        <v>109</v>
+      </c>
+      <c r="M22" s="51"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="51"/>
+      <c r="P22" s="51"/>
+      <c r="Q22" s="51"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="11"/>
+      <c r="AE22" s="11"/>
+      <c r="AF22" s="11"/>
+      <c r="AG22" s="11"/>
+      <c r="AH22" s="11"/>
+      <c r="AI22" s="11"/>
+      <c r="AJ22" s="11"/>
+      <c r="AK22" s="11"/>
+      <c r="AL22" s="11"/>
+      <c r="AM22" s="11"/>
+      <c r="AN22" s="11"/>
+      <c r="AO22" s="11"/>
+      <c r="AP22" s="11"/>
+    </row>
+    <row r="23" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B23" s="56">
+        <v>108</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>506</v>
+      </c>
+      <c r="D23" s="49" t="s">
+        <v>507</v>
+      </c>
+      <c r="E23" s="49">
+        <v>1</v>
+      </c>
+      <c r="F23" s="45"/>
+      <c r="I23" s="51" t="s">
+        <v>458</v>
+      </c>
+      <c r="J23" s="51" t="s">
+        <v>482</v>
+      </c>
+      <c r="K23" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L23" s="54">
+        <v>110</v>
+      </c>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="11"/>
+      <c r="AE23" s="11"/>
+      <c r="AF23" s="11"/>
+      <c r="AG23" s="11"/>
+      <c r="AH23" s="11"/>
+      <c r="AI23" s="11"/>
+      <c r="AJ23" s="11"/>
+      <c r="AK23" s="11"/>
+      <c r="AL23" s="11"/>
+      <c r="AM23" s="11"/>
+      <c r="AN23" s="11"/>
+      <c r="AO23" s="11"/>
+      <c r="AP23" s="11"/>
+    </row>
+    <row r="24" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B24" s="56">
+        <v>109</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>481</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>481</v>
+      </c>
+      <c r="E24" s="49">
+        <v>1</v>
+      </c>
+      <c r="F24" s="45"/>
+      <c r="I24" s="51" t="s">
+        <v>458</v>
+      </c>
+      <c r="J24" s="51" t="s">
+        <v>483</v>
+      </c>
+      <c r="K24" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L24" s="54">
+        <v>112</v>
+      </c>
+      <c r="M24" s="51"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="51"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="11"/>
+      <c r="AE24" s="11"/>
+      <c r="AF24" s="11"/>
+      <c r="AG24" s="11"/>
+      <c r="AH24" s="11"/>
+      <c r="AI24" s="11"/>
+      <c r="AJ24" s="11"/>
+      <c r="AK24" s="11"/>
+      <c r="AL24" s="11"/>
+      <c r="AM24" s="11"/>
+      <c r="AN24" s="11"/>
+      <c r="AO24" s="11"/>
+      <c r="AP24" s="11"/>
+    </row>
+    <row r="25" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B25" s="56">
+        <v>110</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>482</v>
+      </c>
+      <c r="D25" s="49" t="s">
+        <v>508</v>
+      </c>
+      <c r="E25" s="49">
+        <v>2</v>
+      </c>
+      <c r="F25" s="45"/>
+      <c r="I25" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J25" s="51" t="s">
+        <v>484</v>
+      </c>
+      <c r="K25" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L25" s="54">
+        <v>114</v>
+      </c>
+      <c r="M25" s="51"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="51"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="11"/>
+      <c r="AE25" s="11"/>
+      <c r="AF25" s="11"/>
+      <c r="AG25" s="11"/>
+      <c r="AH25" s="11"/>
+      <c r="AI25" s="11"/>
+      <c r="AJ25" s="11"/>
+      <c r="AK25" s="11"/>
+      <c r="AL25" s="11"/>
+      <c r="AM25" s="11"/>
+      <c r="AN25" s="11"/>
+      <c r="AO25" s="11"/>
+      <c r="AP25" s="11"/>
+    </row>
+    <row r="26" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B26" s="56">
+        <v>112</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>483</v>
+      </c>
+      <c r="D26" s="49" t="s">
+        <v>509</v>
+      </c>
+      <c r="E26" s="49">
+        <v>2</v>
+      </c>
+      <c r="F26" s="45"/>
+      <c r="I26" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J26" s="51" t="s">
+        <v>485</v>
+      </c>
+      <c r="K26" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L26" s="54">
+        <v>118</v>
+      </c>
+      <c r="M26" s="51"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="51"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="11"/>
+      <c r="AC26" s="11"/>
+      <c r="AD26" s="11"/>
+      <c r="AE26" s="11"/>
+      <c r="AF26" s="11"/>
+      <c r="AG26" s="11"/>
+      <c r="AH26" s="11"/>
+      <c r="AI26" s="11"/>
+      <c r="AJ26" s="11"/>
+      <c r="AK26" s="11"/>
+      <c r="AL26" s="11"/>
+      <c r="AM26" s="11"/>
+      <c r="AN26" s="11"/>
+      <c r="AO26" s="11"/>
+      <c r="AP26" s="11"/>
+    </row>
+    <row r="27" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B27" s="56">
+        <v>114</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>484</v>
+      </c>
+      <c r="D27" s="49" t="s">
+        <v>484</v>
+      </c>
+      <c r="E27" s="49">
+        <v>4</v>
+      </c>
+      <c r="F27" s="45"/>
+      <c r="I27" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="J27" s="51" t="s">
+        <v>486</v>
+      </c>
+      <c r="K27" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="L27" s="54">
+        <v>119</v>
+      </c>
+      <c r="M27" s="51"/>
+      <c r="N27" s="51"/>
+      <c r="O27" s="51"/>
+      <c r="P27" s="51"/>
+      <c r="Q27" s="51"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="11"/>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="11"/>
+      <c r="AA27" s="11"/>
+      <c r="AB27" s="11"/>
+      <c r="AC27" s="11"/>
+      <c r="AD27" s="11"/>
+      <c r="AE27" s="11"/>
+      <c r="AF27" s="11"/>
+      <c r="AG27" s="11"/>
+      <c r="AH27" s="11"/>
+      <c r="AI27" s="11"/>
+      <c r="AJ27" s="11"/>
+      <c r="AK27" s="11"/>
+      <c r="AL27" s="11"/>
+      <c r="AM27" s="11"/>
+      <c r="AN27" s="11"/>
+      <c r="AO27" s="11"/>
+      <c r="AP27" s="11"/>
+    </row>
+    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B28" s="56">
+        <v>118</v>
+      </c>
+      <c r="C28" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="48">
+        <v>1</v>
+      </c>
+      <c r="F28" s="45"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="54"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="51"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="51"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="11"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
+      <c r="AA28" s="11"/>
+      <c r="AB28" s="11"/>
+      <c r="AC28" s="11"/>
+      <c r="AD28" s="11"/>
+      <c r="AE28" s="11"/>
+      <c r="AF28" s="11"/>
+      <c r="AG28" s="11"/>
+      <c r="AH28" s="11"/>
+      <c r="AI28" s="11"/>
+      <c r="AJ28" s="11"/>
+      <c r="AK28" s="11"/>
+      <c r="AL28" s="11"/>
+      <c r="AM28" s="11"/>
+      <c r="AN28" s="11"/>
+      <c r="AO28" s="11"/>
+      <c r="AP28" s="11"/>
+    </row>
+    <row r="29" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B29" s="56">
+        <v>119</v>
+      </c>
+      <c r="C29" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="48">
+        <v>1</v>
+      </c>
+      <c r="F29" s="45"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="51"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="51"/>
+      <c r="O29" s="51"/>
+      <c r="P29" s="51"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+      <c r="X29" s="11"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="11"/>
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="11"/>
+      <c r="AC29" s="11"/>
+      <c r="AD29" s="11"/>
+      <c r="AE29" s="11"/>
+      <c r="AF29" s="11"/>
+      <c r="AG29" s="11"/>
+      <c r="AH29" s="11"/>
+      <c r="AI29" s="11"/>
+      <c r="AJ29" s="11"/>
+      <c r="AK29" s="11"/>
+      <c r="AL29" s="11"/>
+      <c r="AM29" s="11"/>
+      <c r="AN29" s="11"/>
+      <c r="AO29" s="11"/>
+      <c r="AP29" s="11"/>
+    </row>
+    <row r="30" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f>SUM(E3:E29)</f>
+        <v>120</v>
+      </c>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="51"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="51"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11"/>
+      <c r="X30" s="11"/>
+      <c r="Y30" s="11"/>
+      <c r="Z30" s="11"/>
+      <c r="AA30" s="11"/>
+      <c r="AB30" s="11"/>
+      <c r="AC30" s="11"/>
+      <c r="AD30" s="11"/>
+      <c r="AE30" s="11"/>
+      <c r="AF30" s="11"/>
+      <c r="AG30" s="11"/>
+      <c r="AH30" s="11"/>
+      <c r="AI30" s="11"/>
+      <c r="AJ30" s="11"/>
+      <c r="AK30" s="11"/>
+      <c r="AL30" s="11"/>
+      <c r="AM30" s="11"/>
+      <c r="AN30" s="11"/>
+      <c r="AO30" s="11"/>
+      <c r="AP30" s="11"/>
+    </row>
+    <row r="31" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="51"/>
+      <c r="O31" s="51"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="51"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="11"/>
+      <c r="X31" s="11"/>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="11"/>
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="11"/>
+      <c r="AC31" s="11"/>
+      <c r="AD31" s="11"/>
+      <c r="AE31" s="11"/>
+      <c r="AF31" s="11"/>
+      <c r="AG31" s="11"/>
+      <c r="AH31" s="11"/>
+      <c r="AI31" s="11"/>
+      <c r="AJ31" s="11"/>
+      <c r="AK31" s="11"/>
+      <c r="AL31" s="11"/>
+      <c r="AM31" s="11"/>
+      <c r="AN31" s="11"/>
+      <c r="AO31" s="11"/>
+      <c r="AP31" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D13"/>
   <sheetViews>
@@ -3486,7 +5471,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="57" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3497,7 +5482,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
@@ -3606,7 +5591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D12"/>
   <sheetViews>
@@ -3639,7 +5624,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="57" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3650,7 +5635,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
@@ -3748,7 +5733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D52"/>
   <sheetViews>
@@ -3803,7 +5788,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="57" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3814,7 +5799,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="48"/>
+      <c r="D8" s="57"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -4009,7 +5994,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="48" t="s">
+      <c r="D28" s="57" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4020,7 +6005,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="48"/>
+      <c r="D29" s="57"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
@@ -4252,7 +6237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:C5"/>
   <sheetViews>
@@ -4280,7 +6265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J41"/>
   <sheetViews>

</xml_diff>

<commit_message>
Support partial update on Network config
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="518">
   <si>
     <t>Offset</t>
   </si>
@@ -1562,6 +1562,24 @@
   </si>
   <si>
     <t xml:space="preserve">A9 9A 74 E 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 F 0 1 0 45 53 50 31 35 35 36 36 37 31 37 0 0 0 0 0 0 0 0 0 31 32 33 34 35 36 37 38 0 0 0 0 0 0 0 0 0 0 0 0 1 0 50 0 1 0 34 23 3C 23 0 0 0 0 CD ED </t>
+  </si>
+  <si>
+    <t>0F</t>
+  </si>
+  <si>
+    <t>Partial network config update</t>
+  </si>
+  <si>
+    <t>{offset} {data….}</t>
+  </si>
+  <si>
+    <t>A9 9A 04 0F 08 01 1C ED</t>
+  </si>
+  <si>
+    <t>A9 9A 17 0F 0A 53 75 70 65 72 31 36 39 00 00 00 00 00 00 00 00 00 00 00 00 DF ED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2131,13 +2149,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N54"/>
+  <dimension ref="B2:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M23" sqref="M23"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2145,8 +2163,8 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" style="20" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" style="20" customWidth="1"/>
     <col min="6" max="6" width="39.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="29" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="13.85546875" style="1" customWidth="1"/>
@@ -2488,7 +2506,9 @@
       <c r="C21" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="D21" s="17"/>
+      <c r="D21" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E21" s="23"/>
       <c r="F21" s="4" t="s">
         <v>428</v>
@@ -2511,7 +2531,9 @@
       <c r="C22" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="D22" s="17"/>
+      <c r="D22" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E22" s="23"/>
       <c r="F22" s="4" t="s">
         <v>510</v>
@@ -2534,7 +2556,9 @@
       <c r="C23" s="4" t="s">
         <v>448</v>
       </c>
-      <c r="D23" s="17"/>
+      <c r="D23" s="17" t="s">
+        <v>123</v>
+      </c>
       <c r="E23" s="23"/>
       <c r="F23" s="4" t="s">
         <v>449</v>
@@ -2554,167 +2578,172 @@
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="5">
-        <v>11</v>
+      <c r="B24" s="5" t="s">
+        <v>512</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>45</v>
+        <v>513</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>514</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G24" s="4"/>
+        <v>515</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>517</v>
+      </c>
       <c r="I24" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G25" s="4"/>
       <c r="I25" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G26" s="4"/>
       <c r="I26" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="3">
-        <v>14</v>
+      <c r="B27" s="5">
+        <v>13</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G27" s="4"/>
       <c r="I27" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="41"/>
+        <v>66</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>78</v>
+      </c>
       <c r="F28" s="4" t="s">
-        <v>345</v>
+        <v>68</v>
       </c>
       <c r="G28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="I28" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="J28" s="4" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>77</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="4" t="s">
-        <v>71</v>
+        <v>345</v>
       </c>
       <c r="G29" s="4"/>
-      <c r="I29" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>70</v>
@@ -2723,7 +2752,7 @@
         <v>77</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G30" s="4"/>
       <c r="I30" s="4" t="s">
@@ -2736,21 +2765,21 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="23" t="s">
-        <v>203</v>
+      <c r="E31" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G31" s="4"/>
       <c r="I31" s="4" t="s">
@@ -2760,55 +2789,53 @@
         <v>96</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E32" s="18" t="s">
-        <v>191</v>
+      <c r="E32" s="23" t="s">
+        <v>203</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>173</v>
+        <v>75</v>
       </c>
       <c r="G32" s="4"/>
       <c r="I32" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>170</v>
+        <v>76</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E33" s="28" t="s">
-        <v>51</v>
+        <v>70</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>172</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
         <v>111</v>
       </c>
@@ -2821,21 +2848,23 @@
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G34" s="12"/>
+        <v>171</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>172</v>
+      </c>
       <c r="I34" s="4" t="s">
         <v>111</v>
       </c>
@@ -2848,23 +2877,21 @@
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>187</v>
+        <v>45</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>219</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="G35" s="12"/>
       <c r="I35" s="4" t="s">
         <v>111</v>
       </c>
@@ -2877,21 +2904,23 @@
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="G36" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>219</v>
+      </c>
       <c r="I36" s="4" t="s">
         <v>111</v>
       </c>
@@ -2904,10 +2933,10 @@
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>59</v>
@@ -2916,7 +2945,7 @@
         <v>179</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G37" s="12"/>
       <c r="I37" s="4" t="s">
@@ -2931,23 +2960,21 @@
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="3">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>185</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="G38" s="12"/>
       <c r="I38" s="4" t="s">
         <v>111</v>
       </c>
@@ -2955,26 +2982,28 @@
         <v>112</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>186</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E39" s="26" t="s">
-        <v>6</v>
+        <v>81</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>220</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="G39" s="4"/>
+        <v>184</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="I39" s="4" t="s">
         <v>111</v>
       </c>
@@ -2982,24 +3011,24 @@
         <v>112</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>157</v>
+        <v>6</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G40" s="4"/>
       <c r="I40" s="4" t="s">
@@ -3013,20 +3042,20 @@
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
-        <v>159</v>
+      <c r="B41" s="3">
+        <v>42</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>161</v>
+        <v>225</v>
       </c>
       <c r="G41" s="4"/>
       <c r="I41" s="4" t="s">
@@ -3040,243 +3069,243 @@
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="3">
-        <v>60</v>
+      <c r="B42" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>204</v>
+        <v>160</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E42" s="32" t="s">
+      <c r="E42" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>205</v>
+        <v>161</v>
       </c>
       <c r="G42" s="4"/>
       <c r="I42" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>206</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E43" s="18" t="s">
-        <v>82</v>
+        <v>58</v>
+      </c>
+      <c r="E43" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>80</v>
+        <v>205</v>
       </c>
       <c r="G43" s="4"/>
       <c r="I43" s="4" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>118</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D44" s="25" t="s">
-        <v>93</v>
+        <v>105</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>214</v>
+        <v>82</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>213</v>
+        <v>80</v>
       </c>
       <c r="G44" s="4"/>
       <c r="I44" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="3">
+        <v>62</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G45" s="4"/>
+      <c r="I45" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="J44" s="4" t="s">
+      <c r="J45" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="K44" s="4" t="s">
+      <c r="K45" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="35">
+    <row r="46" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="35">
         <v>63</v>
       </c>
-      <c r="C45" s="36" t="s">
+      <c r="C46" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="D45" s="36" t="s">
+      <c r="D46" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="37" t="s">
+      <c r="E46" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="F45" s="36" t="s">
+      <c r="F46" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="G45" s="36"/>
-      <c r="I45" s="36" t="s">
+      <c r="G46" s="36"/>
+      <c r="I46" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="J45" s="36" t="s">
+      <c r="J46" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="K45" s="36" t="s">
+      <c r="K46" s="36" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="3">
-        <v>68</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="G46" s="4"/>
-      <c r="I46" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="3">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="D47" s="25"/>
-      <c r="E47" s="42"/>
+        <v>346</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" s="42" t="s">
+        <v>214</v>
+      </c>
       <c r="F47" s="4" t="s">
-        <v>417</v>
+        <v>347</v>
       </c>
       <c r="G47" s="4"/>
       <c r="I47" s="4" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>113</v>
+        <v>417</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="3">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E48" s="18" t="s">
-        <v>121</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="D48" s="25"/>
+      <c r="E48" s="42"/>
       <c r="F48" s="4" t="s">
-        <v>122</v>
+        <v>417</v>
       </c>
       <c r="G48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
+      <c r="I48" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E49" s="18"/>
-      <c r="F49" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="G49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
     </row>
-    <row r="50" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E50" s="18" t="s">
+      <c r="E50" s="18"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+    </row>
+    <row r="51" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" s="3">
+        <v>74</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E51" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="F50" s="17" t="s">
+      <c r="F51" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="G50" s="4"/>
-      <c r="I50" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K50" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="3">
-        <v>75</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E51" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>222</v>
       </c>
       <c r="G51" s="4"/>
       <c r="I51" s="4" t="s">
@@ -3286,66 +3315,66 @@
         <v>112</v>
       </c>
       <c r="K51" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="3">
+        <v>75</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="G52" s="4"/>
+      <c r="I52" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K52" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="3"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-    </row>
-    <row r="53" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C53" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D53" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="E53" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="F53" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="G53" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="I53" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="J53" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="K53" s="36" t="s">
-        <v>113</v>
-      </c>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="3"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
     </row>
     <row r="54" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="35" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C54" s="36" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="E54" s="37" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F54" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="G54" s="36"/>
+        <v>86</v>
+      </c>
+      <c r="G54" s="36" t="s">
+        <v>87</v>
+      </c>
       <c r="I54" s="36" t="s">
         <v>111</v>
       </c>
@@ -3353,6 +3382,33 @@
         <v>112</v>
       </c>
       <c r="K54" s="36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D55" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="F55" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="G55" s="36"/>
+      <c r="I55" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="J55" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="K55" s="36" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3740,7 +3796,7 @@
   <dimension ref="B1:AV31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add support for servo tuning of HaiLzd servo
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="525">
   <si>
     <t>Offset</t>
   </si>
@@ -1580,17 +1580,45 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Get servo type</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes {2}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nil</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>A9 9A 02 10 12 ED</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes {1}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes {7}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>{type}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1598,7 +1626,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1608,7 +1636,7 @@
       <u/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1618,14 +1646,21 @@
       <u/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2149,16 +2184,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N55"/>
+  <dimension ref="B2:N56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -2443,7 +2478,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>53</v>
       </c>
@@ -2611,166 +2646,166 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>45</v>
+        <v>518</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>519</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>520</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G25" s="4"/>
+        <v>521</v>
+      </c>
+      <c r="G25" s="12"/>
       <c r="I25" s="4" t="s">
-        <v>109</v>
+        <v>523</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>94</v>
+        <v>522</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>101</v>
+        <v>524</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G26" s="4"/>
       <c r="I26" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G27" s="4"/>
       <c r="I27" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="3">
-        <v>14</v>
+      <c r="B28" s="5">
+        <v>13</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G28" s="4"/>
       <c r="I28" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="41"/>
+        <v>66</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>78</v>
+      </c>
       <c r="F29" s="4" t="s">
-        <v>345</v>
+        <v>68</v>
       </c>
       <c r="G29" s="4"/>
-      <c r="I29" s="4"/>
+      <c r="I29" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="J29" s="4" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>77</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="41"/>
       <c r="F30" s="4" t="s">
-        <v>71</v>
+        <v>345</v>
       </c>
       <c r="G30" s="4"/>
-      <c r="I30" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>70</v>
@@ -2779,7 +2814,7 @@
         <v>77</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G31" s="4"/>
       <c r="I31" s="4" t="s">
@@ -2792,21 +2827,21 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E32" s="23" t="s">
-        <v>203</v>
+      <c r="E32" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G32" s="4"/>
       <c r="I32" s="4" t="s">
@@ -2816,55 +2851,53 @@
         <v>96</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="18" t="s">
-        <v>191</v>
+      <c r="E33" s="23" t="s">
+        <v>203</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>173</v>
+        <v>75</v>
       </c>
       <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>170</v>
+        <v>76</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E34" s="28" t="s">
-        <v>51</v>
+        <v>70</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>172</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="G34" s="4"/>
       <c r="I34" s="4" t="s">
         <v>111</v>
       </c>
@@ -2877,21 +2910,23 @@
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G35" s="12"/>
+        <v>171</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>172</v>
+      </c>
       <c r="I35" s="4" t="s">
         <v>111</v>
       </c>
@@ -2904,23 +2939,21 @@
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>187</v>
+        <v>45</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>219</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="G36" s="12"/>
       <c r="I36" s="4" t="s">
         <v>111</v>
       </c>
@@ -2933,21 +2966,23 @@
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="G37" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>219</v>
+      </c>
       <c r="I37" s="4" t="s">
         <v>111</v>
       </c>
@@ -2960,10 +2995,10 @@
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>59</v>
@@ -2972,7 +3007,7 @@
         <v>179</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G38" s="12"/>
       <c r="I38" s="4" t="s">
@@ -2987,23 +3022,21 @@
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>185</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="G39" s="12"/>
       <c r="I39" s="4" t="s">
         <v>111</v>
       </c>
@@ -3011,26 +3044,28 @@
         <v>112</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>186</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>6</v>
+        <v>81</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>220</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="G40" s="4"/>
+        <v>184</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="I40" s="4" t="s">
         <v>111</v>
       </c>
@@ -3038,24 +3073,24 @@
         <v>112</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>157</v>
+        <v>6</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G41" s="4"/>
       <c r="I41" s="4" t="s">
@@ -3069,20 +3104,20 @@
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="3" t="s">
-        <v>159</v>
+      <c r="B42" s="3">
+        <v>42</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>161</v>
+        <v>225</v>
       </c>
       <c r="G42" s="4"/>
       <c r="I42" s="4" t="s">
@@ -3096,243 +3131,243 @@
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="3">
-        <v>60</v>
+      <c r="B43" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>204</v>
+        <v>160</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="32" t="s">
+      <c r="E43" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>205</v>
+        <v>161</v>
       </c>
       <c r="G43" s="4"/>
       <c r="I43" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>206</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>82</v>
+        <v>58</v>
+      </c>
+      <c r="E44" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>80</v>
+        <v>205</v>
       </c>
       <c r="G44" s="4"/>
       <c r="I44" s="4" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>118</v>
+        <v>206</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D45" s="25" t="s">
-        <v>93</v>
+        <v>105</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>214</v>
+        <v>82</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>213</v>
+        <v>80</v>
       </c>
       <c r="G45" s="4"/>
       <c r="I45" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="3">
+        <v>62</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G46" s="4"/>
+      <c r="I46" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="J45" s="4" t="s">
+      <c r="J46" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="K46" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="35">
+    <row r="47" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="35">
         <v>63</v>
       </c>
-      <c r="C46" s="36" t="s">
+      <c r="C47" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="D46" s="36" t="s">
+      <c r="D47" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E46" s="37" t="s">
+      <c r="E47" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="F46" s="36" t="s">
+      <c r="F47" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="G46" s="36"/>
-      <c r="I46" s="36" t="s">
+      <c r="G47" s="36"/>
+      <c r="I47" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="J46" s="36" t="s">
+      <c r="J47" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="K46" s="36" t="s">
+      <c r="K47" s="36" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="3">
-        <v>68</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="D47" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="G47" s="4"/>
-      <c r="I47" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="3">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="D48" s="25"/>
-      <c r="E48" s="42"/>
+        <v>346</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" s="42" t="s">
+        <v>214</v>
+      </c>
       <c r="F48" s="4" t="s">
-        <v>417</v>
+        <v>347</v>
       </c>
       <c r="G48" s="4"/>
       <c r="I48" s="4" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>113</v>
+        <v>417</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="3">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E49" s="18" t="s">
-        <v>121</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="D49" s="25"/>
+      <c r="E49" s="42"/>
       <c r="F49" s="4" t="s">
-        <v>122</v>
+        <v>417</v>
       </c>
       <c r="G49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
+      <c r="I49" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E50" s="18"/>
-      <c r="F50" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="G50" s="4"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
     </row>
-    <row r="51" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E51" s="18" t="s">
+      <c r="E51" s="18"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+    </row>
+    <row r="52" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B52" s="3">
+        <v>74</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F52" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="G51" s="4"/>
-      <c r="I51" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K51" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="3">
-        <v>75</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E52" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>222</v>
       </c>
       <c r="G52" s="4"/>
       <c r="I52" s="4" t="s">
@@ -3342,66 +3377,66 @@
         <v>112</v>
       </c>
       <c r="K52" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="3">
+        <v>75</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="G53" s="4"/>
+      <c r="I53" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K53" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="3"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-    </row>
-    <row r="54" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D54" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="E54" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="F54" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="G54" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="I54" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="J54" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="K54" s="36" t="s">
-        <v>113</v>
-      </c>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="3"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
     </row>
     <row r="55" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="35" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C55" s="36" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D55" s="36" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="E55" s="37" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F55" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="G55" s="36"/>
+        <v>86</v>
+      </c>
+      <c r="G55" s="36" t="s">
+        <v>87</v>
+      </c>
       <c r="I55" s="36" t="s">
         <v>111</v>
       </c>
@@ -3412,8 +3447,37 @@
         <v>113</v>
       </c>
     </row>
+    <row r="56" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="F56" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="G56" s="36"/>
+      <c r="I56" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="J56" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="K56" s="36" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3425,7 +3489,7 @@
       <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -3787,6 +3851,7 @@
   <mergeCells count="1">
     <mergeCell ref="D3:D4"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3799,7 +3864,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -5489,6 +5554,7 @@
   <mergeCells count="1">
     <mergeCell ref="D3:D4"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5502,7 +5568,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -5643,6 +5709,7 @@
   <mergeCells count="1">
     <mergeCell ref="D3:D4"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5655,7 +5722,7 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
@@ -5785,6 +5852,7 @@
   <mergeCells count="1">
     <mergeCell ref="D3:D4"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5797,7 +5865,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -5808,12 +5876,12 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>147</v>
       </c>
@@ -6027,7 +6095,7 @@
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>190</v>
       </c>
@@ -6288,6 +6356,7 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="D28:D29"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
 </worksheet>
@@ -6301,12 +6370,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="158.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:3" ht="63" x14ac:dyDescent="0.25">
       <c r="C2" s="24" t="s">
         <v>129</v>
       </c>
@@ -6317,6 +6386,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6329,7 +6399,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
@@ -7099,6 +7169,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Special feature for initialization of HaiLzd Servo
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="528">
   <si>
     <t>Offset</t>
   </si>
@@ -1608,17 +1608,26 @@
   <si>
     <t>{type}</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HaiLzd Servo Command</t>
+  </si>
+  <si>
+    <t>{cmd} {parm….}</t>
+  </si>
+  <si>
+    <t>A9 9A 03 16 01 1A ED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1626,7 +1635,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1636,7 +1645,7 @@
       <u/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1646,19 +1655,19 @@
       <u/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1717,7 +1726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1876,6 +1885,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2184,16 +2196,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N56"/>
+  <dimension ref="B2:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -2207,7 +2219,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2215,7 +2227,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -2226,7 +2238,7 @@
       <c r="G3" s="13"/>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -2238,7 +2250,7 @@
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -2250,7 +2262,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -2266,7 +2278,7 @@
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14">
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -2275,7 +2287,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14">
       <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
@@ -2284,7 +2296,7 @@
       </c>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14">
       <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
@@ -2293,7 +2305,7 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14">
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
@@ -2322,7 +2334,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14">
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
@@ -2351,7 +2363,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
@@ -2380,7 +2392,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14">
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
@@ -2409,7 +2421,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
@@ -2432,7 +2444,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13">
       <c r="B17" s="5" t="s">
         <v>134</v>
       </c>
@@ -2455,7 +2467,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13">
       <c r="B18" s="5" t="s">
         <v>194</v>
       </c>
@@ -2478,7 +2490,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="45">
       <c r="B19" s="5" t="s">
         <v>53</v>
       </c>
@@ -2507,7 +2519,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13">
       <c r="B20" s="5" t="s">
         <v>215</v>
       </c>
@@ -2534,7 +2546,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13">
       <c r="B21" s="5" t="s">
         <v>426</v>
       </c>
@@ -2559,7 +2571,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13">
       <c r="B22" s="5" t="s">
         <v>443</v>
       </c>
@@ -2584,7 +2596,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13">
       <c r="B23" s="5" t="s">
         <v>447</v>
       </c>
@@ -2612,7 +2624,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13">
       <c r="B24" s="5" t="s">
         <v>512</v>
       </c>
@@ -2644,7 +2656,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13">
       <c r="B25" s="5">
         <v>10</v>
       </c>
@@ -2671,7 +2683,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13">
       <c r="B26" s="5">
         <v>11</v>
       </c>
@@ -2698,7 +2710,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13">
       <c r="B27" s="5">
         <v>12</v>
       </c>
@@ -2725,7 +2737,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13">
       <c r="B28" s="5">
         <v>13</v>
       </c>
@@ -2752,7 +2764,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13">
       <c r="B29" s="3">
         <v>14</v>
       </c>
@@ -2779,7 +2791,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13">
       <c r="B30" s="3">
         <v>15</v>
       </c>
@@ -2800,39 +2812,33 @@
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13">
       <c r="B31" s="3">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>69</v>
+        <v>525</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="18" t="s">
-        <v>77</v>
+      <c r="E31" s="57" t="s">
+        <v>526</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>71</v>
+        <v>527</v>
       </c>
       <c r="G31" s="4"/>
-      <c r="I31" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="2:13">
       <c r="B32" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>70</v>
@@ -2841,7 +2847,7 @@
         <v>77</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G32" s="4"/>
       <c r="I32" s="4" t="s">
@@ -2854,21 +2860,21 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11">
       <c r="B33" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="23" t="s">
-        <v>203</v>
+      <c r="E33" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
@@ -2878,55 +2884,53 @@
         <v>96</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="30">
       <c r="B34" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>191</v>
+      <c r="E34" s="23" t="s">
+        <v>203</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>173</v>
+        <v>75</v>
       </c>
       <c r="G34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11">
       <c r="B35" s="3">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>170</v>
+        <v>76</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>51</v>
+        <v>70</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>172</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="G35" s="4"/>
       <c r="I35" s="4" t="s">
         <v>111</v>
       </c>
@@ -2937,23 +2941,25 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11">
       <c r="B36" s="3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G36" s="12"/>
+        <v>171</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>172</v>
+      </c>
       <c r="I36" s="4" t="s">
         <v>111</v>
       </c>
@@ -2964,25 +2970,23 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11">
       <c r="B37" s="3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>187</v>
+        <v>45</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>219</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="G37" s="12"/>
       <c r="I37" s="4" t="s">
         <v>111</v>
       </c>
@@ -2993,23 +2997,25 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11">
       <c r="B38" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="G38" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>219</v>
+      </c>
       <c r="I38" s="4" t="s">
         <v>111</v>
       </c>
@@ -3020,12 +3026,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11">
       <c r="B39" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>59</v>
@@ -3034,7 +3040,7 @@
         <v>179</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G39" s="12"/>
       <c r="I39" s="4" t="s">
@@ -3047,25 +3053,23 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11">
       <c r="B40" s="3">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>185</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="G40" s="12"/>
       <c r="I40" s="4" t="s">
         <v>111</v>
       </c>
@@ -3073,26 +3077,28 @@
         <v>112</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11">
       <c r="B41" s="3">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" s="26" t="s">
-        <v>6</v>
+        <v>81</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>220</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="G41" s="4"/>
+        <v>184</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="I41" s="4" t="s">
         <v>111</v>
       </c>
@@ -3100,24 +3106,24 @@
         <v>112</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11">
       <c r="B42" s="3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>157</v>
+        <v>6</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G42" s="4"/>
       <c r="I42" s="4" t="s">
@@ -3130,21 +3136,21 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
-        <v>159</v>
+    <row r="43" spans="2:11">
+      <c r="B43" s="3">
+        <v>42</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>161</v>
+        <v>225</v>
       </c>
       <c r="G43" s="4"/>
       <c r="I43" s="4" t="s">
@@ -3157,244 +3163,244 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="3">
-        <v>60</v>
+    <row r="44" spans="2:11">
+      <c r="B44" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>204</v>
+        <v>160</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="32" t="s">
+      <c r="E44" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>205</v>
+        <v>161</v>
       </c>
       <c r="G44" s="4"/>
       <c r="I44" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11">
       <c r="B45" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" s="18" t="s">
-        <v>82</v>
+        <v>58</v>
+      </c>
+      <c r="E45" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>80</v>
+        <v>205</v>
       </c>
       <c r="G45" s="4"/>
       <c r="I45" s="4" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11">
       <c r="B46" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>93</v>
+        <v>105</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>214</v>
+        <v>82</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>213</v>
+        <v>80</v>
       </c>
       <c r="G46" s="4"/>
       <c r="I46" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11">
+      <c r="B47" s="3">
+        <v>62</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G47" s="4"/>
+      <c r="I47" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="J46" s="4" t="s">
+      <c r="J47" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="K46" s="4" t="s">
+      <c r="K47" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="35">
+    <row r="48" spans="2:11" s="38" customFormat="1">
+      <c r="B48" s="35">
         <v>63</v>
       </c>
-      <c r="C47" s="36" t="s">
+      <c r="C48" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="D47" s="36" t="s">
+      <c r="D48" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E47" s="37" t="s">
+      <c r="E48" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="F47" s="36" t="s">
+      <c r="F48" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="G47" s="36"/>
-      <c r="I47" s="36" t="s">
+      <c r="G48" s="36"/>
+      <c r="I48" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="J47" s="36" t="s">
+      <c r="J48" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="K47" s="36" t="s">
+      <c r="K48" s="36" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="3">
+    <row r="49" spans="2:11">
+      <c r="B49" s="3">
         <v>68</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C49" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="D48" s="25" t="s">
+      <c r="D49" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="E48" s="42" t="s">
+      <c r="E49" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F49" s="4" t="s">
         <v>347</v>
-      </c>
-      <c r="G48" s="4"/>
-      <c r="I48" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="K48" s="4" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="3">
-        <v>69</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="D49" s="25"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="4" t="s">
-        <v>417</v>
       </c>
       <c r="G49" s="4"/>
       <c r="I49" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11">
+      <c r="B50" s="3">
+        <v>69</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="D50" s="25"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="G50" s="4"/>
+      <c r="I50" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="J49" s="4" t="s">
+      <c r="J50" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="K49" s="4" t="s">
+      <c r="K50" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="3">
+    <row r="51" spans="2:11">
+      <c r="B51" s="3">
         <v>71</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E50" s="18" t="s">
+      <c r="E51" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F51" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="3">
-        <v>72</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E51" s="18"/>
-      <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
     </row>
-    <row r="52" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11">
       <c r="B52" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E52" s="18" t="s">
+      <c r="E52" s="18"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+    </row>
+    <row r="53" spans="2:11" ht="30">
+      <c r="B53" s="3">
+        <v>74</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E53" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="F52" s="17" t="s">
+      <c r="F53" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="G52" s="4"/>
-      <c r="I52" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K52" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="3">
-        <v>75</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E53" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>222</v>
       </c>
       <c r="G53" s="4"/>
       <c r="I53" s="4" t="s">
@@ -3404,66 +3410,66 @@
         <v>112</v>
       </c>
       <c r="K53" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11">
+      <c r="B54" s="3">
+        <v>75</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="G54" s="4"/>
+      <c r="I54" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K54" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="3"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-    </row>
-    <row r="55" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="35" t="s">
+    <row r="55" spans="2:11">
+      <c r="B55" s="3"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+    </row>
+    <row r="56" spans="2:11" s="38" customFormat="1">
+      <c r="B56" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C55" s="36" t="s">
+      <c r="C56" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D55" s="36" t="s">
+      <c r="D56" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="E55" s="37" t="s">
+      <c r="E56" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="F55" s="36" t="s">
+      <c r="F56" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="G55" s="36" t="s">
+      <c r="G56" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="I55" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="J55" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="K55" s="36" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="56" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="C56" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="D56" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="E56" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="F56" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="G56" s="36"/>
       <c r="I56" s="36" t="s">
         <v>111</v>
       </c>
@@ -3471,6 +3477,33 @@
         <v>112</v>
       </c>
       <c r="K56" s="36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" s="38" customFormat="1">
+      <c r="B57" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E57" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="F57" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="G57" s="36"/>
+      <c r="I57" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="J57" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="K57" s="36" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3489,7 +3522,7 @@
       <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -3497,7 +3530,7 @@
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3511,29 +3544,29 @@
         <v>393</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="58" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="45"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="57"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="45"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -3545,7 +3578,7 @@
       </c>
       <c r="E5" s="45"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -3557,7 +3590,7 @@
       </c>
       <c r="E6" s="45"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -3571,7 +3604,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
         <v>134</v>
       </c>
@@ -3585,7 +3618,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
         <v>194</v>
       </c>
@@ -3599,7 +3632,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
         <v>411</v>
       </c>
@@ -3613,7 +3646,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5">
       <c r="B11" s="3" t="s">
         <v>359</v>
       </c>
@@ -3627,7 +3660,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5">
       <c r="B12" s="3" t="s">
         <v>362</v>
       </c>
@@ -3641,7 +3674,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5">
       <c r="B13" s="3" t="s">
         <v>364</v>
       </c>
@@ -3655,7 +3688,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5">
       <c r="B14" s="3" t="s">
         <v>368</v>
       </c>
@@ -3669,7 +3702,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5">
       <c r="B15" s="3">
         <v>18</v>
       </c>
@@ -3683,7 +3716,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5">
       <c r="B16" s="3">
         <v>21</v>
       </c>
@@ -3697,7 +3730,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <v>22</v>
       </c>
@@ -3711,7 +3744,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <v>23</v>
       </c>
@@ -3725,7 +3758,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <v>24</v>
       </c>
@@ -3739,7 +3772,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <v>31</v>
       </c>
@@ -3753,7 +3786,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <v>32</v>
       </c>
@@ -3767,7 +3800,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <v>33</v>
       </c>
@@ -3781,7 +3814,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <v>41</v>
       </c>
@@ -3795,7 +3828,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <v>42</v>
       </c>
@@ -3809,7 +3842,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <v>43</v>
       </c>
@@ -3823,7 +3856,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <v>58</v>
       </c>
@@ -3835,7 +3868,7 @@
       </c>
       <c r="E26" s="45"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5">
       <c r="B27" s="3">
         <v>59</v>
       </c>
@@ -3864,7 +3897,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -3880,7 +3913,7 @@
     <col min="18" max="48" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:42">
       <c r="I1" s="52" t="s">
         <v>452</v>
       </c>
@@ -3894,7 +3927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:42">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3953,14 +3986,14 @@
       <c r="AO2" s="11"/>
       <c r="AP2" s="11"/>
     </row>
-    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:42">
       <c r="B3" s="55">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="58" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="48">
@@ -4010,14 +4043,14 @@
       <c r="AO3" s="11"/>
       <c r="AP3" s="11"/>
     </row>
-    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:42">
       <c r="B4" s="56">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="57"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="48">
         <v>1</v>
       </c>
@@ -4065,7 +4098,7 @@
       <c r="AO4" s="11"/>
       <c r="AP4" s="11"/>
     </row>
-    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:42">
       <c r="B5" s="56">
         <v>2</v>
       </c>
@@ -4122,7 +4155,7 @@
       <c r="AO5" s="11"/>
       <c r="AP5" s="11"/>
     </row>
-    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:42">
       <c r="B6" s="56">
         <v>3</v>
       </c>
@@ -4179,7 +4212,7 @@
       <c r="AO6" s="11"/>
       <c r="AP6" s="11"/>
     </row>
-    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:42">
       <c r="B7" s="56">
         <v>4</v>
       </c>
@@ -4236,7 +4269,7 @@
       <c r="AO7" s="11"/>
       <c r="AP7" s="11"/>
     </row>
-    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:42">
       <c r="B8" s="56">
         <v>5</v>
       </c>
@@ -4293,7 +4326,7 @@
       <c r="AO8" s="11"/>
       <c r="AP8" s="11"/>
     </row>
-    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:42">
       <c r="B9" s="56">
         <v>6</v>
       </c>
@@ -4350,7 +4383,7 @@
       <c r="AO9" s="11"/>
       <c r="AP9" s="11"/>
     </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:42">
       <c r="B10" s="56">
         <v>8</v>
       </c>
@@ -4407,7 +4440,7 @@
       <c r="AO10" s="11"/>
       <c r="AP10" s="11"/>
     </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:42">
       <c r="B11" s="56">
         <v>9</v>
       </c>
@@ -4464,7 +4497,7 @@
       <c r="AO11" s="11"/>
       <c r="AP11" s="11"/>
     </row>
-    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:42">
       <c r="B12" s="56">
         <v>10</v>
       </c>
@@ -4521,7 +4554,7 @@
       <c r="AO12" s="11"/>
       <c r="AP12" s="11"/>
     </row>
-    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:42">
       <c r="B13" s="56">
         <v>40</v>
       </c>
@@ -4578,7 +4611,7 @@
       <c r="AO13" s="11"/>
       <c r="AP13" s="11"/>
     </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:42">
       <c r="B14" s="56">
         <v>60</v>
       </c>
@@ -4635,7 +4668,7 @@
       <c r="AO14" s="11"/>
       <c r="AP14" s="11"/>
     </row>
-    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:42">
       <c r="B15" s="56">
         <v>61</v>
       </c>
@@ -4692,7 +4725,7 @@
       <c r="AO15" s="11"/>
       <c r="AP15" s="11"/>
     </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:42">
       <c r="B16" s="56">
         <v>62</v>
       </c>
@@ -4749,7 +4782,7 @@
       <c r="AO16" s="11"/>
       <c r="AP16" s="11"/>
     </row>
-    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:42">
       <c r="B17" s="56">
         <v>63</v>
       </c>
@@ -4806,7 +4839,7 @@
       <c r="AO17" s="11"/>
       <c r="AP17" s="11"/>
     </row>
-    <row r="18" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:42">
       <c r="B18" s="56">
         <v>64</v>
       </c>
@@ -4863,7 +4896,7 @@
       <c r="AO18" s="11"/>
       <c r="AP18" s="11"/>
     </row>
-    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:42">
       <c r="B19" s="56">
         <v>84</v>
       </c>
@@ -4920,7 +4953,7 @@
       <c r="AO19" s="11"/>
       <c r="AP19" s="11"/>
     </row>
-    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:42">
       <c r="B20" s="56">
         <v>104</v>
       </c>
@@ -4977,7 +5010,7 @@
       <c r="AO20" s="11"/>
       <c r="AP20" s="11"/>
     </row>
-    <row r="21" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:42">
       <c r="B21" s="56">
         <v>105</v>
       </c>
@@ -5034,7 +5067,7 @@
       <c r="AO21" s="11"/>
       <c r="AP21" s="11"/>
     </row>
-    <row r="22" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:42">
       <c r="B22" s="56">
         <v>106</v>
       </c>
@@ -5091,7 +5124,7 @@
       <c r="AO22" s="11"/>
       <c r="AP22" s="11"/>
     </row>
-    <row r="23" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:42">
       <c r="B23" s="56">
         <v>108</v>
       </c>
@@ -5148,7 +5181,7 @@
       <c r="AO23" s="11"/>
       <c r="AP23" s="11"/>
     </row>
-    <row r="24" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:42">
       <c r="B24" s="56">
         <v>109</v>
       </c>
@@ -5205,7 +5238,7 @@
       <c r="AO24" s="11"/>
       <c r="AP24" s="11"/>
     </row>
-    <row r="25" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:42">
       <c r="B25" s="56">
         <v>110</v>
       </c>
@@ -5262,7 +5295,7 @@
       <c r="AO25" s="11"/>
       <c r="AP25" s="11"/>
     </row>
-    <row r="26" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:42">
       <c r="B26" s="56">
         <v>112</v>
       </c>
@@ -5319,7 +5352,7 @@
       <c r="AO26" s="11"/>
       <c r="AP26" s="11"/>
     </row>
-    <row r="27" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:42">
       <c r="B27" s="56">
         <v>114</v>
       </c>
@@ -5376,7 +5409,7 @@
       <c r="AO27" s="11"/>
       <c r="AP27" s="11"/>
     </row>
-    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:42">
       <c r="B28" s="56">
         <v>118</v>
       </c>
@@ -5425,7 +5458,7 @@
       <c r="AO28" s="11"/>
       <c r="AP28" s="11"/>
     </row>
-    <row r="29" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:42">
       <c r="B29" s="56">
         <v>119</v>
       </c>
@@ -5474,7 +5507,7 @@
       <c r="AO29" s="11"/>
       <c r="AP29" s="11"/>
     </row>
-    <row r="30" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:42">
       <c r="E30">
         <f>SUM(E3:E29)</f>
         <v>120</v>
@@ -5514,7 +5547,7 @@
       <c r="AO30" s="11"/>
       <c r="AP30" s="11"/>
     </row>
-    <row r="31" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:42">
       <c r="I31" s="51"/>
       <c r="J31" s="51"/>
       <c r="K31" s="51"/>
@@ -5568,14 +5601,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -5586,27 +5619,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="58" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="57"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="58"/>
+    </row>
+    <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5617,7 +5650,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -5628,7 +5661,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -5639,7 +5672,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" s="5" t="s">
         <v>432</v>
       </c>
@@ -5650,7 +5683,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4">
       <c r="B9" s="5" t="s">
         <v>435</v>
       </c>
@@ -5661,7 +5694,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4">
       <c r="B10" s="5" t="s">
         <v>438</v>
       </c>
@@ -5672,7 +5705,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="B11" s="3" t="s">
         <v>441</v>
       </c>
@@ -5683,7 +5716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4">
       <c r="B12" s="3">
         <v>58</v>
       </c>
@@ -5694,7 +5727,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="B13" s="3">
         <v>59</v>
       </c>
@@ -5722,14 +5755,14 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" s="1" customFormat="1">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -5740,27 +5773,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" s="1" customFormat="1">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="58" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" s="1" customFormat="1">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="57"/>
-    </row>
-    <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="58"/>
+    </row>
+    <row r="5" spans="2:4" s="1" customFormat="1">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5771,7 +5804,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" s="1" customFormat="1">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -5782,7 +5815,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" s="1" customFormat="1">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -5793,7 +5826,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="8" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" s="1" customFormat="1">
       <c r="B8" s="5" t="s">
         <v>354</v>
       </c>
@@ -5804,7 +5837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" s="1" customFormat="1">
       <c r="B9" s="3" t="s">
         <v>350</v>
       </c>
@@ -5815,7 +5848,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" s="1" customFormat="1">
       <c r="B10" s="3" t="s">
         <v>351</v>
       </c>
@@ -5826,7 +5859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" s="1" customFormat="1">
       <c r="B11" s="3">
         <v>58</v>
       </c>
@@ -5837,7 +5870,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" s="1" customFormat="1">
       <c r="B12" s="3">
         <v>59</v>
       </c>
@@ -5865,7 +5898,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -5876,12 +5909,12 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18.75">
       <c r="A2" s="8" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="27" t="s">
         <v>147</v>
       </c>
@@ -5889,12 +5922,12 @@
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -5905,27 +5938,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="57" t="s">
+      <c r="D7" s="58" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="57"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="58"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -5936,7 +5969,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -5947,7 +5980,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
@@ -5958,7 +5991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12" s="5" t="s">
         <v>134</v>
       </c>
@@ -5969,7 +6002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13" s="3" t="s">
         <v>135</v>
       </c>
@@ -5980,7 +6013,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14" s="3">
         <v>26</v>
       </c>
@@ -5991,7 +6024,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="B15" s="3">
         <v>27</v>
       </c>
@@ -6002,7 +6035,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="3">
         <v>28</v>
       </c>
@@ -6013,7 +6046,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="B17" s="3">
         <v>29</v>
       </c>
@@ -6024,7 +6057,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="B18" s="3" t="s">
         <v>137</v>
       </c>
@@ -6035,7 +6068,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="B19" s="3" t="s">
         <v>132</v>
       </c>
@@ -6046,7 +6079,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="B20" s="3" t="s">
         <v>138</v>
       </c>
@@ -6057,7 +6090,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="B21" s="3" t="s">
         <v>139</v>
       </c>
@@ -6068,7 +6101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="B22" s="3">
         <v>58</v>
       </c>
@@ -6079,7 +6112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="B23" s="3">
         <v>59</v>
       </c>
@@ -6090,17 +6123,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="18.75">
       <c r="A25" s="8" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
@@ -6111,27 +6144,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="B28" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="57" t="s">
+      <c r="D28" s="58" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="B29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="57"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="58"/>
+    </row>
+    <row r="30" spans="1:4">
       <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
@@ -6142,7 +6175,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="B31" s="5" t="s">
         <v>22</v>
       </c>
@@ -6153,7 +6186,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="B32" s="5" t="s">
         <v>23</v>
       </c>
@@ -6164,7 +6197,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4">
       <c r="B33" s="5" t="s">
         <v>134</v>
       </c>
@@ -6175,7 +6208,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4">
       <c r="B34" s="5" t="s">
         <v>194</v>
       </c>
@@ -6186,7 +6219,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4">
       <c r="B35" s="5" t="s">
         <v>195</v>
       </c>
@@ -6197,7 +6230,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4">
       <c r="B36" s="3" t="s">
         <v>196</v>
       </c>
@@ -6208,7 +6241,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4">
       <c r="B37" s="3" t="s">
         <v>197</v>
       </c>
@@ -6219,7 +6252,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4">
       <c r="B38" s="3" t="s">
         <v>198</v>
       </c>
@@ -6230,7 +6263,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4">
       <c r="B39" s="3">
         <v>51</v>
       </c>
@@ -6241,7 +6274,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4">
       <c r="B40" s="3">
         <v>52</v>
       </c>
@@ -6252,7 +6285,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4">
       <c r="B41" s="3">
         <v>53</v>
       </c>
@@ -6263,7 +6296,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4">
       <c r="B42" s="3">
         <v>54</v>
       </c>
@@ -6274,7 +6307,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4">
       <c r="B43" s="3">
         <v>55</v>
       </c>
@@ -6285,7 +6318,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4">
       <c r="B44" s="3" t="s">
         <v>210</v>
       </c>
@@ -6296,7 +6329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4">
       <c r="B45" s="3">
         <v>58</v>
       </c>
@@ -6307,7 +6340,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4">
       <c r="B46" s="3">
         <v>59</v>
       </c>
@@ -6318,17 +6351,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4">
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4">
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4">
       <c r="C49" s="1" t="s">
         <v>148</v>
       </c>
@@ -6336,17 +6369,17 @@
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4">
       <c r="D50" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4">
       <c r="D51" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4">
       <c r="D52" s="1" t="s">
         <v>152</v>
       </c>
@@ -6370,17 +6403,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="158.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:3" ht="60">
       <c r="C2" s="24" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:3">
       <c r="C5" t="s">
         <v>145</v>
       </c>
@@ -6399,7 +6432,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
@@ -6409,7 +6442,7 @@
     <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10">
       <c r="B3" s="40" t="s">
         <v>229</v>
       </c>
@@ -6436,7 +6469,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="B4" s="39" t="s">
         <v>237</v>
       </c>
@@ -6462,7 +6495,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="B5" t="s">
         <v>228</v>
       </c>
@@ -6488,7 +6521,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="B6" t="s">
         <v>338</v>
       </c>
@@ -6514,7 +6547,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10">
       <c r="B7" t="s">
         <v>341</v>
       </c>
@@ -6540,7 +6573,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="B8" t="s">
         <v>226</v>
       </c>
@@ -6566,7 +6599,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="B9" t="s">
         <v>227</v>
       </c>
@@ -6592,7 +6625,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="B10" t="s">
         <v>289</v>
       </c>
@@ -6612,7 +6645,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="B11" t="s">
         <v>290</v>
       </c>
@@ -6632,7 +6665,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10">
       <c r="B12" t="s">
         <v>288</v>
       </c>
@@ -6652,7 +6685,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10">
       <c r="B13" t="s">
         <v>296</v>
       </c>
@@ -6672,7 +6705,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10">
       <c r="B15" t="s">
         <v>267</v>
       </c>
@@ -6689,7 +6722,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10">
       <c r="B16" t="s">
         <v>268</v>
       </c>
@@ -6709,7 +6742,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9">
       <c r="B18" t="s">
         <v>238</v>
       </c>
@@ -6732,7 +6765,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9">
       <c r="B20" t="s">
         <v>241</v>
       </c>
@@ -6755,7 +6788,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9">
       <c r="B21" t="s">
         <v>245</v>
       </c>
@@ -6778,7 +6811,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9">
       <c r="B22" t="s">
         <v>252</v>
       </c>
@@ -6801,7 +6834,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9">
       <c r="B23" t="s">
         <v>330</v>
       </c>
@@ -6821,7 +6854,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9">
       <c r="B24" t="s">
         <v>331</v>
       </c>
@@ -6841,7 +6874,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9">
       <c r="B25" t="s">
         <v>332</v>
       </c>
@@ -6861,7 +6894,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9">
       <c r="B27" t="s">
         <v>246</v>
       </c>
@@ -6884,7 +6917,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9">
       <c r="B28" t="s">
         <v>247</v>
       </c>
@@ -6907,7 +6940,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9">
       <c r="B29" t="s">
         <v>251</v>
       </c>
@@ -6930,7 +6963,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9">
       <c r="B30" t="s">
         <v>255</v>
       </c>
@@ -6953,7 +6986,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9">
       <c r="B31" t="s">
         <v>256</v>
       </c>
@@ -6976,7 +7009,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9">
       <c r="B32" t="s">
         <v>257</v>
       </c>
@@ -6999,7 +7032,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9">
       <c r="B33" t="s">
         <v>273</v>
       </c>
@@ -7019,7 +7052,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9">
       <c r="B34" t="s">
         <v>274</v>
       </c>
@@ -7039,7 +7072,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9">
       <c r="B35" t="s">
         <v>276</v>
       </c>
@@ -7059,7 +7092,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" t="s">
         <v>285</v>
       </c>
@@ -7082,7 +7115,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9">
       <c r="B38" t="s">
         <v>261</v>
       </c>
@@ -7105,7 +7138,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9">
       <c r="B39" t="s">
         <v>278</v>
       </c>
@@ -7125,7 +7158,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9">
       <c r="B40" t="s">
         <v>279</v>
       </c>
@@ -7145,7 +7178,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9">
       <c r="B41" t="s">
         <v>283</v>
       </c>

</xml_diff>

<commit_message>
- Add support for generic HaiLzd command
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -188,13 +188,6 @@
     <t>A9 9A 02 0A 0C ED</t>
   </si>
   <si>
-    <t>A9 9A 07 0A 00 01 01 01 01 15 ED</t>
-  </si>
-  <si>
-    <t>For enquiry, set {len}=2 (i.e. no parm)
-For set, {len}=7, 5 on/off flag for (V1,V2,BT,CB,SV)</t>
-  </si>
-  <si>
     <t>Fix {len}</t>
   </si>
   <si>
@@ -1617,6 +1610,13 @@
   </si>
   <si>
     <t>A9 9A 03 16 01 1A ED</t>
+  </si>
+  <si>
+    <t>A9 9A 08 0A 00 01 01 01 01 01 17 ED</t>
+  </si>
+  <si>
+    <t>For enquiry, set {len}=2 (i.e. no parm)
+For set, {len}=8, 6 on/off flag for (V1,V2,BT,CB,SV, HAILZD)</t>
   </si>
 </sst>
 </file>
@@ -2202,7 +2202,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2313,7 +2313,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>44</v>
@@ -2325,13 +2325,13 @@
         <v>50</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="2:14">
@@ -2342,25 +2342,25 @@
         <v>40</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>46</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="2:14">
@@ -2371,7 +2371,7 @@
         <v>41</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>51</v>
@@ -2383,13 +2383,13 @@
         <v>48</v>
       </c>
       <c r="I14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="15" spans="2:14">
@@ -2400,7 +2400,7 @@
         <v>42</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>51</v>
@@ -2409,16 +2409,16 @@
         <v>52</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="16" spans="2:14">
@@ -2426,68 +2426,68 @@
         <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="43"/>
       <c r="F16" s="4" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="43"/>
       <c r="F17" s="4" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G17" s="4"/>
       <c r="I17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K17" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="46"/>
       <c r="F18" s="4" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G18" s="4"/>
       <c r="I18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K18" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="45">
@@ -2495,165 +2495,165 @@
         <v>53</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>56</v>
+        <v>527</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>54</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>55</v>
+        <v>526</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="2:13">
       <c r="B20" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>45</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G20" s="12"/>
       <c r="I20" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="2:13">
       <c r="B21" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G21" s="12"/>
       <c r="I21" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="22" spans="2:13">
       <c r="B22" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E22" s="23"/>
       <c r="F22" s="4" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="G22" s="12"/>
       <c r="I22" s="4" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="23" spans="2:13">
       <c r="B23" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E23" s="23"/>
       <c r="F23" s="4" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G23" s="12"/>
       <c r="I23" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K23" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="J23" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>113</v>
-      </c>
       <c r="M23" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="24" spans="2:13">
       <c r="B24" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="23" t="s">
         <v>512</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="23" t="s">
+      <c r="G24" s="12" t="s">
         <v>514</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="H24" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="G24" s="12" t="s">
-        <v>516</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>517</v>
-      </c>
       <c r="I24" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K24" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -2661,26 +2661,26 @@
         <v>10</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>517</v>
+      </c>
+      <c r="E25" s="23" t="s">
         <v>518</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="F25" s="4" t="s">
         <v>519</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>520</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>521</v>
       </c>
       <c r="G25" s="12"/>
       <c r="I25" s="4" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="J25" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="K25" s="4" t="s">
         <v>522</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="26" spans="2:13">
@@ -2688,26 +2688,26 @@
         <v>11</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>45</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G26" s="4"/>
       <c r="I26" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -2715,26 +2715,26 @@
         <v>12</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G27" s="4"/>
       <c r="I27" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="2:13">
@@ -2742,26 +2742,26 @@
         <v>13</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>45</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G28" s="4"/>
       <c r="I28" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -2769,26 +2769,26 @@
         <v>14</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="G29" s="4"/>
       <c r="I29" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -2796,20 +2796,20 @@
         <v>15</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="41"/>
       <c r="F30" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -2817,16 +2817,16 @@
         <v>16</v>
       </c>
       <c r="C31" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="57" t="s">
+        <v>524</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>525</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E31" s="57" t="s">
-        <v>526</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>527</v>
       </c>
       <c r="G31" s="4"/>
       <c r="I31" s="4"/>
@@ -2838,26 +2838,26 @@
         <v>21</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="G32" s="4"/>
       <c r="I32" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="2:11">
@@ -2865,26 +2865,26 @@
         <v>22</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="2:11" ht="30">
@@ -2892,26 +2892,26 @@
         <v>23</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="2:11">
@@ -2919,26 +2919,26 @@
         <v>24</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G35" s="4"/>
       <c r="I35" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K35" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="36" spans="2:11">
@@ -2946,28 +2946,28 @@
         <v>31</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>51</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I36" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K36" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="37" spans="2:11">
@@ -2975,26 +2975,26 @@
         <v>32</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E37" s="28" t="s">
         <v>45</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G37" s="12"/>
       <c r="I37" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K37" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="38" spans="2:11">
@@ -3002,28 +3002,28 @@
         <v>33</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I38" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K38" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="39" spans="2:11">
@@ -3031,26 +3031,26 @@
         <v>34</v>
       </c>
       <c r="C39" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E39" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="G39" s="12"/>
       <c r="I39" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K39" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="40" spans="2:11">
@@ -3058,26 +3058,26 @@
         <v>35</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G40" s="12"/>
       <c r="I40" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K40" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="41" spans="2:11">
@@ -3085,28 +3085,28 @@
         <v>36</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G41" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E41" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="F41" s="4" t="s">
+      <c r="I41" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K41" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="42" spans="2:11">
@@ -3114,26 +3114,26 @@
         <v>41</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E42" s="26" t="s">
         <v>6</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G42" s="4"/>
       <c r="I42" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K42" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="43" spans="2:11">
@@ -3141,53 +3141,53 @@
         <v>42</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G43" s="4"/>
       <c r="I43" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K43" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K43" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="44" spans="2:11">
       <c r="B44" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E44" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G44" s="4"/>
       <c r="I44" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K44" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="45" spans="2:11">
@@ -3195,26 +3195,26 @@
         <v>60</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E45" s="32" t="s">
         <v>45</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G45" s="4"/>
       <c r="I45" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="46" spans="2:11">
@@ -3222,26 +3222,26 @@
         <v>61</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G46" s="4"/>
       <c r="I46" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="2:11">
@@ -3249,26 +3249,26 @@
         <v>62</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G47" s="4"/>
       <c r="I47" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K47" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="48" spans="2:11" s="38" customFormat="1">
@@ -3276,26 +3276,26 @@
         <v>63</v>
       </c>
       <c r="C48" s="36" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E48" s="37" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F48" s="36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G48" s="36"/>
       <c r="I48" s="36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J48" s="36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K48" s="36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="2:11">
@@ -3303,26 +3303,26 @@
         <v>68</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E49" s="42" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G49" s="4"/>
       <c r="I49" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="50" spans="2:11">
@@ -3330,22 +3330,22 @@
         <v>69</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D50" s="25"/>
       <c r="E50" s="42"/>
       <c r="F50" s="4" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G50" s="4"/>
       <c r="I50" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K50" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K50" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="51" spans="2:11">
@@ -3353,16 +3353,16 @@
         <v>71</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G51" s="4"/>
       <c r="I51" s="4"/>
@@ -3374,10 +3374,10 @@
         <v>72</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E52" s="18"/>
       <c r="F52" s="4"/>
@@ -3391,26 +3391,26 @@
         <v>74</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G53" s="4"/>
       <c r="I53" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K53" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="54" spans="2:11">
@@ -3418,26 +3418,26 @@
         <v>75</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E54" s="26" t="s">
         <v>6</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G54" s="4"/>
       <c r="I54" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="2:11">
@@ -3453,58 +3453,58 @@
     </row>
     <row r="56" spans="2:11" s="38" customFormat="1">
       <c r="B56" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="E56" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="C56" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D56" s="36" t="s">
+      <c r="F56" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="E56" s="37" t="s">
+      <c r="G56" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="F56" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="G56" s="36" t="s">
-        <v>87</v>
-      </c>
       <c r="I56" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="J56" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="K56" s="36" t="s">
         <v>111</v>
-      </c>
-      <c r="J56" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="K56" s="36" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="57" spans="2:11" s="38" customFormat="1">
       <c r="B57" s="35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C57" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E57" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="D57" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="E57" s="37" t="s">
-        <v>91</v>
-      </c>
       <c r="F57" s="36" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G57" s="36"/>
       <c r="I57" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="J57" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="K57" s="36" t="s">
         <v>111</v>
-      </c>
-      <c r="J57" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="K57" s="36" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -3541,7 +3541,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="2:5">
@@ -3571,10 +3571,10 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D5" s="43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E5" s="45"/>
     </row>
@@ -3583,10 +3583,10 @@
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E6" s="45"/>
     </row>
@@ -3595,111 +3595,111 @@
         <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D7" s="43" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E7" s="45" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D8" s="43" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E8" s="45" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D9" s="43" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E9" s="45" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="D10" s="43" t="s">
         <v>411</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="E10" s="45" t="s">
         <v>412</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>413</v>
-      </c>
-      <c r="E10" s="45" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="D11" s="43" t="s">
         <v>359</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>361</v>
-      </c>
       <c r="E11" s="45" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E12" s="45" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D13" s="43" t="s">
         <v>365</v>
       </c>
-      <c r="D13" s="43" t="s">
-        <v>367</v>
-      </c>
       <c r="E13" s="45" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="D14" s="43" t="s">
         <v>368</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>370</v>
-      </c>
       <c r="E14" s="45" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="15" spans="2:5">
@@ -3707,13 +3707,13 @@
         <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>418</v>
+      </c>
+      <c r="E15" s="45" t="s">
         <v>419</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>420</v>
-      </c>
-      <c r="E15" s="45" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="16" spans="2:5">
@@ -3721,13 +3721,13 @@
         <v>21</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E16" s="45" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="2:5">
@@ -3735,13 +3735,13 @@
         <v>22</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E17" s="45" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="18" spans="2:5">
@@ -3749,13 +3749,13 @@
         <v>23</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D18" s="43" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E18" s="45" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="19" spans="2:5">
@@ -3763,13 +3763,13 @@
         <v>24</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D19" s="43" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E19" s="45" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="20" spans="2:5">
@@ -3777,13 +3777,13 @@
         <v>31</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D20" s="43" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E20" s="45" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="21" spans="2:5">
@@ -3791,13 +3791,13 @@
         <v>32</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E21" s="45" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="22" spans="2:5">
@@ -3805,13 +3805,13 @@
         <v>33</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E22" s="45" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="23" spans="2:5">
@@ -3819,13 +3819,13 @@
         <v>41</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D23" s="43" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E23" s="45" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="24" spans="2:5">
@@ -3833,13 +3833,13 @@
         <v>42</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E24" s="45" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="25" spans="2:5">
@@ -3847,13 +3847,13 @@
         <v>43</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D25" s="43" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E25" s="45" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="26" spans="2:5">
@@ -3915,13 +3915,13 @@
   <sheetData>
     <row r="1" spans="2:42">
       <c r="I1" s="52" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J1" s="52" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="K1" s="52" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L1" s="53">
         <v>0</v>
@@ -3938,19 +3938,19 @@
         <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I2" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="K2" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L2" s="54">
         <v>1</v>
@@ -4001,13 +4001,13 @@
       </c>
       <c r="F3" s="45"/>
       <c r="I3" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="K3" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L3" s="54">
         <v>2</v>
@@ -4056,13 +4056,13 @@
       </c>
       <c r="F4" s="45"/>
       <c r="I4" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J4" s="51" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K4" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L4" s="54">
         <v>3</v>
@@ -4103,23 +4103,23 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E5" s="48">
         <v>1</v>
       </c>
       <c r="F5" s="45"/>
       <c r="I5" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J5" s="51" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="K5" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L5" s="54">
         <v>4</v>
@@ -4160,23 +4160,23 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E6" s="48">
         <v>1</v>
       </c>
       <c r="F6" s="45"/>
       <c r="I6" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J6" s="51" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K6" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L6" s="54">
         <v>5</v>
@@ -4217,23 +4217,23 @@
         <v>4</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E7" s="49">
         <v>1</v>
       </c>
       <c r="F7" s="45"/>
       <c r="I7" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J7" s="51" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="K7" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L7" s="54">
         <v>6</v>
@@ -4274,23 +4274,23 @@
         <v>5</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D8" s="49" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E8" s="49">
         <v>1</v>
       </c>
       <c r="F8" s="45"/>
       <c r="I8" s="51" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="J8" s="51" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="K8" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L8" s="54">
         <v>8</v>
@@ -4331,23 +4331,23 @@
         <v>6</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E9" s="49">
         <v>2</v>
       </c>
       <c r="F9" s="45"/>
       <c r="I9" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J9" s="51" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="K9" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L9" s="54">
         <v>9</v>
@@ -4388,23 +4388,23 @@
         <v>8</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E10" s="49">
         <v>1</v>
       </c>
       <c r="F10" s="45"/>
       <c r="I10" s="51" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="J10" s="51" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K10" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L10" s="54">
         <v>10</v>
@@ -4445,23 +4445,23 @@
         <v>9</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E11" s="49">
         <v>1</v>
       </c>
       <c r="F11" s="45"/>
       <c r="I11" s="51" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="J11" s="51" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="K11" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L11" s="54">
         <v>40</v>
@@ -4502,23 +4502,23 @@
         <v>10</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E12" s="49">
         <v>30</v>
       </c>
       <c r="F12" s="45"/>
       <c r="I12" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J12" s="51" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K12" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L12" s="54">
         <v>60</v>
@@ -4559,23 +4559,23 @@
         <v>40</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E13" s="49">
         <v>20</v>
       </c>
       <c r="F13" s="45"/>
       <c r="I13" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J13" s="51" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="K13" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L13" s="54">
         <v>61</v>
@@ -4616,23 +4616,23 @@
         <v>60</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E14" s="49">
         <v>1</v>
       </c>
       <c r="F14" s="45"/>
       <c r="I14" s="51" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="J14" s="51" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="K14" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L14" s="54">
         <v>62</v>
@@ -4673,23 +4673,23 @@
         <v>61</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D15" s="49" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E15" s="49">
         <v>1</v>
       </c>
       <c r="F15" s="45"/>
       <c r="I15" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J15" s="51" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="K15" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L15" s="54">
         <v>63</v>
@@ -4730,23 +4730,23 @@
         <v>62</v>
       </c>
       <c r="C16" s="49" t="s">
+        <v>494</v>
+      </c>
+      <c r="D16" s="49" t="s">
         <v>496</v>
-      </c>
-      <c r="D16" s="49" t="s">
-        <v>498</v>
       </c>
       <c r="E16" s="49">
         <v>1</v>
       </c>
       <c r="F16" s="45"/>
       <c r="I16" s="51" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="J16" s="51" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K16" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L16" s="54">
         <v>64</v>
@@ -4787,23 +4787,23 @@
         <v>63</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="E17" s="49">
         <v>1</v>
       </c>
       <c r="F17" s="45"/>
       <c r="I17" s="51" t="s">
+        <v>455</v>
+      </c>
+      <c r="J17" s="51" t="s">
+        <v>474</v>
+      </c>
+      <c r="K17" s="51" t="s">
         <v>457</v>
-      </c>
-      <c r="J17" s="51" t="s">
-        <v>476</v>
-      </c>
-      <c r="K17" s="51" t="s">
-        <v>459</v>
       </c>
       <c r="L17" s="54">
         <v>84</v>
@@ -4844,23 +4844,23 @@
         <v>64</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E18" s="49">
         <v>20</v>
       </c>
       <c r="F18" s="45"/>
       <c r="I18" s="51" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="J18" s="51" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="K18" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L18" s="54">
         <v>104</v>
@@ -4901,23 +4901,23 @@
         <v>84</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D19" s="49" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E19" s="49">
         <v>20</v>
       </c>
       <c r="F19" s="45"/>
       <c r="I19" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J19" s="51" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="K19" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L19" s="54">
         <v>105</v>
@@ -4958,23 +4958,23 @@
         <v>104</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E20" s="49">
         <v>1</v>
       </c>
       <c r="F20" s="45"/>
       <c r="I20" s="51" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="J20" s="51" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="K20" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L20" s="54">
         <v>106</v>
@@ -5015,23 +5015,23 @@
         <v>105</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D21" s="49" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E21" s="49">
         <v>1</v>
       </c>
       <c r="F21" s="45"/>
       <c r="I21" s="51" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="J21" s="51" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="K21" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L21" s="54">
         <v>108</v>
@@ -5072,23 +5072,23 @@
         <v>106</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D22" s="49" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E22" s="49">
         <v>2</v>
       </c>
       <c r="F22" s="45"/>
       <c r="I22" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J22" s="51" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="K22" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L22" s="54">
         <v>109</v>
@@ -5129,23 +5129,23 @@
         <v>108</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E23" s="49">
         <v>1</v>
       </c>
       <c r="F23" s="45"/>
       <c r="I23" s="51" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="J23" s="51" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="K23" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L23" s="54">
         <v>110</v>
@@ -5186,23 +5186,23 @@
         <v>109</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E24" s="49">
         <v>1</v>
       </c>
       <c r="F24" s="45"/>
       <c r="I24" s="51" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="J24" s="51" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="K24" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L24" s="54">
         <v>112</v>
@@ -5243,23 +5243,23 @@
         <v>110</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E25" s="49">
         <v>2</v>
       </c>
       <c r="F25" s="45"/>
       <c r="I25" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J25" s="51" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="K25" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L25" s="54">
         <v>114</v>
@@ -5300,23 +5300,23 @@
         <v>112</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D26" s="49" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E26" s="49">
         <v>2</v>
       </c>
       <c r="F26" s="45"/>
       <c r="I26" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J26" s="51" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="K26" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L26" s="54">
         <v>118</v>
@@ -5357,23 +5357,23 @@
         <v>114</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E27" s="49">
         <v>4</v>
       </c>
       <c r="F27" s="45"/>
       <c r="I27" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J27" s="51" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="K27" s="51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L27" s="54">
         <v>119</v>
@@ -5644,10 +5644,10 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -5655,10 +5655,10 @@
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="2:4">
@@ -5666,48 +5666,48 @@
         <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D8" s="47" t="s">
         <v>432</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="D9" s="47" t="s">
         <v>435</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="D10" s="47" t="s">
         <v>438</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="D10" s="47" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="3" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
@@ -5798,10 +5798,10 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="2:4" s="1" customFormat="1">
@@ -5809,10 +5809,10 @@
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="2:4" s="1" customFormat="1">
@@ -5823,12 +5823,12 @@
         <v>26</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="2:4" s="1" customFormat="1">
       <c r="B8" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
@@ -5839,18 +5839,18 @@
     </row>
     <row r="9" spans="2:4" s="1" customFormat="1">
       <c r="B9" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="D9" s="42" t="s">
         <v>350</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="10" spans="2:4" s="1" customFormat="1">
       <c r="B10" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
@@ -5911,12 +5911,12 @@
   <sheetData>
     <row r="2" spans="1:4" ht="18.75">
       <c r="A2" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
@@ -5963,10 +5963,10 @@
         <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5974,10 +5974,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5993,7 +5993,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>4</v>
@@ -6004,13 +6004,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="B13" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -6021,7 +6021,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -6032,7 +6032,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -6051,26 +6051,26 @@
         <v>29</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="B18" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="B19" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>13</v>
@@ -6081,18 +6081,18 @@
     </row>
     <row r="20" spans="1:4">
       <c r="B20" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="B21" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>4</v>
@@ -6130,7 +6130,7 @@
     </row>
     <row r="25" spans="1:4" ht="18.75">
       <c r="A25" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -6169,10 +6169,10 @@
         <v>21</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -6180,10 +6180,10 @@
         <v>22</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -6191,7 +6191,7 @@
         <v>23</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>6</v>
@@ -6199,7 +6199,7 @@
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>26</v>
@@ -6210,7 +6210,7 @@
     </row>
     <row r="34" spans="2:4">
       <c r="B34" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>27</v>
@@ -6221,18 +6221,18 @@
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>30</v>
@@ -6243,24 +6243,24 @@
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="2:4">
@@ -6268,10 +6268,10 @@
         <v>51</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="2:4">
@@ -6279,10 +6279,10 @@
         <v>52</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D40" s="29" t="s">
         <v>166</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="41" spans="2:4">
@@ -6290,10 +6290,10 @@
         <v>53</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41" s="29" t="s">
         <v>167</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="42" spans="2:4">
@@ -6301,10 +6301,10 @@
         <v>54</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="43" spans="2:4">
@@ -6312,15 +6312,15 @@
         <v>55</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D43" s="34" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="2:4">
       <c r="B44" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>4</v>
@@ -6363,25 +6363,25 @@
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="D50" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="D51" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="D52" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -6410,12 +6410,12 @@
   <sheetData>
     <row r="2" spans="3:3" ht="60">
       <c r="C2" s="24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -6444,761 +6444,761 @@
   <sheetData>
     <row r="3" spans="2:10">
       <c r="B3" s="40" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C3" s="40" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G3" s="40"/>
       <c r="H3" s="40" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I3" s="40" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="2:10">
       <c r="B4" s="39" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="2:10">
       <c r="B5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="2:10">
       <c r="B6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C6" t="s">
+        <v>337</v>
+      </c>
+      <c r="D6" t="s">
         <v>338</v>
       </c>
-      <c r="C6" t="s">
-        <v>339</v>
-      </c>
-      <c r="D6" t="s">
-        <v>340</v>
-      </c>
       <c r="E6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="2:10">
       <c r="B7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D7" t="s">
         <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="2:10">
       <c r="B8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D8" t="s">
         <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D9" t="s">
         <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="2:10">
       <c r="B10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D10" t="s">
         <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H10" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="2:10">
       <c r="B11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D11" t="s">
         <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="2:10">
       <c r="B12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H12" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="2:10">
       <c r="B13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C13" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D13" t="s">
         <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="2:10">
       <c r="B15" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C15" t="s">
         <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H15" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="2:10">
       <c r="B16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C16" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H16" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J16" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" t="s">
+        <v>237</v>
+      </c>
+      <c r="D18" t="s">
         <v>238</v>
       </c>
-      <c r="C18" t="s">
-        <v>239</v>
-      </c>
-      <c r="D18" t="s">
-        <v>240</v>
-      </c>
       <c r="E18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H18" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I18" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" t="s">
+        <v>239</v>
+      </c>
+      <c r="C20" t="s">
+        <v>240</v>
+      </c>
+      <c r="D20" t="s">
         <v>241</v>
       </c>
-      <c r="C20" t="s">
-        <v>242</v>
-      </c>
-      <c r="D20" t="s">
-        <v>243</v>
-      </c>
       <c r="E20" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H20" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I20" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D21" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E21" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I21" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="2:9">
       <c r="B22" t="s">
+        <v>250</v>
+      </c>
+      <c r="C22" t="s">
+        <v>251</v>
+      </c>
+      <c r="D22" t="s">
         <v>252</v>
       </c>
-      <c r="C22" t="s">
-        <v>253</v>
-      </c>
-      <c r="D22" t="s">
-        <v>254</v>
-      </c>
       <c r="E22" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H22" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I22" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" spans="2:9">
       <c r="B23" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C23" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D23" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H23" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="2:9">
       <c r="B24" t="s">
+        <v>329</v>
+      </c>
+      <c r="C24" t="s">
         <v>331</v>
       </c>
-      <c r="C24" t="s">
-        <v>333</v>
-      </c>
       <c r="D24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E24" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H24" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="25" spans="2:9">
       <c r="B25" t="s">
+        <v>330</v>
+      </c>
+      <c r="C25" t="s">
         <v>332</v>
-      </c>
-      <c r="C25" t="s">
-        <v>334</v>
       </c>
       <c r="D25" t="s">
         <v>45</v>
       </c>
       <c r="E25" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H25" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="27" spans="2:9">
       <c r="B27" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D27" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E27" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H27" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I27" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="28" spans="2:9">
       <c r="B28" t="s">
+        <v>245</v>
+      </c>
+      <c r="C28" t="s">
         <v>247</v>
       </c>
-      <c r="C28" t="s">
-        <v>249</v>
-      </c>
       <c r="D28" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F28" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I28" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="2:9">
       <c r="B29" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C29" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D29" t="s">
         <v>45</v>
       </c>
       <c r="E29" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H29" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I29" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="30" spans="2:9">
       <c r="B30" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E30" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F30" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H30" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I30" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="31" spans="2:9">
       <c r="B31" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C31" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D31" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H31" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I31" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="32" spans="2:9">
       <c r="B32" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C32" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D32" t="s">
         <v>45</v>
       </c>
       <c r="E32" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H32" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I32" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" spans="2:9">
       <c r="B33" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C33" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D33" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E33" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H33" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="34" spans="2:9">
       <c r="B34" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C34" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D34" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E34" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F34" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H34" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="35" spans="2:9">
       <c r="B35" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C35" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D35" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E35" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F35" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H35" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" spans="2:9">
       <c r="B36" t="s">
+        <v>283</v>
+      </c>
+      <c r="C36" t="s">
+        <v>284</v>
+      </c>
+      <c r="D36" t="s">
         <v>285</v>
       </c>
-      <c r="C36" t="s">
-        <v>286</v>
-      </c>
-      <c r="D36" t="s">
-        <v>287</v>
-      </c>
       <c r="E36" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F36" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H36" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I36" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="38" spans="2:9">
       <c r="B38" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C38" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D38" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E38" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H38" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I38" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="2:9">
       <c r="B39" t="s">
+        <v>276</v>
+      </c>
+      <c r="C39" t="s">
         <v>278</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
+        <v>238</v>
+      </c>
+      <c r="E39" t="s">
         <v>280</v>
       </c>
-      <c r="D39" t="s">
-        <v>240</v>
-      </c>
-      <c r="E39" t="s">
-        <v>282</v>
-      </c>
       <c r="F39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H39" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="40" spans="2:9">
       <c r="B40" t="s">
+        <v>277</v>
+      </c>
+      <c r="C40" t="s">
         <v>279</v>
       </c>
-      <c r="C40" t="s">
-        <v>281</v>
-      </c>
       <c r="D40" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E40" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H40" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="41" spans="2:9">
       <c r="B41" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C41" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D41" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E41" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H41" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I41" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add version for firmware
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="533">
   <si>
     <t>Offset</t>
   </si>
@@ -1612,22 +1612,43 @@
     <t>A9 9A 03 16 01 1A ED</t>
   </si>
   <si>
-    <t>A9 9A 08 0A 00 01 01 01 01 01 17 ED</t>
-  </si>
-  <si>
     <t>For enquiry, set {len}=2 (i.e. no parm)
 For set, {len}=8, 6 on/off flag for (V1,V2,BT,CB,SV, HAILZD)</t>
+  </si>
+  <si>
+    <t>FF</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get Control Board Version</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes {2} </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nil</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>A9 9A 02 FF 01 ED</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>A9 9A 08 0A 00 01 01 01 01 01 17 ED</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1635,7 +1656,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1645,7 +1666,7 @@
       <u/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1655,19 +1676,19 @@
       <u/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2196,16 +2217,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N57"/>
+  <dimension ref="B2:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -2219,7 +2240,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2227,7 +2248,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -2238,7 +2259,7 @@
       <c r="G3" s="13"/>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -2250,7 +2271,7 @@
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -2262,7 +2283,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -2278,7 +2299,7 @@
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -2287,7 +2308,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
@@ -2296,7 +2317,7 @@
       </c>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
@@ -2305,7 +2326,7 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="12" spans="2:14">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
@@ -2334,7 +2355,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
@@ -2363,7 +2384,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
@@ -2392,7 +2413,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
@@ -2421,7 +2442,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="2:14">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
@@ -2444,7 +2465,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>132</v>
       </c>
@@ -2467,7 +2488,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>192</v>
       </c>
@@ -2490,7 +2511,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="45">
+    <row r="19" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>53</v>
       </c>
@@ -2501,13 +2522,13 @@
         <v>58</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>54</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>105</v>
@@ -2519,7 +2540,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="2:13">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>213</v>
       </c>
@@ -2546,7 +2567,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="2:13">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>424</v>
       </c>
@@ -2571,7 +2592,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="22" spans="2:13">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>441</v>
       </c>
@@ -2596,7 +2617,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>445</v>
       </c>
@@ -2624,7 +2645,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="24" spans="2:13">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>510</v>
       </c>
@@ -2656,7 +2677,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="2:13">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
         <v>10</v>
       </c>
@@ -2683,7 +2704,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="26" spans="2:13">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
         <v>11</v>
       </c>
@@ -2710,7 +2731,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="2:13">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
         <v>12</v>
       </c>
@@ -2737,7 +2758,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="2:13">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
         <v>13</v>
       </c>
@@ -2764,7 +2785,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="2:13">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <v>14</v>
       </c>
@@ -2791,7 +2812,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="2:13">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>15</v>
       </c>
@@ -2812,7 +2833,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="2:13">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
         <v>16</v>
       </c>
@@ -2833,7 +2854,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="2:13">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
         <v>21</v>
       </c>
@@ -2860,7 +2881,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="2:11">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <v>22</v>
       </c>
@@ -2887,7 +2908,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="30">
+    <row r="34" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
         <v>23</v>
       </c>
@@ -2914,7 +2935,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="2:11">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
         <v>24</v>
       </c>
@@ -2941,7 +2962,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="2:11">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
         <v>31</v>
       </c>
@@ -2970,7 +2991,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="2:11">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
         <v>32</v>
       </c>
@@ -2997,7 +3018,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="2:11">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="3">
         <v>33</v>
       </c>
@@ -3026,7 +3047,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="2:11">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
         <v>34</v>
       </c>
@@ -3053,7 +3074,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="2:11">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
         <v>35</v>
       </c>
@@ -3080,7 +3101,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="2:11">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
         <v>36</v>
       </c>
@@ -3109,7 +3130,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="2:11">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="3">
         <v>41</v>
       </c>
@@ -3136,7 +3157,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="2:11">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
         <v>42</v>
       </c>
@@ -3163,7 +3184,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="2:11">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>157</v>
       </c>
@@ -3190,7 +3211,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="2:11">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
         <v>60</v>
       </c>
@@ -3217,7 +3238,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="46" spans="2:11">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
         <v>61</v>
       </c>
@@ -3244,7 +3265,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="2:11">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="3">
         <v>62</v>
       </c>
@@ -3271,7 +3292,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="2:11" s="38" customFormat="1">
+    <row r="48" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="35">
         <v>63</v>
       </c>
@@ -3298,7 +3319,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="2:11">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="3">
         <v>68</v>
       </c>
@@ -3325,7 +3346,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="50" spans="2:11">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="3">
         <v>69</v>
       </c>
@@ -3348,7 +3369,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="2:11">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="3">
         <v>71</v>
       </c>
@@ -3369,7 +3390,7 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
     </row>
-    <row r="52" spans="2:11">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="3">
         <v>72</v>
       </c>
@@ -3386,7 +3407,7 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="2:11" ht="30">
+    <row r="53" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B53" s="3">
         <v>74</v>
       </c>
@@ -3413,7 +3434,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="2:11">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" s="3">
         <v>75</v>
       </c>
@@ -3440,7 +3461,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="55" spans="2:11">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -3451,7 +3472,7 @@
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
     </row>
-    <row r="56" spans="2:11" s="38" customFormat="1">
+    <row r="56" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="35" t="s">
         <v>81</v>
       </c>
@@ -3480,7 +3501,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="2:11" s="38" customFormat="1">
+    <row r="57" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="35" t="s">
         <v>86</v>
       </c>
@@ -3505,6 +3526,23 @@
       </c>
       <c r="K57" s="36" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>530</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>531</v>
       </c>
     </row>
   </sheetData>
@@ -3522,7 +3560,7 @@
       <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -3530,7 +3568,7 @@
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3544,7 +3582,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -3556,7 +3594,7 @@
       </c>
       <c r="E3" s="45"/>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -3566,7 +3604,7 @@
       <c r="D4" s="58"/>
       <c r="E4" s="45"/>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -3578,7 +3616,7 @@
       </c>
       <c r="E5" s="45"/>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -3590,7 +3628,7 @@
       </c>
       <c r="E6" s="45"/>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -3604,7 +3642,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>132</v>
       </c>
@@ -3618,7 +3656,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>192</v>
       </c>
@@ -3632,7 +3670,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>409</v>
       </c>
@@ -3646,7 +3684,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>357</v>
       </c>
@@ -3660,7 +3698,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>360</v>
       </c>
@@ -3674,7 +3712,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>362</v>
       </c>
@@ -3688,7 +3726,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>366</v>
       </c>
@@ -3702,7 +3740,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>18</v>
       </c>
@@ -3716,7 +3754,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>21</v>
       </c>
@@ -3730,7 +3768,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>22</v>
       </c>
@@ -3744,7 +3782,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>23</v>
       </c>
@@ -3758,7 +3796,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>24</v>
       </c>
@@ -3772,7 +3810,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>31</v>
       </c>
@@ -3786,7 +3824,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>32</v>
       </c>
@@ -3800,7 +3838,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>33</v>
       </c>
@@ -3814,7 +3852,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>41</v>
       </c>
@@ -3828,7 +3866,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <v>42</v>
       </c>
@@ -3842,7 +3880,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <v>43</v>
       </c>
@@ -3856,7 +3894,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>58</v>
       </c>
@@ -3868,7 +3906,7 @@
       </c>
       <c r="E26" s="45"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <v>59</v>
       </c>
@@ -3897,7 +3935,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -3913,7 +3951,7 @@
     <col min="18" max="48" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42">
+    <row r="1" spans="2:42" x14ac:dyDescent="0.25">
       <c r="I1" s="52" t="s">
         <v>450</v>
       </c>
@@ -3927,7 +3965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:42">
+    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3986,7 +4024,7 @@
       <c r="AO2" s="11"/>
       <c r="AP2" s="11"/>
     </row>
-    <row r="3" spans="2:42">
+    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B3" s="55">
         <v>0</v>
       </c>
@@ -4043,7 +4081,7 @@
       <c r="AO3" s="11"/>
       <c r="AP3" s="11"/>
     </row>
-    <row r="4" spans="2:42">
+    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B4" s="56">
         <v>1</v>
       </c>
@@ -4098,7 +4136,7 @@
       <c r="AO4" s="11"/>
       <c r="AP4" s="11"/>
     </row>
-    <row r="5" spans="2:42">
+    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B5" s="56">
         <v>2</v>
       </c>
@@ -4155,7 +4193,7 @@
       <c r="AO5" s="11"/>
       <c r="AP5" s="11"/>
     </row>
-    <row r="6" spans="2:42">
+    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B6" s="56">
         <v>3</v>
       </c>
@@ -4212,7 +4250,7 @@
       <c r="AO6" s="11"/>
       <c r="AP6" s="11"/>
     </row>
-    <row r="7" spans="2:42">
+    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B7" s="56">
         <v>4</v>
       </c>
@@ -4269,7 +4307,7 @@
       <c r="AO7" s="11"/>
       <c r="AP7" s="11"/>
     </row>
-    <row r="8" spans="2:42">
+    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B8" s="56">
         <v>5</v>
       </c>
@@ -4326,7 +4364,7 @@
       <c r="AO8" s="11"/>
       <c r="AP8" s="11"/>
     </row>
-    <row r="9" spans="2:42">
+    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B9" s="56">
         <v>6</v>
       </c>
@@ -4383,7 +4421,7 @@
       <c r="AO9" s="11"/>
       <c r="AP9" s="11"/>
     </row>
-    <row r="10" spans="2:42">
+    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B10" s="56">
         <v>8</v>
       </c>
@@ -4440,7 +4478,7 @@
       <c r="AO10" s="11"/>
       <c r="AP10" s="11"/>
     </row>
-    <row r="11" spans="2:42">
+    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B11" s="56">
         <v>9</v>
       </c>
@@ -4497,7 +4535,7 @@
       <c r="AO11" s="11"/>
       <c r="AP11" s="11"/>
     </row>
-    <row r="12" spans="2:42">
+    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B12" s="56">
         <v>10</v>
       </c>
@@ -4554,7 +4592,7 @@
       <c r="AO12" s="11"/>
       <c r="AP12" s="11"/>
     </row>
-    <row r="13" spans="2:42">
+    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B13" s="56">
         <v>40</v>
       </c>
@@ -4611,7 +4649,7 @@
       <c r="AO13" s="11"/>
       <c r="AP13" s="11"/>
     </row>
-    <row r="14" spans="2:42">
+    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B14" s="56">
         <v>60</v>
       </c>
@@ -4668,7 +4706,7 @@
       <c r="AO14" s="11"/>
       <c r="AP14" s="11"/>
     </row>
-    <row r="15" spans="2:42">
+    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B15" s="56">
         <v>61</v>
       </c>
@@ -4725,7 +4763,7 @@
       <c r="AO15" s="11"/>
       <c r="AP15" s="11"/>
     </row>
-    <row r="16" spans="2:42">
+    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B16" s="56">
         <v>62</v>
       </c>
@@ -4782,7 +4820,7 @@
       <c r="AO16" s="11"/>
       <c r="AP16" s="11"/>
     </row>
-    <row r="17" spans="2:42">
+    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B17" s="56">
         <v>63</v>
       </c>
@@ -4839,7 +4877,7 @@
       <c r="AO17" s="11"/>
       <c r="AP17" s="11"/>
     </row>
-    <row r="18" spans="2:42">
+    <row r="18" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B18" s="56">
         <v>64</v>
       </c>
@@ -4896,7 +4934,7 @@
       <c r="AO18" s="11"/>
       <c r="AP18" s="11"/>
     </row>
-    <row r="19" spans="2:42">
+    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B19" s="56">
         <v>84</v>
       </c>
@@ -4953,7 +4991,7 @@
       <c r="AO19" s="11"/>
       <c r="AP19" s="11"/>
     </row>
-    <row r="20" spans="2:42">
+    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B20" s="56">
         <v>104</v>
       </c>
@@ -5010,7 +5048,7 @@
       <c r="AO20" s="11"/>
       <c r="AP20" s="11"/>
     </row>
-    <row r="21" spans="2:42">
+    <row r="21" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B21" s="56">
         <v>105</v>
       </c>
@@ -5067,7 +5105,7 @@
       <c r="AO21" s="11"/>
       <c r="AP21" s="11"/>
     </row>
-    <row r="22" spans="2:42">
+    <row r="22" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B22" s="56">
         <v>106</v>
       </c>
@@ -5124,7 +5162,7 @@
       <c r="AO22" s="11"/>
       <c r="AP22" s="11"/>
     </row>
-    <row r="23" spans="2:42">
+    <row r="23" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B23" s="56">
         <v>108</v>
       </c>
@@ -5181,7 +5219,7 @@
       <c r="AO23" s="11"/>
       <c r="AP23" s="11"/>
     </row>
-    <row r="24" spans="2:42">
+    <row r="24" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B24" s="56">
         <v>109</v>
       </c>
@@ -5238,7 +5276,7 @@
       <c r="AO24" s="11"/>
       <c r="AP24" s="11"/>
     </row>
-    <row r="25" spans="2:42">
+    <row r="25" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B25" s="56">
         <v>110</v>
       </c>
@@ -5295,7 +5333,7 @@
       <c r="AO25" s="11"/>
       <c r="AP25" s="11"/>
     </row>
-    <row r="26" spans="2:42">
+    <row r="26" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B26" s="56">
         <v>112</v>
       </c>
@@ -5352,7 +5390,7 @@
       <c r="AO26" s="11"/>
       <c r="AP26" s="11"/>
     </row>
-    <row r="27" spans="2:42">
+    <row r="27" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B27" s="56">
         <v>114</v>
       </c>
@@ -5409,7 +5447,7 @@
       <c r="AO27" s="11"/>
       <c r="AP27" s="11"/>
     </row>
-    <row r="28" spans="2:42">
+    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B28" s="56">
         <v>118</v>
       </c>
@@ -5458,7 +5496,7 @@
       <c r="AO28" s="11"/>
       <c r="AP28" s="11"/>
     </row>
-    <row r="29" spans="2:42">
+    <row r="29" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B29" s="56">
         <v>119</v>
       </c>
@@ -5507,7 +5545,7 @@
       <c r="AO29" s="11"/>
       <c r="AP29" s="11"/>
     </row>
-    <row r="30" spans="2:42">
+    <row r="30" spans="2:42" x14ac:dyDescent="0.25">
       <c r="E30">
         <f>SUM(E3:E29)</f>
         <v>120</v>
@@ -5547,7 +5585,7 @@
       <c r="AO30" s="11"/>
       <c r="AP30" s="11"/>
     </row>
-    <row r="31" spans="2:42">
+    <row r="31" spans="2:42" x14ac:dyDescent="0.25">
       <c r="I31" s="51"/>
       <c r="J31" s="51"/>
       <c r="K31" s="51"/>
@@ -5601,14 +5639,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -5619,7 +5657,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -5630,7 +5668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -5639,7 +5677,7 @@
       </c>
       <c r="D4" s="58"/>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5650,7 +5688,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -5661,7 +5699,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -5672,7 +5710,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>430</v>
       </c>
@@ -5683,7 +5721,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>433</v>
       </c>
@@ -5694,7 +5732,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>436</v>
       </c>
@@ -5705,7 +5743,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>439</v>
       </c>
@@ -5716,7 +5754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>58</v>
       </c>
@@ -5727,7 +5765,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>59</v>
       </c>
@@ -5755,14 +5793,14 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="1" customFormat="1">
+    <row r="2" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -5773,7 +5811,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" s="1" customFormat="1">
+    <row r="3" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -5784,7 +5822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="1" customFormat="1">
+    <row r="4" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -5793,7 +5831,7 @@
       </c>
       <c r="D4" s="58"/>
     </row>
-    <row r="5" spans="2:4" s="1" customFormat="1">
+    <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5804,7 +5842,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="2:4" s="1" customFormat="1">
+    <row r="6" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -5815,7 +5853,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="1" customFormat="1">
+    <row r="7" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -5826,7 +5864,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="8" spans="2:4" s="1" customFormat="1">
+    <row r="8" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>352</v>
       </c>
@@ -5837,7 +5875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="1" customFormat="1">
+    <row r="9" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>348</v>
       </c>
@@ -5848,7 +5886,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="2:4" s="1" customFormat="1">
+    <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>349</v>
       </c>
@@ -5859,7 +5897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" s="1" customFormat="1">
+    <row r="11" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>58</v>
       </c>
@@ -5870,7 +5908,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:4" s="1" customFormat="1">
+    <row r="12" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>59</v>
       </c>
@@ -5898,7 +5936,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -5909,12 +5947,12 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="18.75">
+    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>145</v>
       </c>
@@ -5922,12 +5960,12 @@
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -5938,7 +5976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
@@ -5949,7 +5987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
@@ -5958,7 +5996,7 @@
       </c>
       <c r="D8" s="58"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -5969,7 +6007,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -5980,7 +6018,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
@@ -5991,7 +6029,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>132</v>
       </c>
@@ -6002,7 +6040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>133</v>
       </c>
@@ -6013,7 +6051,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>26</v>
       </c>
@@ -6024,7 +6062,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>27</v>
       </c>
@@ -6035,7 +6073,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>28</v>
       </c>
@@ -6046,7 +6084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>29</v>
       </c>
@@ -6057,7 +6095,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>135</v>
       </c>
@@ -6068,7 +6106,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>130</v>
       </c>
@@ -6079,7 +6117,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>136</v>
       </c>
@@ -6090,7 +6128,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>137</v>
       </c>
@@ -6101,7 +6139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>58</v>
       </c>
@@ -6112,7 +6150,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>59</v>
       </c>
@@ -6123,17 +6161,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" ht="18.75">
+    <row r="25" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
@@ -6144,7 +6182,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>19</v>
       </c>
@@ -6155,7 +6193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>20</v>
       </c>
@@ -6164,7 +6202,7 @@
       </c>
       <c r="D29" s="58"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
@@ -6175,7 +6213,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>22</v>
       </c>
@@ -6186,7 +6224,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>23</v>
       </c>
@@ -6197,7 +6235,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>132</v>
       </c>
@@ -6208,7 +6246,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>192</v>
       </c>
@@ -6219,7 +6257,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>193</v>
       </c>
@@ -6230,7 +6268,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>194</v>
       </c>
@@ -6241,7 +6279,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>195</v>
       </c>
@@ -6252,7 +6290,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>196</v>
       </c>
@@ -6263,7 +6301,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
         <v>51</v>
       </c>
@@ -6274,7 +6312,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
         <v>52</v>
       </c>
@@ -6285,7 +6323,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
         <v>53</v>
       </c>
@@ -6296,7 +6334,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="42" spans="2:4">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="3">
         <v>54</v>
       </c>
@@ -6307,7 +6345,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
         <v>55</v>
       </c>
@@ -6318,7 +6356,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>208</v>
       </c>
@@ -6329,7 +6367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
         <v>58</v>
       </c>
@@ -6340,7 +6378,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
         <v>59</v>
       </c>
@@ -6351,17 +6389,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
     </row>
-    <row r="49" spans="3:4">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>146</v>
       </c>
@@ -6369,17 +6407,17 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="3:4">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D50" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="51" spans="3:4">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D51" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="3:4">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D52" s="1" t="s">
         <v>150</v>
       </c>
@@ -6403,17 +6441,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="158.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:3" ht="60">
+    <row r="2" spans="3:3" ht="63" x14ac:dyDescent="0.25">
       <c r="C2" s="24" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="3:3">
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>143</v>
       </c>
@@ -6432,7 +6470,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
@@ -6442,7 +6480,7 @@
     <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="40" t="s">
         <v>227</v>
       </c>
@@ -6469,7 +6507,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="39" t="s">
         <v>235</v>
       </c>
@@ -6495,7 +6533,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>226</v>
       </c>
@@ -6521,7 +6559,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>336</v>
       </c>
@@ -6547,7 +6585,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>339</v>
       </c>
@@ -6573,7 +6611,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>224</v>
       </c>
@@ -6599,7 +6637,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>225</v>
       </c>
@@ -6625,7 +6663,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>287</v>
       </c>
@@ -6645,7 +6683,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>288</v>
       </c>
@@ -6665,7 +6703,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>286</v>
       </c>
@@ -6685,7 +6723,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>294</v>
       </c>
@@ -6705,7 +6743,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>265</v>
       </c>
@@ -6722,7 +6760,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>266</v>
       </c>
@@ -6742,7 +6780,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>236</v>
       </c>
@@ -6765,7 +6803,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>239</v>
       </c>
@@ -6788,7 +6826,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>243</v>
       </c>
@@ -6811,7 +6849,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>250</v>
       </c>
@@ -6834,7 +6872,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>328</v>
       </c>
@@ -6854,7 +6892,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>329</v>
       </c>
@@ -6874,7 +6912,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>330</v>
       </c>
@@ -6894,7 +6932,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>244</v>
       </c>
@@ -6917,7 +6955,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>245</v>
       </c>
@@ -6940,7 +6978,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>249</v>
       </c>
@@ -6963,7 +7001,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>253</v>
       </c>
@@ -6986,7 +7024,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>254</v>
       </c>
@@ -7009,7 +7047,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>255</v>
       </c>
@@ -7032,7 +7070,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>271</v>
       </c>
@@ -7052,7 +7090,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>272</v>
       </c>
@@ -7072,7 +7110,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>274</v>
       </c>
@@ -7092,7 +7130,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>283</v>
       </c>
@@ -7115,7 +7153,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>259</v>
       </c>
@@ -7138,7 +7176,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>276</v>
       </c>
@@ -7158,7 +7196,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>277</v>
       </c>
@@ -7178,7 +7216,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>281</v>
       </c>

</xml_diff>

<commit_message>
Update generic command to set angle (for Hailzd only)
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="536">
   <si>
     <t>Offset</t>
   </si>
@@ -1638,17 +1638,26 @@
   <si>
     <t>A9 9A 08 0A 00 01 01 01 01 01 17 ED</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set current angle</t>
+  </si>
+  <si>
+    <t>{id}{angle}{minor}</t>
+  </si>
+  <si>
+    <t>A9 9A 05 18 01 5A 00 78 ED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1656,7 +1665,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1666,7 +1675,7 @@
       <u/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1676,19 +1685,19 @@
       <u/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1747,7 +1756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1906,6 +1915,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2217,16 +2229,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N59"/>
+  <dimension ref="B2:N60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -2240,7 +2252,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2248,7 +2260,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -2259,7 +2271,7 @@
       <c r="G3" s="13"/>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -2271,7 +2283,7 @@
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -2283,7 +2295,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -2299,7 +2311,7 @@
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14">
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -2308,7 +2320,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14">
       <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
@@ -2317,7 +2329,7 @@
       </c>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14">
       <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
@@ -2326,7 +2338,7 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14">
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
@@ -2355,7 +2367,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14">
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
@@ -2384,7 +2396,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
@@ -2413,7 +2425,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14">
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
@@ -2442,7 +2454,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
@@ -2465,7 +2477,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13">
       <c r="B17" s="5" t="s">
         <v>132</v>
       </c>
@@ -2488,7 +2500,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13">
       <c r="B18" s="5" t="s">
         <v>192</v>
       </c>
@@ -2511,7 +2523,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="45">
       <c r="B19" s="5" t="s">
         <v>53</v>
       </c>
@@ -2540,7 +2552,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13">
       <c r="B20" s="5" t="s">
         <v>213</v>
       </c>
@@ -2567,7 +2579,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13">
       <c r="B21" s="5" t="s">
         <v>424</v>
       </c>
@@ -2592,7 +2604,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13">
       <c r="B22" s="5" t="s">
         <v>441</v>
       </c>
@@ -2617,7 +2629,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13">
       <c r="B23" s="5" t="s">
         <v>445</v>
       </c>
@@ -2645,7 +2657,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13">
       <c r="B24" s="5" t="s">
         <v>510</v>
       </c>
@@ -2677,7 +2689,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13">
       <c r="B25" s="5">
         <v>10</v>
       </c>
@@ -2704,7 +2716,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13">
       <c r="B26" s="5">
         <v>11</v>
       </c>
@@ -2731,7 +2743,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13">
       <c r="B27" s="5">
         <v>12</v>
       </c>
@@ -2758,7 +2770,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13">
       <c r="B28" s="5">
         <v>13</v>
       </c>
@@ -2785,7 +2797,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13">
       <c r="B29" s="3">
         <v>14</v>
       </c>
@@ -2812,7 +2824,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13">
       <c r="B30" s="3">
         <v>15</v>
       </c>
@@ -2833,7 +2845,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13">
       <c r="B31" s="3">
         <v>16</v>
       </c>
@@ -2854,39 +2866,37 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13">
       <c r="B32" s="3">
+        <v>18</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="58" t="s">
+        <v>534</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11">
+      <c r="B33" s="3">
         <v>21</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G32" s="4"/>
-      <c r="I32" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="3">
-        <v>22</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>68</v>
@@ -2895,7 +2905,7 @@
         <v>75</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G33" s="4"/>
       <c r="I33" s="4" t="s">
@@ -2908,21 +2918,21 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11">
       <c r="B34" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E34" s="23" t="s">
-        <v>201</v>
+      <c r="E34" s="18" t="s">
+        <v>75</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G34" s="4"/>
       <c r="I34" s="4" t="s">
@@ -2932,55 +2942,53 @@
         <v>94</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="30">
       <c r="B35" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="18" t="s">
-        <v>189</v>
+      <c r="E35" s="23" t="s">
+        <v>201</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="G35" s="4"/>
       <c r="I35" s="4" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11">
       <c r="B36" s="3">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>168</v>
+        <v>74</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E36" s="28" t="s">
-        <v>51</v>
+        <v>68</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>189</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>170</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="G36" s="4"/>
       <c r="I36" s="4" t="s">
         <v>109</v>
       </c>
@@ -2991,23 +2999,25 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11">
       <c r="B37" s="3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G37" s="12"/>
+        <v>169</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>170</v>
+      </c>
       <c r="I37" s="4" t="s">
         <v>109</v>
       </c>
@@ -3018,25 +3028,23 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11">
       <c r="B38" s="3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>185</v>
+        <v>45</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>217</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="G38" s="12"/>
       <c r="I38" s="4" t="s">
         <v>109</v>
       </c>
@@ -3047,23 +3055,25 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11">
       <c r="B39" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="G39" s="12"/>
+        <v>175</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>217</v>
+      </c>
       <c r="I39" s="4" t="s">
         <v>109</v>
       </c>
@@ -3074,12 +3084,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11">
       <c r="B40" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>57</v>
@@ -3088,7 +3098,7 @@
         <v>177</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G40" s="12"/>
       <c r="I40" s="4" t="s">
@@ -3101,25 +3111,23 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11">
       <c r="B41" s="3">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>218</v>
+        <v>177</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>183</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="G41" s="12"/>
       <c r="I41" s="4" t="s">
         <v>109</v>
       </c>
@@ -3127,26 +3135,28 @@
         <v>110</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11">
       <c r="B42" s="3">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E42" s="26" t="s">
-        <v>6</v>
+        <v>79</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>218</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="G42" s="4"/>
+        <v>182</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>183</v>
+      </c>
       <c r="I42" s="4" t="s">
         <v>109</v>
       </c>
@@ -3154,24 +3164,24 @@
         <v>110</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11">
       <c r="B43" s="3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>155</v>
+        <v>6</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G43" s="4"/>
       <c r="I43" s="4" t="s">
@@ -3184,21 +3194,21 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
-        <v>157</v>
+    <row r="44" spans="2:11">
+      <c r="B44" s="3">
+        <v>42</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>45</v>
+        <v>155</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>159</v>
+        <v>223</v>
       </c>
       <c r="G44" s="4"/>
       <c r="I44" s="4" t="s">
@@ -3211,244 +3221,244 @@
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="3">
-        <v>60</v>
+    <row r="45" spans="2:11">
+      <c r="B45" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>202</v>
+        <v>158</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E45" s="32" t="s">
+      <c r="E45" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>203</v>
+        <v>159</v>
       </c>
       <c r="G45" s="4"/>
       <c r="I45" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11">
       <c r="B46" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>103</v>
+        <v>202</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E46" s="18" t="s">
-        <v>80</v>
+        <v>56</v>
+      </c>
+      <c r="E46" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>78</v>
+        <v>203</v>
       </c>
       <c r="G46" s="4"/>
       <c r="I46" s="4" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>141</v>
+        <v>92</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11">
       <c r="B47" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D47" s="25" t="s">
-        <v>91</v>
+        <v>103</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>212</v>
+        <v>80</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>211</v>
+        <v>78</v>
       </c>
       <c r="G47" s="4"/>
       <c r="I47" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11">
+      <c r="B48" s="3">
+        <v>62</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G48" s="4"/>
+      <c r="I48" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="J48" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="K47" s="4" t="s">
+      <c r="K48" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="35">
+    <row r="49" spans="2:11" s="38" customFormat="1">
+      <c r="B49" s="35">
         <v>63</v>
       </c>
-      <c r="C48" s="36" t="s">
+      <c r="C49" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="D48" s="36" t="s">
+      <c r="D49" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E48" s="37" t="s">
+      <c r="E49" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="F48" s="36" t="s">
+      <c r="F49" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="G48" s="36"/>
-      <c r="I48" s="36" t="s">
+      <c r="G49" s="36"/>
+      <c r="I49" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="J48" s="36" t="s">
+      <c r="J49" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="K48" s="36" t="s">
+      <c r="K49" s="36" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="3">
+    <row r="50" spans="2:11">
+      <c r="B50" s="3">
         <v>68</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D50" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="E49" s="42" t="s">
+      <c r="E50" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="F50" s="4" t="s">
         <v>345</v>
-      </c>
-      <c r="G49" s="4"/>
-      <c r="I49" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="K49" s="4" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="3">
-        <v>69</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="D50" s="25"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="4" t="s">
-        <v>415</v>
       </c>
       <c r="G50" s="4"/>
       <c r="I50" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11">
+      <c r="B51" s="3">
+        <v>69</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="D51" s="25"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="G51" s="4"/>
+      <c r="I51" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="J50" s="4" t="s">
+      <c r="J51" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="K50" s="4" t="s">
+      <c r="K51" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="3">
+    <row r="52" spans="2:11">
+      <c r="B52" s="3">
         <v>71</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E51" s="18" t="s">
+      <c r="E52" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="F52" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="G51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="3">
-        <v>72</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E52" s="18"/>
-      <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11">
       <c r="B53" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E53" s="18" t="s">
+      <c r="E53" s="18"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+    </row>
+    <row r="54" spans="2:11" ht="30">
+      <c r="B54" s="3">
+        <v>74</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E54" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F54" s="17" t="s">
         <v>142</v>
-      </c>
-      <c r="G53" s="4"/>
-      <c r="I53" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="3">
-        <v>75</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E54" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>220</v>
       </c>
       <c r="G54" s="4"/>
       <c r="I54" s="4" t="s">
@@ -3458,66 +3468,66 @@
         <v>110</v>
       </c>
       <c r="K54" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11">
+      <c r="B55" s="3">
+        <v>75</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E55" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G55" s="4"/>
+      <c r="I55" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K55" s="4" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B55" s="3"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-    </row>
-    <row r="56" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="35" t="s">
+    <row r="56" spans="2:11">
+      <c r="B56" s="3"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+    </row>
+    <row r="57" spans="2:11" s="38" customFormat="1">
+      <c r="B57" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C56" s="36" t="s">
+      <c r="C57" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="D56" s="36" t="s">
+      <c r="D57" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="E56" s="37" t="s">
+      <c r="E57" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="F56" s="36" t="s">
+      <c r="F57" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="G56" s="36" t="s">
+      <c r="G57" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="I56" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="J56" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="K56" s="36" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="57" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="C57" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D57" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E57" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="F57" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="G57" s="36"/>
       <c r="I57" s="36" t="s">
         <v>109</v>
       </c>
@@ -3528,20 +3538,47 @@
         <v>111</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="2" t="s">
+    <row r="58" spans="2:11" s="38" customFormat="1">
+      <c r="B58" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D58" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E58" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="F58" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="G58" s="36"/>
+      <c r="I58" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="J58" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="K58" s="36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11">
+      <c r="B60" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="E59" s="20" t="s">
+      <c r="E60" s="20" t="s">
         <v>530</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>531</v>
       </c>
     </row>
@@ -3560,7 +3597,7 @@
       <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -3568,7 +3605,7 @@
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3582,29 +3619,29 @@
         <v>391</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="59" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="45"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="58"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="45"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -3616,7 +3653,7 @@
       </c>
       <c r="E5" s="45"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -3628,7 +3665,7 @@
       </c>
       <c r="E6" s="45"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -3642,7 +3679,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
         <v>132</v>
       </c>
@@ -3656,7 +3693,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
         <v>192</v>
       </c>
@@ -3670,7 +3707,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
         <v>409</v>
       </c>
@@ -3684,7 +3721,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5">
       <c r="B11" s="3" t="s">
         <v>357</v>
       </c>
@@ -3698,7 +3735,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5">
       <c r="B12" s="3" t="s">
         <v>360</v>
       </c>
@@ -3712,7 +3749,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5">
       <c r="B13" s="3" t="s">
         <v>362</v>
       </c>
@@ -3726,7 +3763,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5">
       <c r="B14" s="3" t="s">
         <v>366</v>
       </c>
@@ -3740,7 +3777,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5">
       <c r="B15" s="3">
         <v>18</v>
       </c>
@@ -3754,7 +3791,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5">
       <c r="B16" s="3">
         <v>21</v>
       </c>
@@ -3768,7 +3805,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <v>22</v>
       </c>
@@ -3782,7 +3819,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <v>23</v>
       </c>
@@ -3796,7 +3833,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <v>24</v>
       </c>
@@ -3810,7 +3847,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <v>31</v>
       </c>
@@ -3824,7 +3861,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <v>32</v>
       </c>
@@ -3838,7 +3875,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <v>33</v>
       </c>
@@ -3852,7 +3889,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <v>41</v>
       </c>
@@ -3866,7 +3903,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <v>42</v>
       </c>
@@ -3880,7 +3917,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <v>43</v>
       </c>
@@ -3894,7 +3931,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <v>58</v>
       </c>
@@ -3906,7 +3943,7 @@
       </c>
       <c r="E26" s="45"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5">
       <c r="B27" s="3">
         <v>59</v>
       </c>
@@ -3935,7 +3972,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -3951,7 +3988,7 @@
     <col min="18" max="48" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:42">
       <c r="I1" s="52" t="s">
         <v>450</v>
       </c>
@@ -3965,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:42">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -4024,14 +4061,14 @@
       <c r="AO2" s="11"/>
       <c r="AP2" s="11"/>
     </row>
-    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:42">
       <c r="B3" s="55">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="59" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="48">
@@ -4081,14 +4118,14 @@
       <c r="AO3" s="11"/>
       <c r="AP3" s="11"/>
     </row>
-    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:42">
       <c r="B4" s="56">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="58"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="48">
         <v>1</v>
       </c>
@@ -4136,7 +4173,7 @@
       <c r="AO4" s="11"/>
       <c r="AP4" s="11"/>
     </row>
-    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:42">
       <c r="B5" s="56">
         <v>2</v>
       </c>
@@ -4193,7 +4230,7 @@
       <c r="AO5" s="11"/>
       <c r="AP5" s="11"/>
     </row>
-    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:42">
       <c r="B6" s="56">
         <v>3</v>
       </c>
@@ -4250,7 +4287,7 @@
       <c r="AO6" s="11"/>
       <c r="AP6" s="11"/>
     </row>
-    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:42">
       <c r="B7" s="56">
         <v>4</v>
       </c>
@@ -4307,7 +4344,7 @@
       <c r="AO7" s="11"/>
       <c r="AP7" s="11"/>
     </row>
-    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:42">
       <c r="B8" s="56">
         <v>5</v>
       </c>
@@ -4364,7 +4401,7 @@
       <c r="AO8" s="11"/>
       <c r="AP8" s="11"/>
     </row>
-    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:42">
       <c r="B9" s="56">
         <v>6</v>
       </c>
@@ -4421,7 +4458,7 @@
       <c r="AO9" s="11"/>
       <c r="AP9" s="11"/>
     </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:42">
       <c r="B10" s="56">
         <v>8</v>
       </c>
@@ -4478,7 +4515,7 @@
       <c r="AO10" s="11"/>
       <c r="AP10" s="11"/>
     </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:42">
       <c r="B11" s="56">
         <v>9</v>
       </c>
@@ -4535,7 +4572,7 @@
       <c r="AO11" s="11"/>
       <c r="AP11" s="11"/>
     </row>
-    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:42">
       <c r="B12" s="56">
         <v>10</v>
       </c>
@@ -4592,7 +4629,7 @@
       <c r="AO12" s="11"/>
       <c r="AP12" s="11"/>
     </row>
-    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:42">
       <c r="B13" s="56">
         <v>40</v>
       </c>
@@ -4649,7 +4686,7 @@
       <c r="AO13" s="11"/>
       <c r="AP13" s="11"/>
     </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:42">
       <c r="B14" s="56">
         <v>60</v>
       </c>
@@ -4706,7 +4743,7 @@
       <c r="AO14" s="11"/>
       <c r="AP14" s="11"/>
     </row>
-    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:42">
       <c r="B15" s="56">
         <v>61</v>
       </c>
@@ -4763,7 +4800,7 @@
       <c r="AO15" s="11"/>
       <c r="AP15" s="11"/>
     </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:42">
       <c r="B16" s="56">
         <v>62</v>
       </c>
@@ -4820,7 +4857,7 @@
       <c r="AO16" s="11"/>
       <c r="AP16" s="11"/>
     </row>
-    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:42">
       <c r="B17" s="56">
         <v>63</v>
       </c>
@@ -4877,7 +4914,7 @@
       <c r="AO17" s="11"/>
       <c r="AP17" s="11"/>
     </row>
-    <row r="18" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:42">
       <c r="B18" s="56">
         <v>64</v>
       </c>
@@ -4934,7 +4971,7 @@
       <c r="AO18" s="11"/>
       <c r="AP18" s="11"/>
     </row>
-    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:42">
       <c r="B19" s="56">
         <v>84</v>
       </c>
@@ -4991,7 +5028,7 @@
       <c r="AO19" s="11"/>
       <c r="AP19" s="11"/>
     </row>
-    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:42">
       <c r="B20" s="56">
         <v>104</v>
       </c>
@@ -5048,7 +5085,7 @@
       <c r="AO20" s="11"/>
       <c r="AP20" s="11"/>
     </row>
-    <row r="21" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:42">
       <c r="B21" s="56">
         <v>105</v>
       </c>
@@ -5105,7 +5142,7 @@
       <c r="AO21" s="11"/>
       <c r="AP21" s="11"/>
     </row>
-    <row r="22" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:42">
       <c r="B22" s="56">
         <v>106</v>
       </c>
@@ -5162,7 +5199,7 @@
       <c r="AO22" s="11"/>
       <c r="AP22" s="11"/>
     </row>
-    <row r="23" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:42">
       <c r="B23" s="56">
         <v>108</v>
       </c>
@@ -5219,7 +5256,7 @@
       <c r="AO23" s="11"/>
       <c r="AP23" s="11"/>
     </row>
-    <row r="24" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:42">
       <c r="B24" s="56">
         <v>109</v>
       </c>
@@ -5276,7 +5313,7 @@
       <c r="AO24" s="11"/>
       <c r="AP24" s="11"/>
     </row>
-    <row r="25" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:42">
       <c r="B25" s="56">
         <v>110</v>
       </c>
@@ -5333,7 +5370,7 @@
       <c r="AO25" s="11"/>
       <c r="AP25" s="11"/>
     </row>
-    <row r="26" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:42">
       <c r="B26" s="56">
         <v>112</v>
       </c>
@@ -5390,7 +5427,7 @@
       <c r="AO26" s="11"/>
       <c r="AP26" s="11"/>
     </row>
-    <row r="27" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:42">
       <c r="B27" s="56">
         <v>114</v>
       </c>
@@ -5447,7 +5484,7 @@
       <c r="AO27" s="11"/>
       <c r="AP27" s="11"/>
     </row>
-    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:42">
       <c r="B28" s="56">
         <v>118</v>
       </c>
@@ -5496,7 +5533,7 @@
       <c r="AO28" s="11"/>
       <c r="AP28" s="11"/>
     </row>
-    <row r="29" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:42">
       <c r="B29" s="56">
         <v>119</v>
       </c>
@@ -5545,7 +5582,7 @@
       <c r="AO29" s="11"/>
       <c r="AP29" s="11"/>
     </row>
-    <row r="30" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:42">
       <c r="E30">
         <f>SUM(E3:E29)</f>
         <v>120</v>
@@ -5585,7 +5622,7 @@
       <c r="AO30" s="11"/>
       <c r="AP30" s="11"/>
     </row>
-    <row r="31" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:42">
       <c r="I31" s="51"/>
       <c r="J31" s="51"/>
       <c r="K31" s="51"/>
@@ -5639,14 +5676,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -5657,27 +5694,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="59" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="58"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="59"/>
+    </row>
+    <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5688,7 +5725,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -5699,7 +5736,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -5710,7 +5747,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" s="5" t="s">
         <v>430</v>
       </c>
@@ -5721,7 +5758,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4">
       <c r="B9" s="5" t="s">
         <v>433</v>
       </c>
@@ -5732,7 +5769,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4">
       <c r="B10" s="5" t="s">
         <v>436</v>
       </c>
@@ -5743,7 +5780,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="B11" s="3" t="s">
         <v>439</v>
       </c>
@@ -5754,7 +5791,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4">
       <c r="B12" s="3">
         <v>58</v>
       </c>
@@ -5765,7 +5802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="B13" s="3">
         <v>59</v>
       </c>
@@ -5793,14 +5830,14 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" s="1" customFormat="1">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -5811,27 +5848,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" s="1" customFormat="1">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="59" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" s="1" customFormat="1">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="58"/>
-    </row>
-    <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="59"/>
+    </row>
+    <row r="5" spans="2:4" s="1" customFormat="1">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5842,7 +5879,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" s="1" customFormat="1">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -5853,7 +5890,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" s="1" customFormat="1">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -5864,7 +5901,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="8" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" s="1" customFormat="1">
       <c r="B8" s="5" t="s">
         <v>352</v>
       </c>
@@ -5875,7 +5912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" s="1" customFormat="1">
       <c r="B9" s="3" t="s">
         <v>348</v>
       </c>
@@ -5886,7 +5923,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" s="1" customFormat="1">
       <c r="B10" s="3" t="s">
         <v>349</v>
       </c>
@@ -5897,7 +5934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" s="1" customFormat="1">
       <c r="B11" s="3">
         <v>58</v>
       </c>
@@ -5908,7 +5945,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" s="1" customFormat="1">
       <c r="B12" s="3">
         <v>59</v>
       </c>
@@ -5936,7 +5973,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -5947,12 +5984,12 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18.75">
       <c r="A2" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="27" t="s">
         <v>145</v>
       </c>
@@ -5960,12 +5997,12 @@
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -5976,27 +6013,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="59" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="58"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="59"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -6007,7 +6044,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -6018,7 +6055,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
@@ -6029,7 +6066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12" s="5" t="s">
         <v>132</v>
       </c>
@@ -6040,7 +6077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13" s="3" t="s">
         <v>133</v>
       </c>
@@ -6051,7 +6088,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14" s="3">
         <v>26</v>
       </c>
@@ -6062,7 +6099,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="B15" s="3">
         <v>27</v>
       </c>
@@ -6073,7 +6110,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="3">
         <v>28</v>
       </c>
@@ -6084,7 +6121,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="B17" s="3">
         <v>29</v>
       </c>
@@ -6095,7 +6132,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="B18" s="3" t="s">
         <v>135</v>
       </c>
@@ -6106,7 +6143,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="B19" s="3" t="s">
         <v>130</v>
       </c>
@@ -6117,7 +6154,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="B20" s="3" t="s">
         <v>136</v>
       </c>
@@ -6128,7 +6165,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="B21" s="3" t="s">
         <v>137</v>
       </c>
@@ -6139,7 +6176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="B22" s="3">
         <v>58</v>
       </c>
@@ -6150,7 +6187,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="B23" s="3">
         <v>59</v>
       </c>
@@ -6161,17 +6198,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="18.75">
       <c r="A25" s="8" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
@@ -6182,27 +6219,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="B28" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="58" t="s">
+      <c r="D28" s="59" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="B29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="58"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="59"/>
+    </row>
+    <row r="30" spans="1:4">
       <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
@@ -6213,7 +6250,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="B31" s="5" t="s">
         <v>22</v>
       </c>
@@ -6224,7 +6261,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="B32" s="5" t="s">
         <v>23</v>
       </c>
@@ -6235,7 +6272,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4">
       <c r="B33" s="5" t="s">
         <v>132</v>
       </c>
@@ -6246,7 +6283,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4">
       <c r="B34" s="5" t="s">
         <v>192</v>
       </c>
@@ -6257,7 +6294,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4">
       <c r="B35" s="5" t="s">
         <v>193</v>
       </c>
@@ -6268,7 +6305,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4">
       <c r="B36" s="3" t="s">
         <v>194</v>
       </c>
@@ -6279,7 +6316,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4">
       <c r="B37" s="3" t="s">
         <v>195</v>
       </c>
@@ -6290,7 +6327,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4">
       <c r="B38" s="3" t="s">
         <v>196</v>
       </c>
@@ -6301,7 +6338,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4">
       <c r="B39" s="3">
         <v>51</v>
       </c>
@@ -6312,7 +6349,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4">
       <c r="B40" s="3">
         <v>52</v>
       </c>
@@ -6323,7 +6360,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4">
       <c r="B41" s="3">
         <v>53</v>
       </c>
@@ -6334,7 +6371,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4">
       <c r="B42" s="3">
         <v>54</v>
       </c>
@@ -6345,7 +6382,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4">
       <c r="B43" s="3">
         <v>55</v>
       </c>
@@ -6356,7 +6393,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4">
       <c r="B44" s="3" t="s">
         <v>208</v>
       </c>
@@ -6367,7 +6404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4">
       <c r="B45" s="3">
         <v>58</v>
       </c>
@@ -6378,7 +6415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4">
       <c r="B46" s="3">
         <v>59</v>
       </c>
@@ -6389,17 +6426,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4">
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4">
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4">
       <c r="C49" s="1" t="s">
         <v>146</v>
       </c>
@@ -6407,17 +6444,17 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4">
       <c r="D50" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4">
       <c r="D51" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4">
       <c r="D52" s="1" t="s">
         <v>150</v>
       </c>
@@ -6441,17 +6478,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="158.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:3" ht="60">
       <c r="C2" s="24" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:3">
       <c r="C5" t="s">
         <v>143</v>
       </c>
@@ -6470,7 +6507,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
@@ -6480,7 +6517,7 @@
     <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10">
       <c r="B3" s="40" t="s">
         <v>227</v>
       </c>
@@ -6507,7 +6544,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="B4" s="39" t="s">
         <v>235</v>
       </c>
@@ -6533,7 +6570,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="B5" t="s">
         <v>226</v>
       </c>
@@ -6559,7 +6596,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="B6" t="s">
         <v>336</v>
       </c>
@@ -6585,7 +6622,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10">
       <c r="B7" t="s">
         <v>339</v>
       </c>
@@ -6611,7 +6648,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="B8" t="s">
         <v>224</v>
       </c>
@@ -6637,7 +6674,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="B9" t="s">
         <v>225</v>
       </c>
@@ -6663,7 +6700,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="B10" t="s">
         <v>287</v>
       </c>
@@ -6683,7 +6720,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="B11" t="s">
         <v>288</v>
       </c>
@@ -6703,7 +6740,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10">
       <c r="B12" t="s">
         <v>286</v>
       </c>
@@ -6723,7 +6760,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10">
       <c r="B13" t="s">
         <v>294</v>
       </c>
@@ -6743,7 +6780,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10">
       <c r="B15" t="s">
         <v>265</v>
       </c>
@@ -6760,7 +6797,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10">
       <c r="B16" t="s">
         <v>266</v>
       </c>
@@ -6780,7 +6817,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9">
       <c r="B18" t="s">
         <v>236</v>
       </c>
@@ -6803,7 +6840,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9">
       <c r="B20" t="s">
         <v>239</v>
       </c>
@@ -6826,7 +6863,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9">
       <c r="B21" t="s">
         <v>243</v>
       </c>
@@ -6849,7 +6886,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9">
       <c r="B22" t="s">
         <v>250</v>
       </c>
@@ -6872,7 +6909,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9">
       <c r="B23" t="s">
         <v>328</v>
       </c>
@@ -6892,7 +6929,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9">
       <c r="B24" t="s">
         <v>329</v>
       </c>
@@ -6912,7 +6949,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9">
       <c r="B25" t="s">
         <v>330</v>
       </c>
@@ -6932,7 +6969,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9">
       <c r="B27" t="s">
         <v>244</v>
       </c>
@@ -6955,7 +6992,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9">
       <c r="B28" t="s">
         <v>245</v>
       </c>
@@ -6978,7 +7015,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9">
       <c r="B29" t="s">
         <v>249</v>
       </c>
@@ -7001,7 +7038,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9">
       <c r="B30" t="s">
         <v>253</v>
       </c>
@@ -7024,7 +7061,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9">
       <c r="B31" t="s">
         <v>254</v>
       </c>
@@ -7047,7 +7084,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9">
       <c r="B32" t="s">
         <v>255</v>
       </c>
@@ -7070,7 +7107,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9">
       <c r="B33" t="s">
         <v>271</v>
       </c>
@@ -7090,7 +7127,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9">
       <c r="B34" t="s">
         <v>272</v>
       </c>
@@ -7110,7 +7147,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9">
       <c r="B35" t="s">
         <v>274</v>
       </c>
@@ -7130,7 +7167,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" t="s">
         <v>283</v>
       </c>
@@ -7153,7 +7190,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9">
       <c r="B38" t="s">
         <v>259</v>
       </c>
@@ -7176,7 +7213,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9">
       <c r="B39" t="s">
         <v>276</v>
       </c>
@@ -7196,7 +7233,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9">
       <c r="B40" t="s">
         <v>277</v>
       </c>
@@ -7216,7 +7253,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9">
       <c r="B41" t="s">
         <v>281</v>
       </c>

</xml_diff>

<commit_message>
2.1.1 [Fix 2] - The time passing to generic robot library should be in ms, but in old version, UBT action time has been converted to the count of 20ms. Which cause the action running 20 times faster than expected.
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -2189,14 +2189,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2503,11 +2503,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H26" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="H14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H55" sqref="H55"/>
+      <selection pane="bottomRight" activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3883,8 +3883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3907,21 +3907,21 @@
       <c r="F1" s="50" t="s">
         <v>616</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="G1" s="61" t="s">
         <v>615</v>
       </c>
-      <c r="H1" s="62" t="s">
+      <c r="H1" s="61" t="s">
         <v>620</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="61" t="s">
         <v>621</v>
       </c>
-      <c r="K1" s="63" t="s">
+      <c r="K1" s="62" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="2" spans="2:11">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="60" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -3950,7 +3950,7 @@
       <c r="K2" s="10"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="60" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -3979,7 +3979,7 @@
       <c r="K3" s="10"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="60" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -4008,7 +4008,7 @@
       <c r="K4" s="10"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="60" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -4020,7 +4020,7 @@
       <c r="E5" s="50" t="s">
         <v>536</v>
       </c>
-      <c r="F5" s="62">
+      <c r="F5" s="61">
         <v>60</v>
       </c>
       <c r="G5" s="50">
@@ -4037,7 +4037,7 @@
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="60" t="s">
         <v>130</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -4049,7 +4049,7 @@
       <c r="E6" s="50" t="s">
         <v>537</v>
       </c>
-      <c r="F6" s="62">
+      <c r="F6" s="61">
         <v>7</v>
       </c>
       <c r="G6" s="50">
@@ -4066,7 +4066,7 @@
       <c r="K6" s="10"/>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="60" t="s">
         <v>190</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -4078,7 +4078,7 @@
       <c r="E7" s="50" t="s">
         <v>538</v>
       </c>
-      <c r="F7" s="62">
+      <c r="F7" s="61">
         <v>7</v>
       </c>
       <c r="G7" s="50">
@@ -4095,7 +4095,7 @@
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="60" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -4107,7 +4107,7 @@
       <c r="E8" s="50" t="s">
         <v>539</v>
       </c>
-      <c r="F8" s="62">
+      <c r="F8" s="61">
         <v>11</v>
       </c>
       <c r="G8" s="50">
@@ -4124,7 +4124,7 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="60" t="s">
         <v>211</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -4136,7 +4136,7 @@
       <c r="E9" s="50" t="s">
         <v>540</v>
       </c>
-      <c r="F9" s="62">
+      <c r="F9" s="61">
         <v>9</v>
       </c>
       <c r="G9" s="50">
@@ -4153,7 +4153,7 @@
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="2:11">
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="60" t="s">
         <v>422</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -4165,7 +4165,7 @@
       <c r="E10" s="50" t="s">
         <v>425</v>
       </c>
-      <c r="F10" s="62">
+      <c r="F10" s="61">
         <v>60</v>
       </c>
       <c r="G10" s="50">
@@ -4182,7 +4182,7 @@
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="2:11">
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="60" t="s">
         <v>439</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -4194,7 +4194,7 @@
       <c r="E11" s="50" t="s">
         <v>541</v>
       </c>
-      <c r="F11" s="62">
+      <c r="F11" s="61">
         <v>120</v>
       </c>
       <c r="G11" s="50">
@@ -4211,7 +4211,7 @@
       <c r="K11" s="10"/>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="60" t="s">
         <v>443</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -4223,7 +4223,7 @@
       <c r="E12" s="50" t="s">
         <v>542</v>
       </c>
-      <c r="F12" s="62">
+      <c r="F12" s="61">
         <v>7</v>
       </c>
       <c r="G12" s="50">
@@ -4240,7 +4240,7 @@
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="2:11">
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="60" t="s">
         <v>508</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -4252,7 +4252,7 @@
       <c r="E13" s="50" t="s">
         <v>543</v>
       </c>
-      <c r="F13" s="62">
+      <c r="F13" s="61">
         <v>7</v>
       </c>
       <c r="G13" s="50">
@@ -4269,7 +4269,7 @@
       <c r="K13" s="10"/>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="61">
+      <c r="B14" s="60">
         <v>10</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -4281,7 +4281,7 @@
       <c r="E14" s="50" t="s">
         <v>544</v>
       </c>
-      <c r="F14" s="62">
+      <c r="F14" s="61">
         <v>7</v>
       </c>
       <c r="G14" s="50">
@@ -4298,7 +4298,7 @@
       <c r="K14" s="10"/>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="61">
+      <c r="B15" s="60">
         <v>11</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -4310,7 +4310,7 @@
       <c r="E15" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="F15" s="62">
+      <c r="F15" s="61">
         <v>38</v>
       </c>
       <c r="G15" s="50">
@@ -4327,7 +4327,7 @@
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="61">
+      <c r="B16" s="60">
         <v>12</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -4339,7 +4339,7 @@
       <c r="E16" s="50" t="s">
         <v>546</v>
       </c>
-      <c r="F16" s="62">
+      <c r="F16" s="61">
         <v>9</v>
       </c>
       <c r="G16" s="50">
@@ -4356,7 +4356,7 @@
       <c r="K16" s="10"/>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="61">
+      <c r="B17" s="60">
         <v>13</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -4368,7 +4368,7 @@
       <c r="E17" s="50" t="s">
         <v>547</v>
       </c>
-      <c r="F17" s="62">
+      <c r="F17" s="61">
         <v>38</v>
       </c>
       <c r="G17" s="50">
@@ -4397,7 +4397,7 @@
       <c r="E18" s="50" t="s">
         <v>548</v>
       </c>
-      <c r="F18" s="62">
+      <c r="F18" s="61">
         <v>9</v>
       </c>
       <c r="G18" s="50">
@@ -4426,7 +4426,7 @@
       <c r="E19" s="50" t="s">
         <v>549</v>
       </c>
-      <c r="F19" s="62">
+      <c r="F19" s="61">
         <v>0</v>
       </c>
       <c r="G19" s="50">
@@ -4455,7 +4455,7 @@
       <c r="E20" s="50" t="s">
         <v>550</v>
       </c>
-      <c r="F20" s="62">
+      <c r="F20" s="61">
         <v>0</v>
       </c>
       <c r="G20" s="50">
@@ -4484,7 +4484,7 @@
       <c r="E21" s="50" t="s">
         <v>551</v>
       </c>
-      <c r="F21" s="62">
+      <c r="F21" s="61">
         <v>0</v>
       </c>
       <c r="G21" s="50">
@@ -4513,8 +4513,8 @@
       <c r="E22" s="50" t="s">
         <v>552</v>
       </c>
-      <c r="F22" s="62">
-        <v>0</v>
+      <c r="F22" s="61">
+        <v>9</v>
       </c>
       <c r="G22" s="50">
         <v>0</v>
@@ -4525,7 +4525,7 @@
       <c r="I22" s="10"/>
       <c r="J22" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>public static CMD_INFO LOCKSERVO = new CMD_INFO(0x21,0,0,0);</v>
+        <v>public static CMD_INFO LOCKSERVO = new CMD_INFO(0x21,9,0,0);</v>
       </c>
       <c r="K22" s="10"/>
     </row>
@@ -4542,8 +4542,8 @@
       <c r="E23" s="50" t="s">
         <v>553</v>
       </c>
-      <c r="F23" s="62">
-        <v>0</v>
+      <c r="F23" s="61">
+        <v>9</v>
       </c>
       <c r="G23" s="50">
         <v>0</v>
@@ -4554,7 +4554,7 @@
       <c r="I23" s="10"/>
       <c r="J23" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>public static CMD_INFO UNLOCKSERVO = new CMD_INFO(0x22,0,0,0);</v>
+        <v>public static CMD_INFO UNLOCKSERVO = new CMD_INFO(0x22,9,0,0);</v>
       </c>
       <c r="K23" s="10"/>
     </row>
@@ -4571,8 +4571,8 @@
       <c r="E24" s="50" t="s">
         <v>554</v>
       </c>
-      <c r="F24" s="62">
-        <v>0</v>
+      <c r="F24" s="61">
+        <v>10</v>
       </c>
       <c r="G24" s="50">
         <v>0</v>
@@ -4583,7 +4583,7 @@
       <c r="I24" s="10"/>
       <c r="J24" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>public static CMD_INFO SERVOMOVE = new CMD_INFO(0x23,0,0,0);</v>
+        <v>public static CMD_INFO SERVOMOVE = new CMD_INFO(0x23,10,0,0);</v>
       </c>
       <c r="K24" s="10"/>
     </row>
@@ -4600,7 +4600,7 @@
       <c r="E25" s="50" t="s">
         <v>555</v>
       </c>
-      <c r="F25" s="62">
+      <c r="F25" s="61">
         <v>7</v>
       </c>
       <c r="G25" s="50">
@@ -4629,7 +4629,7 @@
       <c r="E26" s="50" t="s">
         <v>556</v>
       </c>
-      <c r="F26" s="62">
+      <c r="F26" s="61">
         <v>7</v>
       </c>
       <c r="G26" s="50">
@@ -4658,7 +4658,7 @@
       <c r="E27" s="50" t="s">
         <v>557</v>
       </c>
-      <c r="F27" s="62">
+      <c r="F27" s="61">
         <v>7</v>
       </c>
       <c r="G27" s="50">
@@ -4687,7 +4687,7 @@
       <c r="E28" s="50" t="s">
         <v>558</v>
       </c>
-      <c r="F28" s="62">
+      <c r="F28" s="61">
         <v>7</v>
       </c>
       <c r="G28" s="50">
@@ -4716,7 +4716,7 @@
       <c r="E29" s="50" t="s">
         <v>559</v>
       </c>
-      <c r="F29" s="62">
+      <c r="F29" s="61">
         <v>7</v>
       </c>
       <c r="G29" s="50">
@@ -4745,7 +4745,7 @@
       <c r="E30" s="50" t="s">
         <v>560</v>
       </c>
-      <c r="F30" s="62">
+      <c r="F30" s="61">
         <v>7</v>
       </c>
       <c r="G30" s="50">
@@ -4774,7 +4774,7 @@
       <c r="E31" s="50" t="s">
         <v>561</v>
       </c>
-      <c r="F31" s="62">
+      <c r="F31" s="61">
         <v>7</v>
       </c>
       <c r="G31" s="50">
@@ -4803,7 +4803,7 @@
       <c r="E32" s="50" t="s">
         <v>562</v>
       </c>
-      <c r="F32" s="62">
+      <c r="F32" s="61">
         <v>7</v>
       </c>
       <c r="G32" s="50">
@@ -4832,7 +4832,7 @@
       <c r="E33" s="50" t="s">
         <v>563</v>
       </c>
-      <c r="F33" s="62">
+      <c r="F33" s="61">
         <v>7</v>
       </c>
       <c r="G33" s="50">
@@ -4861,7 +4861,7 @@
       <c r="E34" s="50" t="s">
         <v>564</v>
       </c>
-      <c r="F34" s="62">
+      <c r="F34" s="61">
         <v>7</v>
       </c>
       <c r="G34" s="50">
@@ -4890,7 +4890,7 @@
       <c r="E35" s="50" t="s">
         <v>565</v>
       </c>
-      <c r="F35" s="62">
+      <c r="F35" s="61">
         <v>738</v>
       </c>
       <c r="G35" s="50">
@@ -4919,7 +4919,7 @@
       <c r="E36" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="F36" s="62">
+      <c r="F36" s="61">
         <v>60</v>
       </c>
       <c r="G36" s="50">
@@ -4948,7 +4948,7 @@
       <c r="E37" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="F37" s="62">
+      <c r="F37" s="61">
         <v>60</v>
       </c>
       <c r="G37" s="50">
@@ -4977,7 +4977,7 @@
       <c r="E38" s="50" t="s">
         <v>344</v>
       </c>
-      <c r="F38" s="62">
+      <c r="F38" s="61">
         <v>60</v>
       </c>
       <c r="G38" s="50">
@@ -5006,7 +5006,7 @@
       <c r="E39" s="50" t="s">
         <v>566</v>
       </c>
-      <c r="F39" s="62">
+      <c r="F39" s="61">
         <v>7</v>
       </c>
       <c r="G39" s="50">
@@ -5035,7 +5035,7 @@
       <c r="E40" s="50" t="s">
         <v>567</v>
       </c>
-      <c r="F40" s="62">
+      <c r="F40" s="61">
         <v>7</v>
       </c>
       <c r="G40" s="50">
@@ -5064,7 +5064,7 @@
       <c r="E41" s="50" t="s">
         <v>568</v>
       </c>
-      <c r="F41" s="62">
+      <c r="F41" s="61">
         <v>7</v>
       </c>
       <c r="G41" s="50">
@@ -5093,7 +5093,7 @@
       <c r="E42" s="50" t="s">
         <v>446</v>
       </c>
-      <c r="F42" s="62">
+      <c r="F42" s="61">
         <v>7</v>
       </c>
       <c r="G42" s="50">
@@ -5122,7 +5122,7 @@
       <c r="E43" s="50" t="s">
         <v>569</v>
       </c>
-      <c r="F43" s="62">
+      <c r="F43" s="61">
         <v>7</v>
       </c>
       <c r="G43" s="50">
@@ -5151,7 +5151,7 @@
       <c r="E44" s="50" t="s">
         <v>570</v>
       </c>
-      <c r="F44" s="62">
+      <c r="F44" s="61">
         <v>10</v>
       </c>
       <c r="G44" s="50">
@@ -5210,7 +5210,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="63" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="45"/>
@@ -5222,7 +5222,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="45"/>
     </row>
     <row r="5" spans="2:5">
@@ -5652,7 +5652,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="63" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="48">
@@ -5709,7 +5709,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="48">
         <v>1</v>
       </c>
@@ -7285,7 +7285,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="63" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7296,7 +7296,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="63"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
@@ -7439,7 +7439,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="63" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7450,7 +7450,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="63"/>
     </row>
     <row r="5" spans="2:4" s="1" customFormat="1">
       <c r="B5" s="5" t="s">
@@ -7604,7 +7604,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="63" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7615,7 +7615,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="60"/>
+      <c r="D8" s="63"/>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="5" t="s">
@@ -7810,7 +7810,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="63" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7821,7 +7821,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="60"/>
+      <c r="D29" s="63"/>
     </row>
     <row r="30" spans="1:4">
       <c r="B30" s="5" t="s">

</xml_diff>

<commit_message>
v2.1.2 - Add MPU function - check mpu and get mpu data - Fix on SimpleWiiManager - Change router enable flag before using router - Update some command setting in info.xlsx
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="636">
   <si>
     <t>Offset</t>
   </si>
@@ -1905,7 +1905,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1926,7 +1926,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1937,7 +1937,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1954,7 +1954,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1965,7 +1965,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1981,7 +1981,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1998,7 +1998,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -2011,16 +2011,68 @@
     <t>Yes {*}</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>Check MPU Exists</t>
+  </si>
+  <si>
+    <t>Yes {0}</t>
+  </si>
+  <si>
+    <t>A9 9A 02 81 83 ED</t>
+  </si>
+  <si>
+    <t>A9 9A 02 82 84 ED</t>
+  </si>
+  <si>
+    <t>Get MPU Data</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{ax}{ay}{az}{?}{gx}{gy}{gz} - all in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H/L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> format</t>
+    </r>
+  </si>
+  <si>
+    <t>Yes {14}</t>
+  </si>
+  <si>
+    <t>Yes {20}</t>
+  </si>
+  <si>
+    <t>No {7 + 2*n}</t>
+  </si>
+  <si>
+    <t>No {7 + 4*n}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2028,7 +2080,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2038,7 +2090,7 @@
       <u/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2048,19 +2100,19 @@
       <u/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2068,9 +2120,16 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2127,7 +2186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2301,6 +2360,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2608,30 +2670,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N60"/>
+  <dimension ref="B2:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
+      <selection pane="bottomRight" activeCell="I33" sqref="I33:I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="39.85546875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="39.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="69.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="69.5703125" style="1" hidden="1" customWidth="1"/>
     <col min="8" max="10" width="13.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="47.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2639,7 +2701,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -2650,7 +2712,7 @@
       <c r="G3" s="13"/>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -2662,7 +2724,7 @@
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -2674,7 +2736,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -2690,7 +2752,7 @@
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14">
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -2699,7 +2761,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14">
       <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
@@ -2708,7 +2770,7 @@
       </c>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14">
       <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
@@ -2717,7 +2779,7 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14">
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
@@ -2746,7 +2808,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14">
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
@@ -2775,7 +2837,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
@@ -2804,7 +2866,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14">
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
@@ -2833,7 +2895,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
@@ -2856,7 +2918,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13">
       <c r="B17" s="5" t="s">
         <v>126</v>
       </c>
@@ -2879,7 +2941,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13">
       <c r="B18" s="5" t="s">
         <v>186</v>
       </c>
@@ -2902,7 +2964,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="45">
       <c r="B19" s="5" t="s">
         <v>53</v>
       </c>
@@ -2931,7 +2993,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13">
       <c r="B20" s="5" t="s">
         <v>205</v>
       </c>
@@ -2958,7 +3020,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13">
       <c r="B21" s="5" t="s">
         <v>416</v>
       </c>
@@ -2983,7 +3045,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13">
       <c r="B22" s="5" t="s">
         <v>433</v>
       </c>
@@ -3008,7 +3070,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13">
       <c r="B23" s="5" t="s">
         <v>437</v>
       </c>
@@ -3036,7 +3098,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13">
       <c r="B24" s="5" t="s">
         <v>502</v>
       </c>
@@ -3068,7 +3130,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13">
       <c r="B25" s="5">
         <v>10</v>
       </c>
@@ -3095,7 +3157,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13">
       <c r="B26" s="5">
         <v>11</v>
       </c>
@@ -3122,7 +3184,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13">
       <c r="B27" s="5">
         <v>12</v>
       </c>
@@ -3149,7 +3211,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13">
       <c r="B28" s="5">
         <v>13</v>
       </c>
@@ -3176,7 +3238,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13">
       <c r="B29" s="3">
         <v>14</v>
       </c>
@@ -3203,7 +3265,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13">
       <c r="B30" s="3">
         <v>15</v>
       </c>
@@ -3224,7 +3286,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13">
       <c r="B31" s="3">
         <v>16</v>
       </c>
@@ -3245,7 +3307,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13">
       <c r="B32" s="3">
         <v>18</v>
       </c>
@@ -3270,7 +3332,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11">
       <c r="B33" s="3">
         <v>21</v>
       </c>
@@ -3287,8 +3349,8 @@
         <v>69</v>
       </c>
       <c r="G33" s="4"/>
-      <c r="I33" s="4" t="s">
-        <v>68</v>
+      <c r="I33" s="25" t="s">
+        <v>634</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>93</v>
@@ -3297,7 +3359,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11">
       <c r="B34" s="3">
         <v>22</v>
       </c>
@@ -3314,8 +3376,8 @@
         <v>71</v>
       </c>
       <c r="G34" s="4"/>
-      <c r="I34" s="4" t="s">
-        <v>68</v>
+      <c r="I34" s="25" t="s">
+        <v>634</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>93</v>
@@ -3324,7 +3386,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" ht="30">
       <c r="B35" s="3">
         <v>23</v>
       </c>
@@ -3341,8 +3403,8 @@
         <v>618</v>
       </c>
       <c r="G35" s="4"/>
-      <c r="I35" s="4" t="s">
-        <v>68</v>
+      <c r="I35" s="25" t="s">
+        <v>635</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>625</v>
@@ -3351,7 +3413,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11">
       <c r="B36" s="3">
         <v>24</v>
       </c>
@@ -3378,7 +3440,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11">
       <c r="B37" s="3">
         <v>31</v>
       </c>
@@ -3407,7 +3469,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11">
       <c r="B38" s="3">
         <v>32</v>
       </c>
@@ -3434,7 +3496,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11">
       <c r="B39" s="3">
         <v>33</v>
       </c>
@@ -3463,7 +3525,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11">
       <c r="B40" s="3">
         <v>34</v>
       </c>
@@ -3490,7 +3552,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11">
       <c r="B41" s="3">
         <v>35</v>
       </c>
@@ -3517,7 +3579,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11">
       <c r="B42" s="3">
         <v>36</v>
       </c>
@@ -3546,7 +3608,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11">
       <c r="B43" s="3">
         <v>41</v>
       </c>
@@ -3573,7 +3635,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11">
       <c r="B44" s="3">
         <v>42</v>
       </c>
@@ -3600,7 +3662,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11">
       <c r="B45" s="3" t="s">
         <v>151</v>
       </c>
@@ -3627,7 +3689,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11">
       <c r="B46" s="3">
         <v>60</v>
       </c>
@@ -3654,7 +3716,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11">
       <c r="B47" s="3">
         <v>61</v>
       </c>
@@ -3681,7 +3743,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11">
       <c r="B48" s="3">
         <v>62</v>
       </c>
@@ -3708,7 +3770,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" s="38" customFormat="1">
       <c r="B49" s="35">
         <v>63</v>
       </c>
@@ -3735,7 +3797,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11">
       <c r="B50" s="3">
         <v>68</v>
       </c>
@@ -3762,7 +3824,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11">
       <c r="B51" s="3">
         <v>69</v>
       </c>
@@ -3785,7 +3847,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11">
       <c r="B52" s="3">
         <v>71</v>
       </c>
@@ -3810,7 +3872,7 @@
       </c>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11">
       <c r="B53" s="3">
         <v>72</v>
       </c>
@@ -3831,7 +3893,7 @@
       </c>
       <c r="K53" s="4"/>
     </row>
-    <row r="54" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" ht="30">
       <c r="B54" s="3">
         <v>74</v>
       </c>
@@ -3858,7 +3920,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11">
       <c r="B55" s="3">
         <v>75</v>
       </c>
@@ -3866,7 +3928,7 @@
         <v>211</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="E55" s="26" t="s">
         <v>6</v>
@@ -3885,97 +3947,169 @@
         <v>213</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11">
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
-      <c r="E56" s="18"/>
+      <c r="E56" s="63"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
     </row>
-    <row r="57" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="35" t="s">
+    <row r="57" spans="2:11">
+      <c r="B57" s="3">
+        <v>81</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="E57" s="63"/>
+      <c r="F57" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="G57" s="4"/>
+      <c r="I57" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11">
+      <c r="B58" s="3">
+        <v>82</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="E58" s="63"/>
+      <c r="F58" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="G58" s="4"/>
+      <c r="I58" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11">
+      <c r="B59" s="3"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="63"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+    </row>
+    <row r="60" spans="2:11">
+      <c r="B60" s="3"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+    </row>
+    <row r="61" spans="2:11" s="38" customFormat="1">
+      <c r="B61" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C57" s="36" t="s">
+      <c r="C61" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="D57" s="36" t="s">
+      <c r="D61" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="37" t="s">
+      <c r="E61" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="F57" s="36" t="s">
+      <c r="F61" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="G57" s="36" t="s">
+      <c r="G61" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="I57" s="36" t="s">
+      <c r="I61" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="J57" s="36" t="s">
+      <c r="J61" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="K57" s="36" t="s">
+      <c r="K61" s="36" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="35" t="s">
+    <row r="62" spans="2:11" s="38" customFormat="1">
+      <c r="B62" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="C58" s="36" t="s">
+      <c r="C62" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="D58" s="36" t="s">
+      <c r="D62" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E58" s="37" t="s">
+      <c r="E62" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="F58" s="36" t="s">
+      <c r="F62" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="G58" s="36"/>
-      <c r="I58" s="36" t="s">
+      <c r="G62" s="36"/>
+      <c r="I62" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="J58" s="36" t="s">
+      <c r="J62" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="K58" s="36" t="s">
+      <c r="K62" s="36" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B60" s="3" t="s">
+    <row r="64" spans="2:11">
+      <c r="B64" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D64" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="E60" s="59" t="s">
+      <c r="E64" s="59" t="s">
         <v>522</v>
       </c>
-      <c r="F60" s="4" t="s">
+      <c r="F64" s="4" t="s">
         <v>612</v>
       </c>
-      <c r="G60" s="4"/>
-      <c r="I60" s="4" t="s">
+      <c r="G64" s="4"/>
+      <c r="I64" s="4" t="s">
         <v>611</v>
       </c>
-      <c r="J60" s="4" t="s">
+      <c r="J64" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="K60" s="4" t="s">
+      <c r="K64" s="4" t="s">
         <v>613</v>
       </c>
     </row>
@@ -3994,7 +4128,7 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="50"/>
     <col min="3" max="3" width="38.42578125" style="50" bestFit="1" customWidth="1"/>
@@ -4004,7 +4138,7 @@
     <col min="10" max="16384" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11">
       <c r="D1" s="50" t="s">
         <v>608</v>
       </c>
@@ -4027,7 +4161,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11">
       <c r="B2" s="60" t="s">
         <v>20</v>
       </c>
@@ -4056,7 +4190,7 @@
       </c>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11">
       <c r="B3" s="60" t="s">
         <v>21</v>
       </c>
@@ -4085,7 +4219,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11">
       <c r="B4" s="60" t="s">
         <v>22</v>
       </c>
@@ -4114,7 +4248,7 @@
       </c>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11">
       <c r="B5" s="60" t="s">
         <v>23</v>
       </c>
@@ -4143,7 +4277,7 @@
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11">
       <c r="B6" s="60" t="s">
         <v>126</v>
       </c>
@@ -4172,7 +4306,7 @@
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11">
       <c r="B7" s="60" t="s">
         <v>186</v>
       </c>
@@ -4201,7 +4335,7 @@
       </c>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11">
       <c r="B8" s="60" t="s">
         <v>53</v>
       </c>
@@ -4230,7 +4364,7 @@
       </c>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11">
       <c r="B9" s="60" t="s">
         <v>205</v>
       </c>
@@ -4259,7 +4393,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11">
       <c r="B10" s="60" t="s">
         <v>416</v>
       </c>
@@ -4288,7 +4422,7 @@
       </c>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11">
       <c r="B11" s="60" t="s">
         <v>433</v>
       </c>
@@ -4317,7 +4451,7 @@
       </c>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11">
       <c r="B12" s="60" t="s">
         <v>437</v>
       </c>
@@ -4346,7 +4480,7 @@
       </c>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11">
       <c r="B13" s="60" t="s">
         <v>502</v>
       </c>
@@ -4375,7 +4509,7 @@
       </c>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11">
       <c r="B14" s="60">
         <v>10</v>
       </c>
@@ -4404,7 +4538,7 @@
       </c>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11">
       <c r="B15" s="60">
         <v>11</v>
       </c>
@@ -4433,7 +4567,7 @@
       </c>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11">
       <c r="B16" s="60">
         <v>12</v>
       </c>
@@ -4462,7 +4596,7 @@
       </c>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11">
       <c r="B17" s="60">
         <v>13</v>
       </c>
@@ -4491,7 +4625,7 @@
       </c>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11">
       <c r="B18" s="9">
         <v>14</v>
       </c>
@@ -4520,7 +4654,7 @@
       </c>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11">
       <c r="B19" s="9">
         <v>15</v>
       </c>
@@ -4549,7 +4683,7 @@
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11">
       <c r="B20" s="9">
         <v>16</v>
       </c>
@@ -4578,7 +4712,7 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11">
       <c r="B21" s="9">
         <v>18</v>
       </c>
@@ -4607,7 +4741,7 @@
       </c>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11">
       <c r="B22" s="9">
         <v>21</v>
       </c>
@@ -4636,7 +4770,7 @@
       </c>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11">
       <c r="B23" s="9">
         <v>22</v>
       </c>
@@ -4665,7 +4799,7 @@
       </c>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11">
       <c r="B24" s="9">
         <v>23</v>
       </c>
@@ -4694,7 +4828,7 @@
       </c>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11">
       <c r="B25" s="9">
         <v>24</v>
       </c>
@@ -4723,7 +4857,7 @@
       </c>
       <c r="K25" s="10"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11">
       <c r="B26" s="9">
         <v>31</v>
       </c>
@@ -4752,7 +4886,7 @@
       </c>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11">
       <c r="B27" s="9">
         <v>32</v>
       </c>
@@ -4781,7 +4915,7 @@
       </c>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11">
       <c r="B28" s="9">
         <v>33</v>
       </c>
@@ -4810,7 +4944,7 @@
       </c>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11">
       <c r="B29" s="9">
         <v>34</v>
       </c>
@@ -4839,7 +4973,7 @@
       </c>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11">
       <c r="B30" s="9">
         <v>35</v>
       </c>
@@ -4868,7 +5002,7 @@
       </c>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11">
       <c r="B31" s="9">
         <v>36</v>
       </c>
@@ -4897,7 +5031,7 @@
       </c>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11">
       <c r="B32" s="9">
         <v>41</v>
       </c>
@@ -4926,7 +5060,7 @@
       </c>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11">
       <c r="B33" s="9">
         <v>42</v>
       </c>
@@ -4955,7 +5089,7 @@
       </c>
       <c r="K33" s="10"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11">
       <c r="B34" s="9" t="s">
         <v>151</v>
       </c>
@@ -4984,7 +5118,7 @@
       </c>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11">
       <c r="B35" s="9">
         <v>60</v>
       </c>
@@ -5013,7 +5147,7 @@
       </c>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11">
       <c r="B36" s="9">
         <v>61</v>
       </c>
@@ -5042,7 +5176,7 @@
       </c>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11">
       <c r="B37" s="9">
         <v>62</v>
       </c>
@@ -5071,7 +5205,7 @@
       </c>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11">
       <c r="B38" s="9">
         <v>68</v>
       </c>
@@ -5100,7 +5234,7 @@
       </c>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11">
       <c r="B39" s="9">
         <v>69</v>
       </c>
@@ -5129,7 +5263,7 @@
       </c>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11">
       <c r="B40" s="9">
         <v>71</v>
       </c>
@@ -5158,7 +5292,7 @@
       </c>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11">
       <c r="B41" s="9">
         <v>72</v>
       </c>
@@ -5187,7 +5321,7 @@
       </c>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11">
       <c r="B42" s="9">
         <v>74</v>
       </c>
@@ -5216,7 +5350,7 @@
       </c>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11">
       <c r="B43" s="9">
         <v>75</v>
       </c>
@@ -5245,7 +5379,7 @@
       </c>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11">
       <c r="B44" s="9" t="s">
         <v>519</v>
       </c>
@@ -5289,7 +5423,7 @@
       <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -5297,7 +5431,7 @@
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -5311,29 +5445,29 @@
         <v>383</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="64" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="45"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="63"/>
+      <c r="D4" s="64"/>
       <c r="E4" s="45"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5345,7 +5479,7 @@
       </c>
       <c r="E5" s="45"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -5357,7 +5491,7 @@
       </c>
       <c r="E6" s="45"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -5371,7 +5505,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
         <v>126</v>
       </c>
@@ -5385,7 +5519,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
         <v>186</v>
       </c>
@@ -5399,7 +5533,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
         <v>401</v>
       </c>
@@ -5413,7 +5547,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5">
       <c r="B11" s="3" t="s">
         <v>349</v>
       </c>
@@ -5427,7 +5561,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5">
       <c r="B12" s="3" t="s">
         <v>352</v>
       </c>
@@ -5441,7 +5575,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5">
       <c r="B13" s="3" t="s">
         <v>354</v>
       </c>
@@ -5455,7 +5589,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5">
       <c r="B14" s="3" t="s">
         <v>358</v>
       </c>
@@ -5469,7 +5603,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5">
       <c r="B15" s="3">
         <v>18</v>
       </c>
@@ -5483,7 +5617,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5">
       <c r="B16" s="3">
         <v>21</v>
       </c>
@@ -5497,7 +5631,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <v>22</v>
       </c>
@@ -5511,7 +5645,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <v>23</v>
       </c>
@@ -5525,7 +5659,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <v>24</v>
       </c>
@@ -5539,7 +5673,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <v>31</v>
       </c>
@@ -5553,7 +5687,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <v>32</v>
       </c>
@@ -5567,7 +5701,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <v>33</v>
       </c>
@@ -5581,7 +5715,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <v>41</v>
       </c>
@@ -5595,7 +5729,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <v>42</v>
       </c>
@@ -5609,7 +5743,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <v>43</v>
       </c>
@@ -5623,7 +5757,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <v>58</v>
       </c>
@@ -5635,7 +5769,7 @@
       </c>
       <c r="E26" s="45"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5">
       <c r="B27" s="3">
         <v>59</v>
       </c>
@@ -5664,7 +5798,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -5680,7 +5814,7 @@
     <col min="18" max="48" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:42">
       <c r="I1" s="52" t="s">
         <v>442</v>
       </c>
@@ -5694,7 +5828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:42">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -5753,14 +5887,14 @@
       <c r="AO2" s="11"/>
       <c r="AP2" s="11"/>
     </row>
-    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:42">
       <c r="B3" s="55">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="64" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="48">
@@ -5810,14 +5944,14 @@
       <c r="AO3" s="11"/>
       <c r="AP3" s="11"/>
     </row>
-    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:42">
       <c r="B4" s="56">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="63"/>
+      <c r="D4" s="64"/>
       <c r="E4" s="48">
         <v>1</v>
       </c>
@@ -5865,7 +5999,7 @@
       <c r="AO4" s="11"/>
       <c r="AP4" s="11"/>
     </row>
-    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:42">
       <c r="B5" s="56">
         <v>2</v>
       </c>
@@ -5922,7 +6056,7 @@
       <c r="AO5" s="11"/>
       <c r="AP5" s="11"/>
     </row>
-    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:42">
       <c r="B6" s="56">
         <v>3</v>
       </c>
@@ -5979,7 +6113,7 @@
       <c r="AO6" s="11"/>
       <c r="AP6" s="11"/>
     </row>
-    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:42">
       <c r="B7" s="56">
         <v>4</v>
       </c>
@@ -6036,7 +6170,7 @@
       <c r="AO7" s="11"/>
       <c r="AP7" s="11"/>
     </row>
-    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:42">
       <c r="B8" s="56">
         <v>5</v>
       </c>
@@ -6093,7 +6227,7 @@
       <c r="AO8" s="11"/>
       <c r="AP8" s="11"/>
     </row>
-    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:42">
       <c r="B9" s="56">
         <v>6</v>
       </c>
@@ -6150,7 +6284,7 @@
       <c r="AO9" s="11"/>
       <c r="AP9" s="11"/>
     </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:42">
       <c r="B10" s="56">
         <v>8</v>
       </c>
@@ -6207,7 +6341,7 @@
       <c r="AO10" s="11"/>
       <c r="AP10" s="11"/>
     </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:42">
       <c r="B11" s="56">
         <v>9</v>
       </c>
@@ -6264,7 +6398,7 @@
       <c r="AO11" s="11"/>
       <c r="AP11" s="11"/>
     </row>
-    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:42">
       <c r="B12" s="56">
         <v>10</v>
       </c>
@@ -6321,7 +6455,7 @@
       <c r="AO12" s="11"/>
       <c r="AP12" s="11"/>
     </row>
-    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:42">
       <c r="B13" s="56">
         <v>40</v>
       </c>
@@ -6378,7 +6512,7 @@
       <c r="AO13" s="11"/>
       <c r="AP13" s="11"/>
     </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:42">
       <c r="B14" s="56">
         <v>60</v>
       </c>
@@ -6435,7 +6569,7 @@
       <c r="AO14" s="11"/>
       <c r="AP14" s="11"/>
     </row>
-    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:42">
       <c r="B15" s="56">
         <v>61</v>
       </c>
@@ -6492,7 +6626,7 @@
       <c r="AO15" s="11"/>
       <c r="AP15" s="11"/>
     </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:42">
       <c r="B16" s="56">
         <v>62</v>
       </c>
@@ -6549,7 +6683,7 @@
       <c r="AO16" s="11"/>
       <c r="AP16" s="11"/>
     </row>
-    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:42">
       <c r="B17" s="56">
         <v>63</v>
       </c>
@@ -6606,7 +6740,7 @@
       <c r="AO17" s="11"/>
       <c r="AP17" s="11"/>
     </row>
-    <row r="18" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:42">
       <c r="B18" s="56">
         <v>64</v>
       </c>
@@ -6663,7 +6797,7 @@
       <c r="AO18" s="11"/>
       <c r="AP18" s="11"/>
     </row>
-    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:42">
       <c r="B19" s="56">
         <v>84</v>
       </c>
@@ -6720,7 +6854,7 @@
       <c r="AO19" s="11"/>
       <c r="AP19" s="11"/>
     </row>
-    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:42">
       <c r="B20" s="56">
         <v>104</v>
       </c>
@@ -6777,7 +6911,7 @@
       <c r="AO20" s="11"/>
       <c r="AP20" s="11"/>
     </row>
-    <row r="21" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:42">
       <c r="B21" s="56">
         <v>105</v>
       </c>
@@ -6834,7 +6968,7 @@
       <c r="AO21" s="11"/>
       <c r="AP21" s="11"/>
     </row>
-    <row r="22" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:42">
       <c r="B22" s="56">
         <v>106</v>
       </c>
@@ -6891,7 +7025,7 @@
       <c r="AO22" s="11"/>
       <c r="AP22" s="11"/>
     </row>
-    <row r="23" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:42">
       <c r="B23" s="56">
         <v>108</v>
       </c>
@@ -6948,7 +7082,7 @@
       <c r="AO23" s="11"/>
       <c r="AP23" s="11"/>
     </row>
-    <row r="24" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:42">
       <c r="B24" s="56">
         <v>109</v>
       </c>
@@ -7005,7 +7139,7 @@
       <c r="AO24" s="11"/>
       <c r="AP24" s="11"/>
     </row>
-    <row r="25" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:42">
       <c r="B25" s="56">
         <v>110</v>
       </c>
@@ -7062,7 +7196,7 @@
       <c r="AO25" s="11"/>
       <c r="AP25" s="11"/>
     </row>
-    <row r="26" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:42">
       <c r="B26" s="56">
         <v>112</v>
       </c>
@@ -7119,7 +7253,7 @@
       <c r="AO26" s="11"/>
       <c r="AP26" s="11"/>
     </row>
-    <row r="27" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:42">
       <c r="B27" s="56">
         <v>114</v>
       </c>
@@ -7176,7 +7310,7 @@
       <c r="AO27" s="11"/>
       <c r="AP27" s="11"/>
     </row>
-    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:42">
       <c r="B28" s="56">
         <v>118</v>
       </c>
@@ -7225,7 +7359,7 @@
       <c r="AO28" s="11"/>
       <c r="AP28" s="11"/>
     </row>
-    <row r="29" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:42">
       <c r="B29" s="56">
         <v>119</v>
       </c>
@@ -7274,7 +7408,7 @@
       <c r="AO29" s="11"/>
       <c r="AP29" s="11"/>
     </row>
-    <row r="30" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:42">
       <c r="E30">
         <f>SUM(E3:E29)</f>
         <v>120</v>
@@ -7314,7 +7448,7 @@
       <c r="AO30" s="11"/>
       <c r="AP30" s="11"/>
     </row>
-    <row r="31" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:42">
       <c r="I31" s="51"/>
       <c r="J31" s="51"/>
       <c r="K31" s="51"/>
@@ -7368,14 +7502,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -7386,27 +7520,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="64" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="63"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="64"/>
+    </row>
+    <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -7417,7 +7551,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -7428,7 +7562,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -7439,7 +7573,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" s="5" t="s">
         <v>422</v>
       </c>
@@ -7450,7 +7584,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4">
       <c r="B9" s="5" t="s">
         <v>425</v>
       </c>
@@ -7461,7 +7595,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4">
       <c r="B10" s="5" t="s">
         <v>428</v>
       </c>
@@ -7472,7 +7606,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="B11" s="3" t="s">
         <v>431</v>
       </c>
@@ -7483,7 +7617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4">
       <c r="B12" s="3">
         <v>58</v>
       </c>
@@ -7494,7 +7628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="B13" s="3">
         <v>59</v>
       </c>
@@ -7522,14 +7656,14 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" s="1" customFormat="1">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -7540,27 +7674,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" s="1" customFormat="1">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="64" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" s="1" customFormat="1">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="63"/>
-    </row>
-    <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="64"/>
+    </row>
+    <row r="5" spans="2:4" s="1" customFormat="1">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -7571,7 +7705,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" s="1" customFormat="1">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -7582,7 +7716,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" s="1" customFormat="1">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -7593,7 +7727,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="8" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" s="1" customFormat="1">
       <c r="B8" s="5" t="s">
         <v>344</v>
       </c>
@@ -7604,7 +7738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" s="1" customFormat="1">
       <c r="B9" s="3" t="s">
         <v>340</v>
       </c>
@@ -7615,7 +7749,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" s="1" customFormat="1">
       <c r="B10" s="3" t="s">
         <v>341</v>
       </c>
@@ -7626,7 +7760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" s="1" customFormat="1">
       <c r="B11" s="3">
         <v>58</v>
       </c>
@@ -7637,7 +7771,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" s="1" customFormat="1">
       <c r="B12" s="3">
         <v>59</v>
       </c>
@@ -7665,7 +7799,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -7676,12 +7810,12 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18.75">
       <c r="A2" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="27" t="s">
         <v>139</v>
       </c>
@@ -7689,12 +7823,12 @@
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -7705,27 +7839,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="64" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="63"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="64"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -7736,7 +7870,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -7747,7 +7881,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
@@ -7758,7 +7892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12" s="5" t="s">
         <v>126</v>
       </c>
@@ -7769,7 +7903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13" s="3" t="s">
         <v>127</v>
       </c>
@@ -7780,7 +7914,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14" s="3">
         <v>26</v>
       </c>
@@ -7791,7 +7925,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="B15" s="3">
         <v>27</v>
       </c>
@@ -7802,7 +7936,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="3">
         <v>28</v>
       </c>
@@ -7813,7 +7947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="B17" s="3">
         <v>29</v>
       </c>
@@ -7824,7 +7958,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="B18" s="3" t="s">
         <v>129</v>
       </c>
@@ -7835,7 +7969,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="B19" s="3" t="s">
         <v>124</v>
       </c>
@@ -7846,7 +7980,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="B20" s="3" t="s">
         <v>130</v>
       </c>
@@ -7857,7 +7991,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="B21" s="3" t="s">
         <v>131</v>
       </c>
@@ -7868,7 +8002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="B22" s="3">
         <v>58</v>
       </c>
@@ -7879,7 +8013,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="B23" s="3">
         <v>59</v>
       </c>
@@ -7890,17 +8024,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="18.75">
       <c r="A25" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
@@ -7911,27 +8045,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="B28" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="63" t="s">
+      <c r="D28" s="64" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="B29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="63"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="64"/>
+    </row>
+    <row r="30" spans="1:4">
       <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
@@ -7942,7 +8076,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="B31" s="5" t="s">
         <v>22</v>
       </c>
@@ -7953,7 +8087,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="B32" s="5" t="s">
         <v>23</v>
       </c>
@@ -7964,7 +8098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4">
       <c r="B33" s="5" t="s">
         <v>126</v>
       </c>
@@ -7975,7 +8109,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4">
       <c r="B34" s="5" t="s">
         <v>186</v>
       </c>
@@ -7986,7 +8120,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4">
       <c r="B35" s="5" t="s">
         <v>187</v>
       </c>
@@ -7997,7 +8131,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4">
       <c r="B36" s="3" t="s">
         <v>188</v>
       </c>
@@ -8008,7 +8142,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4">
       <c r="B37" s="3" t="s">
         <v>189</v>
       </c>
@@ -8019,7 +8153,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4">
       <c r="B38" s="3" t="s">
         <v>190</v>
       </c>
@@ -8030,7 +8164,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4">
       <c r="B39" s="3">
         <v>51</v>
       </c>
@@ -8041,7 +8175,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4">
       <c r="B40" s="3">
         <v>52</v>
       </c>
@@ -8052,7 +8186,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4">
       <c r="B41" s="3">
         <v>53</v>
       </c>
@@ -8063,7 +8197,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4">
       <c r="B42" s="3">
         <v>54</v>
       </c>
@@ -8074,7 +8208,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4">
       <c r="B43" s="3">
         <v>55</v>
       </c>
@@ -8085,7 +8219,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4">
       <c r="B44" s="3" t="s">
         <v>201</v>
       </c>
@@ -8096,7 +8230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4">
       <c r="B45" s="3">
         <v>58</v>
       </c>
@@ -8107,7 +8241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4">
       <c r="B46" s="3">
         <v>59</v>
       </c>
@@ -8118,17 +8252,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4">
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4">
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4">
       <c r="C49" s="1" t="s">
         <v>140</v>
       </c>
@@ -8136,17 +8270,17 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4">
       <c r="D50" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4">
       <c r="D51" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4">
       <c r="D52" s="1" t="s">
         <v>144</v>
       </c>
@@ -8170,17 +8304,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="158.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:3" ht="60">
       <c r="C2" s="24" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:3">
       <c r="C5" t="s">
         <v>137</v>
       </c>
@@ -8199,7 +8333,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
@@ -8209,7 +8343,7 @@
     <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10">
       <c r="B3" s="40" t="s">
         <v>219</v>
       </c>
@@ -8236,7 +8370,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="B4" s="39" t="s">
         <v>227</v>
       </c>
@@ -8262,7 +8396,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="B5" t="s">
         <v>218</v>
       </c>
@@ -8288,7 +8422,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="B6" t="s">
         <v>328</v>
       </c>
@@ -8314,7 +8448,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10">
       <c r="B7" t="s">
         <v>331</v>
       </c>
@@ -8340,7 +8474,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="B8" t="s">
         <v>216</v>
       </c>
@@ -8366,7 +8500,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="B9" t="s">
         <v>217</v>
       </c>
@@ -8392,7 +8526,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="B10" t="s">
         <v>279</v>
       </c>
@@ -8412,7 +8546,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="B11" t="s">
         <v>280</v>
       </c>
@@ -8432,7 +8566,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10">
       <c r="B12" t="s">
         <v>278</v>
       </c>
@@ -8452,7 +8586,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10">
       <c r="B13" t="s">
         <v>286</v>
       </c>
@@ -8472,7 +8606,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10">
       <c r="B15" t="s">
         <v>257</v>
       </c>
@@ -8489,7 +8623,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10">
       <c r="B16" t="s">
         <v>258</v>
       </c>
@@ -8509,7 +8643,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9">
       <c r="B18" t="s">
         <v>228</v>
       </c>
@@ -8532,7 +8666,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9">
       <c r="B20" t="s">
         <v>231</v>
       </c>
@@ -8555,7 +8689,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9">
       <c r="B21" t="s">
         <v>235</v>
       </c>
@@ -8578,7 +8712,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9">
       <c r="B22" t="s">
         <v>242</v>
       </c>
@@ -8601,7 +8735,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9">
       <c r="B23" t="s">
         <v>320</v>
       </c>
@@ -8621,7 +8755,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9">
       <c r="B24" t="s">
         <v>321</v>
       </c>
@@ -8641,7 +8775,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9">
       <c r="B25" t="s">
         <v>322</v>
       </c>
@@ -8661,7 +8795,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9">
       <c r="B27" t="s">
         <v>236</v>
       </c>
@@ -8684,7 +8818,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9">
       <c r="B28" t="s">
         <v>237</v>
       </c>
@@ -8707,7 +8841,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9">
       <c r="B29" t="s">
         <v>241</v>
       </c>
@@ -8730,7 +8864,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9">
       <c r="B30" t="s">
         <v>245</v>
       </c>
@@ -8753,7 +8887,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9">
       <c r="B31" t="s">
         <v>246</v>
       </c>
@@ -8776,7 +8910,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9">
       <c r="B32" t="s">
         <v>247</v>
       </c>
@@ -8799,7 +8933,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9">
       <c r="B33" t="s">
         <v>263</v>
       </c>
@@ -8819,7 +8953,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9">
       <c r="B34" t="s">
         <v>264</v>
       </c>
@@ -8839,7 +8973,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9">
       <c r="B35" t="s">
         <v>266</v>
       </c>
@@ -8859,7 +8993,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" t="s">
         <v>275</v>
       </c>
@@ -8882,7 +9016,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9">
       <c r="B38" t="s">
         <v>251</v>
       </c>
@@ -8905,7 +9039,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9">
       <c r="B39" t="s">
         <v>268</v>
       </c>
@@ -8925,7 +9059,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9">
       <c r="B40" t="s">
         <v>269</v>
       </c>
@@ -8945,7 +9079,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9">
       <c r="B41" t="s">
         <v>273</v>
       </c>

</xml_diff>

<commit_message>
Updated to change event data batch size to 8
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="713">
   <si>
     <t>Offset</t>
   </si>
@@ -2099,18 +2099,10 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Event Header</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Event Data (12 bytes)</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>10 x {EventData}</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Starting index</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -2139,14 +2131,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>06~125</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Length of header data = 122</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>0x92</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -2159,10 +2143,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>0x7A</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Yes {128}</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -2175,10 +2155,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Event Data Batch</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>{refer to Event Data Batch}</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -2231,18 +2207,10 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>0 - idle, else - busy</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Event count (only support 255 event at this version)</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Event count (only support 255 event at this version)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>A9 9A 02 0B 0D ED</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -2255,10 +2223,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Reserved for command code; return 90 - idle, 91 - busy</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>seq</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -2344,6 +2308,70 @@
   </si>
   <si>
     <t>Action: parm_2, parm_3 (byte) or parm_u16 (UInt16)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Event Header as result of 0x91</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00 - idle, 0x01 - busy</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of events in this batch</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Event Data Batch as result of 0x92; leave more space for future use, only 8 events everytime</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>8 x {EventData}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>06</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>{mode}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>07 ~ 15</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>reserved</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 ~ 111</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>112 ~ 125</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>reserved</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x7C</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length of header data = 124</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -2469,7 +2497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2657,6 +2685,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2968,7 +2999,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F60" sqref="F60"/>
+      <selection pane="bottomRight" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3299,7 +3330,7 @@
         <v>45</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="G20" s="12"/>
       <c r="I20" s="4" t="s">
@@ -4316,14 +4347,14 @@
         <v>91</v>
       </c>
       <c r="C60" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="D60" s="17" t="s">
         <v>668</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>674</v>
       </c>
       <c r="E60" s="64"/>
       <c r="F60" s="4" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="G60" s="4"/>
       <c r="I60" s="4" t="s">
@@ -4339,16 +4370,16 @@
         <v>92</v>
       </c>
       <c r="C61" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="E61" s="64" t="s">
         <v>670</v>
       </c>
-      <c r="D61" s="4" t="s">
-        <v>675</v>
-      </c>
-      <c r="E61" s="64" t="s">
-        <v>676</v>
-      </c>
       <c r="F61" s="4" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="G61" s="4"/>
       <c r="I61" s="4"/>
@@ -4360,14 +4391,14 @@
         <v>93</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="E62" s="64"/>
       <c r="F62" s="4" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="G62" s="4"/>
       <c r="I62" s="4"/>
@@ -4382,11 +4413,11 @@
         <v>636</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="E63" s="64"/>
       <c r="F63" s="4" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="G63" s="4"/>
       <c r="I63" s="4"/>
@@ -5280,22 +5311,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D37"/>
+  <dimension ref="B2:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>644</v>
+        <v>697</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -5316,7 +5347,7 @@
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="68" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5327,7 +5358,7 @@
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="65"/>
+      <c r="D5" s="68"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
@@ -5345,7 +5376,7 @@
         <v>22</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="D7" s="64" t="s">
         <v>122</v>
@@ -5353,18 +5384,18 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
       <c r="D8" s="64" t="s">
-        <v>677</v>
+        <v>698</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>637</v>
@@ -5375,29 +5406,29 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>639</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>4</v>
@@ -5430,7 +5461,7 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>663</v>
+        <v>700</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -5440,7 +5471,7 @@
       <c r="C17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="65" t="s">
+      <c r="D17" s="68" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5451,198 +5482,231 @@
       <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="65"/>
+      <c r="D18" s="68"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>659</v>
+        <v>711</v>
       </c>
       <c r="D19" s="64" t="s">
-        <v>655</v>
+        <v>712</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>656</v>
-      </c>
-      <c r="D20" s="64" t="s">
-        <v>683</v>
+        <v>652</v>
+      </c>
+      <c r="D20" s="65" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>648</v>
-      </c>
-      <c r="D21" s="64" t="s">
-        <v>647</v>
+        <v>703</v>
+      </c>
+      <c r="D21" s="65" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="D22" s="64" t="s">
-        <v>678</v>
+        <v>645</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="66" t="s">
-        <v>654</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>646</v>
-      </c>
-      <c r="D23" s="45" t="s">
-        <v>649</v>
+      <c r="B23" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="D23" s="64" t="s">
+        <v>699</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="45">
+      <c r="B24" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="66" t="s">
+        <v>707</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>701</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="66" t="s">
+        <v>708</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>709</v>
+      </c>
+      <c r="D26" s="45" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="45">
         <v>126</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="64" t="s">
+      <c r="D27" s="64" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="45">
-        <v>127</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="64" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="45">
-        <v>0</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>684</v>
-      </c>
-      <c r="D28" s="45" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="45">
-        <v>1</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>685</v>
-      </c>
-      <c r="D29" s="45" t="s">
-        <v>697</v>
+        <v>127</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="64" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="45">
-        <v>2</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>686</v>
-      </c>
-      <c r="D30" s="45" t="s">
-        <v>698</v>
+      <c r="B30" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="45">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C31" s="16" t="s">
+        <v>675</v>
+      </c>
+      <c r="D31" s="45" t="s">
         <v>687</v>
-      </c>
-      <c r="D31" s="45" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="45">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C32" s="16" t="s">
+        <v>676</v>
+      </c>
+      <c r="D32" s="45" t="s">
         <v>688</v>
-      </c>
-      <c r="D32" s="45" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="45">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C33" s="16" t="s">
+        <v>677</v>
+      </c>
+      <c r="D33" s="45" t="s">
         <v>689</v>
       </c>
-      <c r="D33" s="45" t="s">
-        <v>701</v>
-      </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="67" t="s">
-        <v>691</v>
+      <c r="B34" s="45">
+        <v>3</v>
       </c>
       <c r="C34" s="16" t="s">
+        <v>678</v>
+      </c>
+      <c r="D34" s="45" t="s">
         <v>690</v>
-      </c>
-      <c r="D34" s="45" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="45">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>692</v>
+        <v>679</v>
       </c>
       <c r="D35" s="45" t="s">
-        <v>703</v>
+        <v>691</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="45">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>693</v>
+        <v>680</v>
       </c>
       <c r="D36" s="45" t="s">
-        <v>704</v>
+        <v>692</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="67" t="s">
+        <v>682</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>681</v>
+      </c>
+      <c r="D37" s="45" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="45">
+        <v>8</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>683</v>
+      </c>
+      <c r="D38" s="45" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="45">
+        <v>9</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>684</v>
+      </c>
+      <c r="D39" s="45" t="s">
         <v>695</v>
       </c>
-      <c r="C37" s="16" t="s">
-        <v>694</v>
-      </c>
-      <c r="D37" s="45" t="s">
-        <v>705</v>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="67" t="s">
+        <v>686</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>685</v>
+      </c>
+      <c r="D40" s="45" t="s">
+        <v>696</v>
       </c>
     </row>
   </sheetData>
@@ -6988,7 +7052,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="68" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="45"/>
@@ -7000,7 +7064,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="68"/>
       <c r="E4" s="45"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -7430,7 +7494,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="68" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="48">
@@ -7487,7 +7551,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="68"/>
       <c r="E4" s="48">
         <v>1</v>
       </c>
@@ -9063,7 +9127,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="68" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9074,7 +9138,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="68"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
@@ -9217,7 +9281,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="68" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9228,7 +9292,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="68"/>
     </row>
     <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
@@ -9382,7 +9446,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="68" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9393,7 +9457,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="65"/>
+      <c r="D8" s="68"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -9588,7 +9652,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="65" t="s">
+      <c r="D28" s="68" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9599,7 +9663,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="65"/>
+      <c r="D29" s="68"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">

</xml_diff>

<commit_message>
Working, still have bug in saving events
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="714">
   <si>
     <t>Offset</t>
   </si>
@@ -1903,7 +1903,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1924,7 +1924,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1935,7 +1935,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1952,7 +1952,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1963,7 +1963,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1979,7 +1979,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1996,7 +1996,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -2029,7 +2029,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2039,7 +2039,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2151,10 +2151,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>{refer to Event Header}</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>{refer to Event Data Batch}</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -2219,10 +2215,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>A9 9A 04 92 00 10 A6 ED</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>seq</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -2373,17 +2365,26 @@
   <si>
     <t>Length of header data = 124</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>A9 9A 0C 93 00 00 05 02 00 00 00 00 00 00 A6 ED</t>
+  </si>
+  <si>
+    <t>A9 9A 04 92 00 00 96 ED</t>
+  </si>
+  <si>
+    <t>A9 9A 0C 93 00 01 05 01 00 00 00 00 00 00 A6 ED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2391,7 +2392,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2401,7 +2402,7 @@
       <u/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2411,19 +2412,19 @@
       <u/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2431,7 +2432,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2439,7 +2440,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2995,28 +2996,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="F50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D52" sqref="D52"/>
+      <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.85546875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="39.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="69.5703125" style="1" customWidth="1"/>
     <col min="8" max="10" width="13.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="47.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3024,7 +3025,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -3035,7 +3036,7 @@
       <c r="G3" s="13"/>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -3047,7 +3048,7 @@
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -3059,7 +3060,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -3075,7 +3076,7 @@
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14">
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -3084,7 +3085,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14">
       <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
@@ -3093,7 +3094,7 @@
       </c>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14">
       <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
@@ -3102,7 +3103,7 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14">
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
@@ -3131,7 +3132,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14">
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
@@ -3160,7 +3161,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
@@ -3189,7 +3190,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14">
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
@@ -3218,7 +3219,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
@@ -3241,7 +3242,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13">
       <c r="B17" s="5" t="s">
         <v>126</v>
       </c>
@@ -3264,7 +3265,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13">
       <c r="B18" s="5" t="s">
         <v>186</v>
       </c>
@@ -3287,7 +3288,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="45">
       <c r="B19" s="5" t="s">
         <v>53</v>
       </c>
@@ -3316,7 +3317,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13">
       <c r="B20" s="5" t="s">
         <v>205</v>
       </c>
@@ -3330,7 +3331,7 @@
         <v>45</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G20" s="12"/>
       <c r="I20" s="4" t="s">
@@ -3343,7 +3344,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13">
       <c r="B21" s="5" t="s">
         <v>415</v>
       </c>
@@ -3368,7 +3369,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13">
       <c r="B22" s="5" t="s">
         <v>432</v>
       </c>
@@ -3393,7 +3394,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13">
       <c r="B23" s="5" t="s">
         <v>436</v>
       </c>
@@ -3421,7 +3422,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13">
       <c r="B24" s="5" t="s">
         <v>501</v>
       </c>
@@ -3453,7 +3454,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13">
       <c r="B25" s="5">
         <v>10</v>
       </c>
@@ -3480,7 +3481,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13">
       <c r="B26" s="5">
         <v>11</v>
       </c>
@@ -3507,7 +3508,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13">
       <c r="B27" s="5">
         <v>12</v>
       </c>
@@ -3534,7 +3535,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13">
       <c r="B28" s="5">
         <v>13</v>
       </c>
@@ -3561,7 +3562,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13">
       <c r="B29" s="3">
         <v>14</v>
       </c>
@@ -3588,7 +3589,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13">
       <c r="B30" s="3">
         <v>15</v>
       </c>
@@ -3609,7 +3610,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13">
       <c r="B31" s="3">
         <v>16</v>
       </c>
@@ -3630,7 +3631,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13">
       <c r="B32" s="3">
         <v>18</v>
       </c>
@@ -3655,7 +3656,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11">
       <c r="B33" s="3">
         <v>21</v>
       </c>
@@ -3682,7 +3683,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11">
       <c r="B34" s="3">
         <v>22</v>
       </c>
@@ -3709,7 +3710,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" ht="30">
       <c r="B35" s="3">
         <v>23</v>
       </c>
@@ -3736,7 +3737,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11">
       <c r="B36" s="3">
         <v>24</v>
       </c>
@@ -3763,7 +3764,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11">
       <c r="B37" s="3">
         <v>31</v>
       </c>
@@ -3792,7 +3793,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11">
       <c r="B38" s="3">
         <v>32</v>
       </c>
@@ -3819,7 +3820,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11">
       <c r="B39" s="3">
         <v>33</v>
       </c>
@@ -3848,7 +3849,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11">
       <c r="B40" s="3">
         <v>34</v>
       </c>
@@ -3875,7 +3876,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11">
       <c r="B41" s="3">
         <v>35</v>
       </c>
@@ -3902,7 +3903,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11">
       <c r="B42" s="3">
         <v>36</v>
       </c>
@@ -3931,7 +3932,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11">
       <c r="B43" s="3">
         <v>41</v>
       </c>
@@ -3958,7 +3959,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11">
       <c r="B44" s="3">
         <v>42</v>
       </c>
@@ -3985,7 +3986,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11">
       <c r="B45" s="3" t="s">
         <v>151</v>
       </c>
@@ -4012,7 +4013,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11">
       <c r="B46" s="3">
         <v>60</v>
       </c>
@@ -4039,7 +4040,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11">
       <c r="B47" s="3">
         <v>61</v>
       </c>
@@ -4066,7 +4067,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11">
       <c r="B48" s="3">
         <v>62</v>
       </c>
@@ -4093,7 +4094,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" s="38" customFormat="1">
       <c r="B49" s="35">
         <v>63</v>
       </c>
@@ -4120,7 +4121,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11">
       <c r="B50" s="3">
         <v>68</v>
       </c>
@@ -4147,7 +4148,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11">
       <c r="B51" s="3">
         <v>69</v>
       </c>
@@ -4170,7 +4171,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11">
       <c r="B52" s="3">
         <v>71</v>
       </c>
@@ -4195,7 +4196,7 @@
       </c>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11">
       <c r="B53" s="3">
         <v>72</v>
       </c>
@@ -4216,7 +4217,7 @@
       </c>
       <c r="K53" s="4"/>
     </row>
-    <row r="54" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" ht="30">
       <c r="B54" s="3">
         <v>74</v>
       </c>
@@ -4243,7 +4244,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11">
       <c r="B55" s="3">
         <v>75</v>
       </c>
@@ -4270,7 +4271,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11">
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -4281,7 +4282,7 @@
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11">
       <c r="B57" s="3">
         <v>81</v>
       </c>
@@ -4306,7 +4307,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11">
       <c r="B58" s="3">
         <v>82</v>
       </c>
@@ -4331,7 +4332,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11">
       <c r="B59" s="3"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -4342,19 +4343,19 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11">
       <c r="B60" s="3">
         <v>91</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E60" s="64"/>
       <c r="F60" s="4" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G60" s="4"/>
       <c r="I60" s="4" t="s">
@@ -4365,47 +4366,49 @@
       </c>
       <c r="K60" s="4"/>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11">
       <c r="B61" s="3">
         <v>92</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D61" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="E61" s="64" t="s">
         <v>669</v>
       </c>
-      <c r="E61" s="64" t="s">
-        <v>670</v>
-      </c>
       <c r="F61" s="4" t="s">
-        <v>674</v>
+        <v>712</v>
       </c>
       <c r="G61" s="4"/>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11">
       <c r="B62" s="3">
         <v>93</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>656</v>
       </c>
       <c r="E62" s="64"/>
       <c r="F62" s="4" t="s">
-        <v>657</v>
-      </c>
-      <c r="G62" s="4"/>
+        <v>713</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>711</v>
+      </c>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11">
       <c r="B63" s="3">
         <v>94</v>
       </c>
@@ -4417,14 +4420,14 @@
       </c>
       <c r="E63" s="64"/>
       <c r="F63" s="4" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G63" s="4"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11">
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
@@ -4435,7 +4438,7 @@
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
     </row>
-    <row r="65" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11" s="38" customFormat="1">
       <c r="B65" s="35" t="s">
         <v>80</v>
       </c>
@@ -4464,7 +4467,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="66" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11" s="38" customFormat="1">
       <c r="B66" s="35" t="s">
         <v>85</v>
       </c>
@@ -4491,7 +4494,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:11">
       <c r="B68" s="3" t="s">
         <v>518</v>
       </c>
@@ -4533,7 +4536,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
@@ -4543,7 +4546,7 @@
     <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10">
       <c r="B3" s="40" t="s">
         <v>218</v>
       </c>
@@ -4570,7 +4573,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="B4" s="39" t="s">
         <v>226</v>
       </c>
@@ -4596,7 +4599,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="B5" t="s">
         <v>217</v>
       </c>
@@ -4622,7 +4625,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="B6" t="s">
         <v>327</v>
       </c>
@@ -4648,7 +4651,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10">
       <c r="B7" t="s">
         <v>330</v>
       </c>
@@ -4674,7 +4677,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="B8" t="s">
         <v>215</v>
       </c>
@@ -4700,7 +4703,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="B9" t="s">
         <v>216</v>
       </c>
@@ -4726,7 +4729,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="B10" t="s">
         <v>278</v>
       </c>
@@ -4746,7 +4749,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="B11" t="s">
         <v>279</v>
       </c>
@@ -4766,7 +4769,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10">
       <c r="B12" t="s">
         <v>277</v>
       </c>
@@ -4786,7 +4789,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10">
       <c r="B13" t="s">
         <v>285</v>
       </c>
@@ -4806,7 +4809,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10">
       <c r="B15" t="s">
         <v>256</v>
       </c>
@@ -4823,7 +4826,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10">
       <c r="B16" t="s">
         <v>257</v>
       </c>
@@ -4843,7 +4846,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9">
       <c r="B18" t="s">
         <v>227</v>
       </c>
@@ -4866,7 +4869,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9">
       <c r="B20" t="s">
         <v>230</v>
       </c>
@@ -4889,7 +4892,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9">
       <c r="B21" t="s">
         <v>234</v>
       </c>
@@ -4912,7 +4915,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9">
       <c r="B22" t="s">
         <v>241</v>
       </c>
@@ -4935,7 +4938,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9">
       <c r="B23" t="s">
         <v>319</v>
       </c>
@@ -4955,7 +4958,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9">
       <c r="B24" t="s">
         <v>320</v>
       </c>
@@ -4975,7 +4978,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9">
       <c r="B25" t="s">
         <v>321</v>
       </c>
@@ -4995,7 +4998,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9">
       <c r="B27" t="s">
         <v>235</v>
       </c>
@@ -5018,7 +5021,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9">
       <c r="B28" t="s">
         <v>236</v>
       </c>
@@ -5041,7 +5044,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9">
       <c r="B29" t="s">
         <v>240</v>
       </c>
@@ -5064,7 +5067,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9">
       <c r="B30" t="s">
         <v>244</v>
       </c>
@@ -5087,7 +5090,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9">
       <c r="B31" t="s">
         <v>245</v>
       </c>
@@ -5110,7 +5113,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9">
       <c r="B32" t="s">
         <v>246</v>
       </c>
@@ -5133,7 +5136,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9">
       <c r="B33" t="s">
         <v>262</v>
       </c>
@@ -5153,7 +5156,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9">
       <c r="B34" t="s">
         <v>263</v>
       </c>
@@ -5173,7 +5176,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9">
       <c r="B35" t="s">
         <v>265</v>
       </c>
@@ -5193,7 +5196,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" t="s">
         <v>274</v>
       </c>
@@ -5216,7 +5219,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9">
       <c r="B38" t="s">
         <v>250</v>
       </c>
@@ -5239,7 +5242,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9">
       <c r="B39" t="s">
         <v>267</v>
       </c>
@@ -5259,7 +5262,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9">
       <c r="B40" t="s">
         <v>268</v>
       </c>
@@ -5279,7 +5282,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9">
       <c r="B41" t="s">
         <v>272</v>
       </c>
@@ -5313,23 +5316,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -5340,7 +5343,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
@@ -5351,7 +5354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
@@ -5360,7 +5363,7 @@
       </c>
       <c r="D5" s="68"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
@@ -5371,7 +5374,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
@@ -5382,18 +5385,18 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" s="5" t="s">
         <v>649</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D8" s="64" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
       <c r="B9" s="5" t="s">
         <v>653</v>
       </c>
@@ -5404,31 +5407,31 @@
         <v>638</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4">
       <c r="B10" s="5" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>639</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
       <c r="B11" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="D11" s="64" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="3" t="s">
         <v>666</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="D11" s="64" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>667</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>4</v>
@@ -5437,7 +5440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="B13" s="3">
         <v>14</v>
       </c>
@@ -5448,7 +5451,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4">
       <c r="B14" s="3">
         <v>15</v>
       </c>
@@ -5459,12 +5462,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4">
       <c r="B16" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
@@ -5475,7 +5478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4">
       <c r="B18" s="5" t="s">
         <v>20</v>
       </c>
@@ -5484,18 +5487,18 @@
       </c>
       <c r="D18" s="68"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4">
       <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D19" s="64" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
       <c r="B20" s="5" t="s">
         <v>648</v>
       </c>
@@ -5506,18 +5509,18 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4">
       <c r="B21" s="5" t="s">
         <v>649</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="D21" s="65" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
       <c r="B22" s="5" t="s">
         <v>650</v>
       </c>
@@ -5528,51 +5531,51 @@
         <v>645</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4">
       <c r="B23" s="5" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>651</v>
       </c>
       <c r="D23" s="64" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="66" t="s">
+        <v>705</v>
+      </c>
+      <c r="C25" s="16" t="s">
         <v>699</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>704</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>705</v>
-      </c>
-      <c r="D24" s="65" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="66" t="s">
-        <v>707</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>701</v>
       </c>
       <c r="D25" s="45" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4">
       <c r="B26" s="66" t="s">
+        <v>706</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>707</v>
+      </c>
+      <c r="D26" s="45" t="s">
         <v>708</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>709</v>
-      </c>
-      <c r="D26" s="45" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:4">
       <c r="B27" s="45">
         <v>126</v>
       </c>
@@ -5583,7 +5586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4">
       <c r="B28" s="45">
         <v>127</v>
       </c>
@@ -5594,119 +5597,119 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4">
       <c r="B30" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4">
       <c r="B31" s="45">
         <v>0</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D31" s="45" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
       <c r="B32" s="45">
         <v>1</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="D32" s="45" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
       <c r="B33" s="45">
         <v>2</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D33" s="45" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
       <c r="B34" s="45">
         <v>3</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D34" s="45" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
       <c r="B35" s="45">
         <v>4</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D35" s="45" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
       <c r="B36" s="45">
         <v>5</v>
       </c>
       <c r="C36" s="16" t="s">
+        <v>678</v>
+      </c>
+      <c r="D36" s="45" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="67" t="s">
         <v>680</v>
       </c>
-      <c r="D36" s="45" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="67" t="s">
-        <v>682</v>
-      </c>
       <c r="C37" s="16" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D37" s="45" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
       <c r="B38" s="45">
         <v>8</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D38" s="45" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
       <c r="B39" s="45">
         <v>9</v>
       </c>
       <c r="C39" s="16" t="s">
+        <v>682</v>
+      </c>
+      <c r="D39" s="45" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="67" t="s">
         <v>684</v>
       </c>
-      <c r="D39" s="45" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="67" t="s">
-        <v>686</v>
-      </c>
       <c r="C40" s="16" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D40" s="45" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
   </sheetData>
@@ -5728,7 +5731,7 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="50"/>
     <col min="3" max="3" width="38.42578125" style="50" bestFit="1" customWidth="1"/>
@@ -5738,7 +5741,7 @@
     <col min="10" max="16384" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11">
       <c r="D1" s="50" t="s">
         <v>607</v>
       </c>
@@ -5761,7 +5764,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11">
       <c r="B2" s="60" t="s">
         <v>20</v>
       </c>
@@ -5790,7 +5793,7 @@
       </c>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11">
       <c r="B3" s="60" t="s">
         <v>21</v>
       </c>
@@ -5819,7 +5822,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11">
       <c r="B4" s="60" t="s">
         <v>22</v>
       </c>
@@ -5848,7 +5851,7 @@
       </c>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11">
       <c r="B5" s="60" t="s">
         <v>23</v>
       </c>
@@ -5877,7 +5880,7 @@
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11">
       <c r="B6" s="60" t="s">
         <v>126</v>
       </c>
@@ -5906,7 +5909,7 @@
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11">
       <c r="B7" s="60" t="s">
         <v>186</v>
       </c>
@@ -5935,7 +5938,7 @@
       </c>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11">
       <c r="B8" s="60" t="s">
         <v>53</v>
       </c>
@@ -5964,7 +5967,7 @@
       </c>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11">
       <c r="B9" s="60" t="s">
         <v>205</v>
       </c>
@@ -5993,7 +5996,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11">
       <c r="B10" s="60" t="s">
         <v>415</v>
       </c>
@@ -6022,7 +6025,7 @@
       </c>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11">
       <c r="B11" s="60" t="s">
         <v>432</v>
       </c>
@@ -6051,7 +6054,7 @@
       </c>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11">
       <c r="B12" s="60" t="s">
         <v>436</v>
       </c>
@@ -6080,7 +6083,7 @@
       </c>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11">
       <c r="B13" s="60" t="s">
         <v>501</v>
       </c>
@@ -6109,7 +6112,7 @@
       </c>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11">
       <c r="B14" s="60">
         <v>10</v>
       </c>
@@ -6138,7 +6141,7 @@
       </c>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11">
       <c r="B15" s="60">
         <v>11</v>
       </c>
@@ -6167,7 +6170,7 @@
       </c>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11">
       <c r="B16" s="60">
         <v>12</v>
       </c>
@@ -6196,7 +6199,7 @@
       </c>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11">
       <c r="B17" s="60">
         <v>13</v>
       </c>
@@ -6225,7 +6228,7 @@
       </c>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11">
       <c r="B18" s="9">
         <v>14</v>
       </c>
@@ -6254,7 +6257,7 @@
       </c>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11">
       <c r="B19" s="9">
         <v>15</v>
       </c>
@@ -6283,7 +6286,7 @@
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11">
       <c r="B20" s="9">
         <v>16</v>
       </c>
@@ -6312,7 +6315,7 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11">
       <c r="B21" s="9">
         <v>18</v>
       </c>
@@ -6341,7 +6344,7 @@
       </c>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11">
       <c r="B22" s="9">
         <v>21</v>
       </c>
@@ -6370,7 +6373,7 @@
       </c>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11">
       <c r="B23" s="9">
         <v>22</v>
       </c>
@@ -6399,7 +6402,7 @@
       </c>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11">
       <c r="B24" s="9">
         <v>23</v>
       </c>
@@ -6428,7 +6431,7 @@
       </c>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11">
       <c r="B25" s="9">
         <v>24</v>
       </c>
@@ -6457,7 +6460,7 @@
       </c>
       <c r="K25" s="10"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11">
       <c r="B26" s="9">
         <v>31</v>
       </c>
@@ -6486,7 +6489,7 @@
       </c>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11">
       <c r="B27" s="9">
         <v>32</v>
       </c>
@@ -6515,7 +6518,7 @@
       </c>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11">
       <c r="B28" s="9">
         <v>33</v>
       </c>
@@ -6544,7 +6547,7 @@
       </c>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11">
       <c r="B29" s="9">
         <v>34</v>
       </c>
@@ -6573,7 +6576,7 @@
       </c>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11">
       <c r="B30" s="9">
         <v>35</v>
       </c>
@@ -6602,7 +6605,7 @@
       </c>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11">
       <c r="B31" s="9">
         <v>36</v>
       </c>
@@ -6631,7 +6634,7 @@
       </c>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11">
       <c r="B32" s="9">
         <v>41</v>
       </c>
@@ -6660,7 +6663,7 @@
       </c>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11">
       <c r="B33" s="9">
         <v>42</v>
       </c>
@@ -6689,7 +6692,7 @@
       </c>
       <c r="K33" s="10"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11">
       <c r="B34" s="9" t="s">
         <v>151</v>
       </c>
@@ -6718,7 +6721,7 @@
       </c>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11">
       <c r="B35" s="9">
         <v>60</v>
       </c>
@@ -6747,7 +6750,7 @@
       </c>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11">
       <c r="B36" s="9">
         <v>61</v>
       </c>
@@ -6776,7 +6779,7 @@
       </c>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11">
       <c r="B37" s="9">
         <v>62</v>
       </c>
@@ -6805,7 +6808,7 @@
       </c>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11">
       <c r="B38" s="9">
         <v>68</v>
       </c>
@@ -6834,7 +6837,7 @@
       </c>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11">
       <c r="B39" s="9">
         <v>69</v>
       </c>
@@ -6863,7 +6866,7 @@
       </c>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11">
       <c r="B40" s="9">
         <v>71</v>
       </c>
@@ -6892,7 +6895,7 @@
       </c>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11">
       <c r="B41" s="9">
         <v>72</v>
       </c>
@@ -6921,7 +6924,7 @@
       </c>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11">
       <c r="B42" s="9">
         <v>74</v>
       </c>
@@ -6950,7 +6953,7 @@
       </c>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11">
       <c r="B43" s="9">
         <v>75</v>
       </c>
@@ -6979,7 +6982,7 @@
       </c>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11">
       <c r="B44" s="9" t="s">
         <v>518</v>
       </c>
@@ -7023,7 +7026,7 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -7031,7 +7034,7 @@
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -7045,7 +7048,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -7057,7 +7060,7 @@
       </c>
       <c r="E3" s="45"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -7067,7 +7070,7 @@
       <c r="D4" s="68"/>
       <c r="E4" s="45"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -7079,7 +7082,7 @@
       </c>
       <c r="E5" s="45"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -7091,7 +7094,7 @@
       </c>
       <c r="E6" s="45"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -7105,7 +7108,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
         <v>126</v>
       </c>
@@ -7119,7 +7122,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
         <v>186</v>
       </c>
@@ -7133,7 +7136,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
         <v>400</v>
       </c>
@@ -7147,7 +7150,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5">
       <c r="B11" s="3" t="s">
         <v>348</v>
       </c>
@@ -7161,7 +7164,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5">
       <c r="B12" s="3" t="s">
         <v>351</v>
       </c>
@@ -7175,7 +7178,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5">
       <c r="B13" s="3" t="s">
         <v>353</v>
       </c>
@@ -7189,7 +7192,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5">
       <c r="B14" s="3" t="s">
         <v>357</v>
       </c>
@@ -7203,7 +7206,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5">
       <c r="B15" s="3">
         <v>18</v>
       </c>
@@ -7217,7 +7220,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5">
       <c r="B16" s="3">
         <v>21</v>
       </c>
@@ -7231,7 +7234,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <v>22</v>
       </c>
@@ -7245,7 +7248,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <v>23</v>
       </c>
@@ -7259,7 +7262,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <v>24</v>
       </c>
@@ -7273,7 +7276,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <v>31</v>
       </c>
@@ -7287,7 +7290,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <v>32</v>
       </c>
@@ -7301,7 +7304,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <v>33</v>
       </c>
@@ -7315,7 +7318,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <v>41</v>
       </c>
@@ -7329,7 +7332,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <v>42</v>
       </c>
@@ -7343,7 +7346,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <v>43</v>
       </c>
@@ -7357,7 +7360,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <v>58</v>
       </c>
@@ -7369,7 +7372,7 @@
       </c>
       <c r="E26" s="45"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5">
       <c r="B27" s="3">
         <v>59</v>
       </c>
@@ -7398,7 +7401,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -7414,7 +7417,7 @@
     <col min="18" max="48" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:42">
       <c r="I1" s="52" t="s">
         <v>441</v>
       </c>
@@ -7428,7 +7431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:42">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -7487,7 +7490,7 @@
       <c r="AO2" s="11"/>
       <c r="AP2" s="11"/>
     </row>
-    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:42">
       <c r="B3" s="55">
         <v>0</v>
       </c>
@@ -7544,7 +7547,7 @@
       <c r="AO3" s="11"/>
       <c r="AP3" s="11"/>
     </row>
-    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:42">
       <c r="B4" s="56">
         <v>1</v>
       </c>
@@ -7599,7 +7602,7 @@
       <c r="AO4" s="11"/>
       <c r="AP4" s="11"/>
     </row>
-    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:42">
       <c r="B5" s="56">
         <v>2</v>
       </c>
@@ -7656,7 +7659,7 @@
       <c r="AO5" s="11"/>
       <c r="AP5" s="11"/>
     </row>
-    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:42">
       <c r="B6" s="56">
         <v>3</v>
       </c>
@@ -7713,7 +7716,7 @@
       <c r="AO6" s="11"/>
       <c r="AP6" s="11"/>
     </row>
-    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:42">
       <c r="B7" s="56">
         <v>4</v>
       </c>
@@ -7770,7 +7773,7 @@
       <c r="AO7" s="11"/>
       <c r="AP7" s="11"/>
     </row>
-    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:42">
       <c r="B8" s="56">
         <v>5</v>
       </c>
@@ -7827,7 +7830,7 @@
       <c r="AO8" s="11"/>
       <c r="AP8" s="11"/>
     </row>
-    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:42">
       <c r="B9" s="56">
         <v>6</v>
       </c>
@@ -7884,7 +7887,7 @@
       <c r="AO9" s="11"/>
       <c r="AP9" s="11"/>
     </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:42">
       <c r="B10" s="56">
         <v>8</v>
       </c>
@@ -7941,7 +7944,7 @@
       <c r="AO10" s="11"/>
       <c r="AP10" s="11"/>
     </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:42">
       <c r="B11" s="56">
         <v>9</v>
       </c>
@@ -7998,7 +8001,7 @@
       <c r="AO11" s="11"/>
       <c r="AP11" s="11"/>
     </row>
-    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:42">
       <c r="B12" s="56">
         <v>10</v>
       </c>
@@ -8055,7 +8058,7 @@
       <c r="AO12" s="11"/>
       <c r="AP12" s="11"/>
     </row>
-    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:42">
       <c r="B13" s="56">
         <v>40</v>
       </c>
@@ -8112,7 +8115,7 @@
       <c r="AO13" s="11"/>
       <c r="AP13" s="11"/>
     </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:42">
       <c r="B14" s="56">
         <v>60</v>
       </c>
@@ -8169,7 +8172,7 @@
       <c r="AO14" s="11"/>
       <c r="AP14" s="11"/>
     </row>
-    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:42">
       <c r="B15" s="56">
         <v>61</v>
       </c>
@@ -8226,7 +8229,7 @@
       <c r="AO15" s="11"/>
       <c r="AP15" s="11"/>
     </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:42">
       <c r="B16" s="56">
         <v>62</v>
       </c>
@@ -8283,7 +8286,7 @@
       <c r="AO16" s="11"/>
       <c r="AP16" s="11"/>
     </row>
-    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:42">
       <c r="B17" s="56">
         <v>63</v>
       </c>
@@ -8340,7 +8343,7 @@
       <c r="AO17" s="11"/>
       <c r="AP17" s="11"/>
     </row>
-    <row r="18" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:42">
       <c r="B18" s="56">
         <v>64</v>
       </c>
@@ -8397,7 +8400,7 @@
       <c r="AO18" s="11"/>
       <c r="AP18" s="11"/>
     </row>
-    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:42">
       <c r="B19" s="56">
         <v>84</v>
       </c>
@@ -8454,7 +8457,7 @@
       <c r="AO19" s="11"/>
       <c r="AP19" s="11"/>
     </row>
-    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:42">
       <c r="B20" s="56">
         <v>104</v>
       </c>
@@ -8511,7 +8514,7 @@
       <c r="AO20" s="11"/>
       <c r="AP20" s="11"/>
     </row>
-    <row r="21" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:42">
       <c r="B21" s="56">
         <v>105</v>
       </c>
@@ -8568,7 +8571,7 @@
       <c r="AO21" s="11"/>
       <c r="AP21" s="11"/>
     </row>
-    <row r="22" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:42">
       <c r="B22" s="56">
         <v>106</v>
       </c>
@@ -8625,7 +8628,7 @@
       <c r="AO22" s="11"/>
       <c r="AP22" s="11"/>
     </row>
-    <row r="23" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:42">
       <c r="B23" s="56">
         <v>108</v>
       </c>
@@ -8682,7 +8685,7 @@
       <c r="AO23" s="11"/>
       <c r="AP23" s="11"/>
     </row>
-    <row r="24" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:42">
       <c r="B24" s="56">
         <v>109</v>
       </c>
@@ -8739,7 +8742,7 @@
       <c r="AO24" s="11"/>
       <c r="AP24" s="11"/>
     </row>
-    <row r="25" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:42">
       <c r="B25" s="56">
         <v>110</v>
       </c>
@@ -8796,7 +8799,7 @@
       <c r="AO25" s="11"/>
       <c r="AP25" s="11"/>
     </row>
-    <row r="26" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:42">
       <c r="B26" s="56">
         <v>112</v>
       </c>
@@ -8853,7 +8856,7 @@
       <c r="AO26" s="11"/>
       <c r="AP26" s="11"/>
     </row>
-    <row r="27" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:42">
       <c r="B27" s="56">
         <v>114</v>
       </c>
@@ -8910,7 +8913,7 @@
       <c r="AO27" s="11"/>
       <c r="AP27" s="11"/>
     </row>
-    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:42">
       <c r="B28" s="56">
         <v>118</v>
       </c>
@@ -8959,7 +8962,7 @@
       <c r="AO28" s="11"/>
       <c r="AP28" s="11"/>
     </row>
-    <row r="29" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:42">
       <c r="B29" s="56">
         <v>119</v>
       </c>
@@ -9008,7 +9011,7 @@
       <c r="AO29" s="11"/>
       <c r="AP29" s="11"/>
     </row>
-    <row r="30" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:42">
       <c r="E30">
         <f>SUM(E3:E29)</f>
         <v>120</v>
@@ -9048,7 +9051,7 @@
       <c r="AO30" s="11"/>
       <c r="AP30" s="11"/>
     </row>
-    <row r="31" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:42">
       <c r="I31" s="51"/>
       <c r="J31" s="51"/>
       <c r="K31" s="51"/>
@@ -9102,14 +9105,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -9120,7 +9123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -9131,7 +9134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -9140,7 +9143,7 @@
       </c>
       <c r="D4" s="68"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -9151,7 +9154,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -9162,7 +9165,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -9173,7 +9176,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" s="5" t="s">
         <v>421</v>
       </c>
@@ -9184,7 +9187,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4">
       <c r="B9" s="5" t="s">
         <v>424</v>
       </c>
@@ -9195,7 +9198,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4">
       <c r="B10" s="5" t="s">
         <v>427</v>
       </c>
@@ -9206,7 +9209,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="B11" s="3" t="s">
         <v>430</v>
       </c>
@@ -9217,7 +9220,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4">
       <c r="B12" s="3">
         <v>58</v>
       </c>
@@ -9228,7 +9231,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="B13" s="3">
         <v>59</v>
       </c>
@@ -9256,14 +9259,14 @@
       <selection activeCell="B2" sqref="B2:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" s="1" customFormat="1">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -9274,7 +9277,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" s="1" customFormat="1">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -9285,7 +9288,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" s="1" customFormat="1">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -9294,7 +9297,7 @@
       </c>
       <c r="D4" s="68"/>
     </row>
-    <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" s="1" customFormat="1">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -9305,7 +9308,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" s="1" customFormat="1">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -9316,7 +9319,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" s="1" customFormat="1">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -9327,7 +9330,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" s="1" customFormat="1">
       <c r="B8" s="5" t="s">
         <v>343</v>
       </c>
@@ -9338,7 +9341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" s="1" customFormat="1">
       <c r="B9" s="3" t="s">
         <v>339</v>
       </c>
@@ -9349,7 +9352,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" s="1" customFormat="1">
       <c r="B10" s="3" t="s">
         <v>340</v>
       </c>
@@ -9360,7 +9363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" s="1" customFormat="1">
       <c r="B11" s="3">
         <v>58</v>
       </c>
@@ -9371,7 +9374,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" s="1" customFormat="1">
       <c r="B12" s="3">
         <v>59</v>
       </c>
@@ -9399,7 +9402,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -9410,12 +9413,12 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18.75">
       <c r="A2" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="27" t="s">
         <v>139</v>
       </c>
@@ -9423,12 +9426,12 @@
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -9439,7 +9442,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
@@ -9450,7 +9453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
@@ -9459,7 +9462,7 @@
       </c>
       <c r="D8" s="68"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -9470,7 +9473,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -9481,7 +9484,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
@@ -9492,7 +9495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12" s="5" t="s">
         <v>126</v>
       </c>
@@ -9503,7 +9506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13" s="3" t="s">
         <v>127</v>
       </c>
@@ -9514,7 +9517,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14" s="3">
         <v>26</v>
       </c>
@@ -9525,7 +9528,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="B15" s="3">
         <v>27</v>
       </c>
@@ -9536,7 +9539,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="3">
         <v>28</v>
       </c>
@@ -9547,7 +9550,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="B17" s="3">
         <v>29</v>
       </c>
@@ -9558,7 +9561,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="B18" s="3" t="s">
         <v>129</v>
       </c>
@@ -9569,7 +9572,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="B19" s="3" t="s">
         <v>124</v>
       </c>
@@ -9580,7 +9583,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="B20" s="3" t="s">
         <v>130</v>
       </c>
@@ -9591,7 +9594,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="B21" s="3" t="s">
         <v>131</v>
       </c>
@@ -9602,7 +9605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="B22" s="3">
         <v>58</v>
       </c>
@@ -9613,7 +9616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="B23" s="3">
         <v>59</v>
       </c>
@@ -9624,17 +9627,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="18.75">
       <c r="A25" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
@@ -9645,7 +9648,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="B28" s="5" t="s">
         <v>19</v>
       </c>
@@ -9656,7 +9659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="B29" s="5" t="s">
         <v>20</v>
       </c>
@@ -9665,7 +9668,7 @@
       </c>
       <c r="D29" s="68"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
@@ -9676,7 +9679,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="B31" s="5" t="s">
         <v>22</v>
       </c>
@@ -9687,7 +9690,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="B32" s="5" t="s">
         <v>23</v>
       </c>
@@ -9698,7 +9701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4">
       <c r="B33" s="5" t="s">
         <v>126</v>
       </c>
@@ -9709,7 +9712,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4">
       <c r="B34" s="5" t="s">
         <v>186</v>
       </c>
@@ -9720,7 +9723,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4">
       <c r="B35" s="5" t="s">
         <v>187</v>
       </c>
@@ -9731,7 +9734,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4">
       <c r="B36" s="3" t="s">
         <v>188</v>
       </c>
@@ -9742,7 +9745,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4">
       <c r="B37" s="3" t="s">
         <v>189</v>
       </c>
@@ -9753,7 +9756,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4">
       <c r="B38" s="3" t="s">
         <v>190</v>
       </c>
@@ -9764,7 +9767,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4">
       <c r="B39" s="3">
         <v>51</v>
       </c>
@@ -9775,7 +9778,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4">
       <c r="B40" s="3">
         <v>52</v>
       </c>
@@ -9786,7 +9789,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4">
       <c r="B41" s="3">
         <v>53</v>
       </c>
@@ -9797,7 +9800,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4">
       <c r="B42" s="3">
         <v>54</v>
       </c>
@@ -9808,7 +9811,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4">
       <c r="B43" s="3">
         <v>55</v>
       </c>
@@ -9819,7 +9822,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4">
       <c r="B44" s="3" t="s">
         <v>201</v>
       </c>
@@ -9830,7 +9833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4">
       <c r="B45" s="3">
         <v>58</v>
       </c>
@@ -9841,7 +9844,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4">
       <c r="B46" s="3">
         <v>59</v>
       </c>
@@ -9852,17 +9855,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4">
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4">
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4">
       <c r="C49" s="1" t="s">
         <v>140</v>
       </c>
@@ -9870,17 +9873,17 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4">
       <c r="D50" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4">
       <c r="D51" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4">
       <c r="D52" s="1" t="s">
         <v>144</v>
       </c>
@@ -9904,17 +9907,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="158.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:3" ht="60">
       <c r="C2" s="24" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:3">
       <c r="C5" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
Ready to update EventHandler from MyAlphaRobot
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="715">
   <si>
     <t>Offset</t>
   </si>
@@ -1903,7 +1903,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1924,7 +1924,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1935,7 +1935,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1952,7 +1952,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1963,7 +1963,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1979,7 +1979,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1996,7 +1996,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -2029,7 +2029,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2039,7 +2039,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2375,16 +2375,20 @@
   <si>
     <t>A9 9A 0C 93 00 01 05 01 00 00 00 00 00 00 A6 ED</t>
   </si>
+  <si>
+    <t>Event Header as input of 0x93</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2392,7 +2396,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2402,7 +2406,7 @@
       <u/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2412,19 +2416,19 @@
       <u/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2432,7 +2436,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2440,7 +2444,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2498,7 +2502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2686,6 +2690,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2996,14 +3003,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="F50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -3017,7 +3024,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3025,7 +3032,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -3036,7 +3043,7 @@
       <c r="G3" s="13"/>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -3048,7 +3055,7 @@
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -3060,7 +3067,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -3076,7 +3083,7 @@
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -3085,7 +3092,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
@@ -3094,7 +3101,7 @@
       </c>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
@@ -3103,7 +3110,7 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="12" spans="2:14">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
@@ -3132,7 +3139,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
@@ -3161,7 +3168,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
@@ -3190,7 +3197,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
@@ -3219,7 +3226,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="2:14">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
@@ -3242,7 +3249,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>126</v>
       </c>
@@ -3265,7 +3272,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>186</v>
       </c>
@@ -3288,7 +3295,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="45">
+    <row r="19" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>53</v>
       </c>
@@ -3317,7 +3324,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="2:13">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>205</v>
       </c>
@@ -3344,7 +3351,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="2:13">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>415</v>
       </c>
@@ -3369,7 +3376,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="22" spans="2:13">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>432</v>
       </c>
@@ -3394,7 +3401,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>436</v>
       </c>
@@ -3422,7 +3429,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="24" spans="2:13">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>501</v>
       </c>
@@ -3454,7 +3461,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="2:13">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
         <v>10</v>
       </c>
@@ -3481,7 +3488,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="26" spans="2:13">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
         <v>11</v>
       </c>
@@ -3508,7 +3515,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="2:13">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
         <v>12</v>
       </c>
@@ -3535,7 +3542,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="2:13">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
         <v>13</v>
       </c>
@@ -3562,7 +3569,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="29" spans="2:13">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <v>14</v>
       </c>
@@ -3589,7 +3596,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="30" spans="2:13">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>15</v>
       </c>
@@ -3610,7 +3617,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="2:13">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
         <v>16</v>
       </c>
@@ -3631,7 +3638,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="2:13">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
         <v>18</v>
       </c>
@@ -3656,7 +3663,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="2:11">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <v>21</v>
       </c>
@@ -3683,7 +3690,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="2:11">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
         <v>22</v>
       </c>
@@ -3710,7 +3717,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="30">
+    <row r="35" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
         <v>23</v>
       </c>
@@ -3737,7 +3744,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="36" spans="2:11">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
         <v>24</v>
       </c>
@@ -3764,7 +3771,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="2:11">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
         <v>31</v>
       </c>
@@ -3793,7 +3800,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="2:11">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="3">
         <v>32</v>
       </c>
@@ -3820,7 +3827,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="2:11">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
         <v>33</v>
       </c>
@@ -3849,7 +3856,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="2:11">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
         <v>34</v>
       </c>
@@ -3876,7 +3883,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="2:11">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
         <v>35</v>
       </c>
@@ -3903,7 +3910,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="2:11">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="3">
         <v>36</v>
       </c>
@@ -3932,7 +3939,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="43" spans="2:11">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
         <v>41</v>
       </c>
@@ -3959,7 +3966,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="2:11">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
         <v>42</v>
       </c>
@@ -3986,7 +3993,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="2:11">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>151</v>
       </c>
@@ -4013,7 +4020,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="2:11">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
         <v>60</v>
       </c>
@@ -4040,7 +4047,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="47" spans="2:11">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="3">
         <v>61</v>
       </c>
@@ -4067,7 +4074,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="2:11">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="3">
         <v>62</v>
       </c>
@@ -4094,7 +4101,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="2:11" s="38" customFormat="1">
+    <row r="49" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="35">
         <v>63</v>
       </c>
@@ -4121,7 +4128,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="2:11">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="3">
         <v>68</v>
       </c>
@@ -4148,7 +4155,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="51" spans="2:11">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="3">
         <v>69</v>
       </c>
@@ -4171,7 +4178,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="2:11">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="3">
         <v>71</v>
       </c>
@@ -4196,7 +4203,7 @@
       </c>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="2:11">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="3">
         <v>72</v>
       </c>
@@ -4217,7 +4224,7 @@
       </c>
       <c r="K53" s="4"/>
     </row>
-    <row r="54" spans="2:11" ht="30">
+    <row r="54" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B54" s="3">
         <v>74</v>
       </c>
@@ -4244,7 +4251,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="2:11">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="3">
         <v>75</v>
       </c>
@@ -4271,7 +4278,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="2:11">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -4282,7 +4289,7 @@
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
     </row>
-    <row r="57" spans="2:11">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" s="3">
         <v>81</v>
       </c>
@@ -4307,7 +4314,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="58" spans="2:11">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="3">
         <v>82</v>
       </c>
@@ -4332,7 +4339,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="59" spans="2:11">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -4343,7 +4350,7 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
     </row>
-    <row r="60" spans="2:11">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="3">
         <v>91</v>
       </c>
@@ -4366,7 +4373,7 @@
       </c>
       <c r="K60" s="4"/>
     </row>
-    <row r="61" spans="2:11">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" s="3">
         <v>92</v>
       </c>
@@ -4387,7 +4394,7 @@
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
     </row>
-    <row r="62" spans="2:11">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" s="3">
         <v>93</v>
       </c>
@@ -4408,7 +4415,7 @@
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
     </row>
-    <row r="63" spans="2:11">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" s="3">
         <v>94</v>
       </c>
@@ -4427,7 +4434,7 @@
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
     </row>
-    <row r="64" spans="2:11">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
@@ -4438,7 +4445,7 @@
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
     </row>
-    <row r="65" spans="2:11" s="38" customFormat="1">
+    <row r="65" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="35" t="s">
         <v>80</v>
       </c>
@@ -4467,7 +4474,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="66" spans="2:11" s="38" customFormat="1">
+    <row r="66" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="35" t="s">
         <v>85</v>
       </c>
@@ -4494,7 +4501,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="2:11">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
         <v>518</v>
       </c>
@@ -4536,7 +4543,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
@@ -4546,7 +4553,7 @@
     <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="40" t="s">
         <v>218</v>
       </c>
@@ -4573,7 +4580,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="39" t="s">
         <v>226</v>
       </c>
@@ -4599,7 +4606,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>217</v>
       </c>
@@ -4625,7 +4632,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>327</v>
       </c>
@@ -4651,7 +4658,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>330</v>
       </c>
@@ -4677,7 +4684,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>215</v>
       </c>
@@ -4703,7 +4710,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>216</v>
       </c>
@@ -4729,7 +4736,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>278</v>
       </c>
@@ -4749,7 +4756,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>279</v>
       </c>
@@ -4769,7 +4776,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>277</v>
       </c>
@@ -4789,7 +4796,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>285</v>
       </c>
@@ -4809,7 +4816,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>256</v>
       </c>
@@ -4826,7 +4833,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>257</v>
       </c>
@@ -4846,7 +4853,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>227</v>
       </c>
@@ -4869,7 +4876,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>230</v>
       </c>
@@ -4892,7 +4899,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>234</v>
       </c>
@@ -4915,7 +4922,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>241</v>
       </c>
@@ -4938,7 +4945,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>319</v>
       </c>
@@ -4958,7 +4965,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>320</v>
       </c>
@@ -4978,7 +4985,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>321</v>
       </c>
@@ -4998,7 +5005,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>235</v>
       </c>
@@ -5021,7 +5028,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>236</v>
       </c>
@@ -5044,7 +5051,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>240</v>
       </c>
@@ -5067,7 +5074,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>244</v>
       </c>
@@ -5090,7 +5097,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>245</v>
       </c>
@@ -5113,7 +5120,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>246</v>
       </c>
@@ -5136,7 +5143,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>262</v>
       </c>
@@ -5156,7 +5163,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>263</v>
       </c>
@@ -5176,7 +5183,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>265</v>
       </c>
@@ -5196,7 +5203,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>274</v>
       </c>
@@ -5219,7 +5226,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>250</v>
       </c>
@@ -5242,7 +5249,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>267</v>
       </c>
@@ -5262,7 +5269,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>268</v>
       </c>
@@ -5282,7 +5289,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>272</v>
       </c>
@@ -5314,25 +5321,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D40"/>
+  <dimension ref="B2:D55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -5343,27 +5350,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="69" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="68"/>
-    </row>
-    <row r="6" spans="2:4">
+      <c r="D5" s="69"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
@@ -5374,7 +5381,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
@@ -5385,7 +5392,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>649</v>
       </c>
@@ -5396,7 +5403,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>653</v>
       </c>
@@ -5407,7 +5414,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>660</v>
       </c>
@@ -5418,18 +5425,18 @@
         <v>670</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>665</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>658</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="68" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>666</v>
       </c>
@@ -5440,7 +5447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>14</v>
       </c>
@@ -5451,7 +5458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>15</v>
       </c>
@@ -5462,32 +5469,32 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="68" t="s">
+      <c r="D17" s="69" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="68"/>
-    </row>
-    <row r="19" spans="2:4">
+      <c r="D18" s="69"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
@@ -5498,7 +5505,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>648</v>
       </c>
@@ -5509,7 +5516,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>649</v>
       </c>
@@ -5520,7 +5527,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>650</v>
       </c>
@@ -5531,7 +5538,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>700</v>
       </c>
@@ -5542,7 +5549,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>702</v>
       </c>
@@ -5553,7 +5560,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="66" t="s">
         <v>705</v>
       </c>
@@ -5564,7 +5571,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="66" t="s">
         <v>706</v>
       </c>
@@ -5575,7 +5582,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="45">
         <v>126</v>
       </c>
@@ -5586,7 +5593,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="45">
         <v>127</v>
       </c>
@@ -5597,12 +5604,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="45">
         <v>0</v>
       </c>
@@ -5613,7 +5620,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="45">
         <v>1</v>
       </c>
@@ -5624,7 +5631,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="45">
         <v>2</v>
       </c>
@@ -5635,7 +5642,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="45">
         <v>3</v>
       </c>
@@ -5646,7 +5653,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="45">
         <v>4</v>
       </c>
@@ -5657,7 +5664,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="45">
         <v>5</v>
       </c>
@@ -5668,7 +5675,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="67" t="s">
         <v>680</v>
       </c>
@@ -5679,7 +5686,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="45">
         <v>8</v>
       </c>
@@ -5690,7 +5697,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="45">
         <v>9</v>
       </c>
@@ -5701,7 +5708,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="67" t="s">
         <v>684</v>
       </c>
@@ -5712,10 +5719,146 @@
         <v>694</v>
       </c>
     </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" s="69" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="69"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="D47" s="68" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="D48" s="68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="D49" s="68" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>637</v>
+      </c>
+      <c r="D50" s="68" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="D51" s="68" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="D52" s="68" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="3">
+        <v>14</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="68" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="3">
+        <v>15</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="68" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D45:D46"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5731,7 +5874,7 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="50"/>
     <col min="3" max="3" width="38.42578125" style="50" bestFit="1" customWidth="1"/>
@@ -5741,7 +5884,7 @@
     <col min="10" max="16384" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D1" s="50" t="s">
         <v>607</v>
       </c>
@@ -5764,7 +5907,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="60" t="s">
         <v>20</v>
       </c>
@@ -5793,7 +5936,7 @@
       </c>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="60" t="s">
         <v>21</v>
       </c>
@@ -5822,7 +5965,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="60" t="s">
         <v>22</v>
       </c>
@@ -5851,7 +5994,7 @@
       </c>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
         <v>23</v>
       </c>
@@ -5880,7 +6023,7 @@
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="2:11">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="60" t="s">
         <v>126</v>
       </c>
@@ -5909,7 +6052,7 @@
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="60" t="s">
         <v>186</v>
       </c>
@@ -5938,7 +6081,7 @@
       </c>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="60" t="s">
         <v>53</v>
       </c>
@@ -5967,7 +6110,7 @@
       </c>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="60" t="s">
         <v>205</v>
       </c>
@@ -5996,7 +6139,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="60" t="s">
         <v>415</v>
       </c>
@@ -6025,7 +6168,7 @@
       </c>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="60" t="s">
         <v>432</v>
       </c>
@@ -6054,7 +6197,7 @@
       </c>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="2:11">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="60" t="s">
         <v>436</v>
       </c>
@@ -6083,7 +6226,7 @@
       </c>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="60" t="s">
         <v>501</v>
       </c>
@@ -6112,7 +6255,7 @@
       </c>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="60">
         <v>10</v>
       </c>
@@ -6141,7 +6284,7 @@
       </c>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="60">
         <v>11</v>
       </c>
@@ -6170,7 +6313,7 @@
       </c>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="60">
         <v>12</v>
       </c>
@@ -6199,7 +6342,7 @@
       </c>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="2:11">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="60">
         <v>13</v>
       </c>
@@ -6228,7 +6371,7 @@
       </c>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="2:11">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="9">
         <v>14</v>
       </c>
@@ -6257,7 +6400,7 @@
       </c>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="9">
         <v>15</v>
       </c>
@@ -6286,7 +6429,7 @@
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="9">
         <v>16</v>
       </c>
@@ -6315,7 +6458,7 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="9">
         <v>18</v>
       </c>
@@ -6344,7 +6487,7 @@
       </c>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="2:11">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="9">
         <v>21</v>
       </c>
@@ -6373,7 +6516,7 @@
       </c>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="2:11">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="9">
         <v>22</v>
       </c>
@@ -6402,7 +6545,7 @@
       </c>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="2:11">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="9">
         <v>23</v>
       </c>
@@ -6431,7 +6574,7 @@
       </c>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="9">
         <v>24</v>
       </c>
@@ -6460,7 +6603,7 @@
       </c>
       <c r="K25" s="10"/>
     </row>
-    <row r="26" spans="2:11">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="9">
         <v>31</v>
       </c>
@@ -6489,7 +6632,7 @@
       </c>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="2:11">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="9">
         <v>32</v>
       </c>
@@ -6518,7 +6661,7 @@
       </c>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="2:11">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="9">
         <v>33</v>
       </c>
@@ -6547,7 +6690,7 @@
       </c>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="2:11">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="9">
         <v>34</v>
       </c>
@@ -6576,7 +6719,7 @@
       </c>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="2:11">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="9">
         <v>35</v>
       </c>
@@ -6605,7 +6748,7 @@
       </c>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="2:11">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="9">
         <v>36</v>
       </c>
@@ -6634,7 +6777,7 @@
       </c>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="2:11">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="9">
         <v>41</v>
       </c>
@@ -6663,7 +6806,7 @@
       </c>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="2:11">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="9">
         <v>42</v>
       </c>
@@ -6692,7 +6835,7 @@
       </c>
       <c r="K33" s="10"/>
     </row>
-    <row r="34" spans="2:11">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
         <v>151</v>
       </c>
@@ -6721,7 +6864,7 @@
       </c>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="2:11">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="9">
         <v>60</v>
       </c>
@@ -6750,7 +6893,7 @@
       </c>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="2:11">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="9">
         <v>61</v>
       </c>
@@ -6779,7 +6922,7 @@
       </c>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="2:11">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="9">
         <v>62</v>
       </c>
@@ -6808,7 +6951,7 @@
       </c>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="2:11">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="9">
         <v>68</v>
       </c>
@@ -6837,7 +6980,7 @@
       </c>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="2:11">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="9">
         <v>69</v>
       </c>
@@ -6866,7 +7009,7 @@
       </c>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="2:11">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="9">
         <v>71</v>
       </c>
@@ -6895,7 +7038,7 @@
       </c>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="2:11">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="9">
         <v>72</v>
       </c>
@@ -6924,7 +7067,7 @@
       </c>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="2:11">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="9">
         <v>74</v>
       </c>
@@ -6953,7 +7096,7 @@
       </c>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="2:11">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="9">
         <v>75</v>
       </c>
@@ -6982,7 +7125,7 @@
       </c>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="2:11">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="9" t="s">
         <v>518</v>
       </c>
@@ -7026,7 +7169,7 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -7034,7 +7177,7 @@
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -7048,29 +7191,29 @@
         <v>382</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="69" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="45"/>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="69"/>
       <c r="E4" s="45"/>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -7082,7 +7225,7 @@
       </c>
       <c r="E5" s="45"/>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -7094,7 +7237,7 @@
       </c>
       <c r="E6" s="45"/>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -7108,7 +7251,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>126</v>
       </c>
@@ -7122,7 +7265,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>186</v>
       </c>
@@ -7136,7 +7279,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>400</v>
       </c>
@@ -7150,7 +7293,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>348</v>
       </c>
@@ -7164,7 +7307,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>351</v>
       </c>
@@ -7178,7 +7321,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>353</v>
       </c>
@@ -7192,7 +7335,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>357</v>
       </c>
@@ -7206,7 +7349,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>18</v>
       </c>
@@ -7220,7 +7363,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>21</v>
       </c>
@@ -7234,7 +7377,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>22</v>
       </c>
@@ -7248,7 +7391,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>23</v>
       </c>
@@ -7262,7 +7405,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>24</v>
       </c>
@@ -7276,7 +7419,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>31</v>
       </c>
@@ -7290,7 +7433,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>32</v>
       </c>
@@ -7304,7 +7447,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>33</v>
       </c>
@@ -7318,7 +7461,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>41</v>
       </c>
@@ -7332,7 +7475,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <v>42</v>
       </c>
@@ -7346,7 +7489,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <v>43</v>
       </c>
@@ -7360,7 +7503,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>58</v>
       </c>
@@ -7372,7 +7515,7 @@
       </c>
       <c r="E26" s="45"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <v>59</v>
       </c>
@@ -7401,7 +7544,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -7417,7 +7560,7 @@
     <col min="18" max="48" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42">
+    <row r="1" spans="2:42" x14ac:dyDescent="0.25">
       <c r="I1" s="52" t="s">
         <v>441</v>
       </c>
@@ -7431,7 +7574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:42">
+    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -7490,14 +7633,14 @@
       <c r="AO2" s="11"/>
       <c r="AP2" s="11"/>
     </row>
-    <row r="3" spans="2:42">
+    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B3" s="55">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="69" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="48">
@@ -7547,14 +7690,14 @@
       <c r="AO3" s="11"/>
       <c r="AP3" s="11"/>
     </row>
-    <row r="4" spans="2:42">
+    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B4" s="56">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="69"/>
       <c r="E4" s="48">
         <v>1</v>
       </c>
@@ -7602,7 +7745,7 @@
       <c r="AO4" s="11"/>
       <c r="AP4" s="11"/>
     </row>
-    <row r="5" spans="2:42">
+    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B5" s="56">
         <v>2</v>
       </c>
@@ -7659,7 +7802,7 @@
       <c r="AO5" s="11"/>
       <c r="AP5" s="11"/>
     </row>
-    <row r="6" spans="2:42">
+    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B6" s="56">
         <v>3</v>
       </c>
@@ -7716,7 +7859,7 @@
       <c r="AO6" s="11"/>
       <c r="AP6" s="11"/>
     </row>
-    <row r="7" spans="2:42">
+    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B7" s="56">
         <v>4</v>
       </c>
@@ -7773,7 +7916,7 @@
       <c r="AO7" s="11"/>
       <c r="AP7" s="11"/>
     </row>
-    <row r="8" spans="2:42">
+    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B8" s="56">
         <v>5</v>
       </c>
@@ -7830,7 +7973,7 @@
       <c r="AO8" s="11"/>
       <c r="AP8" s="11"/>
     </row>
-    <row r="9" spans="2:42">
+    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B9" s="56">
         <v>6</v>
       </c>
@@ -7887,7 +8030,7 @@
       <c r="AO9" s="11"/>
       <c r="AP9" s="11"/>
     </row>
-    <row r="10" spans="2:42">
+    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B10" s="56">
         <v>8</v>
       </c>
@@ -7944,7 +8087,7 @@
       <c r="AO10" s="11"/>
       <c r="AP10" s="11"/>
     </row>
-    <row r="11" spans="2:42">
+    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B11" s="56">
         <v>9</v>
       </c>
@@ -8001,7 +8144,7 @@
       <c r="AO11" s="11"/>
       <c r="AP11" s="11"/>
     </row>
-    <row r="12" spans="2:42">
+    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B12" s="56">
         <v>10</v>
       </c>
@@ -8058,7 +8201,7 @@
       <c r="AO12" s="11"/>
       <c r="AP12" s="11"/>
     </row>
-    <row r="13" spans="2:42">
+    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B13" s="56">
         <v>40</v>
       </c>
@@ -8115,7 +8258,7 @@
       <c r="AO13" s="11"/>
       <c r="AP13" s="11"/>
     </row>
-    <row r="14" spans="2:42">
+    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B14" s="56">
         <v>60</v>
       </c>
@@ -8172,7 +8315,7 @@
       <c r="AO14" s="11"/>
       <c r="AP14" s="11"/>
     </row>
-    <row r="15" spans="2:42">
+    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B15" s="56">
         <v>61</v>
       </c>
@@ -8229,7 +8372,7 @@
       <c r="AO15" s="11"/>
       <c r="AP15" s="11"/>
     </row>
-    <row r="16" spans="2:42">
+    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B16" s="56">
         <v>62</v>
       </c>
@@ -8286,7 +8429,7 @@
       <c r="AO16" s="11"/>
       <c r="AP16" s="11"/>
     </row>
-    <row r="17" spans="2:42">
+    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B17" s="56">
         <v>63</v>
       </c>
@@ -8343,7 +8486,7 @@
       <c r="AO17" s="11"/>
       <c r="AP17" s="11"/>
     </row>
-    <row r="18" spans="2:42">
+    <row r="18" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B18" s="56">
         <v>64</v>
       </c>
@@ -8400,7 +8543,7 @@
       <c r="AO18" s="11"/>
       <c r="AP18" s="11"/>
     </row>
-    <row r="19" spans="2:42">
+    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B19" s="56">
         <v>84</v>
       </c>
@@ -8457,7 +8600,7 @@
       <c r="AO19" s="11"/>
       <c r="AP19" s="11"/>
     </row>
-    <row r="20" spans="2:42">
+    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B20" s="56">
         <v>104</v>
       </c>
@@ -8514,7 +8657,7 @@
       <c r="AO20" s="11"/>
       <c r="AP20" s="11"/>
     </row>
-    <row r="21" spans="2:42">
+    <row r="21" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B21" s="56">
         <v>105</v>
       </c>
@@ -8571,7 +8714,7 @@
       <c r="AO21" s="11"/>
       <c r="AP21" s="11"/>
     </row>
-    <row r="22" spans="2:42">
+    <row r="22" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B22" s="56">
         <v>106</v>
       </c>
@@ -8628,7 +8771,7 @@
       <c r="AO22" s="11"/>
       <c r="AP22" s="11"/>
     </row>
-    <row r="23" spans="2:42">
+    <row r="23" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B23" s="56">
         <v>108</v>
       </c>
@@ -8685,7 +8828,7 @@
       <c r="AO23" s="11"/>
       <c r="AP23" s="11"/>
     </row>
-    <row r="24" spans="2:42">
+    <row r="24" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B24" s="56">
         <v>109</v>
       </c>
@@ -8742,7 +8885,7 @@
       <c r="AO24" s="11"/>
       <c r="AP24" s="11"/>
     </row>
-    <row r="25" spans="2:42">
+    <row r="25" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B25" s="56">
         <v>110</v>
       </c>
@@ -8799,7 +8942,7 @@
       <c r="AO25" s="11"/>
       <c r="AP25" s="11"/>
     </row>
-    <row r="26" spans="2:42">
+    <row r="26" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B26" s="56">
         <v>112</v>
       </c>
@@ -8856,7 +8999,7 @@
       <c r="AO26" s="11"/>
       <c r="AP26" s="11"/>
     </row>
-    <row r="27" spans="2:42">
+    <row r="27" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B27" s="56">
         <v>114</v>
       </c>
@@ -8913,7 +9056,7 @@
       <c r="AO27" s="11"/>
       <c r="AP27" s="11"/>
     </row>
-    <row r="28" spans="2:42">
+    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B28" s="56">
         <v>118</v>
       </c>
@@ -8962,7 +9105,7 @@
       <c r="AO28" s="11"/>
       <c r="AP28" s="11"/>
     </row>
-    <row r="29" spans="2:42">
+    <row r="29" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B29" s="56">
         <v>119</v>
       </c>
@@ -9011,7 +9154,7 @@
       <c r="AO29" s="11"/>
       <c r="AP29" s="11"/>
     </row>
-    <row r="30" spans="2:42">
+    <row r="30" spans="2:42" x14ac:dyDescent="0.25">
       <c r="E30">
         <f>SUM(E3:E29)</f>
         <v>120</v>
@@ -9051,7 +9194,7 @@
       <c r="AO30" s="11"/>
       <c r="AP30" s="11"/>
     </row>
-    <row r="31" spans="2:42">
+    <row r="31" spans="2:42" x14ac:dyDescent="0.25">
       <c r="I31" s="51"/>
       <c r="J31" s="51"/>
       <c r="K31" s="51"/>
@@ -9105,14 +9248,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -9123,27 +9266,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="69" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
-    </row>
-    <row r="5" spans="2:4">
+      <c r="D4" s="69"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -9154,7 +9297,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -9165,7 +9308,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -9176,7 +9319,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>421</v>
       </c>
@@ -9187,7 +9330,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>424</v>
       </c>
@@ -9198,7 +9341,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>427</v>
       </c>
@@ -9209,7 +9352,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>430</v>
       </c>
@@ -9220,7 +9363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>58</v>
       </c>
@@ -9231,7 +9374,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>59</v>
       </c>
@@ -9259,14 +9402,14 @@
       <selection activeCell="B2" sqref="B2:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="1" customFormat="1">
+    <row r="2" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -9277,27 +9420,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" s="1" customFormat="1">
+    <row r="3" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="69" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="1" customFormat="1">
+    <row r="4" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
-    </row>
-    <row r="5" spans="2:4" s="1" customFormat="1">
+      <c r="D4" s="69"/>
+    </row>
+    <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -9308,7 +9451,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:4" s="1" customFormat="1">
+    <row r="6" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -9319,7 +9462,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="1" customFormat="1">
+    <row r="7" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -9330,7 +9473,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="2:4" s="1" customFormat="1">
+    <row r="8" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>343</v>
       </c>
@@ -9341,7 +9484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="1" customFormat="1">
+    <row r="9" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>339</v>
       </c>
@@ -9352,7 +9495,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="10" spans="2:4" s="1" customFormat="1">
+    <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>340</v>
       </c>
@@ -9363,7 +9506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" s="1" customFormat="1">
+    <row r="11" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>58</v>
       </c>
@@ -9374,7 +9517,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:4" s="1" customFormat="1">
+    <row r="12" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>59</v>
       </c>
@@ -9402,7 +9545,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -9413,12 +9556,12 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="18.75">
+    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>139</v>
       </c>
@@ -9426,12 +9569,12 @@
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -9442,27 +9585,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="69" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="68"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="69"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -9473,7 +9616,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -9484,7 +9627,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
@@ -9495,7 +9638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>126</v>
       </c>
@@ -9506,7 +9649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>127</v>
       </c>
@@ -9517,7 +9660,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>26</v>
       </c>
@@ -9528,7 +9671,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>27</v>
       </c>
@@ -9539,7 +9682,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>28</v>
       </c>
@@ -9550,7 +9693,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>29</v>
       </c>
@@ -9561,7 +9704,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>129</v>
       </c>
@@ -9572,7 +9715,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>124</v>
       </c>
@@ -9583,7 +9726,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>130</v>
       </c>
@@ -9594,7 +9737,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>131</v>
       </c>
@@ -9605,7 +9748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>58</v>
       </c>
@@ -9616,7 +9759,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>59</v>
       </c>
@@ -9627,17 +9770,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" ht="18.75">
+    <row r="25" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
@@ -9648,27 +9791,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="68" t="s">
+      <c r="D28" s="69" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="68"/>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="D29" s="69"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
@@ -9679,7 +9822,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>22</v>
       </c>
@@ -9690,7 +9833,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>23</v>
       </c>
@@ -9701,7 +9844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>126</v>
       </c>
@@ -9712,7 +9855,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>186</v>
       </c>
@@ -9723,7 +9866,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>187</v>
       </c>
@@ -9734,7 +9877,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>188</v>
       </c>
@@ -9745,7 +9888,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>189</v>
       </c>
@@ -9756,7 +9899,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>190</v>
       </c>
@@ -9767,7 +9910,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
         <v>51</v>
       </c>
@@ -9778,7 +9921,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
         <v>52</v>
       </c>
@@ -9789,7 +9932,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
         <v>53</v>
       </c>
@@ -9800,7 +9943,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="2:4">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="3">
         <v>54</v>
       </c>
@@ -9811,7 +9954,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
         <v>55</v>
       </c>
@@ -9822,7 +9965,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>201</v>
       </c>
@@ -9833,7 +9976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
         <v>58</v>
       </c>
@@ -9844,7 +9987,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
         <v>59</v>
       </c>
@@ -9855,17 +9998,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
     </row>
-    <row r="49" spans="3:4">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>140</v>
       </c>
@@ -9873,17 +10016,17 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="3:4">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D50" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="3:4">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D51" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="3:4">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D52" s="1" t="s">
         <v>144</v>
       </c>
@@ -9907,17 +10050,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="158.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:3" ht="60">
+    <row r="2" spans="3:3" ht="63" x14ac:dyDescent="0.25">
       <c r="C2" s="24" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="3:3">
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
2.1.99.7 - Add USB-TTL mode
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="721">
   <si>
     <t>Offset</t>
   </si>
@@ -2389,10 +2389,13 @@
     <t>USB-TTL mode</t>
   </si>
   <si>
-    <t>A9 9A 03 00 01 04 ED</t>
-  </si>
-  <si>
     <t>{0=USER, 1=DEV} {0=Robot,1=SSB}</t>
+  </si>
+  <si>
+    <t>A9 9A 04 07 00 01 0C ED</t>
+  </si>
+  <si>
+    <t>A9 9A 04 07 01 01 0D ED</t>
   </si>
 </sst>
 </file>
@@ -3022,7 +3025,7 @@
   <dimension ref="B2:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
@@ -3324,13 +3327,13 @@
         <v>57</v>
       </c>
       <c r="E19" s="69" t="s">
+        <v>718</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>719</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>718</v>
-      </c>
       <c r="G19" s="4" t="s">
-        <v>156</v>
+        <v>720</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Update information in Info.xlsx Update default_log_level
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -3025,10 +3025,10 @@
   <dimension ref="B2:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3324,7 +3324,7 @@
         <v>717</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="E19" s="69" t="s">
         <v>718</v>

</xml_diff>

<commit_message>
v2.1.99.9 - update configuration file, new command for sub-system board.
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="769">
   <si>
     <t>Offset</t>
   </si>
@@ -1903,7 +1903,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1924,7 +1924,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1935,7 +1935,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1952,7 +1952,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1963,7 +1963,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1979,7 +1979,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1996,7 +1996,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -2029,7 +2029,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2039,7 +2039,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2554,10 +2554,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>36~37</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>38~39</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -2584,17 +2580,23 @@
   <si>
     <t>Enable PSX Button (false)</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>No event handle in ms (100)</t>
+  </si>
+  <si>
+    <t>RC_PSX_NO_EVENT_MS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2602,7 +2604,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2612,7 +2614,7 @@
       <u/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2622,19 +2624,19 @@
       <u/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2642,7 +2644,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2650,7 +2652,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2714,7 +2716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2921,6 +2923,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3234,7 +3239,7 @@
       <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -3248,7 +3253,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3256,7 +3261,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -3267,7 +3272,7 @@
       <c r="G3" s="13"/>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -3279,7 +3284,7 @@
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -3291,7 +3296,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -3307,7 +3312,7 @@
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14">
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -3316,7 +3321,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14">
       <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
@@ -3325,7 +3330,7 @@
       </c>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14">
       <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
@@ -3334,7 +3339,7 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14">
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
@@ -3363,7 +3368,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14">
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
@@ -3392,7 +3397,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
@@ -3421,7 +3426,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14">
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
@@ -3450,7 +3455,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
@@ -3473,7 +3478,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13">
       <c r="B17" s="5" t="s">
         <v>126</v>
       </c>
@@ -3496,7 +3501,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13">
       <c r="B18" s="5" t="s">
         <v>186</v>
       </c>
@@ -3519,7 +3524,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13">
       <c r="B19" s="5" t="s">
         <v>400</v>
       </c>
@@ -3548,7 +3553,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="45">
       <c r="B20" s="5" t="s">
         <v>53</v>
       </c>
@@ -3577,7 +3582,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13">
       <c r="B21" s="5" t="s">
         <v>205</v>
       </c>
@@ -3604,7 +3609,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13">
       <c r="B22" s="5" t="s">
         <v>415</v>
       </c>
@@ -3629,7 +3634,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13">
       <c r="B23" s="5" t="s">
         <v>432</v>
       </c>
@@ -3654,7 +3659,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13">
       <c r="B24" s="5" t="s">
         <v>436</v>
       </c>
@@ -3682,7 +3687,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13">
       <c r="B25" s="5" t="s">
         <v>501</v>
       </c>
@@ -3714,7 +3719,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13">
       <c r="B26" s="5">
         <v>10</v>
       </c>
@@ -3741,7 +3746,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13">
       <c r="B27" s="5">
         <v>11</v>
       </c>
@@ -3768,7 +3773,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13">
       <c r="B28" s="5">
         <v>12</v>
       </c>
@@ -3795,7 +3800,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13">
       <c r="B29" s="5">
         <v>13</v>
       </c>
@@ -3822,7 +3827,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13">
       <c r="B30" s="3">
         <v>14</v>
       </c>
@@ -3849,7 +3854,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13">
       <c r="B31" s="3">
         <v>15</v>
       </c>
@@ -3870,7 +3875,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13">
       <c r="B32" s="3">
         <v>16</v>
       </c>
@@ -3891,7 +3896,7 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11">
       <c r="B33" s="3">
         <v>18</v>
       </c>
@@ -3916,7 +3921,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11">
       <c r="B34" s="3">
         <v>21</v>
       </c>
@@ -3943,7 +3948,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11">
       <c r="B35" s="3">
         <v>22</v>
       </c>
@@ -3970,7 +3975,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" ht="30">
       <c r="B36" s="3">
         <v>23</v>
       </c>
@@ -3997,7 +4002,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11">
       <c r="B37" s="3">
         <v>24</v>
       </c>
@@ -4024,7 +4029,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11">
       <c r="B38" s="3">
         <v>31</v>
       </c>
@@ -4053,7 +4058,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11">
       <c r="B39" s="3">
         <v>32</v>
       </c>
@@ -4080,7 +4085,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11">
       <c r="B40" s="3">
         <v>33</v>
       </c>
@@ -4109,7 +4114,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11">
       <c r="B41" s="3">
         <v>34</v>
       </c>
@@ -4136,7 +4141,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11">
       <c r="B42" s="3">
         <v>35</v>
       </c>
@@ -4163,7 +4168,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11">
       <c r="B43" s="3">
         <v>36</v>
       </c>
@@ -4192,7 +4197,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11">
       <c r="B44" s="3">
         <v>41</v>
       </c>
@@ -4219,7 +4224,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11">
       <c r="B45" s="3">
         <v>42</v>
       </c>
@@ -4246,7 +4251,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11">
       <c r="B46" s="3" t="s">
         <v>151</v>
       </c>
@@ -4273,7 +4278,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11">
       <c r="B47" s="3">
         <v>60</v>
       </c>
@@ -4300,7 +4305,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11">
       <c r="B48" s="3">
         <v>61</v>
       </c>
@@ -4327,7 +4332,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11">
       <c r="B49" s="3">
         <v>62</v>
       </c>
@@ -4354,7 +4359,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" s="38" customFormat="1">
       <c r="B50" s="35">
         <v>63</v>
       </c>
@@ -4381,7 +4386,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11">
       <c r="B51" s="3">
         <v>68</v>
       </c>
@@ -4408,7 +4413,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11">
       <c r="B52" s="3">
         <v>69</v>
       </c>
@@ -4431,7 +4436,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11">
       <c r="B53" s="3">
         <v>71</v>
       </c>
@@ -4456,7 +4461,7 @@
       </c>
       <c r="K53" s="4"/>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11">
       <c r="B54" s="3">
         <v>72</v>
       </c>
@@ -4477,7 +4482,7 @@
       </c>
       <c r="K54" s="4"/>
     </row>
-    <row r="55" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" ht="30">
       <c r="B55" s="3">
         <v>74</v>
       </c>
@@ -4504,7 +4509,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11">
       <c r="B56" s="3">
         <v>75</v>
       </c>
@@ -4531,7 +4536,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11">
       <c r="B57" s="3"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -4542,7 +4547,7 @@
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11">
       <c r="B58" s="3">
         <v>81</v>
       </c>
@@ -4567,7 +4572,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11">
       <c r="B59" s="3">
         <v>82</v>
       </c>
@@ -4592,7 +4597,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11">
       <c r="B60" s="3"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
@@ -4603,7 +4608,7 @@
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11">
       <c r="B61" s="3">
         <v>91</v>
       </c>
@@ -4626,7 +4631,7 @@
       </c>
       <c r="K61" s="4"/>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11">
       <c r="B62" s="3">
         <v>92</v>
       </c>
@@ -4647,7 +4652,7 @@
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11">
       <c r="B63" s="3">
         <v>93</v>
       </c>
@@ -4668,7 +4673,7 @@
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11">
       <c r="B64" s="3">
         <v>94</v>
       </c>
@@ -4687,7 +4692,7 @@
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11">
       <c r="B65" s="3"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
@@ -4698,7 +4703,7 @@
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
     </row>
-    <row r="66" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11" s="38" customFormat="1">
       <c r="B66" s="35" t="s">
         <v>80</v>
       </c>
@@ -4727,7 +4732,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="67" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:11" s="38" customFormat="1">
       <c r="B67" s="35" t="s">
         <v>85</v>
       </c>
@@ -4754,7 +4759,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:11">
       <c r="B69" s="3" t="s">
         <v>518</v>
       </c>
@@ -4796,7 +4801,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
@@ -4806,7 +4811,7 @@
     <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10">
       <c r="B3" s="40" t="s">
         <v>218</v>
       </c>
@@ -4833,7 +4838,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="B4" s="39" t="s">
         <v>226</v>
       </c>
@@ -4859,7 +4864,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="B5" t="s">
         <v>217</v>
       </c>
@@ -4885,7 +4890,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="B6" t="s">
         <v>327</v>
       </c>
@@ -4911,7 +4916,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10">
       <c r="B7" t="s">
         <v>330</v>
       </c>
@@ -4937,7 +4942,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="B8" t="s">
         <v>215</v>
       </c>
@@ -4963,7 +4968,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="B9" t="s">
         <v>216</v>
       </c>
@@ -4989,7 +4994,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="B10" t="s">
         <v>278</v>
       </c>
@@ -5009,7 +5014,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="B11" t="s">
         <v>279</v>
       </c>
@@ -5029,7 +5034,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10">
       <c r="B12" t="s">
         <v>277</v>
       </c>
@@ -5049,7 +5054,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10">
       <c r="B13" t="s">
         <v>285</v>
       </c>
@@ -5069,7 +5074,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10">
       <c r="B15" t="s">
         <v>256</v>
       </c>
@@ -5086,7 +5091,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10">
       <c r="B16" t="s">
         <v>257</v>
       </c>
@@ -5106,7 +5111,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9">
       <c r="B18" t="s">
         <v>227</v>
       </c>
@@ -5129,7 +5134,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9">
       <c r="B20" t="s">
         <v>230</v>
       </c>
@@ -5152,7 +5157,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9">
       <c r="B21" t="s">
         <v>234</v>
       </c>
@@ -5175,7 +5180,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9">
       <c r="B22" t="s">
         <v>241</v>
       </c>
@@ -5198,7 +5203,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9">
       <c r="B23" t="s">
         <v>319</v>
       </c>
@@ -5218,7 +5223,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9">
       <c r="B24" t="s">
         <v>320</v>
       </c>
@@ -5238,7 +5243,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9">
       <c r="B25" t="s">
         <v>321</v>
       </c>
@@ -5258,7 +5263,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9">
       <c r="B27" t="s">
         <v>235</v>
       </c>
@@ -5281,7 +5286,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9">
       <c r="B28" t="s">
         <v>236</v>
       </c>
@@ -5304,7 +5309,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9">
       <c r="B29" t="s">
         <v>240</v>
       </c>
@@ -5327,7 +5332,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9">
       <c r="B30" t="s">
         <v>244</v>
       </c>
@@ -5350,7 +5355,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9">
       <c r="B31" t="s">
         <v>245</v>
       </c>
@@ -5373,7 +5378,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9">
       <c r="B32" t="s">
         <v>246</v>
       </c>
@@ -5396,7 +5401,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9">
       <c r="B33" t="s">
         <v>262</v>
       </c>
@@ -5416,7 +5421,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9">
       <c r="B34" t="s">
         <v>263</v>
       </c>
@@ -5436,7 +5441,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9">
       <c r="B35" t="s">
         <v>265</v>
       </c>
@@ -5456,7 +5461,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" t="s">
         <v>274</v>
       </c>
@@ -5479,7 +5484,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9">
       <c r="B38" t="s">
         <v>250</v>
       </c>
@@ -5502,7 +5507,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9">
       <c r="B39" t="s">
         <v>267</v>
       </c>
@@ -5522,7 +5527,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9">
       <c r="B40" t="s">
         <v>268</v>
       </c>
@@ -5542,7 +5547,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9">
       <c r="B41" t="s">
         <v>272</v>
       </c>
@@ -5580,7 +5585,7 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="50"/>
     <col min="3" max="3" width="38.42578125" style="50" bestFit="1" customWidth="1"/>
@@ -5590,7 +5595,7 @@
     <col min="10" max="16384" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11">
       <c r="D1" s="50" t="s">
         <v>607</v>
       </c>
@@ -5613,7 +5618,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11">
       <c r="B2" s="60" t="s">
         <v>20</v>
       </c>
@@ -5642,7 +5647,7 @@
       </c>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11">
       <c r="B3" s="60" t="s">
         <v>21</v>
       </c>
@@ -5671,7 +5676,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11">
       <c r="B4" s="60" t="s">
         <v>22</v>
       </c>
@@ -5700,7 +5705,7 @@
       </c>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11">
       <c r="B5" s="60" t="s">
         <v>23</v>
       </c>
@@ -5729,7 +5734,7 @@
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11">
       <c r="B6" s="60" t="s">
         <v>126</v>
       </c>
@@ -5758,7 +5763,7 @@
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11">
       <c r="B7" s="60" t="s">
         <v>186</v>
       </c>
@@ -5787,7 +5792,7 @@
       </c>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11">
       <c r="B8" s="60" t="s">
         <v>400</v>
       </c>
@@ -5803,7 +5808,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11">
       <c r="B9" s="60" t="s">
         <v>53</v>
       </c>
@@ -5832,7 +5837,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11">
       <c r="B10" s="60" t="s">
         <v>205</v>
       </c>
@@ -5861,7 +5866,7 @@
       </c>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11">
       <c r="B11" s="60" t="s">
         <v>415</v>
       </c>
@@ -5890,7 +5895,7 @@
       </c>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11">
       <c r="B12" s="60" t="s">
         <v>432</v>
       </c>
@@ -5919,7 +5924,7 @@
       </c>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11">
       <c r="B13" s="60" t="s">
         <v>436</v>
       </c>
@@ -5948,7 +5953,7 @@
       </c>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11">
       <c r="B14" s="60" t="s">
         <v>501</v>
       </c>
@@ -5977,7 +5982,7 @@
       </c>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11">
       <c r="B15" s="60">
         <v>10</v>
       </c>
@@ -6006,7 +6011,7 @@
       </c>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11">
       <c r="B16" s="60">
         <v>11</v>
       </c>
@@ -6035,7 +6040,7 @@
       </c>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11">
       <c r="B17" s="60">
         <v>12</v>
       </c>
@@ -6064,7 +6069,7 @@
       </c>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11">
       <c r="B18" s="60">
         <v>13</v>
       </c>
@@ -6093,7 +6098,7 @@
       </c>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11">
       <c r="B19" s="9">
         <v>14</v>
       </c>
@@ -6122,7 +6127,7 @@
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11">
       <c r="B20" s="9">
         <v>15</v>
       </c>
@@ -6151,7 +6156,7 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11">
       <c r="B21" s="9">
         <v>16</v>
       </c>
@@ -6180,7 +6185,7 @@
       </c>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11">
       <c r="B22" s="9">
         <v>18</v>
       </c>
@@ -6209,7 +6214,7 @@
       </c>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11">
       <c r="B23" s="9">
         <v>21</v>
       </c>
@@ -6238,7 +6243,7 @@
       </c>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11">
       <c r="B24" s="9">
         <v>22</v>
       </c>
@@ -6267,7 +6272,7 @@
       </c>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11">
       <c r="B25" s="9">
         <v>23</v>
       </c>
@@ -6296,7 +6301,7 @@
       </c>
       <c r="K25" s="10"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11">
       <c r="B26" s="9">
         <v>24</v>
       </c>
@@ -6325,7 +6330,7 @@
       </c>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11">
       <c r="B27" s="9">
         <v>31</v>
       </c>
@@ -6354,7 +6359,7 @@
       </c>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11">
       <c r="B28" s="9">
         <v>32</v>
       </c>
@@ -6383,7 +6388,7 @@
       </c>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11">
       <c r="B29" s="9">
         <v>33</v>
       </c>
@@ -6412,7 +6417,7 @@
       </c>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11">
       <c r="B30" s="9">
         <v>34</v>
       </c>
@@ -6441,7 +6446,7 @@
       </c>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11">
       <c r="B31" s="9">
         <v>35</v>
       </c>
@@ -6470,7 +6475,7 @@
       </c>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11">
       <c r="B32" s="9">
         <v>36</v>
       </c>
@@ -6499,7 +6504,7 @@
       </c>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11">
       <c r="B33" s="9">
         <v>41</v>
       </c>
@@ -6528,7 +6533,7 @@
       </c>
       <c r="K33" s="10"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11">
       <c r="B34" s="9">
         <v>42</v>
       </c>
@@ -6557,7 +6562,7 @@
       </c>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11">
       <c r="B35" s="9" t="s">
         <v>151</v>
       </c>
@@ -6586,7 +6591,7 @@
       </c>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11">
       <c r="B36" s="9">
         <v>60</v>
       </c>
@@ -6615,7 +6620,7 @@
       </c>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11">
       <c r="B37" s="9">
         <v>61</v>
       </c>
@@ -6644,7 +6649,7 @@
       </c>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11">
       <c r="B38" s="9">
         <v>62</v>
       </c>
@@ -6673,7 +6678,7 @@
       </c>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11">
       <c r="B39" s="9">
         <v>68</v>
       </c>
@@ -6702,7 +6707,7 @@
       </c>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11">
       <c r="B40" s="9">
         <v>69</v>
       </c>
@@ -6731,7 +6736,7 @@
       </c>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11">
       <c r="B41" s="9">
         <v>71</v>
       </c>
@@ -6760,7 +6765,7 @@
       </c>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11">
       <c r="B42" s="9">
         <v>72</v>
       </c>
@@ -6789,7 +6794,7 @@
       </c>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11">
       <c r="B43" s="9">
         <v>74</v>
       </c>
@@ -6818,7 +6823,7 @@
       </c>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11">
       <c r="B44" s="9">
         <v>75</v>
       </c>
@@ -6847,7 +6852,7 @@
       </c>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11">
       <c r="B45" s="9" t="s">
         <v>518</v>
       </c>
@@ -6891,19 +6896,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -6914,27 +6919,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="76" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="71"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="76"/>
+    </row>
+    <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
@@ -6945,7 +6950,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
@@ -6956,7 +6961,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" s="5" t="s">
         <v>649</v>
       </c>
@@ -6967,7 +6972,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4">
       <c r="B9" s="5" t="s">
         <v>653</v>
       </c>
@@ -6978,7 +6983,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4">
       <c r="B10" s="5" t="s">
         <v>660</v>
       </c>
@@ -6989,7 +6994,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="B11" s="5" t="s">
         <v>665</v>
       </c>
@@ -7000,7 +7005,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4">
       <c r="B12" s="3" t="s">
         <v>666</v>
       </c>
@@ -7011,7 +7016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="B13" s="3">
         <v>14</v>
       </c>
@@ -7022,7 +7027,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4">
       <c r="B14" s="3">
         <v>15</v>
       </c>
@@ -7033,32 +7038,32 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4">
       <c r="B16" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4">
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="71" t="s">
+      <c r="D17" s="76" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4">
       <c r="B18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="71"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="76"/>
+    </row>
+    <row r="19" spans="2:4">
       <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
@@ -7069,7 +7074,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4">
       <c r="B20" s="5" t="s">
         <v>648</v>
       </c>
@@ -7080,7 +7085,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4">
       <c r="B21" s="5" t="s">
         <v>649</v>
       </c>
@@ -7091,7 +7096,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4">
       <c r="B22" s="5" t="s">
         <v>650</v>
       </c>
@@ -7102,7 +7107,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4">
       <c r="B23" s="5" t="s">
         <v>700</v>
       </c>
@@ -7113,7 +7118,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4">
       <c r="B24" s="5" t="s">
         <v>702</v>
       </c>
@@ -7124,7 +7129,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4">
       <c r="B25" s="66" t="s">
         <v>705</v>
       </c>
@@ -7135,7 +7140,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4">
       <c r="B26" s="66" t="s">
         <v>706</v>
       </c>
@@ -7146,7 +7151,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4">
       <c r="B27" s="45">
         <v>126</v>
       </c>
@@ -7157,7 +7162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4">
       <c r="B28" s="45">
         <v>127</v>
       </c>
@@ -7168,12 +7173,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4">
       <c r="B30" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4">
       <c r="B31" s="45">
         <v>0</v>
       </c>
@@ -7184,7 +7189,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4">
       <c r="B32" s="45">
         <v>1</v>
       </c>
@@ -7195,7 +7200,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4">
       <c r="B33" s="45">
         <v>2</v>
       </c>
@@ -7206,7 +7211,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4">
       <c r="B34" s="45">
         <v>3</v>
       </c>
@@ -7217,7 +7222,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4">
       <c r="B35" s="45">
         <v>4</v>
       </c>
@@ -7228,7 +7233,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4">
       <c r="B36" s="45">
         <v>5</v>
       </c>
@@ -7239,7 +7244,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4">
       <c r="B37" s="67" t="s">
         <v>680</v>
       </c>
@@ -7250,7 +7255,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4">
       <c r="B38" s="45">
         <v>8</v>
       </c>
@@ -7261,7 +7266,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4">
       <c r="B39" s="45">
         <v>9</v>
       </c>
@@ -7272,7 +7277,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4">
       <c r="B40" s="67" t="s">
         <v>684</v>
       </c>
@@ -7283,12 +7288,12 @@
         <v>694</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4">
       <c r="B43" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4">
       <c r="B44" s="6" t="s">
         <v>0</v>
       </c>
@@ -7299,27 +7304,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4">
       <c r="B45" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="71" t="s">
+      <c r="D45" s="76" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4">
       <c r="B46" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="71"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="76"/>
+    </row>
+    <row r="47" spans="2:4">
       <c r="B47" s="5" t="s">
         <v>21</v>
       </c>
@@ -7330,7 +7335,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4">
       <c r="B48" s="5" t="s">
         <v>22</v>
       </c>
@@ -7341,7 +7346,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4">
       <c r="B49" s="5" t="s">
         <v>649</v>
       </c>
@@ -7352,7 +7357,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4">
       <c r="B50" s="5" t="s">
         <v>650</v>
       </c>
@@ -7363,7 +7368,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4">
       <c r="B51" s="5" t="s">
         <v>660</v>
       </c>
@@ -7374,7 +7379,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4">
       <c r="B52" s="5" t="s">
         <v>665</v>
       </c>
@@ -7385,7 +7390,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4">
       <c r="B53" s="3" t="s">
         <v>666</v>
       </c>
@@ -7396,7 +7401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4">
       <c r="B54" s="3">
         <v>14</v>
       </c>
@@ -7407,7 +7412,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4">
       <c r="B55" s="3">
         <v>15</v>
       </c>
@@ -7432,13 +7437,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I44"/>
+  <dimension ref="B1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31:F31"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13.5703125" customWidth="1"/>
@@ -7447,7 +7452,7 @@
     <col min="9" max="9" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9">
       <c r="G1" t="s">
         <v>721</v>
       </c>
@@ -7455,7 +7460,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -7472,7 +7477,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -7482,12 +7487,12 @@
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="71" t="s">
+      <c r="E3" s="76" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="45"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -7497,10 +7502,10 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="71"/>
+      <c r="E4" s="76"/>
       <c r="F4" s="45"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -7515,7 +7520,7 @@
       </c>
       <c r="F5" s="45"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -7530,7 +7535,7 @@
       </c>
       <c r="F6" s="45"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -7550,7 +7555,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9">
       <c r="B8" s="5" t="s">
         <v>126</v>
       </c>
@@ -7573,7 +7578,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9">
       <c r="B9" s="5" t="s">
         <v>186</v>
       </c>
@@ -7596,7 +7601,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9">
       <c r="B10" s="5" t="s">
         <v>400</v>
       </c>
@@ -7619,7 +7624,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9">
       <c r="B11" s="5" t="s">
         <v>753</v>
       </c>
@@ -7632,7 +7637,7 @@
       <c r="E11" s="70"/>
       <c r="F11" s="45"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9">
       <c r="B12" s="3" t="s">
         <v>348</v>
       </c>
@@ -7655,7 +7660,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9">
       <c r="B13" s="3" t="s">
         <v>351</v>
       </c>
@@ -7678,7 +7683,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9">
       <c r="B14" s="3" t="s">
         <v>353</v>
       </c>
@@ -7701,7 +7706,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9">
       <c r="B15" s="3" t="s">
         <v>357</v>
       </c>
@@ -7727,7 +7732,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9">
       <c r="B16" s="3">
         <v>18</v>
       </c>
@@ -7750,7 +7755,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8">
       <c r="B17" s="3">
         <v>19</v>
       </c>
@@ -7773,7 +7778,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8">
       <c r="B18" s="3">
         <v>20</v>
       </c>
@@ -7786,7 +7791,7 @@
       <c r="E18" s="70"/>
       <c r="F18" s="45"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8">
       <c r="B19" s="3">
         <v>21</v>
       </c>
@@ -7809,7 +7814,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8">
       <c r="B20" s="3">
         <v>22</v>
       </c>
@@ -7832,7 +7837,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8">
       <c r="B21" s="3">
         <v>23</v>
       </c>
@@ -7855,7 +7860,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8">
       <c r="B22" s="3">
         <v>24</v>
       </c>
@@ -7878,7 +7883,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8">
       <c r="B23" s="3" t="s">
         <v>751</v>
       </c>
@@ -7891,7 +7896,7 @@
       <c r="E23" s="70"/>
       <c r="F23" s="45"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8">
       <c r="B24" s="3">
         <v>31</v>
       </c>
@@ -7914,7 +7919,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8">
       <c r="B25" s="3">
         <v>32</v>
       </c>
@@ -7937,7 +7942,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8">
       <c r="B26" s="3">
         <v>33</v>
       </c>
@@ -7960,7 +7965,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8">
       <c r="B27" s="3">
         <v>34</v>
       </c>
@@ -7973,7 +7978,7 @@
       <c r="E27" s="70"/>
       <c r="F27" s="45"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8">
       <c r="B28" s="3">
         <v>35</v>
       </c>
@@ -7984,29 +7989,29 @@
         <v>1</v>
       </c>
       <c r="E28" s="70" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="F28" s="45"/>
       <c r="G28" t="s">
         <v>725</v>
       </c>
       <c r="H28" s="73" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>760</v>
+        <v>765</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" s="3">
+        <v>36</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="70" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="F29" s="45" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G29" t="s">
         <v>725</v>
@@ -8015,192 +8020,190 @@
         <v>723</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
-        <v>761</v>
+    <row r="30" spans="2:8">
+      <c r="B30" s="3">
+        <v>37</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4">
+        <v>1</v>
+      </c>
+      <c r="E30" s="71" t="s">
+        <v>767</v>
+      </c>
+      <c r="F30" s="45" t="s">
+        <v>768</v>
+      </c>
+      <c r="G30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="73" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4">
         <v>2</v>
       </c>
-      <c r="E30" s="70" t="s">
+      <c r="E31" s="70" t="s">
+        <v>762</v>
+      </c>
+      <c r="F31" s="45" t="s">
         <v>763</v>
       </c>
-      <c r="F30" s="45" t="s">
-        <v>764</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="G31" t="s">
         <v>725</v>
       </c>
-      <c r="H30" s="73" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="3">
+      <c r="H31" s="73" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" s="3">
         <v>40</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>750</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D32" s="4">
         <v>1</v>
       </c>
-      <c r="E31" s="70"/>
-      <c r="F31" s="45"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="3">
+      <c r="E32" s="70"/>
+      <c r="F32" s="45"/>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="3">
         <v>41</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C33" s="25" t="s">
         <v>376</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D33" s="25">
         <v>1</v>
       </c>
-      <c r="E32" s="74" t="s">
+      <c r="E33" s="74" t="s">
         <v>377</v>
       </c>
-      <c r="F32" s="75" t="s">
+      <c r="F33" s="75" t="s">
         <v>396</v>
-      </c>
-      <c r="G32" t="s">
-        <v>723</v>
-      </c>
-      <c r="H32" s="73" t="s">
-        <v>727</v>
-      </c>
-      <c r="I32" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="3">
-        <v>42</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="D33" s="4">
-        <v>1</v>
-      </c>
-      <c r="E33" s="43" t="s">
-        <v>381</v>
-      </c>
-      <c r="F33" s="45" t="s">
-        <v>398</v>
       </c>
       <c r="G33" t="s">
         <v>723</v>
       </c>
-      <c r="H33" s="72" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="73" t="s">
+        <v>727</v>
+      </c>
+      <c r="I33" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
       <c r="B34" s="3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F34" s="45" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G34" t="s">
         <v>723</v>
       </c>
       <c r="H34" s="72" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
       <c r="B35" s="3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>730</v>
+        <v>379</v>
       </c>
       <c r="D35" s="4">
         <v>1</v>
       </c>
-      <c r="E35" s="70" t="s">
-        <v>747</v>
-      </c>
-      <c r="F35" s="70" t="s">
-        <v>729</v>
+      <c r="E35" s="43" t="s">
+        <v>380</v>
+      </c>
+      <c r="F35" s="45" t="s">
+        <v>399</v>
       </c>
       <c r="G35" t="s">
         <v>723</v>
       </c>
-      <c r="H35" s="73" t="s">
+      <c r="H35" s="72" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="3">
+        <v>44</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" s="70" t="s">
+        <v>747</v>
+      </c>
+      <c r="F36" s="70" t="s">
+        <v>729</v>
+      </c>
+      <c r="G36" t="s">
+        <v>723</v>
+      </c>
+      <c r="H36" s="73" t="s">
         <v>744</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I36" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
+    <row r="37" spans="2:9">
+      <c r="B37" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4">
         <v>3</v>
       </c>
-      <c r="E36" s="70" t="s">
+      <c r="E37" s="70" t="s">
         <v>748</v>
       </c>
-      <c r="F36" s="70"/>
-      <c r="H36" s="72" t="s">
+      <c r="F37" s="70"/>
+      <c r="H37" s="72" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
+    <row r="38" spans="2:9">
+      <c r="B38" s="3" t="s">
         <v>754</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>735</v>
-      </c>
-      <c r="D37" s="4">
-        <v>2</v>
-      </c>
-      <c r="E37" s="70" t="s">
-        <v>740</v>
-      </c>
-      <c r="F37" s="45" t="s">
-        <v>731</v>
-      </c>
-      <c r="G37" t="s">
-        <v>723</v>
-      </c>
-      <c r="H37" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>755</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>736</v>
       </c>
       <c r="D38" s="4">
         <v>2</v>
       </c>
       <c r="E38" s="70" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="F38" s="45" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="G38" t="s">
         <v>723</v>
@@ -8209,21 +8212,21 @@
         <v>724</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="3">
-        <v>52</v>
+    <row r="39" spans="2:9">
+      <c r="B39" s="3" t="s">
+        <v>755</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="D39" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" s="70" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="F39" s="45" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G39" t="s">
         <v>723</v>
@@ -8232,21 +8235,21 @@
         <v>724</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9">
       <c r="B40" s="3">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D40" s="4">
         <v>1</v>
       </c>
       <c r="E40" s="70" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F40" s="45" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G40" t="s">
         <v>723</v>
@@ -8255,52 +8258,75 @@
         <v>724</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
+    <row r="41" spans="2:9">
+      <c r="B41" s="3">
+        <v>53</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>737</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1</v>
+      </c>
+      <c r="E41" s="70" t="s">
+        <v>739</v>
+      </c>
+      <c r="F41" s="45" t="s">
+        <v>734</v>
+      </c>
+      <c r="G41" t="s">
+        <v>723</v>
+      </c>
+      <c r="H41" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" s="3" t="s">
         <v>752</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>750</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D42" s="4">
         <v>4</v>
       </c>
-      <c r="E41" s="70"/>
-      <c r="F41" s="45"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="3">
+      <c r="E42" s="70"/>
+      <c r="F42" s="45"/>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" s="3">
         <v>58</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="D42" s="4">
-        <v>1</v>
-      </c>
-      <c r="E42" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="F42" s="45"/>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="3">
-        <v>59</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="D43" s="4">
         <v>1</v>
       </c>
       <c r="E43" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="45"/>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44" s="3">
+        <v>59</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1</v>
+      </c>
+      <c r="E44" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="F43" s="45"/>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D44">
-        <f>SUM(D3:D43)</f>
+      <c r="F44" s="45"/>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="D45">
+        <f>SUM(D3:D44)</f>
         <v>61</v>
       </c>
     </row>
@@ -8322,7 +8348,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -8338,7 +8364,7 @@
     <col min="18" max="48" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:42">
       <c r="I1" s="52" t="s">
         <v>441</v>
       </c>
@@ -8352,7 +8378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:42">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -8411,14 +8437,14 @@
       <c r="AO2" s="11"/>
       <c r="AP2" s="11"/>
     </row>
-    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:42">
       <c r="B3" s="55">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="76" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="48">
@@ -8468,14 +8494,14 @@
       <c r="AO3" s="11"/>
       <c r="AP3" s="11"/>
     </row>
-    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:42">
       <c r="B4" s="56">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="71"/>
+      <c r="D4" s="76"/>
       <c r="E4" s="48">
         <v>1</v>
       </c>
@@ -8523,7 +8549,7 @@
       <c r="AO4" s="11"/>
       <c r="AP4" s="11"/>
     </row>
-    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:42">
       <c r="B5" s="56">
         <v>2</v>
       </c>
@@ -8580,7 +8606,7 @@
       <c r="AO5" s="11"/>
       <c r="AP5" s="11"/>
     </row>
-    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:42">
       <c r="B6" s="56">
         <v>3</v>
       </c>
@@ -8637,7 +8663,7 @@
       <c r="AO6" s="11"/>
       <c r="AP6" s="11"/>
     </row>
-    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:42">
       <c r="B7" s="56">
         <v>4</v>
       </c>
@@ -8694,7 +8720,7 @@
       <c r="AO7" s="11"/>
       <c r="AP7" s="11"/>
     </row>
-    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:42">
       <c r="B8" s="56">
         <v>5</v>
       </c>
@@ -8751,7 +8777,7 @@
       <c r="AO8" s="11"/>
       <c r="AP8" s="11"/>
     </row>
-    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:42">
       <c r="B9" s="56">
         <v>6</v>
       </c>
@@ -8808,7 +8834,7 @@
       <c r="AO9" s="11"/>
       <c r="AP9" s="11"/>
     </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:42">
       <c r="B10" s="56">
         <v>8</v>
       </c>
@@ -8865,7 +8891,7 @@
       <c r="AO10" s="11"/>
       <c r="AP10" s="11"/>
     </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:42">
       <c r="B11" s="56">
         <v>9</v>
       </c>
@@ -8922,7 +8948,7 @@
       <c r="AO11" s="11"/>
       <c r="AP11" s="11"/>
     </row>
-    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:42">
       <c r="B12" s="56">
         <v>10</v>
       </c>
@@ -8979,7 +9005,7 @@
       <c r="AO12" s="11"/>
       <c r="AP12" s="11"/>
     </row>
-    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:42">
       <c r="B13" s="56">
         <v>40</v>
       </c>
@@ -9036,7 +9062,7 @@
       <c r="AO13" s="11"/>
       <c r="AP13" s="11"/>
     </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:42">
       <c r="B14" s="56">
         <v>60</v>
       </c>
@@ -9093,7 +9119,7 @@
       <c r="AO14" s="11"/>
       <c r="AP14" s="11"/>
     </row>
-    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:42">
       <c r="B15" s="56">
         <v>61</v>
       </c>
@@ -9150,7 +9176,7 @@
       <c r="AO15" s="11"/>
       <c r="AP15" s="11"/>
     </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:42">
       <c r="B16" s="56">
         <v>62</v>
       </c>
@@ -9207,7 +9233,7 @@
       <c r="AO16" s="11"/>
       <c r="AP16" s="11"/>
     </row>
-    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:42">
       <c r="B17" s="56">
         <v>63</v>
       </c>
@@ -9264,7 +9290,7 @@
       <c r="AO17" s="11"/>
       <c r="AP17" s="11"/>
     </row>
-    <row r="18" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:42">
       <c r="B18" s="56">
         <v>64</v>
       </c>
@@ -9321,7 +9347,7 @@
       <c r="AO18" s="11"/>
       <c r="AP18" s="11"/>
     </row>
-    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:42">
       <c r="B19" s="56">
         <v>84</v>
       </c>
@@ -9378,7 +9404,7 @@
       <c r="AO19" s="11"/>
       <c r="AP19" s="11"/>
     </row>
-    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:42">
       <c r="B20" s="56">
         <v>104</v>
       </c>
@@ -9435,7 +9461,7 @@
       <c r="AO20" s="11"/>
       <c r="AP20" s="11"/>
     </row>
-    <row r="21" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:42">
       <c r="B21" s="56">
         <v>105</v>
       </c>
@@ -9492,7 +9518,7 @@
       <c r="AO21" s="11"/>
       <c r="AP21" s="11"/>
     </row>
-    <row r="22" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:42">
       <c r="B22" s="56">
         <v>106</v>
       </c>
@@ -9549,7 +9575,7 @@
       <c r="AO22" s="11"/>
       <c r="AP22" s="11"/>
     </row>
-    <row r="23" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:42">
       <c r="B23" s="56">
         <v>108</v>
       </c>
@@ -9606,7 +9632,7 @@
       <c r="AO23" s="11"/>
       <c r="AP23" s="11"/>
     </row>
-    <row r="24" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:42">
       <c r="B24" s="56">
         <v>109</v>
       </c>
@@ -9663,7 +9689,7 @@
       <c r="AO24" s="11"/>
       <c r="AP24" s="11"/>
     </row>
-    <row r="25" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:42">
       <c r="B25" s="56">
         <v>110</v>
       </c>
@@ -9720,7 +9746,7 @@
       <c r="AO25" s="11"/>
       <c r="AP25" s="11"/>
     </row>
-    <row r="26" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:42">
       <c r="B26" s="56">
         <v>112</v>
       </c>
@@ -9777,7 +9803,7 @@
       <c r="AO26" s="11"/>
       <c r="AP26" s="11"/>
     </row>
-    <row r="27" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:42">
       <c r="B27" s="56">
         <v>114</v>
       </c>
@@ -9834,7 +9860,7 @@
       <c r="AO27" s="11"/>
       <c r="AP27" s="11"/>
     </row>
-    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:42">
       <c r="B28" s="56">
         <v>118</v>
       </c>
@@ -9883,7 +9909,7 @@
       <c r="AO28" s="11"/>
       <c r="AP28" s="11"/>
     </row>
-    <row r="29" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:42">
       <c r="B29" s="56">
         <v>119</v>
       </c>
@@ -9932,7 +9958,7 @@
       <c r="AO29" s="11"/>
       <c r="AP29" s="11"/>
     </row>
-    <row r="30" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:42">
       <c r="E30">
         <f>SUM(E3:E29)</f>
         <v>120</v>
@@ -9972,7 +9998,7 @@
       <c r="AO30" s="11"/>
       <c r="AP30" s="11"/>
     </row>
-    <row r="31" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:42">
       <c r="I31" s="51"/>
       <c r="J31" s="51"/>
       <c r="K31" s="51"/>
@@ -10026,14 +10052,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -10044,27 +10070,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="76" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="71"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="76"/>
+    </row>
+    <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -10075,7 +10101,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -10086,7 +10112,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -10097,7 +10123,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" s="5" t="s">
         <v>421</v>
       </c>
@@ -10108,7 +10134,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4">
       <c r="B9" s="5" t="s">
         <v>424</v>
       </c>
@@ -10119,7 +10145,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4">
       <c r="B10" s="5" t="s">
         <v>427</v>
       </c>
@@ -10130,7 +10156,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="B11" s="3" t="s">
         <v>430</v>
       </c>
@@ -10141,7 +10167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4">
       <c r="B12" s="3">
         <v>58</v>
       </c>
@@ -10152,7 +10178,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="B13" s="3">
         <v>59</v>
       </c>
@@ -10180,14 +10206,14 @@
       <selection activeCell="B2" sqref="B2:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" s="1" customFormat="1">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -10198,27 +10224,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" s="1" customFormat="1">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="76" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" s="1" customFormat="1">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="71"/>
-    </row>
-    <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="76"/>
+    </row>
+    <row r="5" spans="2:4" s="1" customFormat="1">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -10229,7 +10255,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" s="1" customFormat="1">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -10240,7 +10266,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" s="1" customFormat="1">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -10251,7 +10277,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" s="1" customFormat="1">
       <c r="B8" s="5" t="s">
         <v>343</v>
       </c>
@@ -10262,7 +10288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" s="1" customFormat="1">
       <c r="B9" s="3" t="s">
         <v>339</v>
       </c>
@@ -10273,7 +10299,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" s="1" customFormat="1">
       <c r="B10" s="3" t="s">
         <v>340</v>
       </c>
@@ -10284,7 +10310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" s="1" customFormat="1">
       <c r="B11" s="3">
         <v>58</v>
       </c>
@@ -10295,7 +10321,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" s="1" customFormat="1">
       <c r="B12" s="3">
         <v>59</v>
       </c>
@@ -10323,7 +10349,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -10334,12 +10360,12 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18.75">
       <c r="A2" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="27" t="s">
         <v>139</v>
       </c>
@@ -10347,12 +10373,12 @@
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -10363,27 +10389,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="71" t="s">
+      <c r="D7" s="76" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="71"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="76"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -10394,7 +10420,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -10405,7 +10431,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
@@ -10416,7 +10442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12" s="5" t="s">
         <v>126</v>
       </c>
@@ -10427,7 +10453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13" s="3" t="s">
         <v>127</v>
       </c>
@@ -10438,7 +10464,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14" s="3">
         <v>26</v>
       </c>
@@ -10449,7 +10475,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="B15" s="3">
         <v>27</v>
       </c>
@@ -10460,7 +10486,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="3">
         <v>28</v>
       </c>
@@ -10471,7 +10497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="B17" s="3">
         <v>29</v>
       </c>
@@ -10482,7 +10508,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="B18" s="3" t="s">
         <v>129</v>
       </c>
@@ -10493,7 +10519,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="B19" s="3" t="s">
         <v>124</v>
       </c>
@@ -10504,7 +10530,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="B20" s="3" t="s">
         <v>130</v>
       </c>
@@ -10515,7 +10541,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="B21" s="3" t="s">
         <v>131</v>
       </c>
@@ -10526,7 +10552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="B22" s="3">
         <v>58</v>
       </c>
@@ -10537,7 +10563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="B23" s="3">
         <v>59</v>
       </c>
@@ -10548,17 +10574,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="18.75">
       <c r="A25" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
@@ -10569,27 +10595,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="B28" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="71" t="s">
+      <c r="D28" s="76" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="B29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="71"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="76"/>
+    </row>
+    <row r="30" spans="1:4">
       <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
@@ -10600,7 +10626,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="B31" s="5" t="s">
         <v>22</v>
       </c>
@@ -10611,7 +10637,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="B32" s="5" t="s">
         <v>23</v>
       </c>
@@ -10622,7 +10648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4">
       <c r="B33" s="5" t="s">
         <v>126</v>
       </c>
@@ -10633,7 +10659,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4">
       <c r="B34" s="5" t="s">
         <v>186</v>
       </c>
@@ -10644,7 +10670,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4">
       <c r="B35" s="5" t="s">
         <v>187</v>
       </c>
@@ -10655,7 +10681,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4">
       <c r="B36" s="3" t="s">
         <v>188</v>
       </c>
@@ -10666,7 +10692,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4">
       <c r="B37" s="3" t="s">
         <v>189</v>
       </c>
@@ -10677,7 +10703,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4">
       <c r="B38" s="3" t="s">
         <v>190</v>
       </c>
@@ -10688,7 +10714,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4">
       <c r="B39" s="3">
         <v>51</v>
       </c>
@@ -10699,7 +10725,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4">
       <c r="B40" s="3">
         <v>52</v>
       </c>
@@ -10710,7 +10736,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4">
       <c r="B41" s="3">
         <v>53</v>
       </c>
@@ -10721,7 +10747,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4">
       <c r="B42" s="3">
         <v>54</v>
       </c>
@@ -10732,7 +10758,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4">
       <c r="B43" s="3">
         <v>55</v>
       </c>
@@ -10743,7 +10769,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4">
       <c r="B44" s="3" t="s">
         <v>201</v>
       </c>
@@ -10754,7 +10780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4">
       <c r="B45" s="3">
         <v>58</v>
       </c>
@@ -10765,7 +10791,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4">
       <c r="B46" s="3">
         <v>59</v>
       </c>
@@ -10776,17 +10802,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4">
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4">
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4">
       <c r="C49" s="1" t="s">
         <v>140</v>
       </c>
@@ -10794,17 +10820,17 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4">
       <c r="D50" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4">
       <c r="D51" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4">
       <c r="D52" s="1" t="s">
         <v>144</v>
       </c>
@@ -10828,17 +10854,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="158.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:3" ht="60">
       <c r="C2" s="24" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:3">
       <c r="C5" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
v2.2.1.0 - add handling for Ultra Sonic Sensor
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,26 +4,27 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
     <sheet name="Event " sheetId="10" r:id="rId3"/>
     <sheet name="ConfigData" sheetId="6" r:id="rId4"/>
-    <sheet name="NetworkConfig" sheetId="8" r:id="rId5"/>
-    <sheet name="GetNetwork" sheetId="7" r:id="rId6"/>
-    <sheet name="ComboData" sheetId="5" r:id="rId7"/>
-    <sheet name="ActionData" sheetId="1" r:id="rId8"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId9"/>
-    <sheet name="CommonMethod" sheetId="4" r:id="rId10"/>
+    <sheet name="ConfigDataV1" sheetId="11" r:id="rId5"/>
+    <sheet name="NetworkConfig" sheetId="8" r:id="rId6"/>
+    <sheet name="GetNetwork" sheetId="7" r:id="rId7"/>
+    <sheet name="ComboData" sheetId="5" r:id="rId8"/>
+    <sheet name="ActionData" sheetId="1" r:id="rId9"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId10"/>
+    <sheet name="CommonMethod" sheetId="4" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="812">
   <si>
     <t>Offset</t>
   </si>
@@ -2613,6 +2614,108 @@
   </si>
   <si>
     <t>{mode}</t>
+  </si>
+  <si>
+    <t>RC_SONIC_ENABLED</t>
+  </si>
+  <si>
+    <t>RC_BATTERY_REF_VOLTAGE</t>
+  </si>
+  <si>
+    <t>RC_BATTERY_MIN_VALUE</t>
+  </si>
+  <si>
+    <t>RC_BATTERY_MAX_VALUE</t>
+  </si>
+  <si>
+    <t>RC_BATTERY_NORAML_SEC</t>
+  </si>
+  <si>
+    <t>RC_BATTERY_ALARM_SEC</t>
+  </si>
+  <si>
+    <t>RC_MAX_SERVO</t>
+  </si>
+  <si>
+    <t>RC_MAX_DETECT_RETRY</t>
+  </si>
+  <si>
+    <t>RC_MAX_COMMAND_WAIT_MS</t>
+  </si>
+  <si>
+    <t>RC_MAX_COMMAND_RETRY</t>
+  </si>
+  <si>
+    <t>filler</t>
+  </si>
+  <si>
+    <t>RC_MP3_ENABLED</t>
+  </si>
+  <si>
+    <t>RC_MP3_VOLUME</t>
+  </si>
+  <si>
+    <t>RC_PSX_ENABLED</t>
+  </si>
+  <si>
+    <t>RC_PSX_CHECK_MS</t>
+  </si>
+  <si>
+    <t>RC_PSX_IGNORE_REPEAT_MS</t>
+  </si>
+  <si>
+    <t>RC_PSX_SHOCK</t>
+  </si>
+  <si>
+    <t>Shock for valid command</t>
+  </si>
+  <si>
+    <t>RC_MPU_ENABLED</t>
+  </si>
+  <si>
+    <t>Enable MPU 6050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC_MPU_CHECK_FREQ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC_MPU_POSITION_CHECK_FREQ </t>
+  </si>
+  <si>
+    <t>44~46</t>
+  </si>
+  <si>
+    <t>48~49</t>
+  </si>
+  <si>
+    <t>50~51</t>
+  </si>
+  <si>
+    <t>RC_TOUCH_ENABLED</t>
+  </si>
+  <si>
+    <t>RC_TOUCH_DETECT_PERIOD</t>
+  </si>
+  <si>
+    <t>RC_TOUCH_RELEASE_PERIOD</t>
+  </si>
+  <si>
+    <t>25~30</t>
+  </si>
+  <si>
+    <t>54~57</t>
+  </si>
+  <si>
+    <t>Enable Sonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Touch </t>
+  </si>
+  <si>
+    <t>Detection period for touch</t>
+  </si>
+  <si>
+    <t>Time to start another touch checking</t>
   </si>
 </sst>
 </file>
@@ -2743,7 +2846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2949,6 +3052,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3256,11 +3365,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="F44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="B14:E22"/>
+      <selection pane="bottomRight" activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4872,6 +4981,35 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="158.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:3" ht="60">
+      <c r="C2" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3">
+      <c r="C5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J41"/>
   <sheetViews>
@@ -6970,8 +7108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D55"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7004,7 +7142,7 @@
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="76" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7015,7 +7153,7 @@
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="75"/>
+      <c r="D5" s="76"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
@@ -7128,7 +7266,7 @@
       <c r="C17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="75" t="s">
+      <c r="D17" s="76" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7139,7 +7277,7 @@
       <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="75"/>
+      <c r="D18" s="76"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="5" t="s">
@@ -7389,7 +7527,7 @@
       <c r="C45" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="75" t="s">
+      <c r="D45" s="76" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7400,7 +7538,7 @@
       <c r="C46" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="75"/>
+      <c r="D46" s="76"/>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="5" t="s">
@@ -7517,8 +7655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7565,7 +7703,7 @@
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="76" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="45"/>
@@ -7580,7 +7718,7 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="75"/>
+      <c r="E4" s="76"/>
       <c r="F4" s="45"/>
     </row>
     <row r="5" spans="2:9">
@@ -8419,6 +8557,676 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>749</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="45"/>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="76"/>
+      <c r="F4" s="45"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="75" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="45"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="75" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="45"/>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="75" t="s">
+        <v>345</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="75" t="s">
+        <v>347</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="75" t="s">
+        <v>375</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="75" t="s">
+        <v>402</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="75"/>
+      <c r="F11" s="45"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2</v>
+      </c>
+      <c r="E12" s="75" t="s">
+        <v>350</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="75" t="s">
+        <v>355</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="75" t="s">
+        <v>356</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="77" t="s">
+        <v>357</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>788</v>
+      </c>
+      <c r="D15" s="25">
+        <v>2</v>
+      </c>
+      <c r="E15" s="72"/>
+      <c r="F15" s="73"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="3">
+        <v>18</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="45" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="3">
+        <v>19</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="45" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="77">
+        <v>20</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>788</v>
+      </c>
+      <c r="D18" s="25">
+        <v>1</v>
+      </c>
+      <c r="E18" s="72"/>
+      <c r="F18" s="73"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="3">
+        <v>21</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="75" t="s">
+        <v>361</v>
+      </c>
+      <c r="F19" s="45" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="3">
+        <v>22</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="75" t="s">
+        <v>363</v>
+      </c>
+      <c r="F20" s="45" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="3">
+        <v>23</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="75" t="s">
+        <v>365</v>
+      </c>
+      <c r="F21" s="45" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="3">
+        <v>24</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="E22" s="75" t="s">
+        <v>367</v>
+      </c>
+      <c r="F22" s="45" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="77" t="s">
+        <v>806</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>788</v>
+      </c>
+      <c r="D23" s="25">
+        <v>6</v>
+      </c>
+      <c r="E23" s="72"/>
+      <c r="F23" s="73"/>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="3">
+        <v>31</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="E24" s="75" t="s">
+        <v>369</v>
+      </c>
+      <c r="F24" s="45" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="3">
+        <v>32</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="75" t="s">
+        <v>371</v>
+      </c>
+      <c r="F25" s="45" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="3">
+        <v>33</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+      <c r="E26" s="75" t="s">
+        <v>373</v>
+      </c>
+      <c r="F26" s="45" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="77">
+        <v>34</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>788</v>
+      </c>
+      <c r="D27" s="25">
+        <v>1</v>
+      </c>
+      <c r="E27" s="72"/>
+      <c r="F27" s="73"/>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="3">
+        <v>35</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>759</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1</v>
+      </c>
+      <c r="E28" s="75" t="s">
+        <v>766</v>
+      </c>
+      <c r="F28" s="45" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="3">
+        <v>36</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+      <c r="E29" s="75" t="s">
+        <v>761</v>
+      </c>
+      <c r="F29" s="45" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="3">
+        <v>37</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4">
+        <v>1</v>
+      </c>
+      <c r="E30" s="75" t="s">
+        <v>767</v>
+      </c>
+      <c r="F30" s="45" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4">
+        <v>2</v>
+      </c>
+      <c r="E31" s="75" t="s">
+        <v>762</v>
+      </c>
+      <c r="F31" s="45" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="3">
+        <v>40</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1</v>
+      </c>
+      <c r="E32" s="75" t="s">
+        <v>795</v>
+      </c>
+      <c r="F32" s="45" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="3">
+        <v>41</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4">
+        <v>1</v>
+      </c>
+      <c r="E33" s="75" t="s">
+        <v>797</v>
+      </c>
+      <c r="F33" s="45" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="3">
+        <v>42</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" s="75"/>
+      <c r="F34" s="45" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="3">
+        <v>43</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+      <c r="E35" s="75"/>
+      <c r="F35" s="45" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="77" t="s">
+        <v>800</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>750</v>
+      </c>
+      <c r="D36" s="25">
+        <v>3</v>
+      </c>
+      <c r="E36" s="72"/>
+      <c r="F36" s="73"/>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="3">
+        <v>47</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4">
+        <v>1</v>
+      </c>
+      <c r="E37" s="75" t="s">
+        <v>809</v>
+      </c>
+      <c r="F37" s="45" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4">
+        <v>2</v>
+      </c>
+      <c r="E38" s="75" t="s">
+        <v>810</v>
+      </c>
+      <c r="F38" s="45" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4">
+        <v>2</v>
+      </c>
+      <c r="E39" s="75" t="s">
+        <v>811</v>
+      </c>
+      <c r="F39" s="45" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" s="77">
+        <v>52</v>
+      </c>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25">
+        <v>1</v>
+      </c>
+      <c r="E40" s="72"/>
+      <c r="F40" s="73"/>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="3">
+        <v>53</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4">
+        <v>1</v>
+      </c>
+      <c r="E41" s="75" t="s">
+        <v>808</v>
+      </c>
+      <c r="F41" s="45" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="77" t="s">
+        <v>807</v>
+      </c>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25">
+        <v>4</v>
+      </c>
+      <c r="E42" s="72"/>
+      <c r="F42" s="73"/>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43" s="3">
+        <v>58</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1</v>
+      </c>
+      <c r="E43" s="75" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="45"/>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="3">
+        <v>59</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1</v>
+      </c>
+      <c r="E44" s="75" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="45"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E3:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AV31"/>
   <sheetViews>
@@ -8522,7 +9330,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="76" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="47">
@@ -8579,7 +9387,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="75"/>
+      <c r="D4" s="76"/>
       <c r="E4" s="47">
         <v>1</v>
       </c>
@@ -10122,7 +10930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D13"/>
   <sheetViews>
@@ -10155,7 +10963,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="76" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10166,7 +10974,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="75"/>
+      <c r="D4" s="76"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
@@ -10276,7 +11084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D12"/>
   <sheetViews>
@@ -10309,7 +11117,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="76" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10320,7 +11128,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="75"/>
+      <c r="D4" s="76"/>
     </row>
     <row r="5" spans="2:4" s="1" customFormat="1">
       <c r="B5" s="5" t="s">
@@ -10419,7 +11227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D52"/>
   <sheetViews>
@@ -10474,7 +11282,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="75" t="s">
+      <c r="D7" s="76" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10485,7 +11293,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="75"/>
+      <c r="D8" s="76"/>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="5" t="s">
@@ -10680,7 +11488,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="75" t="s">
+      <c r="D28" s="76" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10691,7 +11499,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="75"/>
+      <c r="D29" s="76"/>
     </row>
     <row r="30" spans="1:4">
       <c r="B30" s="5" t="s">
@@ -10922,33 +11730,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="158.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:3" ht="60">
-      <c r="C2" s="24" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="3:3">
-      <c r="C5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
v2.2.1.1 - add setting for sonic sensor, frequency and delay after event
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,27 +4,27 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
     <sheet name="Event " sheetId="10" r:id="rId3"/>
-    <sheet name="ConfigData" sheetId="6" r:id="rId4"/>
-    <sheet name="ConfigDataV1" sheetId="11" r:id="rId5"/>
-    <sheet name="NetworkConfig" sheetId="8" r:id="rId6"/>
-    <sheet name="GetNetwork" sheetId="7" r:id="rId7"/>
-    <sheet name="ComboData" sheetId="5" r:id="rId8"/>
-    <sheet name="ActionData" sheetId="1" r:id="rId9"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId10"/>
-    <sheet name="CommonMethod" sheetId="4" r:id="rId11"/>
+    <sheet name="ConfigData" sheetId="11" r:id="rId4"/>
+    <sheet name="NetworkConfig" sheetId="8" r:id="rId5"/>
+    <sheet name="GetNetwork" sheetId="7" r:id="rId6"/>
+    <sheet name="ComboData" sheetId="5" r:id="rId7"/>
+    <sheet name="ActionData" sheetId="1" r:id="rId8"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId9"/>
+    <sheet name="CommonMethod" sheetId="4" r:id="rId10"/>
+    <sheet name="ConfigData.Obsolete" sheetId="6" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="845">
   <si>
     <t>Offset</t>
   </si>
@@ -2703,9 +2703,6 @@
     <t>25~30</t>
   </si>
   <si>
-    <t>54~57</t>
-  </si>
-  <si>
     <t>Enable Sonic</t>
   </si>
   <si>
@@ -2716,6 +2713,108 @@
   </si>
   <si>
     <t>Time to start another touch checking</t>
+  </si>
+  <si>
+    <t>Frequency to check Sonic sensor</t>
+  </si>
+  <si>
+    <t>RC_SONIC_CHECK_FREQ</t>
+  </si>
+  <si>
+    <t>Continue check period in seconds</t>
+  </si>
+  <si>
+    <t>Delay check after event in seconds</t>
+  </si>
+  <si>
+    <t>{batteryAlarmSec}</t>
+  </si>
+  <si>
+    <t>{psxCheckMs}</t>
+  </si>
+  <si>
+    <t>{mpuCheckFreq}</t>
+  </si>
+  <si>
+    <t>{touchReleasePeriod}</t>
+  </si>
+  <si>
+    <t>{sonicCheckFreq}</t>
+  </si>
+  <si>
+    <t>{batteryNomalSec}</t>
+  </si>
+  <si>
+    <t>{mpuEnabled}</t>
+  </si>
+  <si>
+    <t>55~57</t>
+  </si>
+  <si>
+    <t>{mpuPositionCheckFreq}</t>
+  </si>
+  <si>
+    <t>{touchEnabled}</t>
+  </si>
+  <si>
+    <t>{sonicEnabled}</t>
+  </si>
+  <si>
+    <t>{psxShock}</t>
+  </si>
+  <si>
+    <t>{psxIgnoreRepeatMs}</t>
+  </si>
+  <si>
+    <t>{psxNoEventMs}</t>
+  </si>
+  <si>
+    <t>[enableDebug}</t>
+  </si>
+  <si>
+    <t>{connectRouter}</t>
+  </si>
+  <si>
+    <t>{enableOLED}</t>
+  </si>
+  <si>
+    <t>{batteryRefVoltage}</t>
+  </si>
+  <si>
+    <t>{batteryMinValue}</t>
+  </si>
+  <si>
+    <t>{batteryMaxValue}</t>
+  </si>
+  <si>
+    <t>{maxDetectRetry}</t>
+  </si>
+  <si>
+    <t>{maxCommandWaitMs}</t>
+  </si>
+  <si>
+    <t>{maxCommandRetry}</t>
+  </si>
+  <si>
+    <t>{mp3Enabled}</t>
+  </si>
+  <si>
+    <t>{mp3Volume}</t>
+  </si>
+  <si>
+    <t>{mp3Startup}</t>
+  </si>
+  <si>
+    <t>[touchDetectPeriod}</t>
+  </si>
+  <si>
+    <t>RC_SONIC_DELAY_SEC</t>
+  </si>
+  <si>
+    <t>Delay after event handled (in seconds)</t>
+  </si>
+  <si>
+    <t>{sonicDelaySec}</t>
   </si>
 </sst>
 </file>
@@ -2846,7 +2945,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3057,6 +3156,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -4982,35 +5087,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="158.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:3" ht="60">
-      <c r="C2" s="24" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="3:3">
-      <c r="C5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J41"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -5787,6 +5863,911 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9">
+      <c r="G1" t="s">
+        <v>721</v>
+      </c>
+      <c r="H1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9">
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>749</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="45"/>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="78"/>
+      <c r="F4" s="45"/>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="45"/>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="45"/>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>345</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>383</v>
+      </c>
+      <c r="H7" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>347</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>384</v>
+      </c>
+      <c r="G8" t="s">
+        <v>723</v>
+      </c>
+      <c r="H8" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>375</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>397</v>
+      </c>
+      <c r="G9" t="s">
+        <v>723</v>
+      </c>
+      <c r="H9" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>402</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>403</v>
+      </c>
+      <c r="G10" t="s">
+        <v>723</v>
+      </c>
+      <c r="H10" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="68"/>
+      <c r="F11" s="45"/>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>350</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>385</v>
+      </c>
+      <c r="G12" t="s">
+        <v>723</v>
+      </c>
+      <c r="H12" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>355</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>386</v>
+      </c>
+      <c r="G13" t="s">
+        <v>723</v>
+      </c>
+      <c r="H13" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="43" t="s">
+        <v>356</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>387</v>
+      </c>
+      <c r="G14" t="s">
+        <v>723</v>
+      </c>
+      <c r="H14" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>358</v>
+      </c>
+      <c r="D15" s="25">
+        <v>2</v>
+      </c>
+      <c r="E15" s="72" t="s">
+        <v>359</v>
+      </c>
+      <c r="F15" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="G15" t="s">
+        <v>723</v>
+      </c>
+      <c r="H15" s="71" t="s">
+        <v>728</v>
+      </c>
+      <c r="I15" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="3">
+        <v>18</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>757</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>758</v>
+      </c>
+      <c r="G16" t="s">
+        <v>723</v>
+      </c>
+      <c r="H16" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="3">
+        <v>19</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+      <c r="E17" s="68" t="s">
+        <v>409</v>
+      </c>
+      <c r="F17" s="45" t="s">
+        <v>410</v>
+      </c>
+      <c r="G17" t="s">
+        <v>723</v>
+      </c>
+      <c r="H17" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="3">
+        <v>20</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2</v>
+      </c>
+      <c r="E18" s="68"/>
+      <c r="F18" s="45"/>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="3">
+        <v>21</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>361</v>
+      </c>
+      <c r="F19" s="45" t="s">
+        <v>389</v>
+      </c>
+      <c r="G19" t="s">
+        <v>723</v>
+      </c>
+      <c r="H19" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="3">
+        <v>22</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="43" t="s">
+        <v>363</v>
+      </c>
+      <c r="F20" s="45" t="s">
+        <v>390</v>
+      </c>
+      <c r="G20" t="s">
+        <v>723</v>
+      </c>
+      <c r="H20" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="3">
+        <v>23</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>365</v>
+      </c>
+      <c r="F21" s="45" t="s">
+        <v>391</v>
+      </c>
+      <c r="G21" t="s">
+        <v>723</v>
+      </c>
+      <c r="H21" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="3">
+        <v>24</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="E22" s="43" t="s">
+        <v>367</v>
+      </c>
+      <c r="F22" s="45" t="s">
+        <v>392</v>
+      </c>
+      <c r="G22" t="s">
+        <v>723</v>
+      </c>
+      <c r="H22" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="3" t="s">
+        <v>751</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D23" s="4">
+        <v>6</v>
+      </c>
+      <c r="E23" s="68"/>
+      <c r="F23" s="45"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="3">
+        <v>31</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="E24" s="43" t="s">
+        <v>369</v>
+      </c>
+      <c r="F24" s="45" t="s">
+        <v>393</v>
+      </c>
+      <c r="G24" t="s">
+        <v>723</v>
+      </c>
+      <c r="H24" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="3">
+        <v>32</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="43" t="s">
+        <v>371</v>
+      </c>
+      <c r="F25" s="45" t="s">
+        <v>394</v>
+      </c>
+      <c r="G25" t="s">
+        <v>723</v>
+      </c>
+      <c r="H25" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="3">
+        <v>33</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+      <c r="E26" s="43" t="s">
+        <v>373</v>
+      </c>
+      <c r="F26" s="45" t="s">
+        <v>395</v>
+      </c>
+      <c r="G26" t="s">
+        <v>723</v>
+      </c>
+      <c r="H26" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="3">
+        <v>34</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+      <c r="E27" s="68"/>
+      <c r="F27" s="45"/>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" s="3">
+        <v>35</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>759</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1</v>
+      </c>
+      <c r="E28" s="68" t="s">
+        <v>766</v>
+      </c>
+      <c r="F28" s="45"/>
+      <c r="G28" t="s">
+        <v>725</v>
+      </c>
+      <c r="H28" s="71" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" s="3">
+        <v>36</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+      <c r="E29" s="68" t="s">
+        <v>761</v>
+      </c>
+      <c r="F29" s="45" t="s">
+        <v>764</v>
+      </c>
+      <c r="G29" t="s">
+        <v>725</v>
+      </c>
+      <c r="H29" s="71" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="3">
+        <v>37</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4">
+        <v>1</v>
+      </c>
+      <c r="E30" s="69" t="s">
+        <v>767</v>
+      </c>
+      <c r="F30" s="45" t="s">
+        <v>768</v>
+      </c>
+      <c r="G30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="71" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4">
+        <v>2</v>
+      </c>
+      <c r="E31" s="68" t="s">
+        <v>762</v>
+      </c>
+      <c r="F31" s="45" t="s">
+        <v>763</v>
+      </c>
+      <c r="G31" t="s">
+        <v>725</v>
+      </c>
+      <c r="H31" s="71" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" s="3">
+        <v>40</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1</v>
+      </c>
+      <c r="E32" s="68"/>
+      <c r="F32" s="45"/>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="3">
+        <v>41</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="D33" s="25">
+        <v>1</v>
+      </c>
+      <c r="E33" s="72" t="s">
+        <v>377</v>
+      </c>
+      <c r="F33" s="73" t="s">
+        <v>396</v>
+      </c>
+      <c r="G33" t="s">
+        <v>723</v>
+      </c>
+      <c r="H33" s="71" t="s">
+        <v>727</v>
+      </c>
+      <c r="I33" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="3">
+        <v>42</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" s="43" t="s">
+        <v>381</v>
+      </c>
+      <c r="F34" s="45" t="s">
+        <v>398</v>
+      </c>
+      <c r="G34" t="s">
+        <v>723</v>
+      </c>
+      <c r="H34" s="70" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="3">
+        <v>43</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+      <c r="E35" s="43" t="s">
+        <v>380</v>
+      </c>
+      <c r="F35" s="45" t="s">
+        <v>399</v>
+      </c>
+      <c r="G35" t="s">
+        <v>723</v>
+      </c>
+      <c r="H35" s="70" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="3">
+        <v>44</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" s="68" t="s">
+        <v>747</v>
+      </c>
+      <c r="F36" s="68" t="s">
+        <v>729</v>
+      </c>
+      <c r="G36" t="s">
+        <v>723</v>
+      </c>
+      <c r="H36" s="71" t="s">
+        <v>744</v>
+      </c>
+      <c r="I36" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4">
+        <v>3</v>
+      </c>
+      <c r="E37" s="68" t="s">
+        <v>748</v>
+      </c>
+      <c r="F37" s="68"/>
+      <c r="H37" s="70" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="D38" s="4">
+        <v>2</v>
+      </c>
+      <c r="E38" s="68" t="s">
+        <v>740</v>
+      </c>
+      <c r="F38" s="45" t="s">
+        <v>731</v>
+      </c>
+      <c r="G38" t="s">
+        <v>723</v>
+      </c>
+      <c r="H38" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>736</v>
+      </c>
+      <c r="D39" s="4">
+        <v>2</v>
+      </c>
+      <c r="E39" s="68" t="s">
+        <v>741</v>
+      </c>
+      <c r="F39" s="45" t="s">
+        <v>732</v>
+      </c>
+      <c r="G39" t="s">
+        <v>723</v>
+      </c>
+      <c r="H39" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="3">
+        <v>52</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1</v>
+      </c>
+      <c r="E40" s="68" t="s">
+        <v>738</v>
+      </c>
+      <c r="F40" s="45" t="s">
+        <v>733</v>
+      </c>
+      <c r="G40" t="s">
+        <v>723</v>
+      </c>
+      <c r="H40" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="3">
+        <v>53</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>737</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1</v>
+      </c>
+      <c r="E41" s="68" t="s">
+        <v>739</v>
+      </c>
+      <c r="F41" s="45" t="s">
+        <v>734</v>
+      </c>
+      <c r="G41" t="s">
+        <v>723</v>
+      </c>
+      <c r="H41" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" s="3" t="s">
+        <v>752</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D42" s="4">
+        <v>4</v>
+      </c>
+      <c r="E42" s="68"/>
+      <c r="F42" s="45"/>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" s="3">
+        <v>58</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1</v>
+      </c>
+      <c r="E43" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="45"/>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44" s="3">
+        <v>59</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1</v>
+      </c>
+      <c r="E44" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="45"/>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="D45">
+        <f>SUM(D3:D44)</f>
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E3:E4"/>
+  </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7108,7 +8089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -7142,7 +8123,7 @@
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="78" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7153,7 +8134,7 @@
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="76"/>
+      <c r="D5" s="78"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
@@ -7266,7 +8247,7 @@
       <c r="C17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="76" t="s">
+      <c r="D17" s="78" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7277,7 +8258,7 @@
       <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="76"/>
+      <c r="D18" s="78"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="5" t="s">
@@ -7527,7 +8508,7 @@
       <c r="C45" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="76" t="s">
+      <c r="D45" s="78" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7538,7 +8519,7 @@
       <c r="C46" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="76"/>
+      <c r="D46" s="78"/>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="5" t="s">
@@ -7653,921 +8634,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I45"/>
+  <dimension ref="B2:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="44.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:9">
-      <c r="G1" t="s">
-        <v>721</v>
-      </c>
-      <c r="H1" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9">
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>749</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9">
-      <c r="B3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="76" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="45"/>
-    </row>
-    <row r="4" spans="2:9">
-      <c r="B4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="76"/>
-      <c r="F4" s="45"/>
-    </row>
-    <row r="5" spans="2:9">
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" s="45"/>
-    </row>
-    <row r="6" spans="2:9">
-      <c r="B6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="F6" s="45"/>
-    </row>
-    <row r="7" spans="2:9">
-      <c r="B7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="43" t="s">
-        <v>345</v>
-      </c>
-      <c r="F7" s="45" t="s">
-        <v>383</v>
-      </c>
-      <c r="H7" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9">
-      <c r="B8" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>347</v>
-      </c>
-      <c r="F8" s="45" t="s">
-        <v>384</v>
-      </c>
-      <c r="G8" t="s">
-        <v>723</v>
-      </c>
-      <c r="H8" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9">
-      <c r="B9" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="43" t="s">
-        <v>375</v>
-      </c>
-      <c r="F9" s="45" t="s">
-        <v>397</v>
-      </c>
-      <c r="G9" t="s">
-        <v>723</v>
-      </c>
-      <c r="H9" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>401</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>402</v>
-      </c>
-      <c r="F10" s="45" t="s">
-        <v>403</v>
-      </c>
-      <c r="G10" t="s">
-        <v>723</v>
-      </c>
-      <c r="H10" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="5" t="s">
-        <v>753</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>750</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2</v>
-      </c>
-      <c r="E11" s="68"/>
-      <c r="F11" s="45"/>
-    </row>
-    <row r="12" spans="2:9">
-      <c r="B12" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="D12" s="4">
-        <v>2</v>
-      </c>
-      <c r="E12" s="43" t="s">
-        <v>350</v>
-      </c>
-      <c r="F12" s="45" t="s">
-        <v>385</v>
-      </c>
-      <c r="G12" t="s">
-        <v>723</v>
-      </c>
-      <c r="H12" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9">
-      <c r="B13" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-      <c r="E13" s="43" t="s">
-        <v>355</v>
-      </c>
-      <c r="F13" s="45" t="s">
-        <v>386</v>
-      </c>
-      <c r="G13" t="s">
-        <v>723</v>
-      </c>
-      <c r="H13" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9">
-      <c r="B14" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="D14" s="4">
-        <v>2</v>
-      </c>
-      <c r="E14" s="43" t="s">
-        <v>356</v>
-      </c>
-      <c r="F14" s="45" t="s">
-        <v>387</v>
-      </c>
-      <c r="G14" t="s">
-        <v>723</v>
-      </c>
-      <c r="H14" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9">
-      <c r="B15" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>358</v>
-      </c>
-      <c r="D15" s="25">
-        <v>2</v>
-      </c>
-      <c r="E15" s="72" t="s">
-        <v>359</v>
-      </c>
-      <c r="F15" s="73" t="s">
-        <v>388</v>
-      </c>
-      <c r="G15" t="s">
-        <v>723</v>
-      </c>
-      <c r="H15" s="71" t="s">
-        <v>728</v>
-      </c>
-      <c r="I15" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9">
-      <c r="B16" s="3">
-        <v>18</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>756</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
-      <c r="E16" s="44" t="s">
-        <v>757</v>
-      </c>
-      <c r="F16" s="45" t="s">
-        <v>758</v>
-      </c>
-      <c r="G16" t="s">
-        <v>723</v>
-      </c>
-      <c r="H16" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="3">
-        <v>19</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="D17" s="4">
-        <v>1</v>
-      </c>
-      <c r="E17" s="68" t="s">
-        <v>409</v>
-      </c>
-      <c r="F17" s="45" t="s">
-        <v>410</v>
-      </c>
-      <c r="G17" t="s">
-        <v>723</v>
-      </c>
-      <c r="H17" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="3">
-        <v>20</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>750</v>
-      </c>
-      <c r="D18" s="4">
-        <v>2</v>
-      </c>
-      <c r="E18" s="68"/>
-      <c r="F18" s="45"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" s="3">
-        <v>21</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19" s="43" t="s">
-        <v>361</v>
-      </c>
-      <c r="F19" s="45" t="s">
-        <v>389</v>
-      </c>
-      <c r="G19" t="s">
-        <v>723</v>
-      </c>
-      <c r="H19" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="3">
-        <v>22</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20" s="43" t="s">
-        <v>363</v>
-      </c>
-      <c r="F20" s="45" t="s">
-        <v>390</v>
-      </c>
-      <c r="G20" t="s">
-        <v>723</v>
-      </c>
-      <c r="H20" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="3">
-        <v>23</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="E21" s="43" t="s">
-        <v>365</v>
-      </c>
-      <c r="F21" s="45" t="s">
-        <v>391</v>
-      </c>
-      <c r="G21" t="s">
-        <v>723</v>
-      </c>
-      <c r="H21" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="3">
-        <v>24</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="D22" s="4">
-        <v>1</v>
-      </c>
-      <c r="E22" s="43" t="s">
-        <v>367</v>
-      </c>
-      <c r="F22" s="45" t="s">
-        <v>392</v>
-      </c>
-      <c r="G22" t="s">
-        <v>723</v>
-      </c>
-      <c r="H22" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="B23" s="3" t="s">
-        <v>751</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>750</v>
-      </c>
-      <c r="D23" s="4">
-        <v>6</v>
-      </c>
-      <c r="E23" s="68"/>
-      <c r="F23" s="45"/>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="B24" s="3">
-        <v>31</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="D24" s="4">
-        <v>1</v>
-      </c>
-      <c r="E24" s="43" t="s">
-        <v>369</v>
-      </c>
-      <c r="F24" s="45" t="s">
-        <v>393</v>
-      </c>
-      <c r="G24" t="s">
-        <v>723</v>
-      </c>
-      <c r="H24" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="B25" s="3">
-        <v>32</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
-      <c r="E25" s="43" t="s">
-        <v>371</v>
-      </c>
-      <c r="F25" s="45" t="s">
-        <v>394</v>
-      </c>
-      <c r="G25" t="s">
-        <v>723</v>
-      </c>
-      <c r="H25" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" s="3">
-        <v>33</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
-      <c r="E26" s="43" t="s">
-        <v>373</v>
-      </c>
-      <c r="F26" s="45" t="s">
-        <v>395</v>
-      </c>
-      <c r="G26" t="s">
-        <v>723</v>
-      </c>
-      <c r="H26" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8">
-      <c r="B27" s="3">
-        <v>34</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>750</v>
-      </c>
-      <c r="D27" s="4">
-        <v>1</v>
-      </c>
-      <c r="E27" s="68"/>
-      <c r="F27" s="45"/>
-    </row>
-    <row r="28" spans="2:8">
-      <c r="B28" s="3">
-        <v>35</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>759</v>
-      </c>
-      <c r="D28" s="4">
-        <v>1</v>
-      </c>
-      <c r="E28" s="68" t="s">
-        <v>766</v>
-      </c>
-      <c r="F28" s="45"/>
-      <c r="G28" t="s">
-        <v>725</v>
-      </c>
-      <c r="H28" s="71" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8">
-      <c r="B29" s="3">
-        <v>36</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4">
-        <v>1</v>
-      </c>
-      <c r="E29" s="68" t="s">
-        <v>761</v>
-      </c>
-      <c r="F29" s="45" t="s">
-        <v>764</v>
-      </c>
-      <c r="G29" t="s">
-        <v>725</v>
-      </c>
-      <c r="H29" s="71" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8">
-      <c r="B30" s="3">
-        <v>37</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4">
-        <v>1</v>
-      </c>
-      <c r="E30" s="69" t="s">
-        <v>767</v>
-      </c>
-      <c r="F30" s="45" t="s">
-        <v>768</v>
-      </c>
-      <c r="G30" t="s">
-        <v>68</v>
-      </c>
-      <c r="H30" s="71" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8">
-      <c r="B31" s="3" t="s">
-        <v>760</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4">
-        <v>2</v>
-      </c>
-      <c r="E31" s="68" t="s">
-        <v>762</v>
-      </c>
-      <c r="F31" s="45" t="s">
-        <v>763</v>
-      </c>
-      <c r="G31" t="s">
-        <v>725</v>
-      </c>
-      <c r="H31" s="71" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8">
-      <c r="B32" s="3">
-        <v>40</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>750</v>
-      </c>
-      <c r="D32" s="4">
-        <v>1</v>
-      </c>
-      <c r="E32" s="68"/>
-      <c r="F32" s="45"/>
-    </row>
-    <row r="33" spans="2:9">
-      <c r="B33" s="3">
-        <v>41</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>376</v>
-      </c>
-      <c r="D33" s="25">
-        <v>1</v>
-      </c>
-      <c r="E33" s="72" t="s">
-        <v>377</v>
-      </c>
-      <c r="F33" s="73" t="s">
-        <v>396</v>
-      </c>
-      <c r="G33" t="s">
-        <v>723</v>
-      </c>
-      <c r="H33" s="71" t="s">
-        <v>727</v>
-      </c>
-      <c r="I33" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9">
-      <c r="B34" s="3">
-        <v>42</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="D34" s="4">
-        <v>1</v>
-      </c>
-      <c r="E34" s="43" t="s">
-        <v>381</v>
-      </c>
-      <c r="F34" s="45" t="s">
-        <v>398</v>
-      </c>
-      <c r="G34" t="s">
-        <v>723</v>
-      </c>
-      <c r="H34" s="70" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9">
-      <c r="B35" s="3">
-        <v>43</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="D35" s="4">
-        <v>1</v>
-      </c>
-      <c r="E35" s="43" t="s">
-        <v>380</v>
-      </c>
-      <c r="F35" s="45" t="s">
-        <v>399</v>
-      </c>
-      <c r="G35" t="s">
-        <v>723</v>
-      </c>
-      <c r="H35" s="70" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9">
-      <c r="B36" s="3">
-        <v>44</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>730</v>
-      </c>
-      <c r="D36" s="4">
-        <v>1</v>
-      </c>
-      <c r="E36" s="68" t="s">
-        <v>747</v>
-      </c>
-      <c r="F36" s="68" t="s">
-        <v>729</v>
-      </c>
-      <c r="G36" t="s">
-        <v>723</v>
-      </c>
-      <c r="H36" s="71" t="s">
-        <v>744</v>
-      </c>
-      <c r="I36" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9">
-      <c r="B37" s="3" t="s">
-        <v>746</v>
-      </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4">
-        <v>3</v>
-      </c>
-      <c r="E37" s="68" t="s">
-        <v>748</v>
-      </c>
-      <c r="F37" s="68"/>
-      <c r="H37" s="70" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9">
-      <c r="B38" s="3" t="s">
-        <v>754</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>735</v>
-      </c>
-      <c r="D38" s="4">
-        <v>2</v>
-      </c>
-      <c r="E38" s="68" t="s">
-        <v>740</v>
-      </c>
-      <c r="F38" s="45" t="s">
-        <v>731</v>
-      </c>
-      <c r="G38" t="s">
-        <v>723</v>
-      </c>
-      <c r="H38" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9">
-      <c r="B39" s="3" t="s">
-        <v>755</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>736</v>
-      </c>
-      <c r="D39" s="4">
-        <v>2</v>
-      </c>
-      <c r="E39" s="68" t="s">
-        <v>741</v>
-      </c>
-      <c r="F39" s="45" t="s">
-        <v>732</v>
-      </c>
-      <c r="G39" t="s">
-        <v>723</v>
-      </c>
-      <c r="H39" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9">
-      <c r="B40" s="3">
-        <v>52</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>735</v>
-      </c>
-      <c r="D40" s="4">
-        <v>1</v>
-      </c>
-      <c r="E40" s="68" t="s">
-        <v>738</v>
-      </c>
-      <c r="F40" s="45" t="s">
-        <v>733</v>
-      </c>
-      <c r="G40" t="s">
-        <v>723</v>
-      </c>
-      <c r="H40" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9">
-      <c r="B41" s="3">
-        <v>53</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>737</v>
-      </c>
-      <c r="D41" s="4">
-        <v>1</v>
-      </c>
-      <c r="E41" s="68" t="s">
-        <v>739</v>
-      </c>
-      <c r="F41" s="45" t="s">
-        <v>734</v>
-      </c>
-      <c r="G41" t="s">
-        <v>723</v>
-      </c>
-      <c r="H41" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9">
-      <c r="B42" s="3" t="s">
-        <v>752</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>750</v>
-      </c>
-      <c r="D42" s="4">
-        <v>4</v>
-      </c>
-      <c r="E42" s="68"/>
-      <c r="F42" s="45"/>
-    </row>
-    <row r="43" spans="2:9">
-      <c r="B43" s="3">
-        <v>58</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" s="4">
-        <v>1</v>
-      </c>
-      <c r="E43" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" s="45"/>
-    </row>
-    <row r="44" spans="2:9">
-      <c r="B44" s="3">
-        <v>59</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D44" s="4">
-        <v>1</v>
-      </c>
-      <c r="E44" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="F44" s="45"/>
-    </row>
-    <row r="45" spans="2:9">
-      <c r="D45">
-        <f>SUM(D3:D44)</f>
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E3:E4"/>
-  </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F44"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.42578125" customWidth="1"/>
@@ -8600,7 +8676,7 @@
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="78" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="45"/>
@@ -8615,7 +8691,7 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="76"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="45"/>
     </row>
     <row r="5" spans="2:6">
@@ -8670,7 +8746,7 @@
         <v>126</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>346</v>
+        <v>829</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -8687,7 +8763,7 @@
         <v>186</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>374</v>
+        <v>830</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -8704,7 +8780,7 @@
         <v>400</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>401</v>
+        <v>831</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -8717,24 +8793,24 @@
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="79" t="s">
         <v>753</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="25" t="s">
         <v>750</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="25">
         <v>2</v>
       </c>
-      <c r="E11" s="75"/>
-      <c r="F11" s="45"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="73"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="3" t="s">
         <v>348</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>349</v>
+        <v>832</v>
       </c>
       <c r="D12" s="4">
         <v>2</v>
@@ -8751,7 +8827,7 @@
         <v>351</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>352</v>
+        <v>833</v>
       </c>
       <c r="D13" s="4">
         <v>2</v>
@@ -8768,7 +8844,7 @@
         <v>353</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>354</v>
+        <v>834</v>
       </c>
       <c r="D14" s="4">
         <v>2</v>
@@ -8797,9 +8873,15 @@
       <c r="B16" s="3">
         <v>18</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="75"/>
+      <c r="C16" s="4" t="s">
+        <v>820</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="75" t="s">
+        <v>813</v>
+      </c>
       <c r="F16" s="45" t="s">
         <v>782</v>
       </c>
@@ -8808,9 +8890,15 @@
       <c r="B17" s="3">
         <v>19</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="75"/>
+      <c r="C17" s="4" t="s">
+        <v>815</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+      <c r="E17" s="75" t="s">
+        <v>814</v>
+      </c>
       <c r="F17" s="45" t="s">
         <v>783</v>
       </c>
@@ -8850,7 +8938,7 @@
         <v>22</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>362</v>
+        <v>835</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -8867,7 +8955,7 @@
         <v>23</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>364</v>
+        <v>836</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -8884,7 +8972,7 @@
         <v>24</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>366</v>
+        <v>837</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -8914,7 +9002,7 @@
         <v>31</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>368</v>
+        <v>838</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -8931,7 +9019,7 @@
         <v>32</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>370</v>
+        <v>839</v>
       </c>
       <c r="D25" s="4">
         <v>1</v>
@@ -8948,7 +9036,7 @@
         <v>33</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>372</v>
+        <v>840</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
@@ -8994,7 +9082,9 @@
       <c r="B29" s="3">
         <v>36</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>816</v>
+      </c>
       <c r="D29" s="4">
         <v>1</v>
       </c>
@@ -9009,7 +9099,9 @@
       <c r="B30" s="3">
         <v>37</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>828</v>
+      </c>
       <c r="D30" s="4">
         <v>1</v>
       </c>
@@ -9024,7 +9116,9 @@
       <c r="B31" s="3" t="s">
         <v>760</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="4" t="s">
+        <v>827</v>
+      </c>
       <c r="D31" s="4">
         <v>2</v>
       </c>
@@ -9040,7 +9134,7 @@
         <v>40</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>750</v>
+        <v>826</v>
       </c>
       <c r="D32" s="4">
         <v>1</v>
@@ -9056,7 +9150,9 @@
       <c r="B33" s="3">
         <v>41</v>
       </c>
-      <c r="C33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>821</v>
+      </c>
       <c r="D33" s="4">
         <v>1</v>
       </c>
@@ -9071,7 +9167,9 @@
       <c r="B34" s="3">
         <v>42</v>
       </c>
-      <c r="C34" s="4"/>
+      <c r="C34" s="4" t="s">
+        <v>817</v>
+      </c>
       <c r="D34" s="4">
         <v>1</v>
       </c>
@@ -9084,7 +9182,9 @@
       <c r="B35" s="3">
         <v>43</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="C35" s="4" t="s">
+        <v>823</v>
+      </c>
       <c r="D35" s="4">
         <v>1</v>
       </c>
@@ -9098,7 +9198,7 @@
         <v>800</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>750</v>
+        <v>788</v>
       </c>
       <c r="D36" s="25">
         <v>3</v>
@@ -9110,12 +9210,14 @@
       <c r="B37" s="3">
         <v>47</v>
       </c>
-      <c r="C37" s="4"/>
+      <c r="C37" s="4" t="s">
+        <v>824</v>
+      </c>
       <c r="D37" s="4">
         <v>1</v>
       </c>
       <c r="E37" s="75" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F37" s="45" t="s">
         <v>803</v>
@@ -9125,12 +9227,14 @@
       <c r="B38" s="3" t="s">
         <v>801</v>
       </c>
-      <c r="C38" s="4"/>
+      <c r="C38" s="4" t="s">
+        <v>841</v>
+      </c>
       <c r="D38" s="4">
         <v>2</v>
       </c>
       <c r="E38" s="75" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F38" s="45" t="s">
         <v>804</v>
@@ -9140,12 +9244,14 @@
       <c r="B39" s="3" t="s">
         <v>802</v>
       </c>
-      <c r="C39" s="4"/>
+      <c r="C39" s="4" t="s">
+        <v>818</v>
+      </c>
       <c r="D39" s="4">
         <v>2</v>
       </c>
       <c r="E39" s="75" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="F39" s="45" t="s">
         <v>805</v>
@@ -9166,67 +9272,110 @@
       <c r="B41" s="3">
         <v>53</v>
       </c>
-      <c r="C41" s="4"/>
+      <c r="C41" s="4" t="s">
+        <v>825</v>
+      </c>
       <c r="D41" s="4">
         <v>1</v>
       </c>
       <c r="E41" s="75" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F41" s="45" t="s">
         <v>778</v>
       </c>
     </row>
     <row r="42" spans="2:6">
-      <c r="B42" s="77" t="s">
-        <v>807</v>
-      </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25">
-        <v>4</v>
-      </c>
-      <c r="E42" s="72"/>
-      <c r="F42" s="73"/>
+      <c r="B42" s="3">
+        <v>54</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>819</v>
+      </c>
+      <c r="D42" s="4">
+        <v>1</v>
+      </c>
+      <c r="E42" s="76" t="s">
+        <v>811</v>
+      </c>
+      <c r="F42" s="45" t="s">
+        <v>812</v>
+      </c>
     </row>
     <row r="43" spans="2:6">
       <c r="B43" s="3">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>15</v>
+        <v>844</v>
       </c>
       <c r="D43" s="4">
         <v>1</v>
       </c>
-      <c r="E43" s="75" t="s">
+      <c r="E43" s="76" t="s">
+        <v>843</v>
+      </c>
+      <c r="F43" s="45" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="77" t="s">
+        <v>822</v>
+      </c>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25">
+        <v>3</v>
+      </c>
+      <c r="E44" s="72"/>
+      <c r="F44" s="73"/>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="3">
+        <v>58</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="4">
+        <v>1</v>
+      </c>
+      <c r="E45" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="45"/>
-    </row>
-    <row r="44" spans="2:6">
-      <c r="B44" s="3">
+      <c r="F45" s="45"/>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" s="3">
         <v>59</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D46" s="4">
         <v>1</v>
       </c>
-      <c r="E44" s="75" t="s">
+      <c r="E46" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="45"/>
+      <c r="F46" s="45"/>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="D47">
+        <f>SUM(D3:D46)</f>
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AV31"/>
   <sheetViews>
@@ -9330,7 +9479,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="78" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="47">
@@ -9387,7 +9536,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="76"/>
+      <c r="D4" s="78"/>
       <c r="E4" s="47">
         <v>1</v>
       </c>
@@ -10930,7 +11079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D13"/>
   <sheetViews>
@@ -10963,7 +11112,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="78" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10974,7 +11123,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="76"/>
+      <c r="D4" s="78"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
@@ -11084,7 +11233,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D12"/>
   <sheetViews>
@@ -11117,7 +11266,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="78" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11128,7 +11277,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="76"/>
+      <c r="D4" s="78"/>
     </row>
     <row r="5" spans="2:4" s="1" customFormat="1">
       <c r="B5" s="5" t="s">
@@ -11227,7 +11376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D52"/>
   <sheetViews>
@@ -11282,7 +11431,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="76" t="s">
+      <c r="D7" s="78" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11293,7 +11442,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="76"/>
+      <c r="D8" s="78"/>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="5" t="s">
@@ -11488,7 +11637,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="76" t="s">
+      <c r="D28" s="78" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11499,7 +11648,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="76"/>
+      <c r="D29" s="78"/>
     </row>
     <row r="30" spans="1:4">
       <c r="B30" s="5" t="s">
@@ -11730,4 +11879,33 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="158.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:3" ht="60">
+      <c r="C2" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3">
+      <c r="C5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update protocol Remove dummy code in SimpleWiFiManager
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="849">
   <si>
     <t>Offset</t>
   </si>
@@ -1904,7 +1904,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1925,7 +1925,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1936,7 +1936,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1953,7 +1953,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1964,7 +1964,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1980,7 +1980,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1997,7 +1997,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -2030,7 +2030,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2040,7 +2040,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2816,16 +2816,32 @@
   <si>
     <t>{sonicDelaySec}</t>
   </si>
+  <si>
+    <t>Yes {2}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action ID, {play count}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes {3/4}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>A9 9A 04 41 00 02 47 ED</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2833,7 +2849,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2843,7 +2859,7 @@
       <u/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2853,19 +2869,19 @@
       <u/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2873,7 +2889,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2881,7 +2897,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3158,11 +3174,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3470,14 +3486,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F44" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="G31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H65" sqref="H65"/>
+      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -3491,7 +3507,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3499,7 +3515,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -3510,7 +3526,7 @@
       <c r="G3" s="13"/>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -3522,7 +3538,7 @@
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -3534,7 +3550,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -3550,7 +3566,7 @@
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -3559,7 +3575,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
@@ -3568,7 +3584,7 @@
       </c>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
@@ -3577,7 +3593,7 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="12" spans="2:14">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
@@ -3606,7 +3622,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
@@ -3614,7 +3630,7 @@
         <v>40</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>57</v>
+        <v>845</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>155</v>
@@ -3635,7 +3651,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
@@ -3664,7 +3680,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
@@ -3693,7 +3709,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="2:14">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
@@ -3716,7 +3732,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>126</v>
       </c>
@@ -3739,7 +3755,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>186</v>
       </c>
@@ -3762,7 +3778,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:13">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>400</v>
       </c>
@@ -3791,7 +3807,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="2:13">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>769</v>
       </c>
@@ -3816,7 +3832,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="21" spans="2:13">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>772</v>
       </c>
@@ -3845,7 +3861,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="45">
+    <row r="22" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>53</v>
       </c>
@@ -3874,7 +3890,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>205</v>
       </c>
@@ -3901,7 +3917,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="2:13">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>415</v>
       </c>
@@ -3926,7 +3942,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="25" spans="2:13">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>432</v>
       </c>
@@ -3951,7 +3967,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="26" spans="2:13">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>436</v>
       </c>
@@ -3979,7 +3995,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="27" spans="2:13">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>501</v>
       </c>
@@ -4011,7 +4027,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="2:13">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
         <v>10</v>
       </c>
@@ -4038,7 +4054,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="29" spans="2:13">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="5">
         <v>11</v>
       </c>
@@ -4065,7 +4081,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="2:13">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="5">
         <v>12</v>
       </c>
@@ -4092,7 +4108,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="2:13">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
         <v>13</v>
       </c>
@@ -4119,7 +4135,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="32" spans="2:13">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
         <v>14</v>
       </c>
@@ -4146,7 +4162,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="33" spans="2:11">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <v>15</v>
       </c>
@@ -4167,7 +4183,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="2:11">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
         <v>16</v>
       </c>
@@ -4188,7 +4204,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="2:11">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
         <v>18</v>
       </c>
@@ -4213,7 +4229,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="2:11">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
         <v>21</v>
       </c>
@@ -4240,7 +4256,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="2:11">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
         <v>22</v>
       </c>
@@ -4267,7 +4283,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="30">
+    <row r="38" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B38" s="3">
         <v>23</v>
       </c>
@@ -4294,7 +4310,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="39" spans="2:11">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
         <v>24</v>
       </c>
@@ -4321,7 +4337,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="2:11">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
         <v>31</v>
       </c>
@@ -4350,7 +4366,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="2:11">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
         <v>32</v>
       </c>
@@ -4377,7 +4393,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="2:11">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="3">
         <v>33</v>
       </c>
@@ -4406,7 +4422,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="2:11">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
         <v>34</v>
       </c>
@@ -4433,7 +4449,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="2:11">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
         <v>35</v>
       </c>
@@ -4460,7 +4476,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="2:11">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
         <v>36</v>
       </c>
@@ -4489,7 +4505,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="46" spans="2:11">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
         <v>41</v>
       </c>
@@ -4497,15 +4513,17 @@
         <v>147</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>57</v>
+        <v>847</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>6</v>
+        <v>846</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="G46" s="4"/>
+      <c r="G46" s="4" t="s">
+        <v>848</v>
+      </c>
       <c r="I46" s="4" t="s">
         <v>105</v>
       </c>
@@ -4516,7 +4534,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="2:11">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="3">
         <v>42</v>
       </c>
@@ -4543,7 +4561,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="2:11">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>151</v>
       </c>
@@ -4570,7 +4588,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="2:11">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="3">
         <v>60</v>
       </c>
@@ -4597,7 +4615,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="2:11">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="3">
         <v>61</v>
       </c>
@@ -4624,7 +4642,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="2:11">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="3">
         <v>62</v>
       </c>
@@ -4651,7 +4669,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="2:11" s="38" customFormat="1">
+    <row r="52" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="35">
         <v>63</v>
       </c>
@@ -4678,7 +4696,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="2:11">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="3">
         <v>68</v>
       </c>
@@ -4705,7 +4723,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="54" spans="2:11">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" s="3">
         <v>69</v>
       </c>
@@ -4728,7 +4746,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="2:11">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="3">
         <v>71</v>
       </c>
@@ -4753,7 +4771,7 @@
       </c>
       <c r="K55" s="4"/>
     </row>
-    <row r="56" spans="2:11">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="3">
         <v>72</v>
       </c>
@@ -4774,7 +4792,7 @@
       </c>
       <c r="K56" s="4"/>
     </row>
-    <row r="57" spans="2:11" ht="30">
+    <row r="57" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B57" s="3">
         <v>74</v>
       </c>
@@ -4801,7 +4819,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="2:11">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="3">
         <v>75</v>
       </c>
@@ -4828,7 +4846,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="59" spans="2:11">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -4839,7 +4857,7 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
     </row>
-    <row r="60" spans="2:11">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="3">
         <v>81</v>
       </c>
@@ -4864,7 +4882,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="61" spans="2:11">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" s="3">
         <v>82</v>
       </c>
@@ -4889,7 +4907,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="62" spans="2:11">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" s="3"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -4900,7 +4918,7 @@
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
     </row>
-    <row r="63" spans="2:11">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" s="3">
         <v>91</v>
       </c>
@@ -4923,7 +4941,7 @@
       </c>
       <c r="K63" s="4"/>
     </row>
-    <row r="64" spans="2:11">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" s="3">
         <v>92</v>
       </c>
@@ -4944,7 +4962,7 @@
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
     </row>
-    <row r="65" spans="2:11">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" s="3">
         <v>93</v>
       </c>
@@ -4965,7 +4983,7 @@
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
     </row>
-    <row r="66" spans="2:11">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" s="3">
         <v>94</v>
       </c>
@@ -4984,7 +5002,7 @@
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
     </row>
-    <row r="67" spans="2:11">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" s="3"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
@@ -4995,7 +5013,7 @@
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
     </row>
-    <row r="68" spans="2:11" s="38" customFormat="1">
+    <row r="68" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="35" t="s">
         <v>80</v>
       </c>
@@ -5024,7 +5042,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="69" spans="2:11" s="38" customFormat="1">
+    <row r="69" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="35" t="s">
         <v>85</v>
       </c>
@@ -5051,7 +5069,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="71" spans="2:11">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
         <v>518</v>
       </c>
@@ -5093,7 +5111,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
@@ -5103,7 +5121,7 @@
     <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="40" t="s">
         <v>218</v>
       </c>
@@ -5130,7 +5148,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="39" t="s">
         <v>226</v>
       </c>
@@ -5156,7 +5174,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>217</v>
       </c>
@@ -5182,7 +5200,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>327</v>
       </c>
@@ -5208,7 +5226,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>330</v>
       </c>
@@ -5234,7 +5252,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>215</v>
       </c>
@@ -5260,7 +5278,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>216</v>
       </c>
@@ -5286,7 +5304,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>278</v>
       </c>
@@ -5306,7 +5324,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>279</v>
       </c>
@@ -5326,7 +5344,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>277</v>
       </c>
@@ -5346,7 +5364,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>285</v>
       </c>
@@ -5366,7 +5384,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>256</v>
       </c>
@@ -5383,7 +5401,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>257</v>
       </c>
@@ -5403,7 +5421,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>227</v>
       </c>
@@ -5426,7 +5444,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>230</v>
       </c>
@@ -5449,7 +5467,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>234</v>
       </c>
@@ -5472,7 +5490,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>241</v>
       </c>
@@ -5495,7 +5513,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>319</v>
       </c>
@@ -5515,7 +5533,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>320</v>
       </c>
@@ -5535,7 +5553,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>321</v>
       </c>
@@ -5555,7 +5573,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>235</v>
       </c>
@@ -5578,7 +5596,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>236</v>
       </c>
@@ -5601,7 +5619,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>240</v>
       </c>
@@ -5624,7 +5642,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>244</v>
       </c>
@@ -5647,7 +5665,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>245</v>
       </c>
@@ -5670,7 +5688,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>246</v>
       </c>
@@ -5693,7 +5711,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>262</v>
       </c>
@@ -5713,7 +5731,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>263</v>
       </c>
@@ -5733,7 +5751,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>265</v>
       </c>
@@ -5753,7 +5771,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>274</v>
       </c>
@@ -5776,7 +5794,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>250</v>
       </c>
@@ -5799,7 +5817,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>267</v>
       </c>
@@ -5819,7 +5837,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>268</v>
       </c>
@@ -5839,7 +5857,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>272</v>
       </c>
@@ -5877,7 +5895,7 @@
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13.5703125" customWidth="1"/>
@@ -5886,7 +5904,7 @@
     <col min="9" max="9" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
         <v>721</v>
       </c>
@@ -5894,7 +5912,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -5911,7 +5929,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -5921,12 +5939,12 @@
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="78" t="s">
+      <c r="E3" s="79" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="45"/>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -5936,10 +5954,10 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="78"/>
+      <c r="E4" s="79"/>
       <c r="F4" s="45"/>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5954,7 +5972,7 @@
       </c>
       <c r="F5" s="45"/>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -5969,7 +5987,7 @@
       </c>
       <c r="F6" s="45"/>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -5989,7 +6007,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>126</v>
       </c>
@@ -6012,7 +6030,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>186</v>
       </c>
@@ -6035,7 +6053,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>400</v>
       </c>
@@ -6058,7 +6076,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>753</v>
       </c>
@@ -6071,7 +6089,7 @@
       <c r="E11" s="68"/>
       <c r="F11" s="45"/>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>348</v>
       </c>
@@ -6094,7 +6112,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>351</v>
       </c>
@@ -6117,7 +6135,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>353</v>
       </c>
@@ -6140,7 +6158,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>357</v>
       </c>
@@ -6166,7 +6184,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>18</v>
       </c>
@@ -6189,7 +6207,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>19</v>
       </c>
@@ -6212,7 +6230,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>20</v>
       </c>
@@ -6225,7 +6243,7 @@
       <c r="E18" s="68"/>
       <c r="F18" s="45"/>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>21</v>
       </c>
@@ -6248,7 +6266,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>22</v>
       </c>
@@ -6271,7 +6289,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>23</v>
       </c>
@@ -6294,7 +6312,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>24</v>
       </c>
@@ -6317,7 +6335,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>751</v>
       </c>
@@ -6330,7 +6348,7 @@
       <c r="E23" s="68"/>
       <c r="F23" s="45"/>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <v>31</v>
       </c>
@@ -6353,7 +6371,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <v>32</v>
       </c>
@@ -6376,7 +6394,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>33</v>
       </c>
@@ -6399,7 +6417,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <v>34</v>
       </c>
@@ -6412,7 +6430,7 @@
       <c r="E27" s="68"/>
       <c r="F27" s="45"/>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <v>35</v>
       </c>
@@ -6433,7 +6451,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <v>36</v>
       </c>
@@ -6454,7 +6472,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>37</v>
       </c>
@@ -6475,7 +6493,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="2:8">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>760</v>
       </c>
@@ -6496,7 +6514,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="32" spans="2:8">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
         <v>40</v>
       </c>
@@ -6509,7 +6527,7 @@
       <c r="E32" s="68"/>
       <c r="F32" s="45"/>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <v>41</v>
       </c>
@@ -6535,7 +6553,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
         <v>42</v>
       </c>
@@ -6558,7 +6576,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
         <v>43</v>
       </c>
@@ -6581,7 +6599,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
         <v>44</v>
       </c>
@@ -6607,7 +6625,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>746</v>
       </c>
@@ -6623,7 +6641,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>754</v>
       </c>
@@ -6646,7 +6664,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>755</v>
       </c>
@@ -6669,7 +6687,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
         <v>52</v>
       </c>
@@ -6692,7 +6710,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
         <v>53</v>
       </c>
@@ -6715,7 +6733,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="42" spans="2:9">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>752</v>
       </c>
@@ -6728,7 +6746,7 @@
       <c r="E42" s="68"/>
       <c r="F42" s="45"/>
     </row>
-    <row r="43" spans="2:9">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
         <v>58</v>
       </c>
@@ -6743,7 +6761,7 @@
       </c>
       <c r="F43" s="45"/>
     </row>
-    <row r="44" spans="2:9">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
         <v>59</v>
       </c>
@@ -6758,7 +6776,7 @@
       </c>
       <c r="F44" s="45"/>
     </row>
-    <row r="45" spans="2:9">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D45">
         <f>SUM(D3:D44)</f>
         <v>61</v>
@@ -6782,7 +6800,7 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="49"/>
     <col min="3" max="3" width="38.42578125" style="49" bestFit="1" customWidth="1"/>
@@ -6792,7 +6810,7 @@
     <col min="10" max="16384" width="9.140625" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D1" s="49" t="s">
         <v>607</v>
       </c>
@@ -6815,7 +6833,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="59" t="s">
         <v>20</v>
       </c>
@@ -6844,7 +6862,7 @@
       </c>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="59" t="s">
         <v>21</v>
       </c>
@@ -6873,7 +6891,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="59" t="s">
         <v>22</v>
       </c>
@@ -6902,7 +6920,7 @@
       </c>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="59" t="s">
         <v>23</v>
       </c>
@@ -6931,7 +6949,7 @@
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="2:11">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="59" t="s">
         <v>126</v>
       </c>
@@ -6960,7 +6978,7 @@
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="59" t="s">
         <v>186</v>
       </c>
@@ -6989,7 +7007,7 @@
       </c>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="59" t="s">
         <v>400</v>
       </c>
@@ -7005,7 +7023,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="59" t="s">
         <v>53</v>
       </c>
@@ -7034,7 +7052,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="59" t="s">
         <v>205</v>
       </c>
@@ -7063,7 +7081,7 @@
       </c>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="59" t="s">
         <v>415</v>
       </c>
@@ -7092,7 +7110,7 @@
       </c>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="2:11">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="59" t="s">
         <v>432</v>
       </c>
@@ -7121,7 +7139,7 @@
       </c>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="59" t="s">
         <v>436</v>
       </c>
@@ -7150,7 +7168,7 @@
       </c>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="59" t="s">
         <v>501</v>
       </c>
@@ -7179,7 +7197,7 @@
       </c>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="59">
         <v>10</v>
       </c>
@@ -7208,7 +7226,7 @@
       </c>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="59">
         <v>11</v>
       </c>
@@ -7237,7 +7255,7 @@
       </c>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="2:11">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="59">
         <v>12</v>
       </c>
@@ -7266,7 +7284,7 @@
       </c>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="2:11">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="59">
         <v>13</v>
       </c>
@@ -7295,7 +7313,7 @@
       </c>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="9">
         <v>14</v>
       </c>
@@ -7324,7 +7342,7 @@
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="9">
         <v>15</v>
       </c>
@@ -7353,7 +7371,7 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="9">
         <v>16</v>
       </c>
@@ -7382,7 +7400,7 @@
       </c>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="2:11">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="9">
         <v>18</v>
       </c>
@@ -7411,7 +7429,7 @@
       </c>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="2:11">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="9">
         <v>21</v>
       </c>
@@ -7440,7 +7458,7 @@
       </c>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="2:11">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="9">
         <v>22</v>
       </c>
@@ -7469,7 +7487,7 @@
       </c>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="9">
         <v>23</v>
       </c>
@@ -7498,7 +7516,7 @@
       </c>
       <c r="K25" s="10"/>
     </row>
-    <row r="26" spans="2:11">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="9">
         <v>24</v>
       </c>
@@ -7527,7 +7545,7 @@
       </c>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="2:11">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="9">
         <v>31</v>
       </c>
@@ -7556,7 +7574,7 @@
       </c>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="2:11">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="9">
         <v>32</v>
       </c>
@@ -7585,7 +7603,7 @@
       </c>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="2:11">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="9">
         <v>33</v>
       </c>
@@ -7614,7 +7632,7 @@
       </c>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="2:11">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="9">
         <v>34</v>
       </c>
@@ -7643,7 +7661,7 @@
       </c>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="2:11">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="9">
         <v>35</v>
       </c>
@@ -7672,7 +7690,7 @@
       </c>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="2:11">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="9">
         <v>36</v>
       </c>
@@ -7701,7 +7719,7 @@
       </c>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="2:11">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="9">
         <v>41</v>
       </c>
@@ -7730,7 +7748,7 @@
       </c>
       <c r="K33" s="10"/>
     </row>
-    <row r="34" spans="2:11">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="9">
         <v>42</v>
       </c>
@@ -7759,7 +7777,7 @@
       </c>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="2:11">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
         <v>151</v>
       </c>
@@ -7788,7 +7806,7 @@
       </c>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="2:11">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="9">
         <v>60</v>
       </c>
@@ -7817,7 +7835,7 @@
       </c>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="2:11">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="9">
         <v>61</v>
       </c>
@@ -7846,7 +7864,7 @@
       </c>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="2:11">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="9">
         <v>62</v>
       </c>
@@ -7875,7 +7893,7 @@
       </c>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="2:11">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="9">
         <v>68</v>
       </c>
@@ -7904,7 +7922,7 @@
       </c>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="2:11">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="9">
         <v>69</v>
       </c>
@@ -7933,7 +7951,7 @@
       </c>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="2:11">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="9">
         <v>71</v>
       </c>
@@ -7962,7 +7980,7 @@
       </c>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="2:11">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="9">
         <v>72</v>
       </c>
@@ -7991,7 +8009,7 @@
       </c>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="2:11">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="9">
         <v>74</v>
       </c>
@@ -8020,7 +8038,7 @@
       </c>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="2:11">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="9">
         <v>75</v>
       </c>
@@ -8049,7 +8067,7 @@
       </c>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="2:11">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="9" t="s">
         <v>518</v>
       </c>
@@ -8093,19 +8111,19 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -8116,27 +8134,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="79" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="78"/>
-    </row>
-    <row r="6" spans="2:4">
+      <c r="D5" s="79"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
@@ -8147,7 +8165,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
@@ -8158,7 +8176,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>649</v>
       </c>
@@ -8169,7 +8187,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>653</v>
       </c>
@@ -8180,7 +8198,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>660</v>
       </c>
@@ -8191,7 +8209,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>665</v>
       </c>
@@ -8202,7 +8220,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>666</v>
       </c>
@@ -8213,7 +8231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>14</v>
       </c>
@@ -8224,7 +8242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>15</v>
       </c>
@@ -8235,32 +8253,32 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="78" t="s">
+      <c r="D17" s="79" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="78"/>
-    </row>
-    <row r="19" spans="2:4">
+      <c r="D18" s="79"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
@@ -8271,7 +8289,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>648</v>
       </c>
@@ -8282,7 +8300,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>649</v>
       </c>
@@ -8293,7 +8311,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>650</v>
       </c>
@@ -8304,7 +8322,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>700</v>
       </c>
@@ -8315,7 +8333,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>702</v>
       </c>
@@ -8326,7 +8344,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="65" t="s">
         <v>705</v>
       </c>
@@ -8337,7 +8355,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="65" t="s">
         <v>706</v>
       </c>
@@ -8348,7 +8366,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="45">
         <v>126</v>
       </c>
@@ -8359,7 +8377,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="45">
         <v>127</v>
       </c>
@@ -8370,12 +8388,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="45">
         <v>0</v>
       </c>
@@ -8386,7 +8404,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="45">
         <v>1</v>
       </c>
@@ -8397,7 +8415,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="45">
         <v>2</v>
       </c>
@@ -8408,7 +8426,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="45">
         <v>3</v>
       </c>
@@ -8419,7 +8437,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="45">
         <v>4</v>
       </c>
@@ -8430,7 +8448,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="45">
         <v>5</v>
       </c>
@@ -8441,7 +8459,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="66" t="s">
         <v>680</v>
       </c>
@@ -8452,7 +8470,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="45">
         <v>8</v>
       </c>
@@ -8463,7 +8481,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="45">
         <v>9</v>
       </c>
@@ -8474,7 +8492,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="66" t="s">
         <v>684</v>
       </c>
@@ -8485,12 +8503,12 @@
         <v>694</v>
       </c>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>0</v>
       </c>
@@ -8501,27 +8519,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="78" t="s">
+      <c r="D45" s="79" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="78"/>
-    </row>
-    <row r="47" spans="2:4">
+      <c r="D46" s="79"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>21</v>
       </c>
@@ -8532,7 +8550,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>22</v>
       </c>
@@ -8543,7 +8561,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="2:4">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>649</v>
       </c>
@@ -8554,7 +8572,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="50" spans="2:4">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>650</v>
       </c>
@@ -8565,7 +8583,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="51" spans="2:4">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>660</v>
       </c>
@@ -8576,7 +8594,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="52" spans="2:4">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>665</v>
       </c>
@@ -8587,7 +8605,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="53" spans="2:4">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>666</v>
       </c>
@@ -8598,7 +8616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:4">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="3">
         <v>14</v>
       </c>
@@ -8609,7 +8627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="2:4">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="3">
         <v>15</v>
       </c>
@@ -8636,11 +8654,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
@@ -8649,7 +8667,7 @@
     <col min="6" max="6" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -8666,7 +8684,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -8676,12 +8694,12 @@
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="78" t="s">
+      <c r="E3" s="79" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="45"/>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -8691,10 +8709,10 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="78"/>
+      <c r="E4" s="79"/>
       <c r="F4" s="45"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -8709,7 +8727,7 @@
       </c>
       <c r="F5" s="45"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -8724,7 +8742,7 @@
       </c>
       <c r="F6" s="45"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -8741,7 +8759,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>126</v>
       </c>
@@ -8758,7 +8776,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>186</v>
       </c>
@@ -8775,7 +8793,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>400</v>
       </c>
@@ -8792,8 +8810,8 @@
         <v>403</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="79" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="78" t="s">
         <v>753</v>
       </c>
       <c r="C11" s="25" t="s">
@@ -8805,7 +8823,7 @@
       <c r="E11" s="72"/>
       <c r="F11" s="73"/>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>348</v>
       </c>
@@ -8822,7 +8840,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>351</v>
       </c>
@@ -8839,7 +8857,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>353</v>
       </c>
@@ -8856,7 +8874,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="77" t="s">
         <v>357</v>
       </c>
@@ -8869,7 +8887,7 @@
       <c r="E15" s="72"/>
       <c r="F15" s="73"/>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>18</v>
       </c>
@@ -8886,7 +8904,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>19</v>
       </c>
@@ -8903,7 +8921,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="77">
         <v>20</v>
       </c>
@@ -8916,7 +8934,7 @@
       <c r="E18" s="72"/>
       <c r="F18" s="73"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>21</v>
       </c>
@@ -8933,7 +8951,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>22</v>
       </c>
@@ -8950,7 +8968,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>23</v>
       </c>
@@ -8967,7 +8985,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>24</v>
       </c>
@@ -8984,7 +9002,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="77" t="s">
         <v>806</v>
       </c>
@@ -8997,7 +9015,7 @@
       <c r="E23" s="72"/>
       <c r="F23" s="73"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <v>31</v>
       </c>
@@ -9014,7 +9032,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <v>32</v>
       </c>
@@ -9031,7 +9049,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>33</v>
       </c>
@@ -9048,7 +9066,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="77">
         <v>34</v>
       </c>
@@ -9061,7 +9079,7 @@
       <c r="E27" s="72"/>
       <c r="F27" s="73"/>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <v>35</v>
       </c>
@@ -9078,7 +9096,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <v>36</v>
       </c>
@@ -9095,7 +9113,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>37</v>
       </c>
@@ -9112,7 +9130,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>760</v>
       </c>
@@ -9129,7 +9147,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
         <v>40</v>
       </c>
@@ -9146,7 +9164,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <v>41</v>
       </c>
@@ -9163,7 +9181,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
         <v>42</v>
       </c>
@@ -9178,7 +9196,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
         <v>43</v>
       </c>
@@ -9193,7 +9211,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="77" t="s">
         <v>800</v>
       </c>
@@ -9206,7 +9224,7 @@
       <c r="E36" s="72"/>
       <c r="F36" s="73"/>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
         <v>47</v>
       </c>
@@ -9223,7 +9241,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>801</v>
       </c>
@@ -9240,7 +9258,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>802</v>
       </c>
@@ -9257,7 +9275,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="77">
         <v>52</v>
       </c>
@@ -9268,7 +9286,7 @@
       <c r="E40" s="72"/>
       <c r="F40" s="73"/>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
         <v>53</v>
       </c>
@@ -9285,7 +9303,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="3">
         <v>54</v>
       </c>
@@ -9302,7 +9320,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="43" spans="2:6">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
         <v>53</v>
       </c>
@@ -9319,7 +9337,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="44" spans="2:6">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="77" t="s">
         <v>822</v>
       </c>
@@ -9330,7 +9348,7 @@
       <c r="E44" s="72"/>
       <c r="F44" s="73"/>
     </row>
-    <row r="45" spans="2:6">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
         <v>58</v>
       </c>
@@ -9345,7 +9363,7 @@
       </c>
       <c r="F45" s="45"/>
     </row>
-    <row r="46" spans="2:6">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
         <v>59</v>
       </c>
@@ -9360,7 +9378,7 @@
       </c>
       <c r="F46" s="45"/>
     </row>
-    <row r="47" spans="2:6">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D47">
         <f>SUM(D3:D46)</f>
         <v>61</v>
@@ -9370,6 +9388,7 @@
   <mergeCells count="1">
     <mergeCell ref="E3:E4"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -9383,7 +9402,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -9399,7 +9418,7 @@
     <col min="18" max="48" width="9.140625" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42">
+    <row r="1" spans="2:42" x14ac:dyDescent="0.25">
       <c r="I1" s="51" t="s">
         <v>441</v>
       </c>
@@ -9413,7 +9432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:42">
+    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -9472,14 +9491,14 @@
       <c r="AO2" s="11"/>
       <c r="AP2" s="11"/>
     </row>
-    <row r="3" spans="2:42">
+    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B3" s="54">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="79" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="47">
@@ -9529,14 +9548,14 @@
       <c r="AO3" s="11"/>
       <c r="AP3" s="11"/>
     </row>
-    <row r="4" spans="2:42">
+    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B4" s="55">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="78"/>
+      <c r="D4" s="79"/>
       <c r="E4" s="47">
         <v>1</v>
       </c>
@@ -9584,7 +9603,7 @@
       <c r="AO4" s="11"/>
       <c r="AP4" s="11"/>
     </row>
-    <row r="5" spans="2:42">
+    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B5" s="55">
         <v>2</v>
       </c>
@@ -9641,7 +9660,7 @@
       <c r="AO5" s="11"/>
       <c r="AP5" s="11"/>
     </row>
-    <row r="6" spans="2:42">
+    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B6" s="55">
         <v>3</v>
       </c>
@@ -9698,7 +9717,7 @@
       <c r="AO6" s="11"/>
       <c r="AP6" s="11"/>
     </row>
-    <row r="7" spans="2:42">
+    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B7" s="55">
         <v>4</v>
       </c>
@@ -9755,7 +9774,7 @@
       <c r="AO7" s="11"/>
       <c r="AP7" s="11"/>
     </row>
-    <row r="8" spans="2:42">
+    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B8" s="55">
         <v>5</v>
       </c>
@@ -9812,7 +9831,7 @@
       <c r="AO8" s="11"/>
       <c r="AP8" s="11"/>
     </row>
-    <row r="9" spans="2:42">
+    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B9" s="55">
         <v>6</v>
       </c>
@@ -9869,7 +9888,7 @@
       <c r="AO9" s="11"/>
       <c r="AP9" s="11"/>
     </row>
-    <row r="10" spans="2:42">
+    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B10" s="55">
         <v>8</v>
       </c>
@@ -9926,7 +9945,7 @@
       <c r="AO10" s="11"/>
       <c r="AP10" s="11"/>
     </row>
-    <row r="11" spans="2:42">
+    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B11" s="55">
         <v>9</v>
       </c>
@@ -9983,7 +10002,7 @@
       <c r="AO11" s="11"/>
       <c r="AP11" s="11"/>
     </row>
-    <row r="12" spans="2:42">
+    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B12" s="55">
         <v>10</v>
       </c>
@@ -10040,7 +10059,7 @@
       <c r="AO12" s="11"/>
       <c r="AP12" s="11"/>
     </row>
-    <row r="13" spans="2:42">
+    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B13" s="55">
         <v>40</v>
       </c>
@@ -10097,7 +10116,7 @@
       <c r="AO13" s="11"/>
       <c r="AP13" s="11"/>
     </row>
-    <row r="14" spans="2:42">
+    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B14" s="55">
         <v>60</v>
       </c>
@@ -10154,7 +10173,7 @@
       <c r="AO14" s="11"/>
       <c r="AP14" s="11"/>
     </row>
-    <row r="15" spans="2:42">
+    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B15" s="55">
         <v>61</v>
       </c>
@@ -10211,7 +10230,7 @@
       <c r="AO15" s="11"/>
       <c r="AP15" s="11"/>
     </row>
-    <row r="16" spans="2:42">
+    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B16" s="55">
         <v>62</v>
       </c>
@@ -10268,7 +10287,7 @@
       <c r="AO16" s="11"/>
       <c r="AP16" s="11"/>
     </row>
-    <row r="17" spans="2:42">
+    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B17" s="55">
         <v>63</v>
       </c>
@@ -10325,7 +10344,7 @@
       <c r="AO17" s="11"/>
       <c r="AP17" s="11"/>
     </row>
-    <row r="18" spans="2:42">
+    <row r="18" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B18" s="55">
         <v>64</v>
       </c>
@@ -10382,7 +10401,7 @@
       <c r="AO18" s="11"/>
       <c r="AP18" s="11"/>
     </row>
-    <row r="19" spans="2:42">
+    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B19" s="55">
         <v>84</v>
       </c>
@@ -10439,7 +10458,7 @@
       <c r="AO19" s="11"/>
       <c r="AP19" s="11"/>
     </row>
-    <row r="20" spans="2:42">
+    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B20" s="55">
         <v>104</v>
       </c>
@@ -10496,7 +10515,7 @@
       <c r="AO20" s="11"/>
       <c r="AP20" s="11"/>
     </row>
-    <row r="21" spans="2:42">
+    <row r="21" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B21" s="55">
         <v>105</v>
       </c>
@@ -10553,7 +10572,7 @@
       <c r="AO21" s="11"/>
       <c r="AP21" s="11"/>
     </row>
-    <row r="22" spans="2:42">
+    <row r="22" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B22" s="55">
         <v>106</v>
       </c>
@@ -10610,7 +10629,7 @@
       <c r="AO22" s="11"/>
       <c r="AP22" s="11"/>
     </row>
-    <row r="23" spans="2:42">
+    <row r="23" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B23" s="55">
         <v>108</v>
       </c>
@@ -10667,7 +10686,7 @@
       <c r="AO23" s="11"/>
       <c r="AP23" s="11"/>
     </row>
-    <row r="24" spans="2:42">
+    <row r="24" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B24" s="55">
         <v>109</v>
       </c>
@@ -10724,7 +10743,7 @@
       <c r="AO24" s="11"/>
       <c r="AP24" s="11"/>
     </row>
-    <row r="25" spans="2:42">
+    <row r="25" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B25" s="55">
         <v>110</v>
       </c>
@@ -10781,7 +10800,7 @@
       <c r="AO25" s="11"/>
       <c r="AP25" s="11"/>
     </row>
-    <row r="26" spans="2:42">
+    <row r="26" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B26" s="55">
         <v>112</v>
       </c>
@@ -10838,7 +10857,7 @@
       <c r="AO26" s="11"/>
       <c r="AP26" s="11"/>
     </row>
-    <row r="27" spans="2:42">
+    <row r="27" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B27" s="55">
         <v>114</v>
       </c>
@@ -10895,7 +10914,7 @@
       <c r="AO27" s="11"/>
       <c r="AP27" s="11"/>
     </row>
-    <row r="28" spans="2:42">
+    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B28" s="55">
         <v>118</v>
       </c>
@@ -10944,7 +10963,7 @@
       <c r="AO28" s="11"/>
       <c r="AP28" s="11"/>
     </row>
-    <row r="29" spans="2:42">
+    <row r="29" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B29" s="55">
         <v>119</v>
       </c>
@@ -10993,7 +11012,7 @@
       <c r="AO29" s="11"/>
       <c r="AP29" s="11"/>
     </row>
-    <row r="30" spans="2:42">
+    <row r="30" spans="2:42" x14ac:dyDescent="0.25">
       <c r="E30">
         <f>SUM(E3:E29)</f>
         <v>120</v>
@@ -11033,7 +11052,7 @@
       <c r="AO30" s="11"/>
       <c r="AP30" s="11"/>
     </row>
-    <row r="31" spans="2:42">
+    <row r="31" spans="2:42" x14ac:dyDescent="0.25">
       <c r="I31" s="50"/>
       <c r="J31" s="50"/>
       <c r="K31" s="50"/>
@@ -11087,14 +11106,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -11105,27 +11124,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="79" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="78"/>
-    </row>
-    <row r="5" spans="2:4">
+      <c r="D4" s="79"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -11136,7 +11155,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -11147,7 +11166,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -11158,7 +11177,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>421</v>
       </c>
@@ -11169,7 +11188,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>424</v>
       </c>
@@ -11180,7 +11199,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>427</v>
       </c>
@@ -11191,7 +11210,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>430</v>
       </c>
@@ -11202,7 +11221,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>58</v>
       </c>
@@ -11213,7 +11232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>59</v>
       </c>
@@ -11241,14 +11260,14 @@
       <selection activeCell="B2" sqref="B2:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="1" customFormat="1">
+    <row r="2" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -11259,27 +11278,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" s="1" customFormat="1">
+    <row r="3" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="79" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="1" customFormat="1">
+    <row r="4" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="78"/>
-    </row>
-    <row r="5" spans="2:4" s="1" customFormat="1">
+      <c r="D4" s="79"/>
+    </row>
+    <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -11290,7 +11309,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:4" s="1" customFormat="1">
+    <row r="6" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -11301,7 +11320,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="1" customFormat="1">
+    <row r="7" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -11312,7 +11331,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="2:4" s="1" customFormat="1">
+    <row r="8" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>343</v>
       </c>
@@ -11323,7 +11342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="1" customFormat="1">
+    <row r="9" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>339</v>
       </c>
@@ -11334,7 +11353,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="10" spans="2:4" s="1" customFormat="1">
+    <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>340</v>
       </c>
@@ -11345,7 +11364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" s="1" customFormat="1">
+    <row r="11" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>58</v>
       </c>
@@ -11356,7 +11375,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:4" s="1" customFormat="1">
+    <row r="12" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>59</v>
       </c>
@@ -11384,7 +11403,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -11395,12 +11414,12 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="18.75">
+    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>139</v>
       </c>
@@ -11408,12 +11427,12 @@
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -11424,27 +11443,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="78" t="s">
+      <c r="D7" s="79" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="78"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="79"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -11455,7 +11474,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -11466,7 +11485,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
@@ -11477,7 +11496,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>126</v>
       </c>
@@ -11488,7 +11507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>127</v>
       </c>
@@ -11499,7 +11518,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>26</v>
       </c>
@@ -11510,7 +11529,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>27</v>
       </c>
@@ -11521,7 +11540,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>28</v>
       </c>
@@ -11532,7 +11551,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>29</v>
       </c>
@@ -11543,7 +11562,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>129</v>
       </c>
@@ -11554,7 +11573,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>124</v>
       </c>
@@ -11565,7 +11584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>130</v>
       </c>
@@ -11576,7 +11595,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>131</v>
       </c>
@@ -11587,7 +11606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>58</v>
       </c>
@@ -11598,7 +11617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>59</v>
       </c>
@@ -11609,17 +11628,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" ht="18.75">
+    <row r="25" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
@@ -11630,27 +11649,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="78" t="s">
+      <c r="D28" s="79" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="78"/>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="D29" s="79"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
@@ -11661,7 +11680,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>22</v>
       </c>
@@ -11672,7 +11691,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>23</v>
       </c>
@@ -11683,7 +11702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>126</v>
       </c>
@@ -11694,7 +11713,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>186</v>
       </c>
@@ -11705,7 +11724,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>187</v>
       </c>
@@ -11716,7 +11735,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>188</v>
       </c>
@@ -11727,7 +11746,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>189</v>
       </c>
@@ -11738,7 +11757,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>190</v>
       </c>
@@ -11749,7 +11768,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
         <v>51</v>
       </c>
@@ -11760,7 +11779,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
         <v>52</v>
       </c>
@@ -11771,7 +11790,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
         <v>53</v>
       </c>
@@ -11782,7 +11801,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="2:4">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="3">
         <v>54</v>
       </c>
@@ -11793,7 +11812,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
         <v>55</v>
       </c>
@@ -11804,7 +11823,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>201</v>
       </c>
@@ -11815,7 +11834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
         <v>58</v>
       </c>
@@ -11826,7 +11845,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
         <v>59</v>
       </c>
@@ -11837,17 +11856,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
     </row>
-    <row r="49" spans="3:4">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>140</v>
       </c>
@@ -11855,17 +11874,17 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="3:4">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D50" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="3:4">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D51" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="3:4">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D52" s="1" t="s">
         <v>144</v>
       </c>
@@ -11889,17 +11908,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="158.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:3" ht="60">
+    <row r="2" spans="3:3" ht="63" x14ac:dyDescent="0.25">
       <c r="C2" s="24" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="3:3">
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
- Add startup action - Use servo to change direction for maze solver
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="866">
   <si>
     <t>Offset</t>
   </si>
@@ -1904,7 +1904,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1925,7 +1925,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1936,7 +1936,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1953,7 +1953,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1964,7 +1964,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1980,7 +1980,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1997,7 +1997,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -2030,7 +2030,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2040,7 +2040,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2682,9 +2682,6 @@
     <t xml:space="preserve">RC_MPU_POSITION_CHECK_FREQ </t>
   </si>
   <si>
-    <t>44~46</t>
-  </si>
-  <si>
     <t>48~49</t>
   </si>
   <si>
@@ -2700,9 +2697,6 @@
     <t>RC_TOUCH_RELEASE_PERIOD</t>
   </si>
   <si>
-    <t>25~30</t>
-  </si>
-  <si>
     <t>Enable Sonic</t>
   </si>
   <si>
@@ -2748,9 +2742,6 @@
     <t>{mpuEnabled}</t>
   </si>
   <si>
-    <t>55~57</t>
-  </si>
-  <si>
     <t>{mpuPositionCheckFreq}</t>
   </si>
   <si>
@@ -2831,17 +2822,77 @@
   <si>
     <t>A9 9A 04 41 00 02 47 ED</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>I+E31:G78gnore repeat button period in ms (200)</t>
+  </si>
+  <si>
+    <t>{startupAction}</t>
+  </si>
+  <si>
+    <t>Action to be play at startup (0 = none)</t>
+  </si>
+  <si>
+    <t>RC_STARTUP_ACTION</t>
+  </si>
+  <si>
+    <t>Total(byte)</t>
+  </si>
+  <si>
+    <t>{mazeServoId}</t>
+  </si>
+  <si>
+    <t>Servo to be used for maze detection</t>
+  </si>
+  <si>
+    <t>RC_MAZE_SERVO</t>
+  </si>
+  <si>
+    <t>Distance of wall</t>
+  </si>
+  <si>
+    <t>RC_MAZE_WALL_DISTANCE</t>
+  </si>
+  <si>
+    <t>{mazeWallDistance}</t>
+  </si>
+  <si>
+    <t>{mazeServoDirection}</t>
+  </si>
+  <si>
+    <t>{mazeServoMoveMs}</t>
+  </si>
+  <si>
+    <t>{mazeServoWaitMs}</t>
+  </si>
+  <si>
+    <t>Maze servo setting: 0 : 0 = left, 1 : 0 = right</t>
+  </si>
+  <si>
+    <t>RC_MAZE_SERVO_DIRECTION</t>
+  </si>
+  <si>
+    <t>Maze servo move time to next position</t>
+  </si>
+  <si>
+    <t>Maze servo wait time for movement</t>
+  </si>
+  <si>
+    <t>RC_MAZE_SERVO_MOVE_MS</t>
+  </si>
+  <si>
+    <t>RC_MAZE_SERVO_WAIT_MS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2849,7 +2900,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2859,7 +2910,7 @@
       <u/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2869,19 +2920,19 @@
       <u/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2889,7 +2940,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2897,7 +2948,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2961,7 +3012,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3180,6 +3231,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3486,14 +3541,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="G31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -3507,7 +3562,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3515,7 +3570,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -3526,7 +3581,7 @@
       <c r="G3" s="13"/>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -3538,7 +3593,7 @@
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -3550,7 +3605,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -3566,7 +3621,7 @@
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14">
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -3575,7 +3630,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14">
       <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
@@ -3584,7 +3639,7 @@
       </c>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14">
       <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
@@ -3593,7 +3648,7 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14">
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
@@ -3622,7 +3677,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14">
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
@@ -3630,7 +3685,7 @@
         <v>40</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>155</v>
@@ -3651,7 +3706,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
@@ -3680,7 +3735,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14">
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
@@ -3709,7 +3764,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
@@ -3732,7 +3787,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13">
       <c r="B17" s="5" t="s">
         <v>126</v>
       </c>
@@ -3755,7 +3810,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13">
       <c r="B18" s="5" t="s">
         <v>186</v>
       </c>
@@ -3778,7 +3833,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13">
       <c r="B19" s="5" t="s">
         <v>400</v>
       </c>
@@ -3807,7 +3862,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13">
       <c r="B20" s="5" t="s">
         <v>769</v>
       </c>
@@ -3832,7 +3887,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13">
       <c r="B21" s="5" t="s">
         <v>772</v>
       </c>
@@ -3861,7 +3916,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" ht="45">
       <c r="B22" s="5" t="s">
         <v>53</v>
       </c>
@@ -3890,7 +3945,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13">
       <c r="B23" s="5" t="s">
         <v>205</v>
       </c>
@@ -3917,7 +3972,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13">
       <c r="B24" s="5" t="s">
         <v>415</v>
       </c>
@@ -3942,7 +3997,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13">
       <c r="B25" s="5" t="s">
         <v>432</v>
       </c>
@@ -3967,7 +4022,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13">
       <c r="B26" s="5" t="s">
         <v>436</v>
       </c>
@@ -3995,7 +4050,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13">
       <c r="B27" s="5" t="s">
         <v>501</v>
       </c>
@@ -4027,7 +4082,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13">
       <c r="B28" s="5">
         <v>10</v>
       </c>
@@ -4054,7 +4109,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13">
       <c r="B29" s="5">
         <v>11</v>
       </c>
@@ -4081,7 +4136,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13">
       <c r="B30" s="5">
         <v>12</v>
       </c>
@@ -4108,7 +4163,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13">
       <c r="B31" s="5">
         <v>13</v>
       </c>
@@ -4135,7 +4190,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13">
       <c r="B32" s="3">
         <v>14</v>
       </c>
@@ -4162,7 +4217,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11">
       <c r="B33" s="3">
         <v>15</v>
       </c>
@@ -4183,7 +4238,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11">
       <c r="B34" s="3">
         <v>16</v>
       </c>
@@ -4204,7 +4259,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11">
       <c r="B35" s="3">
         <v>18</v>
       </c>
@@ -4229,7 +4284,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11">
       <c r="B36" s="3">
         <v>21</v>
       </c>
@@ -4256,7 +4311,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11">
       <c r="B37" s="3">
         <v>22</v>
       </c>
@@ -4283,7 +4338,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" ht="30">
       <c r="B38" s="3">
         <v>23</v>
       </c>
@@ -4310,7 +4365,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11">
       <c r="B39" s="3">
         <v>24</v>
       </c>
@@ -4337,7 +4392,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11">
       <c r="B40" s="3">
         <v>31</v>
       </c>
@@ -4366,7 +4421,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11">
       <c r="B41" s="3">
         <v>32</v>
       </c>
@@ -4393,7 +4448,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11">
       <c r="B42" s="3">
         <v>33</v>
       </c>
@@ -4422,7 +4477,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11">
       <c r="B43" s="3">
         <v>34</v>
       </c>
@@ -4449,7 +4504,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11">
       <c r="B44" s="3">
         <v>35</v>
       </c>
@@ -4476,7 +4531,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11">
       <c r="B45" s="3">
         <v>36</v>
       </c>
@@ -4505,7 +4560,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11">
       <c r="B46" s="3">
         <v>41</v>
       </c>
@@ -4513,16 +4568,16 @@
         <v>147</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>213</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="I46" s="4" t="s">
         <v>105</v>
@@ -4534,7 +4589,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11">
       <c r="B47" s="3">
         <v>42</v>
       </c>
@@ -4561,7 +4616,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11">
       <c r="B48" s="3" t="s">
         <v>151</v>
       </c>
@@ -4588,7 +4643,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11">
       <c r="B49" s="3">
         <v>60</v>
       </c>
@@ -4615,7 +4670,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11">
       <c r="B50" s="3">
         <v>61</v>
       </c>
@@ -4642,7 +4697,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11">
       <c r="B51" s="3">
         <v>62</v>
       </c>
@@ -4669,7 +4724,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" s="38" customFormat="1">
       <c r="B52" s="35">
         <v>63</v>
       </c>
@@ -4696,7 +4751,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11">
       <c r="B53" s="3">
         <v>68</v>
       </c>
@@ -4723,7 +4778,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11">
       <c r="B54" s="3">
         <v>69</v>
       </c>
@@ -4746,7 +4801,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11">
       <c r="B55" s="3">
         <v>71</v>
       </c>
@@ -4771,7 +4826,7 @@
       </c>
       <c r="K55" s="4"/>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11">
       <c r="B56" s="3">
         <v>72</v>
       </c>
@@ -4792,7 +4847,7 @@
       </c>
       <c r="K56" s="4"/>
     </row>
-    <row r="57" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" ht="30">
       <c r="B57" s="3">
         <v>74</v>
       </c>
@@ -4819,7 +4874,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11">
       <c r="B58" s="3">
         <v>75</v>
       </c>
@@ -4846,7 +4901,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11">
       <c r="B59" s="3"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -4857,7 +4912,7 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11">
       <c r="B60" s="3">
         <v>81</v>
       </c>
@@ -4882,7 +4937,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11">
       <c r="B61" s="3">
         <v>82</v>
       </c>
@@ -4907,7 +4962,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11">
       <c r="B62" s="3"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -4918,7 +4973,7 @@
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11">
       <c r="B63" s="3">
         <v>91</v>
       </c>
@@ -4941,7 +4996,7 @@
       </c>
       <c r="K63" s="4"/>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11">
       <c r="B64" s="3">
         <v>92</v>
       </c>
@@ -4962,7 +5017,7 @@
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11">
       <c r="B65" s="3">
         <v>93</v>
       </c>
@@ -4983,7 +5038,7 @@
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11">
       <c r="B66" s="3">
         <v>94</v>
       </c>
@@ -5002,7 +5057,7 @@
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:11">
       <c r="B67" s="3"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
@@ -5013,7 +5068,7 @@
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
     </row>
-    <row r="68" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:11" s="38" customFormat="1">
       <c r="B68" s="35" t="s">
         <v>80</v>
       </c>
@@ -5042,7 +5097,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="69" spans="2:11" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:11" s="38" customFormat="1">
       <c r="B69" s="35" t="s">
         <v>85</v>
       </c>
@@ -5069,7 +5124,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:11">
       <c r="B71" s="3" t="s">
         <v>518</v>
       </c>
@@ -5111,7 +5166,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
@@ -5121,7 +5176,7 @@
     <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10">
       <c r="B3" s="40" t="s">
         <v>218</v>
       </c>
@@ -5148,7 +5203,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="B4" s="39" t="s">
         <v>226</v>
       </c>
@@ -5174,7 +5229,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="B5" t="s">
         <v>217</v>
       </c>
@@ -5200,7 +5255,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="B6" t="s">
         <v>327</v>
       </c>
@@ -5226,7 +5281,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10">
       <c r="B7" t="s">
         <v>330</v>
       </c>
@@ -5252,7 +5307,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="B8" t="s">
         <v>215</v>
       </c>
@@ -5278,7 +5333,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="B9" t="s">
         <v>216</v>
       </c>
@@ -5304,7 +5359,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="B10" t="s">
         <v>278</v>
       </c>
@@ -5324,7 +5379,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="B11" t="s">
         <v>279</v>
       </c>
@@ -5344,7 +5399,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10">
       <c r="B12" t="s">
         <v>277</v>
       </c>
@@ -5364,7 +5419,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10">
       <c r="B13" t="s">
         <v>285</v>
       </c>
@@ -5384,7 +5439,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10">
       <c r="B15" t="s">
         <v>256</v>
       </c>
@@ -5401,7 +5456,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10">
       <c r="B16" t="s">
         <v>257</v>
       </c>
@@ -5421,7 +5476,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9">
       <c r="B18" t="s">
         <v>227</v>
       </c>
@@ -5444,7 +5499,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9">
       <c r="B20" t="s">
         <v>230</v>
       </c>
@@ -5467,7 +5522,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9">
       <c r="B21" t="s">
         <v>234</v>
       </c>
@@ -5490,7 +5545,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9">
       <c r="B22" t="s">
         <v>241</v>
       </c>
@@ -5513,7 +5568,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9">
       <c r="B23" t="s">
         <v>319</v>
       </c>
@@ -5533,7 +5588,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9">
       <c r="B24" t="s">
         <v>320</v>
       </c>
@@ -5553,7 +5608,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9">
       <c r="B25" t="s">
         <v>321</v>
       </c>
@@ -5573,7 +5628,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9">
       <c r="B27" t="s">
         <v>235</v>
       </c>
@@ -5596,7 +5651,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9">
       <c r="B28" t="s">
         <v>236</v>
       </c>
@@ -5619,7 +5674,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9">
       <c r="B29" t="s">
         <v>240</v>
       </c>
@@ -5642,7 +5697,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9">
       <c r="B30" t="s">
         <v>244</v>
       </c>
@@ -5665,7 +5720,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9">
       <c r="B31" t="s">
         <v>245</v>
       </c>
@@ -5688,7 +5743,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9">
       <c r="B32" t="s">
         <v>246</v>
       </c>
@@ -5711,7 +5766,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9">
       <c r="B33" t="s">
         <v>262</v>
       </c>
@@ -5731,7 +5786,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9">
       <c r="B34" t="s">
         <v>263</v>
       </c>
@@ -5751,7 +5806,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9">
       <c r="B35" t="s">
         <v>265</v>
       </c>
@@ -5771,7 +5826,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" t="s">
         <v>274</v>
       </c>
@@ -5794,7 +5849,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9">
       <c r="B38" t="s">
         <v>250</v>
       </c>
@@ -5817,7 +5872,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9">
       <c r="B39" t="s">
         <v>267</v>
       </c>
@@ -5837,7 +5892,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9">
       <c r="B40" t="s">
         <v>268</v>
       </c>
@@ -5857,7 +5912,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9">
       <c r="B41" t="s">
         <v>272</v>
       </c>
@@ -5895,7 +5950,7 @@
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13.5703125" customWidth="1"/>
@@ -5904,7 +5959,7 @@
     <col min="9" max="9" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9">
       <c r="G1" t="s">
         <v>721</v>
       </c>
@@ -5912,7 +5967,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -5929,7 +5984,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -5944,7 +5999,7 @@
       </c>
       <c r="F3" s="45"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -5957,7 +6012,7 @@
       <c r="E4" s="79"/>
       <c r="F4" s="45"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5972,7 +6027,7 @@
       </c>
       <c r="F5" s="45"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -5987,7 +6042,7 @@
       </c>
       <c r="F6" s="45"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -6007,7 +6062,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9">
       <c r="B8" s="5" t="s">
         <v>126</v>
       </c>
@@ -6030,7 +6085,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9">
       <c r="B9" s="5" t="s">
         <v>186</v>
       </c>
@@ -6053,7 +6108,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9">
       <c r="B10" s="5" t="s">
         <v>400</v>
       </c>
@@ -6076,7 +6131,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9">
       <c r="B11" s="5" t="s">
         <v>753</v>
       </c>
@@ -6089,7 +6144,7 @@
       <c r="E11" s="68"/>
       <c r="F11" s="45"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9">
       <c r="B12" s="3" t="s">
         <v>348</v>
       </c>
@@ -6112,7 +6167,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9">
       <c r="B13" s="3" t="s">
         <v>351</v>
       </c>
@@ -6135,7 +6190,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9">
       <c r="B14" s="3" t="s">
         <v>353</v>
       </c>
@@ -6158,7 +6213,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9">
       <c r="B15" s="3" t="s">
         <v>357</v>
       </c>
@@ -6184,7 +6239,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9">
       <c r="B16" s="3">
         <v>18</v>
       </c>
@@ -6207,7 +6262,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8">
       <c r="B17" s="3">
         <v>19</v>
       </c>
@@ -6230,7 +6285,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8">
       <c r="B18" s="3">
         <v>20</v>
       </c>
@@ -6243,7 +6298,7 @@
       <c r="E18" s="68"/>
       <c r="F18" s="45"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8">
       <c r="B19" s="3">
         <v>21</v>
       </c>
@@ -6266,7 +6321,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8">
       <c r="B20" s="3">
         <v>22</v>
       </c>
@@ -6289,7 +6344,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8">
       <c r="B21" s="3">
         <v>23</v>
       </c>
@@ -6312,7 +6367,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8">
       <c r="B22" s="3">
         <v>24</v>
       </c>
@@ -6335,7 +6390,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8">
       <c r="B23" s="3" t="s">
         <v>751</v>
       </c>
@@ -6348,7 +6403,7 @@
       <c r="E23" s="68"/>
       <c r="F23" s="45"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8">
       <c r="B24" s="3">
         <v>31</v>
       </c>
@@ -6371,7 +6426,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8">
       <c r="B25" s="3">
         <v>32</v>
       </c>
@@ -6394,7 +6449,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8">
       <c r="B26" s="3">
         <v>33</v>
       </c>
@@ -6417,7 +6472,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8">
       <c r="B27" s="3">
         <v>34</v>
       </c>
@@ -6430,7 +6485,7 @@
       <c r="E27" s="68"/>
       <c r="F27" s="45"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8">
       <c r="B28" s="3">
         <v>35</v>
       </c>
@@ -6451,7 +6506,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8">
       <c r="B29" s="3">
         <v>36</v>
       </c>
@@ -6472,7 +6527,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8">
       <c r="B30" s="3">
         <v>37</v>
       </c>
@@ -6493,7 +6548,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8">
       <c r="B31" s="3" t="s">
         <v>760</v>
       </c>
@@ -6514,7 +6569,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8">
       <c r="B32" s="3">
         <v>40</v>
       </c>
@@ -6527,7 +6582,7 @@
       <c r="E32" s="68"/>
       <c r="F32" s="45"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9">
       <c r="B33" s="3">
         <v>41</v>
       </c>
@@ -6553,7 +6608,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9">
       <c r="B34" s="3">
         <v>42</v>
       </c>
@@ -6576,7 +6631,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9">
       <c r="B35" s="3">
         <v>43</v>
       </c>
@@ -6599,7 +6654,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" s="3">
         <v>44</v>
       </c>
@@ -6625,7 +6680,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9">
       <c r="B37" s="3" t="s">
         <v>746</v>
       </c>
@@ -6641,7 +6696,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9">
       <c r="B38" s="3" t="s">
         <v>754</v>
       </c>
@@ -6664,7 +6719,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9">
       <c r="B39" s="3" t="s">
         <v>755</v>
       </c>
@@ -6687,7 +6742,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9">
       <c r="B40" s="3">
         <v>52</v>
       </c>
@@ -6710,7 +6765,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9">
       <c r="B41" s="3">
         <v>53</v>
       </c>
@@ -6733,7 +6788,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9">
       <c r="B42" s="3" t="s">
         <v>752</v>
       </c>
@@ -6746,7 +6801,7 @@
       <c r="E42" s="68"/>
       <c r="F42" s="45"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9">
       <c r="B43" s="3">
         <v>58</v>
       </c>
@@ -6761,7 +6816,7 @@
       </c>
       <c r="F43" s="45"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9">
       <c r="B44" s="3">
         <v>59</v>
       </c>
@@ -6776,7 +6831,7 @@
       </c>
       <c r="F44" s="45"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9">
       <c r="D45">
         <f>SUM(D3:D44)</f>
         <v>61</v>
@@ -6800,7 +6855,7 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="49"/>
     <col min="3" max="3" width="38.42578125" style="49" bestFit="1" customWidth="1"/>
@@ -6810,7 +6865,7 @@
     <col min="10" max="16384" width="9.140625" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11">
       <c r="D1" s="49" t="s">
         <v>607</v>
       </c>
@@ -6833,7 +6888,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11">
       <c r="B2" s="59" t="s">
         <v>20</v>
       </c>
@@ -6862,7 +6917,7 @@
       </c>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11">
       <c r="B3" s="59" t="s">
         <v>21</v>
       </c>
@@ -6891,7 +6946,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11">
       <c r="B4" s="59" t="s">
         <v>22</v>
       </c>
@@ -6920,7 +6975,7 @@
       </c>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11">
       <c r="B5" s="59" t="s">
         <v>23</v>
       </c>
@@ -6949,7 +7004,7 @@
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11">
       <c r="B6" s="59" t="s">
         <v>126</v>
       </c>
@@ -6978,7 +7033,7 @@
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11">
       <c r="B7" s="59" t="s">
         <v>186</v>
       </c>
@@ -7007,7 +7062,7 @@
       </c>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11">
       <c r="B8" s="59" t="s">
         <v>400</v>
       </c>
@@ -7023,7 +7078,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11">
       <c r="B9" s="59" t="s">
         <v>53</v>
       </c>
@@ -7052,7 +7107,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11">
       <c r="B10" s="59" t="s">
         <v>205</v>
       </c>
@@ -7081,7 +7136,7 @@
       </c>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11">
       <c r="B11" s="59" t="s">
         <v>415</v>
       </c>
@@ -7110,7 +7165,7 @@
       </c>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11">
       <c r="B12" s="59" t="s">
         <v>432</v>
       </c>
@@ -7139,7 +7194,7 @@
       </c>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11">
       <c r="B13" s="59" t="s">
         <v>436</v>
       </c>
@@ -7168,7 +7223,7 @@
       </c>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11">
       <c r="B14" s="59" t="s">
         <v>501</v>
       </c>
@@ -7197,7 +7252,7 @@
       </c>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11">
       <c r="B15" s="59">
         <v>10</v>
       </c>
@@ -7226,7 +7281,7 @@
       </c>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11">
       <c r="B16" s="59">
         <v>11</v>
       </c>
@@ -7255,7 +7310,7 @@
       </c>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11">
       <c r="B17" s="59">
         <v>12</v>
       </c>
@@ -7284,7 +7339,7 @@
       </c>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11">
       <c r="B18" s="59">
         <v>13</v>
       </c>
@@ -7313,7 +7368,7 @@
       </c>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11">
       <c r="B19" s="9">
         <v>14</v>
       </c>
@@ -7342,7 +7397,7 @@
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11">
       <c r="B20" s="9">
         <v>15</v>
       </c>
@@ -7371,7 +7426,7 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11">
       <c r="B21" s="9">
         <v>16</v>
       </c>
@@ -7400,7 +7455,7 @@
       </c>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11">
       <c r="B22" s="9">
         <v>18</v>
       </c>
@@ -7429,7 +7484,7 @@
       </c>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11">
       <c r="B23" s="9">
         <v>21</v>
       </c>
@@ -7458,7 +7513,7 @@
       </c>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11">
       <c r="B24" s="9">
         <v>22</v>
       </c>
@@ -7487,7 +7542,7 @@
       </c>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11">
       <c r="B25" s="9">
         <v>23</v>
       </c>
@@ -7516,7 +7571,7 @@
       </c>
       <c r="K25" s="10"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11">
       <c r="B26" s="9">
         <v>24</v>
       </c>
@@ -7545,7 +7600,7 @@
       </c>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11">
       <c r="B27" s="9">
         <v>31</v>
       </c>
@@ -7574,7 +7629,7 @@
       </c>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11">
       <c r="B28" s="9">
         <v>32</v>
       </c>
@@ -7603,7 +7658,7 @@
       </c>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11">
       <c r="B29" s="9">
         <v>33</v>
       </c>
@@ -7632,7 +7687,7 @@
       </c>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11">
       <c r="B30" s="9">
         <v>34</v>
       </c>
@@ -7661,7 +7716,7 @@
       </c>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11">
       <c r="B31" s="9">
         <v>35</v>
       </c>
@@ -7690,7 +7745,7 @@
       </c>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11">
       <c r="B32" s="9">
         <v>36</v>
       </c>
@@ -7719,7 +7774,7 @@
       </c>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11">
       <c r="B33" s="9">
         <v>41</v>
       </c>
@@ -7748,7 +7803,7 @@
       </c>
       <c r="K33" s="10"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11">
       <c r="B34" s="9">
         <v>42</v>
       </c>
@@ -7777,7 +7832,7 @@
       </c>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11">
       <c r="B35" s="9" t="s">
         <v>151</v>
       </c>
@@ -7806,7 +7861,7 @@
       </c>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11">
       <c r="B36" s="9">
         <v>60</v>
       </c>
@@ -7835,7 +7890,7 @@
       </c>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11">
       <c r="B37" s="9">
         <v>61</v>
       </c>
@@ -7864,7 +7919,7 @@
       </c>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11">
       <c r="B38" s="9">
         <v>62</v>
       </c>
@@ -7893,7 +7948,7 @@
       </c>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11">
       <c r="B39" s="9">
         <v>68</v>
       </c>
@@ -7922,7 +7977,7 @@
       </c>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11">
       <c r="B40" s="9">
         <v>69</v>
       </c>
@@ -7951,7 +8006,7 @@
       </c>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11">
       <c r="B41" s="9">
         <v>71</v>
       </c>
@@ -7980,7 +8035,7 @@
       </c>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11">
       <c r="B42" s="9">
         <v>72</v>
       </c>
@@ -8009,7 +8064,7 @@
       </c>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11">
       <c r="B43" s="9">
         <v>74</v>
       </c>
@@ -8038,7 +8093,7 @@
       </c>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11">
       <c r="B44" s="9">
         <v>75</v>
       </c>
@@ -8067,7 +8122,7 @@
       </c>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11">
       <c r="B45" s="9" t="s">
         <v>518</v>
       </c>
@@ -8111,19 +8166,19 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -8134,7 +8189,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
@@ -8145,7 +8200,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
@@ -8154,7 +8209,7 @@
       </c>
       <c r="D5" s="79"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
@@ -8165,7 +8220,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
@@ -8176,7 +8231,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" s="5" t="s">
         <v>649</v>
       </c>
@@ -8187,7 +8242,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4">
       <c r="B9" s="5" t="s">
         <v>653</v>
       </c>
@@ -8198,7 +8253,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4">
       <c r="B10" s="5" t="s">
         <v>660</v>
       </c>
@@ -8209,7 +8264,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="B11" s="5" t="s">
         <v>665</v>
       </c>
@@ -8220,7 +8275,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4">
       <c r="B12" s="3" t="s">
         <v>666</v>
       </c>
@@ -8231,7 +8286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="B13" s="3">
         <v>14</v>
       </c>
@@ -8242,7 +8297,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4">
       <c r="B14" s="3">
         <v>15</v>
       </c>
@@ -8253,12 +8308,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4">
       <c r="B16" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4">
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
@@ -8269,7 +8324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4">
       <c r="B18" s="5" t="s">
         <v>20</v>
       </c>
@@ -8278,7 +8333,7 @@
       </c>
       <c r="D18" s="79"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4">
       <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
@@ -8289,7 +8344,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4">
       <c r="B20" s="5" t="s">
         <v>648</v>
       </c>
@@ -8300,7 +8355,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4">
       <c r="B21" s="5" t="s">
         <v>649</v>
       </c>
@@ -8311,7 +8366,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4">
       <c r="B22" s="5" t="s">
         <v>650</v>
       </c>
@@ -8322,7 +8377,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4">
       <c r="B23" s="5" t="s">
         <v>700</v>
       </c>
@@ -8333,7 +8388,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4">
       <c r="B24" s="5" t="s">
         <v>702</v>
       </c>
@@ -8344,7 +8399,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4">
       <c r="B25" s="65" t="s">
         <v>705</v>
       </c>
@@ -8355,7 +8410,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4">
       <c r="B26" s="65" t="s">
         <v>706</v>
       </c>
@@ -8366,7 +8421,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4">
       <c r="B27" s="45">
         <v>126</v>
       </c>
@@ -8377,7 +8432,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4">
       <c r="B28" s="45">
         <v>127</v>
       </c>
@@ -8388,12 +8443,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4">
       <c r="B30" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4">
       <c r="B31" s="45">
         <v>0</v>
       </c>
@@ -8404,7 +8459,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4">
       <c r="B32" s="45">
         <v>1</v>
       </c>
@@ -8415,7 +8470,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4">
       <c r="B33" s="45">
         <v>2</v>
       </c>
@@ -8426,7 +8481,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4">
       <c r="B34" s="45">
         <v>3</v>
       </c>
@@ -8437,7 +8492,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4">
       <c r="B35" s="45">
         <v>4</v>
       </c>
@@ -8448,7 +8503,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4">
       <c r="B36" s="45">
         <v>5</v>
       </c>
@@ -8459,7 +8514,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4">
       <c r="B37" s="66" t="s">
         <v>680</v>
       </c>
@@ -8470,7 +8525,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4">
       <c r="B38" s="45">
         <v>8</v>
       </c>
@@ -8481,7 +8536,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4">
       <c r="B39" s="45">
         <v>9</v>
       </c>
@@ -8492,7 +8547,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4">
       <c r="B40" s="66" t="s">
         <v>684</v>
       </c>
@@ -8503,12 +8558,12 @@
         <v>694</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4">
       <c r="B43" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4">
       <c r="B44" s="6" t="s">
         <v>0</v>
       </c>
@@ -8519,7 +8574,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4">
       <c r="B45" s="5" t="s">
         <v>19</v>
       </c>
@@ -8530,7 +8585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4">
       <c r="B46" s="5" t="s">
         <v>20</v>
       </c>
@@ -8539,7 +8594,7 @@
       </c>
       <c r="D46" s="79"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4">
       <c r="B47" s="5" t="s">
         <v>21</v>
       </c>
@@ -8550,7 +8605,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4">
       <c r="B48" s="5" t="s">
         <v>22</v>
       </c>
@@ -8561,7 +8616,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4">
       <c r="B49" s="5" t="s">
         <v>649</v>
       </c>
@@ -8572,7 +8627,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4">
       <c r="B50" s="5" t="s">
         <v>650</v>
       </c>
@@ -8583,7 +8638,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4">
       <c r="B51" s="5" t="s">
         <v>660</v>
       </c>
@@ -8594,7 +8649,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4">
       <c r="B52" s="5" t="s">
         <v>665</v>
       </c>
@@ -8605,7 +8660,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4">
       <c r="B53" s="3" t="s">
         <v>666</v>
       </c>
@@ -8616,7 +8671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4">
       <c r="B54" s="3">
         <v>14</v>
       </c>
@@ -8627,7 +8682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4">
       <c r="B55" s="3">
         <v>15</v>
       </c>
@@ -8652,22 +8707,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F47"/>
+  <dimension ref="B2:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -8678,13 +8734,16 @@
         <v>749</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>850</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -8694,12 +8753,16 @@
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="79" t="s">
+      <c r="E3" s="4">
+        <f>SUM(D$3:D3)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="45"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="45"/>
+    </row>
+    <row r="4" spans="2:7">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -8709,10 +8772,14 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="79"/>
-      <c r="F4" s="45"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="4">
+        <f>SUM(D$3:D4)</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="79"/>
+      <c r="G4" s="45"/>
+    </row>
+    <row r="5" spans="2:7">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -8722,12 +8789,16 @@
       <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="4">
+        <f>SUM(D$3:D5)</f>
+        <v>3</v>
+      </c>
+      <c r="F5" s="75" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="45"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="45"/>
+    </row>
+    <row r="6" spans="2:7">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -8737,12 +8808,16 @@
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="75" t="s">
+      <c r="E6" s="4">
+        <f>SUM(D$3:D6)</f>
+        <v>4</v>
+      </c>
+      <c r="F6" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="F6" s="45"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="45"/>
+    </row>
+    <row r="7" spans="2:7">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -8752,65 +8827,81 @@
       <c r="D7" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="75" t="s">
+      <c r="E7" s="4">
+        <f>SUM(D$3:D7)</f>
+        <v>5</v>
+      </c>
+      <c r="F7" s="75" t="s">
         <v>345</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="G7" s="45" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7">
       <c r="B8" s="5" t="s">
         <v>126</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
-      <c r="E8" s="75" t="s">
+      <c r="E8" s="4">
+        <f>SUM(D$3:D8)</f>
+        <v>6</v>
+      </c>
+      <c r="F8" s="75" t="s">
         <v>347</v>
       </c>
-      <c r="F8" s="45" t="s">
+      <c r="G8" s="45" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7">
       <c r="B9" s="5" t="s">
         <v>186</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E9" s="75" t="s">
+      <c r="E9" s="4">
+        <f>SUM(D$3:D9)</f>
+        <v>7</v>
+      </c>
+      <c r="F9" s="75" t="s">
         <v>375</v>
       </c>
-      <c r="F9" s="45" t="s">
+      <c r="G9" s="45" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7">
       <c r="B10" s="5" t="s">
         <v>400</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="75" t="s">
+      <c r="E10" s="4">
+        <f>SUM(D$3:D10)</f>
+        <v>8</v>
+      </c>
+      <c r="F10" s="75" t="s">
         <v>402</v>
       </c>
-      <c r="F10" s="45" t="s">
+      <c r="G10" s="45" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7">
       <c r="B11" s="78" t="s">
         <v>753</v>
       </c>
@@ -8820,61 +8911,77 @@
       <c r="D11" s="25">
         <v>2</v>
       </c>
-      <c r="E11" s="72"/>
-      <c r="F11" s="73"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="4">
+        <f>SUM(D$3:D11)</f>
+        <v>10</v>
+      </c>
+      <c r="F11" s="72"/>
+      <c r="G11" s="73"/>
+    </row>
+    <row r="12" spans="2:7">
       <c r="B12" s="3" t="s">
         <v>348</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="D12" s="4">
         <v>2</v>
       </c>
-      <c r="E12" s="75" t="s">
+      <c r="E12" s="4">
+        <f>SUM(D$3:D12)</f>
+        <v>12</v>
+      </c>
+      <c r="F12" s="75" t="s">
         <v>350</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="G12" s="45" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7">
       <c r="B13" s="3" t="s">
         <v>351</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="D13" s="4">
         <v>2</v>
       </c>
-      <c r="E13" s="75" t="s">
+      <c r="E13" s="4">
+        <f>SUM(D$3:D13)</f>
+        <v>14</v>
+      </c>
+      <c r="F13" s="75" t="s">
         <v>355</v>
       </c>
-      <c r="F13" s="45" t="s">
+      <c r="G13" s="45" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7">
       <c r="B14" s="3" t="s">
         <v>353</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="D14" s="4">
         <v>2</v>
       </c>
-      <c r="E14" s="75" t="s">
+      <c r="E14" s="4">
+        <f>SUM(D$3:D14)</f>
+        <v>16</v>
+      </c>
+      <c r="F14" s="75" t="s">
         <v>356</v>
       </c>
-      <c r="F14" s="45" t="s">
+      <c r="G14" s="45" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7">
       <c r="B15" s="77" t="s">
         <v>357</v>
       </c>
@@ -8884,44 +8991,56 @@
       <c r="D15" s="25">
         <v>2</v>
       </c>
-      <c r="E15" s="72"/>
-      <c r="F15" s="73"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="4">
+        <f>SUM(D$3:D15)</f>
+        <v>18</v>
+      </c>
+      <c r="F15" s="72"/>
+      <c r="G15" s="73"/>
+    </row>
+    <row r="16" spans="2:7">
       <c r="B16" s="3">
         <v>18</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
       </c>
-      <c r="E16" s="75" t="s">
-        <v>813</v>
-      </c>
-      <c r="F16" s="45" t="s">
+      <c r="E16" s="4">
+        <f>SUM(D$3:D16)</f>
+        <v>19</v>
+      </c>
+      <c r="F16" s="75" t="s">
+        <v>811</v>
+      </c>
+      <c r="G16" s="45" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7">
       <c r="B17" s="3">
         <v>19</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
       </c>
-      <c r="E17" s="75" t="s">
-        <v>814</v>
-      </c>
-      <c r="F17" s="45" t="s">
+      <c r="E17" s="4">
+        <f>SUM(D$3:D17)</f>
+        <v>20</v>
+      </c>
+      <c r="F17" s="75" t="s">
+        <v>812</v>
+      </c>
+      <c r="G17" s="45" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7">
       <c r="B18" s="77">
         <v>20</v>
       </c>
@@ -8931,10 +9050,14 @@
       <c r="D18" s="25">
         <v>1</v>
       </c>
-      <c r="E18" s="72"/>
-      <c r="F18" s="73"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="4">
+        <f>SUM(D$3:D18)</f>
+        <v>21</v>
+      </c>
+      <c r="F18" s="72"/>
+      <c r="G18" s="73"/>
+    </row>
+    <row r="19" spans="2:7">
       <c r="B19" s="3">
         <v>21</v>
       </c>
@@ -8944,261 +9067,331 @@
       <c r="D19" s="4">
         <v>1</v>
       </c>
-      <c r="E19" s="75" t="s">
+      <c r="E19" s="4">
+        <f>SUM(D$3:D19)</f>
+        <v>22</v>
+      </c>
+      <c r="F19" s="75" t="s">
         <v>361</v>
       </c>
-      <c r="F19" s="45" t="s">
+      <c r="G19" s="45" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7">
       <c r="B20" s="3">
         <v>22</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
       </c>
-      <c r="E20" s="75" t="s">
+      <c r="E20" s="4">
+        <f>SUM(D$3:D20)</f>
+        <v>23</v>
+      </c>
+      <c r="F20" s="75" t="s">
         <v>363</v>
       </c>
-      <c r="F20" s="45" t="s">
+      <c r="G20" s="45" t="s">
         <v>785</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7">
       <c r="B21" s="3">
         <v>23</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
       </c>
-      <c r="E21" s="75" t="s">
+      <c r="E21" s="4">
+        <f>SUM(D$3:D21)</f>
+        <v>24</v>
+      </c>
+      <c r="F21" s="75" t="s">
         <v>365</v>
       </c>
-      <c r="F21" s="45" t="s">
+      <c r="G21" s="45" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7">
       <c r="B22" s="3">
         <v>24</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
       </c>
-      <c r="E22" s="75" t="s">
+      <c r="E22" s="4">
+        <f>SUM(D$3:D22)</f>
+        <v>25</v>
+      </c>
+      <c r="F22" s="75" t="s">
         <v>367</v>
       </c>
-      <c r="F22" s="45" t="s">
+      <c r="G22" s="45" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="77" t="s">
-        <v>806</v>
-      </c>
-      <c r="C23" s="25" t="s">
+    <row r="23" spans="2:7">
+      <c r="B23" s="65">
+        <v>25</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>857</v>
+      </c>
+      <c r="D23" s="16">
+        <v>1</v>
+      </c>
+      <c r="E23" s="16">
+        <f>SUM(D$3:D23)</f>
+        <v>26</v>
+      </c>
+      <c r="F23" s="80" t="s">
+        <v>860</v>
+      </c>
+      <c r="G23" s="81" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="65">
+        <v>26</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>858</v>
+      </c>
+      <c r="D24" s="16">
+        <v>2</v>
+      </c>
+      <c r="E24" s="16">
+        <f>SUM(D$3:D24)</f>
+        <v>28</v>
+      </c>
+      <c r="F24" s="80" t="s">
+        <v>862</v>
+      </c>
+      <c r="G24" s="81" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="65">
+        <v>28</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>859</v>
+      </c>
+      <c r="D25" s="16">
+        <v>2</v>
+      </c>
+      <c r="E25" s="16">
+        <f>SUM(D$3:D25)</f>
+        <v>30</v>
+      </c>
+      <c r="F25" s="80" t="s">
+        <v>863</v>
+      </c>
+      <c r="G25" s="81" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="77">
+        <v>30</v>
+      </c>
+      <c r="C26" s="25" t="s">
         <v>788</v>
       </c>
-      <c r="D23" s="25">
-        <v>6</v>
-      </c>
-      <c r="E23" s="72"/>
-      <c r="F23" s="73"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="3">
+      <c r="D26" s="25">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4">
+        <f>SUM(D$3:D26)</f>
         <v>31</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>838</v>
-      </c>
-      <c r="D24" s="4">
+      <c r="F26" s="72"/>
+      <c r="G26" s="73"/>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="3">
+        <v>31</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>835</v>
+      </c>
+      <c r="D27" s="4">
         <v>1</v>
       </c>
-      <c r="E24" s="75" t="s">
+      <c r="E27" s="4">
+        <f>SUM(D$3:D27)</f>
+        <v>32</v>
+      </c>
+      <c r="F27" s="75" t="s">
         <v>369</v>
       </c>
-      <c r="F24" s="45" t="s">
+      <c r="G27" s="45" t="s">
         <v>789</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="3">
+    <row r="28" spans="2:7">
+      <c r="B28" s="3">
         <v>32</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>839</v>
-      </c>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
-      <c r="E25" s="75" t="s">
-        <v>371</v>
-      </c>
-      <c r="F25" s="45" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="3">
-        <v>33</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>840</v>
-      </c>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
-      <c r="E26" s="75" t="s">
-        <v>373</v>
-      </c>
-      <c r="F26" s="45" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="77">
-        <v>34</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>788</v>
-      </c>
-      <c r="D27" s="25">
-        <v>1</v>
-      </c>
-      <c r="E27" s="72"/>
-      <c r="F27" s="73"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="3">
-        <v>35</v>
-      </c>
       <c r="C28" s="4" t="s">
-        <v>759</v>
+        <v>836</v>
       </c>
       <c r="D28" s="4">
         <v>1</v>
       </c>
-      <c r="E28" s="75" t="s">
-        <v>766</v>
-      </c>
-      <c r="F28" s="45" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="4">
+        <f>SUM(D$3:D28)</f>
+        <v>33</v>
+      </c>
+      <c r="F28" s="75" t="s">
+        <v>371</v>
+      </c>
+      <c r="G28" s="45" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
       <c r="B29" s="3">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>816</v>
+        <v>837</v>
       </c>
       <c r="D29" s="4">
         <v>1</v>
       </c>
-      <c r="E29" s="75" t="s">
-        <v>761</v>
-      </c>
-      <c r="F29" s="45" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="3">
-        <v>37</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>828</v>
-      </c>
-      <c r="D30" s="4">
+      <c r="E29" s="4">
+        <f>SUM(D$3:D29)</f>
+        <v>34</v>
+      </c>
+      <c r="F29" s="75" t="s">
+        <v>373</v>
+      </c>
+      <c r="G29" s="45" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="65">
+        <v>34</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>847</v>
+      </c>
+      <c r="D30" s="16">
         <v>1</v>
       </c>
-      <c r="E30" s="75" t="s">
-        <v>767</v>
-      </c>
-      <c r="F30" s="45" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
-        <v>760</v>
+      <c r="E30" s="16">
+        <f>SUM(D$3:D30)</f>
+        <v>35</v>
+      </c>
+      <c r="F30" s="80" t="s">
+        <v>848</v>
+      </c>
+      <c r="G30" s="81" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="3">
+        <v>35</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>827</v>
+        <v>759</v>
       </c>
       <c r="D31" s="4">
-        <v>2</v>
-      </c>
-      <c r="E31" s="75" t="s">
-        <v>762</v>
-      </c>
-      <c r="F31" s="45" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E31" s="4">
+        <f>SUM(D$3:D31)</f>
+        <v>36</v>
+      </c>
+      <c r="F31" s="75" t="s">
+        <v>766</v>
+      </c>
+      <c r="G31" s="45" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
       <c r="B32" s="3">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>826</v>
+        <v>814</v>
       </c>
       <c r="D32" s="4">
         <v>1</v>
       </c>
-      <c r="E32" s="75" t="s">
-        <v>795</v>
-      </c>
-      <c r="F32" s="45" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E32" s="4">
+        <f>SUM(D$3:D32)</f>
+        <v>37</v>
+      </c>
+      <c r="F32" s="75" t="s">
+        <v>761</v>
+      </c>
+      <c r="G32" s="45" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
       <c r="B33" s="3">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>821</v>
+        <v>825</v>
       </c>
       <c r="D33" s="4">
         <v>1</v>
       </c>
-      <c r="E33" s="75" t="s">
-        <v>797</v>
-      </c>
-      <c r="F33" s="45" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="3">
-        <v>42</v>
+      <c r="E33" s="4">
+        <f>SUM(D$3:D33)</f>
+        <v>38</v>
+      </c>
+      <c r="F33" s="75" t="s">
+        <v>767</v>
+      </c>
+      <c r="G33" s="45" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="3" t="s">
+        <v>760</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>817</v>
+        <v>824</v>
       </c>
       <c r="D34" s="4">
-        <v>1</v>
-      </c>
-      <c r="E34" s="75"/>
-      <c r="F34" s="45" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E34" s="4">
+        <f>SUM(D$3:D34)</f>
+        <v>40</v>
+      </c>
+      <c r="F34" s="75" t="s">
+        <v>846</v>
+      </c>
+      <c r="G34" s="45" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7">
       <c r="B35" s="3">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>823</v>
@@ -9206,187 +9399,320 @@
       <c r="D35" s="4">
         <v>1</v>
       </c>
-      <c r="E35" s="75"/>
-      <c r="F35" s="45" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="77" t="s">
-        <v>800</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>788</v>
-      </c>
-      <c r="D36" s="25">
-        <v>3</v>
-      </c>
-      <c r="E36" s="72"/>
-      <c r="F36" s="73"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="4">
+        <f>SUM(D$3:D35)</f>
+        <v>41</v>
+      </c>
+      <c r="F35" s="75" t="s">
+        <v>795</v>
+      </c>
+      <c r="G35" s="45" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="3">
+        <v>41</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>819</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" s="4">
+        <f>SUM(D$3:D36)</f>
+        <v>42</v>
+      </c>
+      <c r="F36" s="75" t="s">
+        <v>797</v>
+      </c>
+      <c r="G36" s="45" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
       <c r="B37" s="3">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>824</v>
+        <v>815</v>
       </c>
       <c r="D37" s="4">
         <v>1</v>
       </c>
-      <c r="E37" s="75" t="s">
+      <c r="E37" s="4">
+        <f>SUM(D$3:D37)</f>
+        <v>43</v>
+      </c>
+      <c r="F37" s="75"/>
+      <c r="G37" s="45" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="3">
+        <v>43</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>820</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="E38" s="4">
+        <f>SUM(D$3:D38)</f>
+        <v>44</v>
+      </c>
+      <c r="F38" s="75"/>
+      <c r="G38" s="45" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="77">
+        <v>44</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>788</v>
+      </c>
+      <c r="D39" s="25">
+        <v>3</v>
+      </c>
+      <c r="E39" s="4">
+        <f>SUM(D$3:D39)</f>
+        <v>47</v>
+      </c>
+      <c r="F39" s="72"/>
+      <c r="G39" s="73"/>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" s="3">
+        <v>47</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>821</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1</v>
+      </c>
+      <c r="E40" s="4">
+        <f>SUM(D$3:D40)</f>
+        <v>48</v>
+      </c>
+      <c r="F40" s="75" t="s">
+        <v>806</v>
+      </c>
+      <c r="G40" s="45" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>838</v>
+      </c>
+      <c r="D41" s="4">
+        <v>2</v>
+      </c>
+      <c r="E41" s="4">
+        <f>SUM(D$3:D41)</f>
+        <v>50</v>
+      </c>
+      <c r="F41" s="75" t="s">
+        <v>807</v>
+      </c>
+      <c r="G41" s="45" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>816</v>
+      </c>
+      <c r="D42" s="4">
+        <v>2</v>
+      </c>
+      <c r="E42" s="4">
+        <f>SUM(D$3:D42)</f>
+        <v>52</v>
+      </c>
+      <c r="F42" s="75" t="s">
         <v>808</v>
       </c>
-      <c r="F37" s="45" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>801</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>841</v>
-      </c>
-      <c r="D38" s="4">
-        <v>2</v>
-      </c>
-      <c r="E38" s="75" t="s">
-        <v>809</v>
-      </c>
-      <c r="F38" s="45" t="s">
+      <c r="G42" s="45" t="s">
         <v>804</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
-        <v>802</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>818</v>
-      </c>
-      <c r="D39" s="4">
-        <v>2</v>
-      </c>
-      <c r="E39" s="75" t="s">
-        <v>810</v>
-      </c>
-      <c r="F39" s="45" t="s">
+    <row r="43" spans="2:7">
+      <c r="B43" s="77">
+        <v>52</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>788</v>
+      </c>
+      <c r="D43" s="25">
+        <v>1</v>
+      </c>
+      <c r="E43" s="4">
+        <f>SUM(D$3:D43)</f>
+        <v>53</v>
+      </c>
+      <c r="F43" s="72"/>
+      <c r="G43" s="73"/>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="B44" s="3">
+        <v>53</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>822</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1</v>
+      </c>
+      <c r="E44" s="4">
+        <f>SUM(D$3:D44)</f>
+        <v>54</v>
+      </c>
+      <c r="F44" s="75" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="77">
-        <v>52</v>
-      </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25">
-        <v>1</v>
-      </c>
-      <c r="E40" s="72"/>
-      <c r="F40" s="73"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="3">
-        <v>53</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>825</v>
-      </c>
-      <c r="D41" s="4">
-        <v>1</v>
-      </c>
-      <c r="E41" s="75" t="s">
-        <v>807</v>
-      </c>
-      <c r="F41" s="45" t="s">
+      <c r="G44" s="45" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="3">
+    <row r="45" spans="2:7">
+      <c r="B45" s="3">
         <v>54</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>819</v>
-      </c>
-      <c r="D42" s="4">
-        <v>1</v>
-      </c>
-      <c r="E42" s="76" t="s">
-        <v>811</v>
-      </c>
-      <c r="F42" s="45" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="3">
-        <v>53</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>844</v>
-      </c>
-      <c r="D43" s="4">
-        <v>1</v>
-      </c>
-      <c r="E43" s="76" t="s">
-        <v>843</v>
-      </c>
-      <c r="F43" s="45" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="77" t="s">
-        <v>822</v>
-      </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25">
-        <v>3</v>
-      </c>
-      <c r="E44" s="72"/>
-      <c r="F44" s="73"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="3">
-        <v>58</v>
-      </c>
       <c r="C45" s="4" t="s">
-        <v>15</v>
+        <v>817</v>
       </c>
       <c r="D45" s="4">
         <v>1</v>
       </c>
-      <c r="E45" s="75" t="s">
-        <v>16</v>
-      </c>
-      <c r="F45" s="45"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E45" s="4">
+        <f>SUM(D$3:D45)</f>
+        <v>55</v>
+      </c>
+      <c r="F45" s="76" t="s">
+        <v>809</v>
+      </c>
+      <c r="G45" s="45" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7">
       <c r="B46" s="3">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>17</v>
+        <v>841</v>
       </c>
       <c r="D46" s="4">
         <v>1</v>
       </c>
-      <c r="E46" s="75" t="s">
+      <c r="E46" s="4">
+        <f>SUM(D$3:D46)</f>
+        <v>56</v>
+      </c>
+      <c r="F46" s="76" t="s">
+        <v>840</v>
+      </c>
+      <c r="G46" s="45" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="B47" s="65">
+        <v>56</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>851</v>
+      </c>
+      <c r="D47" s="16">
+        <v>1</v>
+      </c>
+      <c r="E47" s="16">
+        <f>SUM(D$3:D47)</f>
+        <v>57</v>
+      </c>
+      <c r="F47" s="80" t="s">
+        <v>852</v>
+      </c>
+      <c r="G47" s="81" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="B48" s="65">
+        <v>57</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>856</v>
+      </c>
+      <c r="D48" s="16">
+        <v>1</v>
+      </c>
+      <c r="E48" s="16">
+        <f>SUM(D$3:D48)</f>
+        <v>58</v>
+      </c>
+      <c r="F48" s="80" t="s">
+        <v>854</v>
+      </c>
+      <c r="G48" s="81" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7">
+      <c r="B49" s="3">
+        <v>58</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="4">
+        <v>1</v>
+      </c>
+      <c r="E49" s="4">
+        <f>SUM(D$3:D49)</f>
+        <v>59</v>
+      </c>
+      <c r="F49" s="75" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="45"/>
+    </row>
+    <row r="50" spans="2:7">
+      <c r="B50" s="3">
+        <v>59</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="4">
+        <v>1</v>
+      </c>
+      <c r="E50" s="4">
+        <f>SUM(D$3:D50)</f>
+        <v>60</v>
+      </c>
+      <c r="F50" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="F46" s="45"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D47">
-        <f>SUM(D3:D46)</f>
-        <v>61</v>
-      </c>
-    </row>
+      <c r="G50" s="45"/>
+    </row>
+    <row r="51" spans="2:7"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9402,7 +9728,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -9418,7 +9744,7 @@
     <col min="18" max="48" width="9.140625" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:42">
       <c r="I1" s="51" t="s">
         <v>441</v>
       </c>
@@ -9432,7 +9758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:42">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -9491,7 +9817,7 @@
       <c r="AO2" s="11"/>
       <c r="AP2" s="11"/>
     </row>
-    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:42">
       <c r="B3" s="54">
         <v>0</v>
       </c>
@@ -9548,7 +9874,7 @@
       <c r="AO3" s="11"/>
       <c r="AP3" s="11"/>
     </row>
-    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:42">
       <c r="B4" s="55">
         <v>1</v>
       </c>
@@ -9603,7 +9929,7 @@
       <c r="AO4" s="11"/>
       <c r="AP4" s="11"/>
     </row>
-    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:42">
       <c r="B5" s="55">
         <v>2</v>
       </c>
@@ -9660,7 +9986,7 @@
       <c r="AO5" s="11"/>
       <c r="AP5" s="11"/>
     </row>
-    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:42">
       <c r="B6" s="55">
         <v>3</v>
       </c>
@@ -9717,7 +10043,7 @@
       <c r="AO6" s="11"/>
       <c r="AP6" s="11"/>
     </row>
-    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:42">
       <c r="B7" s="55">
         <v>4</v>
       </c>
@@ -9774,7 +10100,7 @@
       <c r="AO7" s="11"/>
       <c r="AP7" s="11"/>
     </row>
-    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:42">
       <c r="B8" s="55">
         <v>5</v>
       </c>
@@ -9831,7 +10157,7 @@
       <c r="AO8" s="11"/>
       <c r="AP8" s="11"/>
     </row>
-    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:42">
       <c r="B9" s="55">
         <v>6</v>
       </c>
@@ -9888,7 +10214,7 @@
       <c r="AO9" s="11"/>
       <c r="AP9" s="11"/>
     </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:42">
       <c r="B10" s="55">
         <v>8</v>
       </c>
@@ -9945,7 +10271,7 @@
       <c r="AO10" s="11"/>
       <c r="AP10" s="11"/>
     </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:42">
       <c r="B11" s="55">
         <v>9</v>
       </c>
@@ -10002,7 +10328,7 @@
       <c r="AO11" s="11"/>
       <c r="AP11" s="11"/>
     </row>
-    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:42">
       <c r="B12" s="55">
         <v>10</v>
       </c>
@@ -10059,7 +10385,7 @@
       <c r="AO12" s="11"/>
       <c r="AP12" s="11"/>
     </row>
-    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:42">
       <c r="B13" s="55">
         <v>40</v>
       </c>
@@ -10116,7 +10442,7 @@
       <c r="AO13" s="11"/>
       <c r="AP13" s="11"/>
     </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:42">
       <c r="B14" s="55">
         <v>60</v>
       </c>
@@ -10173,7 +10499,7 @@
       <c r="AO14" s="11"/>
       <c r="AP14" s="11"/>
     </row>
-    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:42">
       <c r="B15" s="55">
         <v>61</v>
       </c>
@@ -10230,7 +10556,7 @@
       <c r="AO15" s="11"/>
       <c r="AP15" s="11"/>
     </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:42">
       <c r="B16" s="55">
         <v>62</v>
       </c>
@@ -10287,7 +10613,7 @@
       <c r="AO16" s="11"/>
       <c r="AP16" s="11"/>
     </row>
-    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:42">
       <c r="B17" s="55">
         <v>63</v>
       </c>
@@ -10344,7 +10670,7 @@
       <c r="AO17" s="11"/>
       <c r="AP17" s="11"/>
     </row>
-    <row r="18" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:42">
       <c r="B18" s="55">
         <v>64</v>
       </c>
@@ -10401,7 +10727,7 @@
       <c r="AO18" s="11"/>
       <c r="AP18" s="11"/>
     </row>
-    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:42">
       <c r="B19" s="55">
         <v>84</v>
       </c>
@@ -10458,7 +10784,7 @@
       <c r="AO19" s="11"/>
       <c r="AP19" s="11"/>
     </row>
-    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:42">
       <c r="B20" s="55">
         <v>104</v>
       </c>
@@ -10515,7 +10841,7 @@
       <c r="AO20" s="11"/>
       <c r="AP20" s="11"/>
     </row>
-    <row r="21" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:42">
       <c r="B21" s="55">
         <v>105</v>
       </c>
@@ -10572,7 +10898,7 @@
       <c r="AO21" s="11"/>
       <c r="AP21" s="11"/>
     </row>
-    <row r="22" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:42">
       <c r="B22" s="55">
         <v>106</v>
       </c>
@@ -10629,7 +10955,7 @@
       <c r="AO22" s="11"/>
       <c r="AP22" s="11"/>
     </row>
-    <row r="23" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:42">
       <c r="B23" s="55">
         <v>108</v>
       </c>
@@ -10686,7 +11012,7 @@
       <c r="AO23" s="11"/>
       <c r="AP23" s="11"/>
     </row>
-    <row r="24" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:42">
       <c r="B24" s="55">
         <v>109</v>
       </c>
@@ -10743,7 +11069,7 @@
       <c r="AO24" s="11"/>
       <c r="AP24" s="11"/>
     </row>
-    <row r="25" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:42">
       <c r="B25" s="55">
         <v>110</v>
       </c>
@@ -10800,7 +11126,7 @@
       <c r="AO25" s="11"/>
       <c r="AP25" s="11"/>
     </row>
-    <row r="26" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:42">
       <c r="B26" s="55">
         <v>112</v>
       </c>
@@ -10857,7 +11183,7 @@
       <c r="AO26" s="11"/>
       <c r="AP26" s="11"/>
     </row>
-    <row r="27" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:42">
       <c r="B27" s="55">
         <v>114</v>
       </c>
@@ -10914,7 +11240,7 @@
       <c r="AO27" s="11"/>
       <c r="AP27" s="11"/>
     </row>
-    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:42">
       <c r="B28" s="55">
         <v>118</v>
       </c>
@@ -10963,7 +11289,7 @@
       <c r="AO28" s="11"/>
       <c r="AP28" s="11"/>
     </row>
-    <row r="29" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:42">
       <c r="B29" s="55">
         <v>119</v>
       </c>
@@ -11012,7 +11338,7 @@
       <c r="AO29" s="11"/>
       <c r="AP29" s="11"/>
     </row>
-    <row r="30" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:42">
       <c r="E30">
         <f>SUM(E3:E29)</f>
         <v>120</v>
@@ -11052,7 +11378,7 @@
       <c r="AO30" s="11"/>
       <c r="AP30" s="11"/>
     </row>
-    <row r="31" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:42">
       <c r="I31" s="50"/>
       <c r="J31" s="50"/>
       <c r="K31" s="50"/>
@@ -11106,14 +11432,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -11124,7 +11450,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -11135,7 +11461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -11144,7 +11470,7 @@
       </c>
       <c r="D4" s="79"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -11155,7 +11481,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -11166,7 +11492,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -11177,7 +11503,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" s="5" t="s">
         <v>421</v>
       </c>
@@ -11188,7 +11514,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4">
       <c r="B9" s="5" t="s">
         <v>424</v>
       </c>
@@ -11199,7 +11525,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4">
       <c r="B10" s="5" t="s">
         <v>427</v>
       </c>
@@ -11210,7 +11536,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="B11" s="3" t="s">
         <v>430</v>
       </c>
@@ -11221,7 +11547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4">
       <c r="B12" s="3">
         <v>58</v>
       </c>
@@ -11232,7 +11558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="B13" s="3">
         <v>59</v>
       </c>
@@ -11260,14 +11586,14 @@
       <selection activeCell="B2" sqref="B2:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" s="1" customFormat="1">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -11278,7 +11604,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" s="1" customFormat="1">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -11289,7 +11615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" s="1" customFormat="1">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -11298,7 +11624,7 @@
       </c>
       <c r="D4" s="79"/>
     </row>
-    <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" s="1" customFormat="1">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -11309,7 +11635,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" s="1" customFormat="1">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -11320,7 +11646,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" s="1" customFormat="1">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
@@ -11331,7 +11657,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" s="1" customFormat="1">
       <c r="B8" s="5" t="s">
         <v>343</v>
       </c>
@@ -11342,7 +11668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" s="1" customFormat="1">
       <c r="B9" s="3" t="s">
         <v>339</v>
       </c>
@@ -11353,7 +11679,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" s="1" customFormat="1">
       <c r="B10" s="3" t="s">
         <v>340</v>
       </c>
@@ -11364,7 +11690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" s="1" customFormat="1">
       <c r="B11" s="3">
         <v>58</v>
       </c>
@@ -11375,7 +11701,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" s="1" customFormat="1">
       <c r="B12" s="3">
         <v>59</v>
       </c>
@@ -11403,7 +11729,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -11414,12 +11740,12 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18.75">
       <c r="A2" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="27" t="s">
         <v>139</v>
       </c>
@@ -11427,12 +11753,12 @@
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -11443,7 +11769,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
@@ -11454,7 +11780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
@@ -11463,7 +11789,7 @@
       </c>
       <c r="D8" s="79"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -11474,7 +11800,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -11485,7 +11811,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
@@ -11496,7 +11822,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12" s="5" t="s">
         <v>126</v>
       </c>
@@ -11507,7 +11833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13" s="3" t="s">
         <v>127</v>
       </c>
@@ -11518,7 +11844,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14" s="3">
         <v>26</v>
       </c>
@@ -11529,7 +11855,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="B15" s="3">
         <v>27</v>
       </c>
@@ -11540,7 +11866,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="3">
         <v>28</v>
       </c>
@@ -11551,7 +11877,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="B17" s="3">
         <v>29</v>
       </c>
@@ -11562,7 +11888,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="B18" s="3" t="s">
         <v>129</v>
       </c>
@@ -11573,7 +11899,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="B19" s="3" t="s">
         <v>124</v>
       </c>
@@ -11584,7 +11910,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="B20" s="3" t="s">
         <v>130</v>
       </c>
@@ -11595,7 +11921,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="B21" s="3" t="s">
         <v>131</v>
       </c>
@@ -11606,7 +11932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="B22" s="3">
         <v>58</v>
       </c>
@@ -11617,7 +11943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="B23" s="3">
         <v>59</v>
       </c>
@@ -11628,17 +11954,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="18.75">
       <c r="A25" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
@@ -11649,7 +11975,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="B28" s="5" t="s">
         <v>19</v>
       </c>
@@ -11660,7 +11986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="B29" s="5" t="s">
         <v>20</v>
       </c>
@@ -11669,7 +11995,7 @@
       </c>
       <c r="D29" s="79"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
@@ -11680,7 +12006,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="B31" s="5" t="s">
         <v>22</v>
       </c>
@@ -11691,7 +12017,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="B32" s="5" t="s">
         <v>23</v>
       </c>
@@ -11702,7 +12028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4">
       <c r="B33" s="5" t="s">
         <v>126</v>
       </c>
@@ -11713,7 +12039,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4">
       <c r="B34" s="5" t="s">
         <v>186</v>
       </c>
@@ -11724,7 +12050,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4">
       <c r="B35" s="5" t="s">
         <v>187</v>
       </c>
@@ -11735,7 +12061,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4">
       <c r="B36" s="3" t="s">
         <v>188</v>
       </c>
@@ -11746,7 +12072,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4">
       <c r="B37" s="3" t="s">
         <v>189</v>
       </c>
@@ -11757,7 +12083,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4">
       <c r="B38" s="3" t="s">
         <v>190</v>
       </c>
@@ -11768,7 +12094,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4">
       <c r="B39" s="3">
         <v>51</v>
       </c>
@@ -11779,7 +12105,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4">
       <c r="B40" s="3">
         <v>52</v>
       </c>
@@ -11790,7 +12116,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4">
       <c r="B41" s="3">
         <v>53</v>
       </c>
@@ -11801,7 +12127,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4">
       <c r="B42" s="3">
         <v>54</v>
       </c>
@@ -11812,7 +12138,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4">
       <c r="B43" s="3">
         <v>55</v>
       </c>
@@ -11823,7 +12149,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4">
       <c r="B44" s="3" t="s">
         <v>201</v>
       </c>
@@ -11834,7 +12160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4">
       <c r="B45" s="3">
         <v>58</v>
       </c>
@@ -11845,7 +12171,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4">
       <c r="B46" s="3">
         <v>59</v>
       </c>
@@ -11856,17 +12182,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4">
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4">
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4">
       <c r="C49" s="1" t="s">
         <v>140</v>
       </c>
@@ -11874,17 +12200,17 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4">
       <c r="D50" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4">
       <c r="D51" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4">
       <c r="D52" s="1" t="s">
         <v>144</v>
       </c>
@@ -11908,17 +12234,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="158.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:3" ht="60">
       <c r="C2" s="24" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:3">
       <c r="C5" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
v2.2.1.9 - New command to set action speed
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="V2 Command" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="870">
   <si>
     <t>Offset</t>
   </si>
@@ -2882,6 +2882,18 @@
   </si>
   <si>
     <t>RC_MAZE_SERVO_WAIT_MS</t>
+  </si>
+  <si>
+    <t>Set Action Speed</t>
+  </si>
+  <si>
+    <t>Speed (time = time * 100 / speed)</t>
+  </si>
+  <si>
+    <t>A9 9A 03 43 64 AA ED</t>
+  </si>
+  <si>
+    <t>A9 9A 03 43 C8 0E ED</t>
   </si>
 </sst>
 </file>
@@ -3012,7 +3024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3235,6 +3247,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3539,13 +3554,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N71"/>
+  <dimension ref="B2:N72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G31" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
+      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4400,7 +4415,7 @@
         <v>162</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="E40" s="28" t="s">
         <v>51</v>
@@ -4617,101 +4632,97 @@
       </c>
     </row>
     <row r="48" spans="2:11">
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="3">
+        <v>43</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>866</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E48" s="79" t="s">
+        <v>867</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>869</v>
+      </c>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+    </row>
+    <row r="49" spans="2:11">
+      <c r="B49" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C49" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E48" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="G48" s="4"/>
-      <c r="I48" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="K48" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11">
-      <c r="B49" s="3">
-        <v>60</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="32" t="s">
+      <c r="E49" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>196</v>
+        <v>153</v>
       </c>
       <c r="G49" s="4"/>
       <c r="I49" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>197</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="2:11">
       <c r="B50" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>99</v>
+        <v>195</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E50" s="18" t="s">
-        <v>79</v>
+        <v>56</v>
+      </c>
+      <c r="E50" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="G50" s="4"/>
       <c r="I50" s="4" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>110</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="2:11">
       <c r="B51" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>90</v>
+        <v>99</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>619</v>
+        <v>79</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>204</v>
+        <v>77</v>
       </c>
       <c r="G51" s="4"/>
       <c r="I51" s="4" t="s">
@@ -4721,101 +4732,101 @@
         <v>135</v>
       </c>
       <c r="K51" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11">
+      <c r="B52" s="3">
+        <v>62</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>619</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G52" s="4"/>
+      <c r="I52" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K52" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="2:11" s="38" customFormat="1">
-      <c r="B52" s="35">
+    <row r="53" spans="2:11" s="38" customFormat="1">
+      <c r="B53" s="35">
         <v>63</v>
       </c>
-      <c r="C52" s="36" t="s">
+      <c r="C53" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="D52" s="36" t="s">
+      <c r="D53" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E52" s="37" t="s">
+      <c r="E53" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="F52" s="36" t="s">
+      <c r="F53" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="G52" s="36"/>
-      <c r="I52" s="36" t="s">
+      <c r="G53" s="36"/>
+      <c r="I53" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="J52" s="36" t="s">
+      <c r="J53" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="K52" s="36" t="s">
+      <c r="K53" s="36" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11">
-      <c r="B53" s="3">
-        <v>68</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="D53" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="E53" s="42" t="s">
-        <v>618</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="G53" s="4"/>
-      <c r="I53" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="54" spans="2:11">
       <c r="B54" s="3">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="D54" s="25"/>
-      <c r="E54" s="42"/>
+        <v>335</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54" s="42" t="s">
+        <v>618</v>
+      </c>
       <c r="F54" s="4" t="s">
-        <v>406</v>
+        <v>336</v>
       </c>
       <c r="G54" s="4"/>
       <c r="I54" s="4" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>107</v>
+        <v>406</v>
       </c>
     </row>
     <row r="55" spans="2:11">
       <c r="B55" s="3">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E55" s="18" t="s">
-        <v>113</v>
-      </c>
+        <v>411</v>
+      </c>
+      <c r="D55" s="25"/>
+      <c r="E55" s="42"/>
       <c r="F55" s="4" t="s">
-        <v>114</v>
+        <v>406</v>
       </c>
       <c r="G55" s="4"/>
       <c r="I55" s="4" t="s">
@@ -4824,20 +4835,26 @@
       <c r="J55" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="K55" s="4"/>
+      <c r="K55" s="4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="56" spans="2:11">
       <c r="B56" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E56" s="18"/>
-      <c r="F56" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="G56" s="4"/>
       <c r="I56" s="4" t="s">
         <v>105</v>
@@ -4847,22 +4864,18 @@
       </c>
       <c r="K56" s="4"/>
     </row>
-    <row r="57" spans="2:11" ht="30">
+    <row r="57" spans="2:11">
       <c r="B57" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E57" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="F57" s="17" t="s">
-        <v>136</v>
-      </c>
+      <c r="E57" s="18"/>
+      <c r="F57" s="4"/>
       <c r="G57" s="4"/>
       <c r="I57" s="4" t="s">
         <v>105</v>
@@ -4870,25 +4883,23 @@
       <c r="J57" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="K57" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="58" spans="2:11">
+      <c r="K57" s="4"/>
+    </row>
+    <row r="58" spans="2:11" ht="30">
       <c r="B58" s="3">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>635</v>
-      </c>
-      <c r="E58" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>211</v>
+        <v>115</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="G58" s="4"/>
       <c r="I58" s="4" t="s">
@@ -4898,222 +4909,222 @@
         <v>106</v>
       </c>
       <c r="K58" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11">
+      <c r="B59" s="3">
+        <v>75</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>635</v>
+      </c>
+      <c r="E59" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G59" s="4"/>
+      <c r="I59" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="K59" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="59" spans="2:11">
-      <c r="B59" s="3"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="62"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-    </row>
     <row r="60" spans="2:11">
-      <c r="B60" s="3">
-        <v>81</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>625</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>634</v>
-      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
       <c r="E60" s="62"/>
-      <c r="F60" s="4" t="s">
-        <v>626</v>
-      </c>
+      <c r="F60" s="4"/>
       <c r="G60" s="4"/>
-      <c r="I60" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>212</v>
-      </c>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
     </row>
     <row r="61" spans="2:11">
       <c r="B61" s="3">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D61" s="17" t="s">
         <v>634</v>
       </c>
       <c r="E61" s="62"/>
       <c r="F61" s="4" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G61" s="4"/>
       <c r="I61" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11">
+      <c r="B62" s="3">
+        <v>82</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="E62" s="62"/>
+      <c r="F62" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="G62" s="4"/>
+      <c r="I62" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="J61" s="4" t="s">
+      <c r="J62" s="4" t="s">
         <v>630</v>
       </c>
-      <c r="K61" s="4" t="s">
+      <c r="K62" s="4" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="62" spans="2:11">
-      <c r="B62" s="3"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="62"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-    </row>
     <row r="63" spans="2:11">
-      <c r="B63" s="3">
-        <v>91</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>661</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>667</v>
-      </c>
-      <c r="E63" s="63"/>
-      <c r="F63" s="4" t="s">
-        <v>672</v>
-      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="62"/>
+      <c r="F63" s="4"/>
       <c r="G63" s="4"/>
-      <c r="I63" s="4" t="s">
-        <v>642</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>643</v>
-      </c>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
       <c r="K63" s="4"/>
     </row>
     <row r="64" spans="2:11">
       <c r="B64" s="3">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>663</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>668</v>
-      </c>
-      <c r="E64" s="63" t="s">
-        <v>669</v>
-      </c>
+        <v>661</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>667</v>
+      </c>
+      <c r="E64" s="63"/>
       <c r="F64" s="4" t="s">
-        <v>712</v>
+        <v>672</v>
       </c>
       <c r="G64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
+      <c r="I64" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>643</v>
+      </c>
       <c r="K64" s="4"/>
     </row>
     <row r="65" spans="2:11">
       <c r="B65" s="3">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>656</v>
-      </c>
-      <c r="E65" s="63"/>
+        <v>668</v>
+      </c>
+      <c r="E65" s="63" t="s">
+        <v>669</v>
+      </c>
       <c r="F65" s="4" t="s">
-        <v>713</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>711</v>
-      </c>
+        <v>712</v>
+      </c>
+      <c r="G65" s="4"/>
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
     </row>
     <row r="66" spans="2:11">
       <c r="B66" s="3">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>636</v>
+        <v>662</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="E66" s="63"/>
       <c r="F66" s="4" t="s">
-        <v>657</v>
-      </c>
-      <c r="G66" s="4"/>
+        <v>713</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>711</v>
+      </c>
       <c r="I66" s="4"/>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
     </row>
     <row r="67" spans="2:11">
-      <c r="B67" s="3"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="4"/>
+      <c r="B67" s="3">
+        <v>94</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="E67" s="63"/>
+      <c r="F67" s="4" t="s">
+        <v>657</v>
+      </c>
       <c r="G67" s="4"/>
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
     </row>
-    <row r="68" spans="2:11" s="38" customFormat="1">
-      <c r="B68" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="C68" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D68" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="E68" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="F68" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G68" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="I68" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="J68" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="K68" s="36" t="s">
-        <v>107</v>
-      </c>
+    <row r="68" spans="2:11">
+      <c r="B68" s="3"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
     </row>
     <row r="69" spans="2:11" s="38" customFormat="1">
       <c r="B69" s="35" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C69" s="36" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D69" s="36" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="E69" s="37" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F69" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="G69" s="36"/>
+        <v>83</v>
+      </c>
+      <c r="G69" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="I69" s="36" t="s">
         <v>105</v>
       </c>
@@ -5124,30 +5135,57 @@
         <v>107</v>
       </c>
     </row>
-    <row r="71" spans="2:11">
-      <c r="B71" s="3" t="s">
+    <row r="70" spans="2:11" s="38" customFormat="1">
+      <c r="B70" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C70" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D70" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E70" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="F70" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G70" s="36"/>
+      <c r="I70" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="J70" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="K70" s="36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11">
+      <c r="B72" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C72" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D72" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="E71" s="58" t="s">
+      <c r="E72" s="58" t="s">
         <v>521</v>
       </c>
-      <c r="F71" s="4" t="s">
+      <c r="F72" s="4" t="s">
         <v>611</v>
       </c>
-      <c r="G71" s="4"/>
-      <c r="I71" s="4" t="s">
+      <c r="G72" s="4"/>
+      <c r="I72" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="J71" s="4" t="s">
+      <c r="J72" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="K71" s="4" t="s">
+      <c r="K72" s="4" t="s">
         <v>612</v>
       </c>
     </row>
@@ -5994,7 +6032,7 @@
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="79" t="s">
+      <c r="E3" s="82" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="45"/>
@@ -6009,7 +6047,7 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="79"/>
+      <c r="E4" s="82"/>
       <c r="F4" s="45"/>
     </row>
     <row r="5" spans="2:9">
@@ -8196,7 +8234,7 @@
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="82" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8207,7 +8245,7 @@
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="79"/>
+      <c r="D5" s="82"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
@@ -8320,7 +8358,7 @@
       <c r="C17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="79" t="s">
+      <c r="D17" s="82" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8331,7 +8369,7 @@
       <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="79"/>
+      <c r="D18" s="82"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="5" t="s">
@@ -8581,7 +8619,7 @@
       <c r="C45" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="79" t="s">
+      <c r="D45" s="82" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8592,7 +8630,7 @@
       <c r="C46" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="79"/>
+      <c r="D46" s="82"/>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="5" t="s">
@@ -8707,9 +8745,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G51"/>
+  <dimension ref="B2:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -8757,7 +8795,7 @@
         <f>SUM(D$3:D3)</f>
         <v>1</v>
       </c>
-      <c r="F3" s="79" t="s">
+      <c r="F3" s="82" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="45"/>
@@ -8776,7 +8814,7 @@
         <f>SUM(D$3:D4)</f>
         <v>2</v>
       </c>
-      <c r="F4" s="79"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="45"/>
     </row>
     <row r="5" spans="2:7">
@@ -9709,7 +9747,6 @@
       </c>
       <c r="G50" s="45"/>
     </row>
-    <row r="51" spans="2:7"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F3:F4"/>
@@ -9824,7 +9861,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="82" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="47">
@@ -9881,7 +9918,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="79"/>
+      <c r="D4" s="82"/>
       <c r="E4" s="47">
         <v>1</v>
       </c>
@@ -11457,7 +11494,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="82" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11468,7 +11505,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="79"/>
+      <c r="D4" s="82"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
@@ -11611,7 +11648,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="82" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11622,7 +11659,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="79"/>
+      <c r="D4" s="82"/>
     </row>
     <row r="5" spans="2:4" s="1" customFormat="1">
       <c r="B5" s="5" t="s">
@@ -11776,7 +11813,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="79" t="s">
+      <c r="D7" s="82" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11787,7 +11824,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="82"/>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="5" t="s">
@@ -11982,7 +12019,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="79" t="s">
+      <c r="D28" s="82" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11993,7 +12030,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="79"/>
+      <c r="D29" s="82"/>
     </row>
     <row r="30" spans="1:4">
       <c r="B30" s="5" t="s">

</xml_diff>

<commit_message>
v2.2.1.10 - Provide external interface to control the MP3 module directly: new MP3 command sending MP3-TF-16P instruction code directly.
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="874">
   <si>
     <t>Offset</t>
   </si>
@@ -2894,6 +2894,18 @@
   </si>
   <si>
     <t>A9 9A 03 43 C8 0E ED</t>
+  </si>
+  <si>
+    <t>MP3 Send Command</t>
+  </si>
+  <si>
+    <t>&lt;cmd&gt;&lt;parm1&gt;&lt;parm2&gt;</t>
+  </si>
+  <si>
+    <t>A9 9A 05 37 12 00 01 4F ED</t>
+  </si>
+  <si>
+    <t>A9 9A 05 37 16 00 00 52 ED</t>
   </si>
 </sst>
 </file>
@@ -3024,7 +3036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3247,6 +3259,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3554,13 +3569,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N72"/>
+  <dimension ref="B2:N73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
+      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4577,50 +4592,46 @@
     </row>
     <row r="46" spans="2:11">
       <c r="B46" s="3">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>147</v>
+        <v>870</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>844</v>
-      </c>
-      <c r="E46" s="26" t="s">
-        <v>843</v>
+        <v>90</v>
+      </c>
+      <c r="E46" s="82" t="s">
+        <v>871</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>213</v>
+        <v>872</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>845</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>107</v>
-      </c>
+        <v>873</v>
+      </c>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
     </row>
     <row r="47" spans="2:11">
       <c r="B47" s="3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>57</v>
+        <v>844</v>
       </c>
       <c r="E47" s="26" t="s">
-        <v>149</v>
+        <v>843</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G47" s="4"/>
+        <v>213</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>845</v>
+      </c>
       <c r="I47" s="4" t="s">
         <v>105</v>
       </c>
@@ -4633,123 +4644,123 @@
     </row>
     <row r="48" spans="2:11">
       <c r="B48" s="3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>866</v>
+        <v>148</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E48" s="79" t="s">
+      <c r="E48" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="G48" s="4"/>
+      <c r="I48" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11">
+      <c r="B49" s="3">
+        <v>43</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>866</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" s="79" t="s">
         <v>867</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F49" s="4" t="s">
         <v>868</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="G49" s="4" t="s">
         <v>869</v>
       </c>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-    </row>
-    <row r="49" spans="2:11">
-      <c r="B49" s="3" t="s">
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+    </row>
+    <row r="50" spans="2:11">
+      <c r="B50" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E49" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="G49" s="4"/>
-      <c r="I49" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="K49" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11">
-      <c r="B50" s="3">
-        <v>60</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E50" s="32" t="s">
+      <c r="E50" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>196</v>
+        <v>153</v>
       </c>
       <c r="G50" s="4"/>
       <c r="I50" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>197</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="2:11">
       <c r="B51" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>99</v>
+        <v>195</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E51" s="18" t="s">
-        <v>79</v>
+        <v>56</v>
+      </c>
+      <c r="E51" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="G51" s="4"/>
       <c r="I51" s="4" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>110</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="2:11">
       <c r="B52" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>90</v>
+        <v>99</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>619</v>
+        <v>79</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>204</v>
+        <v>77</v>
       </c>
       <c r="G52" s="4"/>
       <c r="I52" s="4" t="s">
@@ -4759,101 +4770,101 @@
         <v>135</v>
       </c>
       <c r="K52" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11">
+      <c r="B53" s="3">
+        <v>62</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>619</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G53" s="4"/>
+      <c r="I53" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K53" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="53" spans="2:11" s="38" customFormat="1">
-      <c r="B53" s="35">
+    <row r="54" spans="2:11" s="38" customFormat="1">
+      <c r="B54" s="35">
         <v>63</v>
       </c>
-      <c r="C53" s="36" t="s">
+      <c r="C54" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="D53" s="36" t="s">
+      <c r="D54" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E53" s="37" t="s">
+      <c r="E54" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="F53" s="36" t="s">
+      <c r="F54" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="G53" s="36"/>
-      <c r="I53" s="36" t="s">
+      <c r="G54" s="36"/>
+      <c r="I54" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="J53" s="36" t="s">
+      <c r="J54" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="K53" s="36" t="s">
+      <c r="K54" s="36" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11">
-      <c r="B54" s="3">
-        <v>68</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="D54" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="E54" s="42" t="s">
-        <v>618</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="G54" s="4"/>
-      <c r="I54" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="J54" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="K54" s="4" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="55" spans="2:11">
       <c r="B55" s="3">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="D55" s="25"/>
-      <c r="E55" s="42"/>
+        <v>335</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E55" s="42" t="s">
+        <v>618</v>
+      </c>
       <c r="F55" s="4" t="s">
-        <v>406</v>
+        <v>336</v>
       </c>
       <c r="G55" s="4"/>
       <c r="I55" s="4" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>107</v>
+        <v>406</v>
       </c>
     </row>
     <row r="56" spans="2:11">
       <c r="B56" s="3">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E56" s="18" t="s">
-        <v>113</v>
-      </c>
+        <v>411</v>
+      </c>
+      <c r="D56" s="25"/>
+      <c r="E56" s="42"/>
       <c r="F56" s="4" t="s">
-        <v>114</v>
+        <v>406</v>
       </c>
       <c r="G56" s="4"/>
       <c r="I56" s="4" t="s">
@@ -4862,20 +4873,26 @@
       <c r="J56" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="K56" s="4"/>
+      <c r="K56" s="4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="57" spans="2:11">
       <c r="B57" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E57" s="18"/>
-      <c r="F57" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="G57" s="4"/>
       <c r="I57" s="4" t="s">
         <v>105</v>
@@ -4885,22 +4902,18 @@
       </c>
       <c r="K57" s="4"/>
     </row>
-    <row r="58" spans="2:11" ht="30">
+    <row r="58" spans="2:11">
       <c r="B58" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E58" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="F58" s="17" t="s">
-        <v>136</v>
-      </c>
+      <c r="E58" s="18"/>
+      <c r="F58" s="4"/>
       <c r="G58" s="4"/>
       <c r="I58" s="4" t="s">
         <v>105</v>
@@ -4908,25 +4921,23 @@
       <c r="J58" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="K58" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="59" spans="2:11">
+      <c r="K58" s="4"/>
+    </row>
+    <row r="59" spans="2:11" ht="30">
       <c r="B59" s="3">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>635</v>
-      </c>
-      <c r="E59" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>211</v>
+        <v>115</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="G59" s="4"/>
       <c r="I59" s="4" t="s">
@@ -4936,222 +4947,222 @@
         <v>106</v>
       </c>
       <c r="K59" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11">
+      <c r="B60" s="3">
+        <v>75</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>635</v>
+      </c>
+      <c r="E60" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G60" s="4"/>
+      <c r="I60" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="K60" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="60" spans="2:11">
-      <c r="B60" s="3"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="62"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-    </row>
     <row r="61" spans="2:11">
-      <c r="B61" s="3">
-        <v>81</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>625</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>634</v>
-      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
       <c r="E61" s="62"/>
-      <c r="F61" s="4" t="s">
-        <v>626</v>
-      </c>
+      <c r="F61" s="4"/>
       <c r="G61" s="4"/>
-      <c r="I61" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>212</v>
-      </c>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
     </row>
     <row r="62" spans="2:11">
       <c r="B62" s="3">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D62" s="17" t="s">
         <v>634</v>
       </c>
       <c r="E62" s="62"/>
       <c r="F62" s="4" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G62" s="4"/>
       <c r="I62" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11">
+      <c r="B63" s="3">
+        <v>82</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="E63" s="62"/>
+      <c r="F63" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="G63" s="4"/>
+      <c r="I63" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="J62" s="4" t="s">
+      <c r="J63" s="4" t="s">
         <v>630</v>
       </c>
-      <c r="K62" s="4" t="s">
+      <c r="K63" s="4" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="63" spans="2:11">
-      <c r="B63" s="3"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="62"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-    </row>
     <row r="64" spans="2:11">
-      <c r="B64" s="3">
-        <v>91</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>661</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>667</v>
-      </c>
-      <c r="E64" s="63"/>
-      <c r="F64" s="4" t="s">
-        <v>672</v>
-      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="62"/>
+      <c r="F64" s="4"/>
       <c r="G64" s="4"/>
-      <c r="I64" s="4" t="s">
-        <v>642</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>643</v>
-      </c>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
       <c r="K64" s="4"/>
     </row>
     <row r="65" spans="2:11">
       <c r="B65" s="3">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>663</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>668</v>
-      </c>
-      <c r="E65" s="63" t="s">
-        <v>669</v>
-      </c>
+        <v>661</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>667</v>
+      </c>
+      <c r="E65" s="63"/>
       <c r="F65" s="4" t="s">
-        <v>712</v>
+        <v>672</v>
       </c>
       <c r="G65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
+      <c r="I65" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>643</v>
+      </c>
       <c r="K65" s="4"/>
     </row>
     <row r="66" spans="2:11">
       <c r="B66" s="3">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>656</v>
-      </c>
-      <c r="E66" s="63"/>
+        <v>668</v>
+      </c>
+      <c r="E66" s="63" t="s">
+        <v>669</v>
+      </c>
       <c r="F66" s="4" t="s">
-        <v>713</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>711</v>
-      </c>
+        <v>712</v>
+      </c>
+      <c r="G66" s="4"/>
       <c r="I66" s="4"/>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
     </row>
     <row r="67" spans="2:11">
       <c r="B67" s="3">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>636</v>
+        <v>662</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="E67" s="63"/>
       <c r="F67" s="4" t="s">
-        <v>657</v>
-      </c>
-      <c r="G67" s="4"/>
+        <v>713</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>711</v>
+      </c>
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
     </row>
     <row r="68" spans="2:11">
-      <c r="B68" s="3"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="4"/>
+      <c r="B68" s="3">
+        <v>94</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="E68" s="63"/>
+      <c r="F68" s="4" t="s">
+        <v>657</v>
+      </c>
       <c r="G68" s="4"/>
       <c r="I68" s="4"/>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
     </row>
-    <row r="69" spans="2:11" s="38" customFormat="1">
-      <c r="B69" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="C69" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D69" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="E69" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="F69" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G69" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="I69" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="J69" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="K69" s="36" t="s">
-        <v>107</v>
-      </c>
+    <row r="69" spans="2:11">
+      <c r="B69" s="3"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
     </row>
     <row r="70" spans="2:11" s="38" customFormat="1">
       <c r="B70" s="35" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C70" s="36" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D70" s="36" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="E70" s="37" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F70" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="G70" s="36"/>
+        <v>83</v>
+      </c>
+      <c r="G70" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="I70" s="36" t="s">
         <v>105</v>
       </c>
@@ -5162,30 +5173,57 @@
         <v>107</v>
       </c>
     </row>
-    <row r="72" spans="2:11">
-      <c r="B72" s="3" t="s">
+    <row r="71" spans="2:11" s="38" customFormat="1">
+      <c r="B71" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D71" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E71" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="F71" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G71" s="36"/>
+      <c r="I71" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="J71" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="K71" s="36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11">
+      <c r="B73" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C73" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D73" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="E72" s="58" t="s">
+      <c r="E73" s="58" t="s">
         <v>521</v>
       </c>
-      <c r="F72" s="4" t="s">
+      <c r="F73" s="4" t="s">
         <v>611</v>
       </c>
-      <c r="G72" s="4"/>
-      <c r="I72" s="4" t="s">
+      <c r="G73" s="4"/>
+      <c r="I73" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="J72" s="4" t="s">
+      <c r="J73" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="K72" s="4" t="s">
+      <c r="K73" s="4" t="s">
         <v>612</v>
       </c>
     </row>
@@ -6032,7 +6070,7 @@
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="82" t="s">
+      <c r="E3" s="83" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="45"/>
@@ -6047,7 +6085,7 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="82"/>
+      <c r="E4" s="83"/>
       <c r="F4" s="45"/>
     </row>
     <row r="5" spans="2:9">
@@ -8234,7 +8272,7 @@
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="83" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8245,7 +8283,7 @@
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="82"/>
+      <c r="D5" s="83"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
@@ -8358,7 +8396,7 @@
       <c r="C17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="82" t="s">
+      <c r="D17" s="83" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8369,7 +8407,7 @@
       <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="82"/>
+      <c r="D18" s="83"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="5" t="s">
@@ -8619,7 +8657,7 @@
       <c r="C45" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="82" t="s">
+      <c r="D45" s="83" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8630,7 +8668,7 @@
       <c r="C46" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="82"/>
+      <c r="D46" s="83"/>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="5" t="s">
@@ -8795,7 +8833,7 @@
         <f>SUM(D$3:D3)</f>
         <v>1</v>
       </c>
-      <c r="F3" s="82" t="s">
+      <c r="F3" s="83" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="45"/>
@@ -8814,7 +8852,7 @@
         <f>SUM(D$3:D4)</f>
         <v>2</v>
       </c>
-      <c r="F4" s="82"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="45"/>
     </row>
     <row r="5" spans="2:7">
@@ -9861,7 +9899,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="83" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="47">
@@ -9918,7 +9956,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="82"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="47">
         <v>1</v>
       </c>
@@ -11494,7 +11532,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="83" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11505,7 +11543,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="82"/>
+      <c r="D4" s="83"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
@@ -11648,7 +11686,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="83" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11659,7 +11697,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="82"/>
+      <c r="D4" s="83"/>
     </row>
     <row r="5" spans="2:4" s="1" customFormat="1">
       <c r="B5" s="5" t="s">
@@ -11813,7 +11851,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="82" t="s">
+      <c r="D7" s="83" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11824,7 +11862,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="82"/>
+      <c r="D8" s="83"/>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="5" t="s">
@@ -12019,7 +12057,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="82" t="s">
+      <c r="D28" s="83" t="s">
         <v>3</v>
       </c>
     </row>
@@ -12030,7 +12068,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="82"/>
+      <c r="D29" s="83"/>
     </row>
     <row r="30" spans="1:4">
       <c r="B30" s="5" t="s">

</xml_diff>

<commit_message>
Enhance checking on config data to align with MyAlphaRobot, also prevent invalid config data due to users switching back to old firmware. New command (0x4E) to retrieve action status for external control
</commit_message>
<xml_diff>
--- a/info/Info.xlsx
+++ b/info/Info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1577" uniqueCount="881">
   <si>
     <t>Offset</t>
   </si>
@@ -2906,6 +2906,27 @@
   </si>
   <si>
     <t>A9 9A 05 37 16 00 00 52 ED</t>
+  </si>
+  <si>
+    <t>4E</t>
+  </si>
+  <si>
+    <t>A9 9A 02 4E 50 ED</t>
+  </si>
+  <si>
+    <t>Yes {12}</t>
+  </si>
+  <si>
+    <t>Yes {6}</t>
+  </si>
+  <si>
+    <t>{status}{comboId}{comboStep}{actionId}{actionPose}</t>
+  </si>
+  <si>
+    <t>Get Action Status (next pose)</t>
+  </si>
+  <si>
+    <t>Information returned is for next pose instead of current pose</t>
   </si>
 </sst>
 </file>
@@ -3036,7 +3057,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3259,6 +3280,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3569,13 +3593,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N73"/>
+  <dimension ref="B2:N74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4669,7 +4693,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="2:11">
+    <row r="49" spans="2:13">
       <c r="B49" s="3">
         <v>43</v>
       </c>
@@ -4692,102 +4716,105 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
     </row>
-    <row r="50" spans="2:11">
+    <row r="50" spans="2:13">
       <c r="B50" s="3" t="s">
-        <v>151</v>
+        <v>874</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>152</v>
+        <v>879</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E50" s="26" t="s">
+      <c r="E50" s="83" t="s">
         <v>45</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>153</v>
+        <v>875</v>
       </c>
       <c r="G50" s="4"/>
       <c r="I50" s="4" t="s">
-        <v>105</v>
+        <v>876</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>106</v>
+        <v>877</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11">
-      <c r="B51" s="3">
-        <v>60</v>
+        <v>878</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13">
+      <c r="B51" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E51" s="32" t="s">
+      <c r="E51" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>196</v>
+        <v>153</v>
       </c>
       <c r="G51" s="4"/>
       <c r="I51" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13">
       <c r="B52" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>99</v>
+        <v>195</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E52" s="18" t="s">
-        <v>79</v>
+        <v>56</v>
+      </c>
+      <c r="E52" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="G52" s="4"/>
       <c r="I52" s="4" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13">
       <c r="B53" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D53" s="25" t="s">
-        <v>90</v>
+        <v>99</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>619</v>
+        <v>79</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>204</v>
+        <v>77</v>
       </c>
       <c r="G53" s="4"/>
       <c r="I53" s="4" t="s">
@@ -4797,101 +4824,101 @@
         <v>135</v>
       </c>
       <c r="K53" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13">
+      <c r="B54" s="3">
+        <v>62</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>619</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G54" s="4"/>
+      <c r="I54" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K54" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="2:11" s="38" customFormat="1">
-      <c r="B54" s="35">
+    <row r="55" spans="2:13" s="38" customFormat="1">
+      <c r="B55" s="35">
         <v>63</v>
       </c>
-      <c r="C54" s="36" t="s">
+      <c r="C55" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="D54" s="36" t="s">
+      <c r="D55" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E54" s="37" t="s">
+      <c r="E55" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="F54" s="36" t="s">
+      <c r="F55" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="G54" s="36"/>
-      <c r="I54" s="36" t="s">
+      <c r="G55" s="36"/>
+      <c r="I55" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="J54" s="36" t="s">
+      <c r="J55" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="K54" s="36" t="s">
+      <c r="K55" s="36" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="2:11">
-      <c r="B55" s="3">
+    <row r="56" spans="2:13">
+      <c r="B56" s="3">
         <v>68</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C56" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="D55" s="25" t="s">
+      <c r="D56" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E55" s="42" t="s">
+      <c r="E56" s="42" t="s">
         <v>618</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F56" s="4" t="s">
         <v>336</v>
-      </c>
-      <c r="G55" s="4"/>
-      <c r="I55" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="J55" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="K55" s="4" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="56" spans="2:11">
-      <c r="B56" s="3">
-        <v>69</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="D56" s="25"/>
-      <c r="E56" s="42"/>
-      <c r="F56" s="4" t="s">
-        <v>406</v>
       </c>
       <c r="G56" s="4"/>
       <c r="I56" s="4" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="57" spans="2:11">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13">
       <c r="B57" s="3">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E57" s="18" t="s">
-        <v>113</v>
-      </c>
+        <v>411</v>
+      </c>
+      <c r="D57" s="25"/>
+      <c r="E57" s="42"/>
       <c r="F57" s="4" t="s">
-        <v>114</v>
+        <v>406</v>
       </c>
       <c r="G57" s="4"/>
       <c r="I57" s="4" t="s">
@@ -4900,20 +4927,26 @@
       <c r="J57" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="K57" s="4"/>
-    </row>
-    <row r="58" spans="2:11">
+      <c r="K57" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13">
       <c r="B58" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E58" s="18"/>
-      <c r="F58" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="G58" s="4"/>
       <c r="I58" s="4" t="s">
         <v>105</v>
@@ -4923,22 +4956,18 @@
       </c>
       <c r="K58" s="4"/>
     </row>
-    <row r="59" spans="2:11" ht="30">
+    <row r="59" spans="2:13">
       <c r="B59" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E59" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="F59" s="17" t="s">
-        <v>136</v>
-      </c>
+      <c r="E59" s="18"/>
+      <c r="F59" s="4"/>
       <c r="G59" s="4"/>
       <c r="I59" s="4" t="s">
         <v>105</v>
@@ -4946,25 +4975,23 @@
       <c r="J59" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="K59" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="60" spans="2:11">
+      <c r="K59" s="4"/>
+    </row>
+    <row r="60" spans="2:13" ht="30">
       <c r="B60" s="3">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>635</v>
-      </c>
-      <c r="E60" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>211</v>
+        <v>115</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="G60" s="4"/>
       <c r="I60" s="4" t="s">
@@ -4974,222 +5001,222 @@
         <v>106</v>
       </c>
       <c r="K60" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13">
+      <c r="B61" s="3">
+        <v>75</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>635</v>
+      </c>
+      <c r="E61" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G61" s="4"/>
+      <c r="I61" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="K61" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="61" spans="2:11">
-      <c r="B61" s="3"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="62"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-    </row>
-    <row r="62" spans="2:11">
-      <c r="B62" s="3">
+    <row r="62" spans="2:13">
+      <c r="B62" s="3"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="62"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+    </row>
+    <row r="63" spans="2:13">
+      <c r="B63" s="3">
         <v>81</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>625</v>
-      </c>
-      <c r="D62" s="17" t="s">
-        <v>634</v>
-      </c>
-      <c r="E62" s="62"/>
-      <c r="F62" s="4" t="s">
-        <v>626</v>
-      </c>
-      <c r="G62" s="4"/>
-      <c r="I62" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="63" spans="2:11">
-      <c r="B63" s="3">
-        <v>82</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>628</v>
       </c>
       <c r="D63" s="17" t="s">
         <v>634</v>
       </c>
       <c r="E63" s="62"/>
       <c r="F63" s="4" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G63" s="4"/>
       <c r="I63" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="K63" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13">
+      <c r="B64" s="3">
+        <v>82</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="E64" s="62"/>
+      <c r="F64" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="G64" s="4"/>
+      <c r="I64" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="J63" s="4" t="s">
+      <c r="J64" s="4" t="s">
         <v>630</v>
       </c>
-      <c r="K63" s="4" t="s">
+      <c r="K64" s="4" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="64" spans="2:11">
-      <c r="B64" s="3"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="62"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-    </row>
     <row r="65" spans="2:11">
-      <c r="B65" s="3">
-        <v>91</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>661</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>667</v>
-      </c>
-      <c r="E65" s="63"/>
-      <c r="F65" s="4" t="s">
-        <v>672</v>
-      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="62"/>
+      <c r="F65" s="4"/>
       <c r="G65" s="4"/>
-      <c r="I65" s="4" t="s">
-        <v>642</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>643</v>
-      </c>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
       <c r="K65" s="4"/>
     </row>
     <row r="66" spans="2:11">
       <c r="B66" s="3">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>663</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>668</v>
-      </c>
-      <c r="E66" s="63" t="s">
-        <v>669</v>
-      </c>
+        <v>661</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>667</v>
+      </c>
+      <c r="E66" s="63"/>
       <c r="F66" s="4" t="s">
-        <v>712</v>
+        <v>672</v>
       </c>
       <c r="G66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
+      <c r="I66" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>643</v>
+      </c>
       <c r="K66" s="4"/>
     </row>
     <row r="67" spans="2:11">
       <c r="B67" s="3">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>656</v>
-      </c>
-      <c r="E67" s="63"/>
+        <v>668</v>
+      </c>
+      <c r="E67" s="63" t="s">
+        <v>669</v>
+      </c>
       <c r="F67" s="4" t="s">
-        <v>713</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>711</v>
-      </c>
+        <v>712</v>
+      </c>
+      <c r="G67" s="4"/>
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
     </row>
     <row r="68" spans="2:11">
       <c r="B68" s="3">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>636</v>
+        <v>662</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="E68" s="63"/>
       <c r="F68" s="4" t="s">
-        <v>657</v>
-      </c>
-      <c r="G68" s="4"/>
+        <v>713</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>711</v>
+      </c>
       <c r="I68" s="4"/>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
     </row>
     <row r="69" spans="2:11">
-      <c r="B69" s="3"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="4"/>
+      <c r="B69" s="3">
+        <v>94</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="E69" s="63"/>
+      <c r="F69" s="4" t="s">
+        <v>657</v>
+      </c>
       <c r="G69" s="4"/>
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
     </row>
-    <row r="70" spans="2:11" s="38" customFormat="1">
-      <c r="B70" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="C70" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D70" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="E70" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="F70" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G70" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="I70" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="J70" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="K70" s="36" t="s">
-        <v>107</v>
-      </c>
+    <row r="70" spans="2:11">
+      <c r="B70" s="3"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
     </row>
     <row r="71" spans="2:11" s="38" customFormat="1">
       <c r="B71" s="35" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C71" s="36" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D71" s="36" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="E71" s="37" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F71" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="G71" s="36"/>
+        <v>83</v>
+      </c>
+      <c r="G71" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="I71" s="36" t="s">
         <v>105</v>
       </c>
@@ -5200,30 +5227,57 @@
         <v>107</v>
       </c>
     </row>
-    <row r="73" spans="2:11">
-      <c r="B73" s="3" t="s">
+    <row r="72" spans="2:11" s="38" customFormat="1">
+      <c r="B72" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D72" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E72" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="F72" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G72" s="36"/>
+      <c r="I72" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="J72" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="K72" s="36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11">
+      <c r="B74" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C74" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D74" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="E73" s="58" t="s">
+      <c r="E74" s="58" t="s">
         <v>521</v>
       </c>
-      <c r="F73" s="4" t="s">
+      <c r="F74" s="4" t="s">
         <v>611</v>
       </c>
-      <c r="G73" s="4"/>
-      <c r="I73" s="4" t="s">
+      <c r="G74" s="4"/>
+      <c r="I74" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="J73" s="4" t="s">
+      <c r="J74" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="K73" s="4" t="s">
+      <c r="K74" s="4" t="s">
         <v>612</v>
       </c>
     </row>
@@ -6070,7 +6124,7 @@
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="83" t="s">
+      <c r="E3" s="84" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="45"/>
@@ -6085,7 +6139,7 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="83"/>
+      <c r="E4" s="84"/>
       <c r="F4" s="45"/>
     </row>
     <row r="5" spans="2:9">
@@ -8272,7 +8326,7 @@
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="84" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8283,7 +8337,7 @@
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="83"/>
+      <c r="D5" s="84"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="5" t="s">
@@ -8396,7 +8450,7 @@
       <c r="C17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="84" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8407,7 +8461,7 @@
       <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="83"/>
+      <c r="D18" s="84"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="5" t="s">
@@ -8657,7 +8711,7 @@
       <c r="C45" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="83" t="s">
+      <c r="D45" s="84" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8668,7 +8722,7 @@
       <c r="C46" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="83"/>
+      <c r="D46" s="84"/>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="5" t="s">
@@ -8833,7 +8887,7 @@
         <f>SUM(D$3:D3)</f>
         <v>1</v>
       </c>
-      <c r="F3" s="83" t="s">
+      <c r="F3" s="84" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="45"/>
@@ -8852,7 +8906,7 @@
         <f>SUM(D$3:D4)</f>
         <v>2</v>
       </c>
-      <c r="F4" s="83"/>
+      <c r="F4" s="84"/>
       <c r="G4" s="45"/>
     </row>
     <row r="5" spans="2:7">
@@ -9899,7 +9953,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="84" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="47">
@@ -9956,7 +10010,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="84"/>
       <c r="E4" s="47">
         <v>1</v>
       </c>
@@ -11532,7 +11586,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="84" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11543,7 +11597,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="84"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="5" t="s">
@@ -11686,7 +11740,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="84" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11697,7 +11751,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="84"/>
     </row>
     <row r="5" spans="2:4" s="1" customFormat="1">
       <c r="B5" s="5" t="s">
@@ -11851,7 +11905,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="84" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11862,7 +11916,7 @@
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="83"/>
+      <c r="D8" s="84"/>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="5" t="s">
@@ -12057,7 +12111,7 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="83" t="s">
+      <c r="D28" s="84" t="s">
         <v>3</v>
       </c>
     </row>
@@ -12068,7 +12122,7 @@
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="83"/>
+      <c r="D29" s="84"/>
     </row>
     <row r="30" spans="1:4">
       <c r="B30" s="5" t="s">

</xml_diff>